<commit_message>
atualizei os dados da bibi e da add
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2540" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2544" uniqueCount="10">
   <si>
     <t>id_produto</t>
   </si>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2533"/>
+  <dimension ref="A1:H2537"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -520,22 +520,22 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2">
-        <v>45800.93197718772</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" s="2">
-        <v>45800.68631944444</v>
+        <v>45803.64980324074</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -952,16 +952,16 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D23" s="2">
-        <v>45799.89540331678</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E23">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F23" s="2">
-        <v>45799.61216435185</v>
+        <v>45803.61216435185</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -978,16 +978,16 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D24" s="2">
-        <v>45800.93197721101</v>
+        <v>45803.62109434994</v>
       </c>
       <c r="E24">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F24" s="2">
-        <v>45800.6955787037</v>
+        <v>45803.62967592593</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1194,22 +1194,22 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>1176</v>
+        <v>1072</v>
       </c>
       <c r="D33" s="2">
-        <v>45800.93197721101</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E33">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="F33" s="2">
-        <v>45800.6955787037</v>
+        <v>45803.49555555556</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="H33" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1589,22 +1589,22 @@
         <v>1</v>
       </c>
       <c r="C49">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D49" s="2">
-        <v>45800.93175380815</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E49">
         <v>110</v>
       </c>
       <c r="F49" s="2">
-        <v>45800.46056712963</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H49" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1765,22 +1765,22 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="D56" s="2">
-        <v>45800.93197721101</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E56">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="F56" s="2">
-        <v>45800.6955787037</v>
+        <v>45803.5318287037</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1817,22 +1817,22 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D58" s="2">
-        <v>45800.93197721101</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E58">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F58" s="2">
-        <v>45800.6955787037</v>
+        <v>45803.5318287037</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H58" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1843,16 +1843,16 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D59" s="2">
-        <v>45800.93175380815</v>
+        <v>45803.62109434994</v>
       </c>
       <c r="E59">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F59" s="2">
-        <v>45800.46056712963</v>
+        <v>45803.62967592593</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2114,22 +2114,22 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D70" s="2">
-        <v>45800.93175380815</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E70">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F70" s="2">
-        <v>45800.46056712963</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H70" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2140,16 +2140,16 @@
         <v>1</v>
       </c>
       <c r="C71">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D71" s="2">
-        <v>45799.89540330523</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E71">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F71" s="2">
-        <v>45799.53100694445</v>
+        <v>45803.38153935185</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -2376,22 +2376,22 @@
         <v>1</v>
       </c>
       <c r="C81">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D81" s="2">
-        <v>45799.89534674662</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E81">
         <v>57</v>
       </c>
       <c r="F81" s="2">
-        <v>45796.76049768519</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H81" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2402,10 +2402,10 @@
         <v>1</v>
       </c>
       <c r="C82">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D82" s="2">
-        <v>45798.96533509644</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E82">
         <v>18</v>
@@ -2414,10 +2414,10 @@
         <v>45798.43265046296</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2428,16 +2428,16 @@
         <v>1</v>
       </c>
       <c r="C83">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D83" s="2">
-        <v>45800.93201925102</v>
+        <v>45803.62109434994</v>
       </c>
       <c r="E83">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F83" s="2">
-        <v>45800.75802083333</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -2477,16 +2477,16 @@
         <v>1</v>
       </c>
       <c r="C85">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D85" s="2">
-        <v>45800.93201925102</v>
+        <v>45803.62109434994</v>
       </c>
       <c r="E85">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F85" s="2">
-        <v>45800.75802083333</v>
+        <v>45803.62967592593</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -2503,22 +2503,22 @@
         <v>1</v>
       </c>
       <c r="C86">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D86" s="2">
-        <v>45800.93184391336</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E86">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F86" s="2">
-        <v>45800.50141203704</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H86" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2529,10 +2529,10 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D87" s="2">
-        <v>45800.93197721101</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E87">
         <v>15</v>
@@ -2541,10 +2541,10 @@
         <v>45800.6955787037</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H87" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2630,22 +2630,22 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D91" s="2">
-        <v>45800.93201925102</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E91">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F91" s="2">
-        <v>45800.75802083333</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H91" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2702,22 +2702,22 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D94" s="2">
-        <v>45800.93175383128</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E94">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F94" s="2">
-        <v>45800.47983796296</v>
+        <v>45803.62967592593</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H94" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2751,10 +2751,10 @@
         <v>1</v>
       </c>
       <c r="C96">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D96" s="2">
-        <v>45799.89532166889</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E96">
         <v>51</v>
@@ -2763,10 +2763,10 @@
         <v>45791.69931712963</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H96" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2800,16 +2800,16 @@
         <v>1</v>
       </c>
       <c r="C98">
-        <v>257</v>
+        <v>157</v>
       </c>
       <c r="D98" s="2">
-        <v>45799.89534673509</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E98">
-        <v>257</v>
+        <v>157</v>
       </c>
       <c r="F98" s="2">
-        <v>45793.60246527778</v>
+        <v>45803.48216435185</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -2872,22 +2872,22 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>2143</v>
+        <v>1856</v>
       </c>
       <c r="D101" s="2">
-        <v>45800.93201925102</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E101">
-        <v>2143</v>
+        <v>2123</v>
       </c>
       <c r="F101" s="2">
-        <v>45800.75802083333</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>267</v>
       </c>
       <c r="H101" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -2921,10 +2921,10 @@
         <v>1</v>
       </c>
       <c r="C103">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D103" s="2">
-        <v>45799.89542739857</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E103">
         <v>40</v>
@@ -2933,10 +2933,10 @@
         <v>45793.38017361111</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H103" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -2993,10 +2993,10 @@
         <v>1</v>
       </c>
       <c r="C106">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D106" s="2">
-        <v>45799.895427387</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E106">
         <v>7</v>
@@ -3005,10 +3005,10 @@
         <v>45799.64056712963</v>
       </c>
       <c r="G106">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H106" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3258,16 +3258,16 @@
         <v>1</v>
       </c>
       <c r="C117">
-        <v>770</v>
+        <v>1202</v>
       </c>
       <c r="D117" s="2">
-        <v>45800.93172920593</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E117">
-        <v>770</v>
+        <v>1202</v>
       </c>
       <c r="F117" s="2">
-        <v>45800.40415509259</v>
+        <v>45802.99459490741</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -3333,10 +3333,10 @@
         <v>1</v>
       </c>
       <c r="C120">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D120" s="2">
-        <v>45799.89534674662</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E120">
         <v>89</v>
@@ -3345,10 +3345,10 @@
         <v>45796.72284722222</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H120" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -3368,7 +3368,7 @@
         <v>52</v>
       </c>
       <c r="F121" s="2">
-        <v>45800.6955787037</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -3408,22 +3408,22 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D123" s="2">
-        <v>45799.895427387</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E123">
         <v>99</v>
       </c>
       <c r="F123" s="2">
-        <v>45799.64056712963</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G123">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H123" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -3846,10 +3846,10 @@
         <v>1</v>
       </c>
       <c r="C141">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="D141" s="2">
-        <v>45799.89540331678</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E141">
         <v>622</v>
@@ -3858,10 +3858,10 @@
         <v>45800.50141203704</v>
       </c>
       <c r="G141">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H141" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -4074,10 +4074,10 @@
         <v>1</v>
       </c>
       <c r="C150">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D150" s="2">
-        <v>45799.89534672352</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E150">
         <v>14</v>
@@ -4086,10 +4086,10 @@
         <v>45792.73215277777</v>
       </c>
       <c r="G150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H150" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -4936,10 +4936,10 @@
         <v>1</v>
       </c>
       <c r="C185">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D185" s="2">
-        <v>45799.89540330523</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E185">
         <v>94</v>
@@ -4948,10 +4948,10 @@
         <v>45799.54621527778</v>
       </c>
       <c r="G185">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H185" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5077,22 +5077,22 @@
         <v>1</v>
       </c>
       <c r="C191">
-        <v>-133</v>
+        <v>257</v>
       </c>
       <c r="D191" s="2">
-        <v>45799.89540330523</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E191">
-        <v>-133</v>
+        <v>267</v>
       </c>
       <c r="F191" s="2">
-        <v>45799.54621527778</v>
+        <v>45802.99361111111</v>
       </c>
       <c r="G191">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H191" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -5112,7 +5112,7 @@
         <v>34</v>
       </c>
       <c r="F192" s="2">
-        <v>45793.40247685185</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G192">
         <v>0</v>
@@ -5449,10 +5449,10 @@
         <v>1</v>
       </c>
       <c r="C206">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D206" s="2">
-        <v>45799.89534672352</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E206">
         <v>10</v>
@@ -5461,10 +5461,10 @@
         <v>45792.73215277777</v>
       </c>
       <c r="G206">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H206" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -5521,16 +5521,16 @@
         <v>1</v>
       </c>
       <c r="C209">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D209" s="2">
-        <v>45799.89532166889</v>
+        <v>45803.62109434994</v>
       </c>
       <c r="E209">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F209" s="2">
-        <v>45791.54950231482</v>
+        <v>45803.62967592593</v>
       </c>
       <c r="G209">
         <v>0</v>
@@ -5711,10 +5711,10 @@
         <v>1</v>
       </c>
       <c r="C217">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D217" s="2">
-        <v>45798.96533509644</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E217">
         <v>128</v>
@@ -5723,10 +5723,10 @@
         <v>45798.62037037037</v>
       </c>
       <c r="G217">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H217" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -5737,10 +5737,10 @@
         <v>1</v>
       </c>
       <c r="C218">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D218" s="2">
-        <v>45799.89534673509</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E218">
         <v>97</v>
@@ -5749,10 +5749,10 @@
         <v>45793.71568287037</v>
       </c>
       <c r="G218">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H218" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -6175,10 +6175,10 @@
         <v>1</v>
       </c>
       <c r="C236">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D236" s="2">
-        <v>45800.93201925102</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E236">
         <v>64</v>
@@ -6187,10 +6187,10 @@
         <v>45800.75763888889</v>
       </c>
       <c r="G236">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H236" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -6627,22 +6627,22 @@
         <v>1</v>
       </c>
       <c r="C255">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D255" s="2">
-        <v>45799.89540331678</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E255">
         <v>133</v>
       </c>
       <c r="F255" s="2">
-        <v>45799.63390046296</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G255">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H255" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -6996,22 +6996,22 @@
         <v>1</v>
       </c>
       <c r="C270">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="D270" s="2">
-        <v>45800.93175380815</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E270">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F270" s="2">
-        <v>45800.46056712963</v>
+        <v>45803.53376157407</v>
       </c>
       <c r="G270">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H270" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="271" spans="1:8">
@@ -7045,16 +7045,16 @@
         <v>1</v>
       </c>
       <c r="C272">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D272" s="2">
-        <v>45799.895451121</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E272">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F272" s="2">
-        <v>45799.64041666667</v>
+        <v>45803.50018518518</v>
       </c>
       <c r="G272">
         <v>0</v>
@@ -7310,10 +7310,10 @@
         <v>1</v>
       </c>
       <c r="C283">
-        <v>7</v>
+        <v>-13</v>
       </c>
       <c r="D283" s="2">
-        <v>45800.93175383128</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E283">
         <v>7</v>
@@ -7322,10 +7322,10 @@
         <v>45800.47983796296</v>
       </c>
       <c r="G283">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H283" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="284" spans="1:8">
@@ -7408,22 +7408,22 @@
         <v>1</v>
       </c>
       <c r="C287">
-        <v>855</v>
+        <v>824</v>
       </c>
       <c r="D287" s="2">
-        <v>45800.93204011993</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E287">
-        <v>855</v>
+        <v>837</v>
       </c>
       <c r="F287" s="2">
-        <v>45800.76359953704</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G287">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H287" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="288" spans="1:8">
@@ -7535,16 +7535,16 @@
         <v>1</v>
       </c>
       <c r="C292">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D292" s="2">
-        <v>45799.895427387</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E292">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F292" s="2">
-        <v>45799.64056712963</v>
+        <v>45803.38153935185</v>
       </c>
       <c r="G292">
         <v>0</v>
@@ -7619,7 +7619,7 @@
         <v>62</v>
       </c>
       <c r="F295" s="2">
-        <v>45800.686875</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G295">
         <v>0</v>
@@ -7887,7 +7887,7 @@
         <v>1</v>
       </c>
       <c r="F306" s="2">
-        <v>45799.62475694445</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G306">
         <v>0</v>
@@ -7953,22 +7953,22 @@
         <v>1</v>
       </c>
       <c r="C309">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="D309" s="2">
-        <v>45799.89534674662</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E309">
         <v>1241</v>
       </c>
       <c r="F309" s="2">
-        <v>45796.61327546297</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G309">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H309" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="310" spans="1:8">
@@ -8071,16 +8071,16 @@
         <v>1</v>
       </c>
       <c r="C314">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D314" s="2">
-        <v>45800.93194931293</v>
+        <v>45803.62109434994</v>
       </c>
       <c r="E314">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F314" s="2">
-        <v>45800.68569444444</v>
+        <v>45803.64980324074</v>
       </c>
       <c r="G314">
         <v>0</v>
@@ -8097,16 +8097,16 @@
         <v>1</v>
       </c>
       <c r="C315">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D315" s="2">
-        <v>45799.89540331678</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E315">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F315" s="2">
-        <v>45799.63390046296</v>
+        <v>45803.50018518518</v>
       </c>
       <c r="G315">
         <v>0</v>
@@ -8178,7 +8178,7 @@
         <v>-5</v>
       </c>
       <c r="F318" s="2">
-        <v>45800.76359953704</v>
+        <v>45803.61013888889</v>
       </c>
       <c r="G318">
         <v>0</v>
@@ -8195,22 +8195,22 @@
         <v>1</v>
       </c>
       <c r="C319">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D319" s="2">
-        <v>45799.8954032937</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E319">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F319" s="2">
-        <v>45799.40421296296</v>
+        <v>45803.61216435185</v>
       </c>
       <c r="G319">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H319" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="320" spans="1:8">
@@ -8374,10 +8374,10 @@
         <v>1</v>
       </c>
       <c r="C326">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D326" s="2">
-        <v>45799.89534674662</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E326">
         <v>18</v>
@@ -8386,10 +8386,10 @@
         <v>45796.65443287037</v>
       </c>
       <c r="G326">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H326" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="327" spans="1:8">
@@ -8870,10 +8870,10 @@
         <v>1</v>
       </c>
       <c r="C346">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D346" s="2">
-        <v>45800.93197722271</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E346">
         <v>106</v>
@@ -8882,10 +8882,10 @@
         <v>45800.40415509259</v>
       </c>
       <c r="G346">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H346" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="347" spans="1:8">
@@ -9066,10 +9066,10 @@
         <v>1</v>
       </c>
       <c r="C354">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D354" s="2">
-        <v>45798.96533509644</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E354">
         <v>29</v>
@@ -9078,10 +9078,10 @@
         <v>45798.62037037037</v>
       </c>
       <c r="G354">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H354" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="355" spans="1:8">
@@ -9164,10 +9164,10 @@
         <v>1</v>
       </c>
       <c r="C358">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D358" s="2">
-        <v>45800.93194931293</v>
+        <v>45803.90694023441</v>
       </c>
       <c r="E358">
         <v>34</v>
@@ -9176,10 +9176,10 @@
         <v>45800.68569444444</v>
       </c>
       <c r="G358">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H358" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="359" spans="1:8">
@@ -9242,16 +9242,16 @@
         <v>1</v>
       </c>
       <c r="C361">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D361" s="2">
-        <v>45800.93197718772</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E361">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="F361" s="2">
-        <v>45800.68631944444</v>
+        <v>45803.57027777778</v>
       </c>
       <c r="G361">
         <v>0</v>
@@ -9291,22 +9291,22 @@
         <v>1</v>
       </c>
       <c r="C363">
-        <v>907</v>
+        <v>900</v>
       </c>
       <c r="D363" s="2">
-        <v>45800.93197718772</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E363">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="F363" s="2">
-        <v>45800.6859837963</v>
+        <v>45803.62967592593</v>
       </c>
       <c r="G363">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H363" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="364" spans="1:8">
@@ -9978,7 +9978,7 @@
         <v>29</v>
       </c>
       <c r="F390" s="2">
-        <v>45800.686875</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G390">
         <v>0</v>
@@ -10070,22 +10070,22 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="D394" s="2">
-        <v>45800.93175380815</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E394">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="F394" s="2">
-        <v>45800.46056712963</v>
+        <v>45803.50018518518</v>
       </c>
       <c r="G394">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H394" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="395" spans="1:8">
@@ -10278,7 +10278,7 @@
         <v>212</v>
       </c>
       <c r="F402" s="2">
-        <v>45797.76128472222</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G402">
         <v>0</v>
@@ -10321,16 +10321,16 @@
         <v>1</v>
       </c>
       <c r="C404">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="D404" s="2">
-        <v>45800.93172920593</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E404">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="F404" s="2">
-        <v>45800.40415509259</v>
+        <v>45803.61216435185</v>
       </c>
       <c r="G404">
         <v>0</v>
@@ -10419,16 +10419,16 @@
         <v>1</v>
       </c>
       <c r="C408">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D408" s="2">
-        <v>45798.96533509644</v>
+        <v>45803.62109434994</v>
       </c>
       <c r="E408">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F408" s="2">
-        <v>45798.44859953703</v>
+        <v>45803.62967592593</v>
       </c>
       <c r="G408">
         <v>0</v>
@@ -10673,10 +10673,10 @@
         <v>1</v>
       </c>
       <c r="C418">
-        <v>350</v>
+        <v>310</v>
       </c>
       <c r="D418" s="2">
-        <v>45799.895427387</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E418">
         <v>350</v>
@@ -10685,10 +10685,10 @@
         <v>45799.64056712963</v>
       </c>
       <c r="G418">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H418" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="419" spans="1:8">
@@ -11728,16 +11728,16 @@
         <v>1</v>
       </c>
       <c r="C461">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D461" s="2">
-        <v>45800.93197718772</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E461">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F461" s="2">
-        <v>45800.686875</v>
+        <v>45803.41005787037</v>
       </c>
       <c r="G461">
         <v>0</v>
@@ -11780,16 +11780,16 @@
         <v>1</v>
       </c>
       <c r="C463">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D463" s="2">
-        <v>45795.04204563411</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E463">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F463" s="2">
-        <v>45749.77075231481</v>
+        <v>45803.41005787037</v>
       </c>
       <c r="G463">
         <v>0</v>
@@ -12207,22 +12207,22 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D480" s="2">
-        <v>45800.93188815672</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E480">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F480" s="2">
-        <v>45800.62752314815</v>
+        <v>45803.38509259259</v>
       </c>
       <c r="G480">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H480" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="481" spans="1:8">
@@ -12951,22 +12951,22 @@
         <v>1</v>
       </c>
       <c r="C510">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="D510" s="2">
-        <v>45800.93197718772</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E510">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="F510" s="2">
-        <v>45800.686875</v>
+        <v>45803.50018518518</v>
       </c>
       <c r="G510">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H510" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="511" spans="1:8">
@@ -13669,10 +13669,10 @@
         <v>1</v>
       </c>
       <c r="C539">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="D539" s="2">
-        <v>45799.89528859723</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E539">
         <v>107</v>
@@ -13681,10 +13681,10 @@
         <v>45784.73082175926</v>
       </c>
       <c r="G539">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H539" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="540" spans="1:8">
@@ -14415,16 +14415,16 @@
         <v>1</v>
       </c>
       <c r="C570">
-        <v>2761</v>
+        <v>2760</v>
       </c>
       <c r="D570" s="2">
-        <v>45800.93172920593</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E570">
-        <v>2761</v>
+        <v>2760</v>
       </c>
       <c r="F570" s="2">
-        <v>45800.40415509259</v>
+        <v>45803.49555555556</v>
       </c>
       <c r="G570">
         <v>0</v>
@@ -14536,16 +14536,16 @@
         <v>1</v>
       </c>
       <c r="C575">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D575" s="2">
-        <v>45799.8954032937</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E575">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F575" s="2">
-        <v>45799.40591435185</v>
+        <v>45803.49555555556</v>
       </c>
       <c r="G575">
         <v>0</v>
@@ -15878,22 +15878,22 @@
         <v>1</v>
       </c>
       <c r="C631">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D631" s="2">
-        <v>45799.89540330523</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E631">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F631" s="2">
-        <v>45799.54766203704</v>
+        <v>45803.38153935185</v>
       </c>
       <c r="G631">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H631" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="632" spans="1:8">
@@ -15956,10 +15956,10 @@
         <v>1</v>
       </c>
       <c r="C634">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D634" s="2">
-        <v>45799.895427387</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E634">
         <v>23</v>
@@ -15968,10 +15968,10 @@
         <v>45799.64056712963</v>
       </c>
       <c r="G634">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H634" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="635" spans="1:8">
@@ -16535,10 +16535,10 @@
         <v>1</v>
       </c>
       <c r="C658">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D658" s="2">
-        <v>45799.89542739857</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E658">
         <v>40</v>
@@ -16547,10 +16547,10 @@
         <v>45793.37982638889</v>
       </c>
       <c r="G658">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H658" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="659" spans="1:8">
@@ -17094,16 +17094,16 @@
         <v>1</v>
       </c>
       <c r="C681">
-        <v>-1</v>
+        <v>-8</v>
       </c>
       <c r="D681" s="2">
-        <v>45800.93188815672</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E681">
-        <v>-1</v>
+        <v>-8</v>
       </c>
       <c r="F681" s="2">
-        <v>45800.62752314815</v>
+        <v>45803.49592592593</v>
       </c>
       <c r="G681">
         <v>0</v>
@@ -17195,10 +17195,10 @@
         <v>1</v>
       </c>
       <c r="C685">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D685" s="2">
-        <v>45800.93204010786</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E685">
         <v>15</v>
@@ -17207,10 +17207,10 @@
         <v>45800.40415509259</v>
       </c>
       <c r="G685">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H685" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="686" spans="1:8">
@@ -17342,10 +17342,10 @@
         <v>1</v>
       </c>
       <c r="C691">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="D691" s="2">
-        <v>45799.89534674662</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E691">
         <v>377</v>
@@ -17354,10 +17354,10 @@
         <v>45796.65443287037</v>
       </c>
       <c r="G691">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H691" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="692" spans="1:8">
@@ -17599,16 +17599,16 @@
         <v>1</v>
       </c>
       <c r="C701">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D701" s="2">
-        <v>45799.89540331678</v>
+        <v>45803.62109434994</v>
       </c>
       <c r="E701">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F701" s="2">
-        <v>45799.63390046296</v>
+        <v>45803.62967592593</v>
       </c>
       <c r="G701">
         <v>0</v>
@@ -17968,16 +17968,16 @@
         <v>1</v>
       </c>
       <c r="C716">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D716" s="2">
-        <v>45798.96533509644</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E716">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F716" s="2">
-        <v>45798.44859953703</v>
+        <v>45803.61216435185</v>
       </c>
       <c r="G716">
         <v>0</v>
@@ -18072,22 +18072,22 @@
         <v>1</v>
       </c>
       <c r="C720">
-        <v>793</v>
+        <v>775</v>
       </c>
       <c r="D720" s="2">
-        <v>45800.93175383128</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E720">
-        <v>793</v>
+        <v>786</v>
       </c>
       <c r="F720" s="2">
-        <v>45800.47983796296</v>
+        <v>45803.49555555556</v>
       </c>
       <c r="G720">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H720" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="721" spans="1:8">
@@ -18303,16 +18303,16 @@
         <v>1</v>
       </c>
       <c r="C729">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="D729" s="2">
-        <v>45799.895427387</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E729">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="F729" s="2">
-        <v>45799.67204861111</v>
+        <v>45803.52103009259</v>
       </c>
       <c r="G729">
         <v>0</v>
@@ -18381,10 +18381,10 @@
         <v>1</v>
       </c>
       <c r="C732">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D732" s="2">
-        <v>45800.93188815672</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E732">
         <v>444</v>
@@ -18393,10 +18393,10 @@
         <v>45800.62752314815</v>
       </c>
       <c r="G732">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H732" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="733" spans="1:8">
@@ -19154,16 +19154,16 @@
         <v>1</v>
       </c>
       <c r="C763">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="D763" s="2">
-        <v>45799.89534673509</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E763">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="F763" s="2">
-        <v>45796.43142361111</v>
+        <v>45803.40251157407</v>
       </c>
       <c r="G763">
         <v>0</v>
@@ -19241,7 +19241,7 @@
         <v>7</v>
       </c>
       <c r="F766" s="2">
-        <v>45796.49008101852</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G766">
         <v>0</v>
@@ -19379,16 +19379,16 @@
         <v>1</v>
       </c>
       <c r="C772">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="D772" s="2">
-        <v>45800.93197718772</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E772">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="F772" s="2">
-        <v>45800.6859837963</v>
+        <v>45803.57027777778</v>
       </c>
       <c r="G772">
         <v>0</v>
@@ -19483,10 +19483,10 @@
         <v>1</v>
       </c>
       <c r="C776">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="D776" s="2">
-        <v>45800.93188815672</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E776">
         <v>78</v>
@@ -19495,10 +19495,10 @@
         <v>45800.62752314815</v>
       </c>
       <c r="G776">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="H776" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="777" spans="1:8">
@@ -19979,10 +19979,10 @@
         <v>1</v>
       </c>
       <c r="C796">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D796" s="2">
-        <v>45799.89536723674</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E796">
         <v>16</v>
@@ -19991,10 +19991,10 @@
         <v>45797.63394675926</v>
       </c>
       <c r="G796">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H796" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="797" spans="1:8">
@@ -20409,16 +20409,16 @@
         <v>1</v>
       </c>
       <c r="C813">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D813" s="2">
-        <v>45799.89542737551</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E813">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F813" s="2">
-        <v>45799.6352662037</v>
+        <v>45803.54020833333</v>
       </c>
       <c r="G813">
         <v>0</v>
@@ -20732,22 +20732,22 @@
         <v>1</v>
       </c>
       <c r="C826">
-        <v>93</v>
+        <v>152</v>
       </c>
       <c r="D826" s="2">
-        <v>45800.93197718772</v>
+        <v>45803.90694023441</v>
       </c>
       <c r="E826">
-        <v>93</v>
+        <v>153</v>
       </c>
       <c r="F826" s="2">
-        <v>45800.686875</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G826">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H826" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="827" spans="1:8">
@@ -21164,16 +21164,16 @@
         <v>1</v>
       </c>
       <c r="C844">
-        <v>-5</v>
+        <v>31</v>
       </c>
       <c r="D844" s="2">
-        <v>45800.93204010786</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E844">
-        <v>-5</v>
+        <v>31</v>
       </c>
       <c r="F844" s="2">
-        <v>45800.75802083333</v>
+        <v>45802.99417824074</v>
       </c>
       <c r="G844">
         <v>0</v>
@@ -21337,10 +21337,10 @@
         <v>1</v>
       </c>
       <c r="C851">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D851" s="2">
-        <v>45799.89532168047</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E851">
         <v>14</v>
@@ -21349,10 +21349,10 @@
         <v>45791.75405092593</v>
       </c>
       <c r="G851">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H851" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="852" spans="1:8">
@@ -21389,22 +21389,22 @@
         <v>1</v>
       </c>
       <c r="C853">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="D853" s="2">
-        <v>45800.93179064643</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E853">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="F853" s="2">
-        <v>45800.48438657408</v>
+        <v>45803.38509259259</v>
       </c>
       <c r="G853">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H853" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="854" spans="1:8">
@@ -21868,22 +21868,22 @@
         <v>1</v>
       </c>
       <c r="C872">
-        <v>760</v>
+        <v>718</v>
       </c>
       <c r="D872" s="2">
-        <v>45800.93197718772</v>
+        <v>45803.90694023441</v>
       </c>
       <c r="E872">
-        <v>760</v>
+        <v>748</v>
       </c>
       <c r="F872" s="2">
-        <v>45800.6859837963</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G872">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H872" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="873" spans="1:8">
@@ -22145,22 +22145,22 @@
         <v>1</v>
       </c>
       <c r="C883">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="D883" s="2">
-        <v>45800.93188815672</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E883">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="F883" s="2">
-        <v>45800.62752314815</v>
+        <v>45803.62967592593</v>
       </c>
       <c r="G883">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H883" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="884" spans="1:8">
@@ -22272,16 +22272,16 @@
         <v>1</v>
       </c>
       <c r="C888">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="D888" s="2">
-        <v>45800.93197719934</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E888">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="F888" s="2">
-        <v>45800.686875</v>
+        <v>45803.57027777778</v>
       </c>
       <c r="G888">
         <v>0</v>
@@ -23187,22 +23187,22 @@
         <v>1</v>
       </c>
       <c r="C924">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D924" s="2">
-        <v>45800.93179064643</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E924">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F924" s="2">
-        <v>45800.48438657408</v>
+        <v>45803.50018518518</v>
       </c>
       <c r="G924">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H924" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="925" spans="1:8">
@@ -23539,10 +23539,10 @@
         <v>1</v>
       </c>
       <c r="C938">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D938" s="2">
-        <v>45799.89534674662</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E938">
         <v>23</v>
@@ -23551,10 +23551,10 @@
         <v>45796.65907407407</v>
       </c>
       <c r="G938">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H938" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="939" spans="1:8">
@@ -24136,22 +24136,22 @@
         <v>1</v>
       </c>
       <c r="C962">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="D962" s="2">
-        <v>45800.93175383128</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E962">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F962" s="2">
-        <v>45800.47983796296</v>
+        <v>45803.38509259259</v>
       </c>
       <c r="G962">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H962" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="963" spans="1:8">
@@ -24162,10 +24162,10 @@
         <v>1</v>
       </c>
       <c r="C963">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="D963" s="2">
-        <v>45798.96533511975</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E963">
         <v>919</v>
@@ -24174,10 +24174,10 @@
         <v>45798.64541666667</v>
       </c>
       <c r="G963">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H963" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="964" spans="1:8">
@@ -25155,16 +25155,16 @@
         <v>1</v>
       </c>
       <c r="C1002">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D1002" s="2">
-        <v>45799.89534674662</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E1002">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F1002" s="2">
-        <v>45796.63792824074</v>
+        <v>45803.38153935185</v>
       </c>
       <c r="G1002">
         <v>0</v>
@@ -25533,16 +25533,16 @@
         <v>1</v>
       </c>
       <c r="C1017">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="D1017" s="2">
-        <v>45800.93197719934</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E1017">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="F1017" s="2">
-        <v>45800.686875</v>
+        <v>45803.57027777778</v>
       </c>
       <c r="G1017">
         <v>0</v>
@@ -26676,22 +26676,22 @@
         <v>1</v>
       </c>
       <c r="C1062">
-        <v>845</v>
+        <v>804</v>
       </c>
       <c r="D1062" s="2">
-        <v>45800.93197718772</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E1062">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="F1062" s="2">
-        <v>45800.68569444444</v>
+        <v>45803.41005787037</v>
       </c>
       <c r="G1062">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="H1062" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1063" spans="1:8">
@@ -27867,10 +27867,10 @@
         <v>1</v>
       </c>
       <c r="C1110">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D1110" s="2">
-        <v>45799.89542737551</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E1110">
         <v>193</v>
@@ -27879,10 +27879,10 @@
         <v>45799.64041666667</v>
       </c>
       <c r="G1110">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H1110" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1111" spans="1:8">
@@ -29120,7 +29120,7 @@
         <v>2</v>
       </c>
       <c r="D1159" s="2">
-        <v>45795.0420164208</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E1159">
         <v>2</v>
@@ -29573,16 +29573,16 @@
         <v>1</v>
       </c>
       <c r="C1177">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D1177" s="2">
-        <v>45798.9653592312</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E1177">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="F1177" s="2">
-        <v>45798.71837962963</v>
+        <v>45803.51891203703</v>
       </c>
       <c r="G1177">
         <v>0</v>
@@ -31372,10 +31372,10 @@
         <v>1</v>
       </c>
       <c r="C1247">
-        <v>4</v>
+        <v>-18</v>
       </c>
       <c r="D1247" s="2">
-        <v>45799.89534674662</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E1247">
         <v>4</v>
@@ -31384,10 +31384,10 @@
         <v>45796.72284722222</v>
       </c>
       <c r="G1247">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H1247" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1248" spans="1:8">
@@ -31450,10 +31450,10 @@
         <v>1</v>
       </c>
       <c r="C1250">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D1250" s="2">
-        <v>45795.04210567895</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E1250">
         <v>200</v>
@@ -31462,10 +31462,10 @@
         <v>45776.51189814815</v>
       </c>
       <c r="G1250">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H1250" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1251" spans="1:8">
@@ -31528,22 +31528,22 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>751</v>
+        <v>695</v>
       </c>
       <c r="D1253" s="2">
-        <v>45800.93184391336</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E1253">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="F1253" s="2">
-        <v>45800.50141203704</v>
+        <v>45803.49555555556</v>
       </c>
       <c r="G1253">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="H1253" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1254" spans="1:8">
@@ -31733,16 +31733,16 @@
         <v>1</v>
       </c>
       <c r="C1261">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D1261" s="2">
-        <v>45800.93204011993</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E1261">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="F1261" s="2">
-        <v>45800.76021990741</v>
+        <v>45803.52199074074</v>
       </c>
       <c r="G1261">
         <v>0</v>
@@ -31837,16 +31837,16 @@
         <v>1</v>
       </c>
       <c r="C1265">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="D1265" s="2">
-        <v>45800.93175380815</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E1265">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F1265" s="2">
-        <v>45800.46056712963</v>
+        <v>45803.53497685185</v>
       </c>
       <c r="G1265">
         <v>0</v>
@@ -33791,22 +33791,22 @@
         <v>1</v>
       </c>
       <c r="C1342">
-        <v>1781</v>
+        <v>1619</v>
       </c>
       <c r="D1342" s="2">
-        <v>45800.9318881683</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E1342">
-        <v>1781</v>
+        <v>1771</v>
       </c>
       <c r="F1342" s="2">
-        <v>45800.63335648148</v>
+        <v>45803.50018518518</v>
       </c>
       <c r="G1342">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="H1342" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1343" spans="1:8">
@@ -34963,16 +34963,16 @@
         <v>1</v>
       </c>
       <c r="C1388">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="D1388" s="2">
-        <v>45800.93175380815</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E1388">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="F1388" s="2">
-        <v>45800.46056712963</v>
+        <v>45803.50018518518</v>
       </c>
       <c r="G1388">
         <v>0</v>
@@ -35041,10 +35041,10 @@
         <v>1</v>
       </c>
       <c r="C1391">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D1391" s="2">
-        <v>45799.89534671205</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E1391">
         <v>115</v>
@@ -35053,10 +35053,10 @@
         <v>45792.45592592593</v>
       </c>
       <c r="G1391">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1391" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1392" spans="1:8">
@@ -35067,10 +35067,10 @@
         <v>1</v>
       </c>
       <c r="C1392">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1392" s="2">
-        <v>45799.89528859723</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E1392">
         <v>8</v>
@@ -35079,10 +35079,10 @@
         <v>45784.64537037037</v>
       </c>
       <c r="G1392">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H1392" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1393" spans="1:8">
@@ -35578,22 +35578,22 @@
         <v>1</v>
       </c>
       <c r="C1412">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D1412" s="2">
-        <v>45800.93197719934</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E1412">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F1412" s="2">
-        <v>45800.686875</v>
+        <v>45803.4153125</v>
       </c>
       <c r="G1412">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1412" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1413" spans="1:8">
@@ -35832,16 +35832,16 @@
         <v>1</v>
       </c>
       <c r="C1422">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D1422" s="2">
-        <v>45799.89532168047</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E1422">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F1422" s="2">
-        <v>45791.75405092593</v>
+        <v>45803.50018518518</v>
       </c>
       <c r="G1422">
         <v>0</v>
@@ -35858,10 +35858,10 @@
         <v>1</v>
       </c>
       <c r="C1423">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D1423" s="2">
-        <v>45799.89534672352</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E1423">
         <v>20</v>
@@ -35870,10 +35870,10 @@
         <v>45792.65011574074</v>
       </c>
       <c r="G1423">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H1423" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1424" spans="1:8">
@@ -40151,7 +40151,7 @@
         <v>69</v>
       </c>
       <c r="F1594" s="2">
-        <v>45800.75802083333</v>
+        <v>45803.64673611111</v>
       </c>
       <c r="G1594">
         <v>0</v>
@@ -40220,22 +40220,22 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>7407</v>
+        <v>7361</v>
       </c>
       <c r="D1597" s="2">
-        <v>45800.93197719934</v>
+        <v>45803.90694023441</v>
       </c>
       <c r="E1597">
-        <v>7407</v>
+        <v>7405</v>
       </c>
       <c r="F1597" s="2">
-        <v>45800.686875</v>
+        <v>45803.49555555556</v>
       </c>
       <c r="G1597">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="H1597" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1598" spans="1:8">
@@ -41083,16 +41083,16 @@
         <v>1</v>
       </c>
       <c r="C1631">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1631" s="2">
-        <v>45799.89532163485</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E1631">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1631" s="2">
-        <v>45785.67143518518</v>
+        <v>45803.50922453704</v>
       </c>
       <c r="G1631">
         <v>0</v>
@@ -41187,22 +41187,22 @@
         <v>1</v>
       </c>
       <c r="C1635">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D1635" s="2">
-        <v>45800.93197719934</v>
+        <v>45803.90692203668</v>
       </c>
       <c r="E1635">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F1635" s="2">
-        <v>45800.686875</v>
+        <v>45803.50018518518</v>
       </c>
       <c r="G1635">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H1635" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1636" spans="1:8">
@@ -41700,16 +41700,16 @@
         <v>1</v>
       </c>
       <c r="C1656">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D1656" s="2">
-        <v>45799.89542739857</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E1656">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F1656" s="2">
-        <v>45792.65766203704</v>
+        <v>45803.49555555556</v>
       </c>
       <c r="G1656">
         <v>0</v>
@@ -42718,10 +42718,10 @@
         <v>1</v>
       </c>
       <c r="C1697">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D1697" s="2">
-        <v>45799.89534672352</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E1697">
         <v>9</v>
@@ -42730,10 +42730,10 @@
         <v>45792.65133101852</v>
       </c>
       <c r="G1697">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H1697" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1698" spans="1:8">
@@ -43528,16 +43528,16 @@
         <v>1</v>
       </c>
       <c r="C1730">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D1730" s="2">
-        <v>45799.89528858563</v>
+        <v>45803.62109434994</v>
       </c>
       <c r="E1730">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F1730" s="2">
-        <v>45782.63311342592</v>
+        <v>45803.6213425926</v>
       </c>
       <c r="G1730">
         <v>0</v>
@@ -47885,10 +47885,10 @@
         <v>1</v>
       </c>
       <c r="C1903">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1903" s="2">
-        <v>45799.89536723674</v>
+        <v>45803.9069220483</v>
       </c>
       <c r="E1903">
         <v>7</v>
@@ -47897,10 +47897,10 @@
         <v>45797.67800925926</v>
       </c>
       <c r="G1903">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1903" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1904" spans="1:8">
@@ -49475,16 +49475,16 @@
         <v>1</v>
       </c>
       <c r="C1966">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1966" s="2">
-        <v>45795.0420164208</v>
+        <v>45803.62109434994</v>
       </c>
       <c r="E1966">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1966" s="2">
-        <v>45726.47736111111</v>
+        <v>45803.50018518518</v>
       </c>
       <c r="G1966">
         <v>0</v>
@@ -51587,16 +51587,16 @@
         <v>1</v>
       </c>
       <c r="C2050">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D2050" s="2">
-        <v>45800.93175380815</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E2050">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F2050" s="2">
-        <v>45800.44972222222</v>
+        <v>45803.38153935185</v>
       </c>
       <c r="G2050">
         <v>0</v>
@@ -54708,19 +54708,19 @@
         <v>1</v>
       </c>
       <c r="C2175">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D2175" s="2">
-        <v>45795.0418106143</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E2175">
         <v>0</v>
       </c>
       <c r="G2175">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H2175" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2176" spans="1:8">
@@ -54835,22 +54835,22 @@
         <v>1</v>
       </c>
       <c r="C2180">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D2180" s="2">
-        <v>45799.89540330523</v>
+        <v>45803.90694022291</v>
       </c>
       <c r="E2180">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F2180" s="2">
-        <v>45799.43446759259</v>
+        <v>45803.38509259259</v>
       </c>
       <c r="G2180">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H2180" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2181" spans="1:8">
@@ -56362,16 +56362,16 @@
         <v>1</v>
       </c>
       <c r="C2240">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D2240" s="2">
-        <v>45799.89536723674</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E2240">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F2240" s="2">
-        <v>45797.53163194445</v>
+        <v>45803.38153935185</v>
       </c>
       <c r="G2240">
         <v>0</v>
@@ -60749,10 +60749,10 @@
         <v>1</v>
       </c>
       <c r="C2416">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="D2416" s="2">
-        <v>45800.93175379655</v>
+        <v>45803.90694023441</v>
       </c>
       <c r="E2416">
         <v>412</v>
@@ -60761,10 +60761,10 @@
         <v>45800.40415509259</v>
       </c>
       <c r="G2416">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H2416" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2417" spans="1:8">
@@ -61954,16 +61954,16 @@
         <v>1</v>
       </c>
       <c r="C2465">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D2465" s="2">
-        <v>45800.93175379655</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E2465">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F2465" s="2">
-        <v>45800.40415509259</v>
+        <v>45803.4153125</v>
       </c>
       <c r="G2465">
         <v>0</v>
@@ -62369,16 +62369,16 @@
         <v>1</v>
       </c>
       <c r="C2482">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="D2482" s="2">
-        <v>45800.93179064643</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E2482">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="F2482" s="2">
-        <v>45800.48438657408</v>
+        <v>45803.61216435185</v>
       </c>
       <c r="G2482">
         <v>0</v>
@@ -62395,16 +62395,16 @@
         <v>1</v>
       </c>
       <c r="C2483">
-        <v>1063</v>
+        <v>1013</v>
       </c>
       <c r="D2483" s="2">
-        <v>45799.89540331678</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E2483">
-        <v>1063</v>
+        <v>1013</v>
       </c>
       <c r="F2483" s="2">
-        <v>45799.61766203704</v>
+        <v>45803.61216435185</v>
       </c>
       <c r="G2483">
         <v>0</v>
@@ -63593,21 +63593,113 @@
         <v>1</v>
       </c>
       <c r="C2533">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D2533" s="2">
-        <v>45800.93204010786</v>
+        <v>45803.62106753104</v>
       </c>
       <c r="E2533">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F2533" s="2">
-        <v>45800.75802083333</v>
+        <v>45803.53655092593</v>
       </c>
       <c r="G2533">
         <v>0</v>
       </c>
       <c r="H2533" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2534" spans="1:8">
+      <c r="A2534">
+        <v>43238724</v>
+      </c>
+      <c r="B2534">
+        <v>1</v>
+      </c>
+      <c r="C2534">
+        <v>0</v>
+      </c>
+      <c r="D2534" s="2">
+        <v>45803.62106753104</v>
+      </c>
+      <c r="E2534">
+        <v>0</v>
+      </c>
+      <c r="G2534">
+        <v>0</v>
+      </c>
+      <c r="H2534" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2535" spans="1:8">
+      <c r="A2535">
+        <v>43239201</v>
+      </c>
+      <c r="B2535">
+        <v>1</v>
+      </c>
+      <c r="C2535">
+        <v>0</v>
+      </c>
+      <c r="D2535" s="2">
+        <v>45803.62106753104</v>
+      </c>
+      <c r="E2535">
+        <v>0</v>
+      </c>
+      <c r="G2535">
+        <v>0</v>
+      </c>
+      <c r="H2535" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2536" spans="1:8">
+      <c r="A2536">
+        <v>43241476</v>
+      </c>
+      <c r="B2536">
+        <v>1</v>
+      </c>
+      <c r="C2536">
+        <v>0</v>
+      </c>
+      <c r="D2536" s="2">
+        <v>45803.62109434994</v>
+      </c>
+      <c r="E2536">
+        <v>0</v>
+      </c>
+      <c r="G2536">
+        <v>0</v>
+      </c>
+      <c r="H2536" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2537" spans="1:8">
+      <c r="A2537">
+        <v>43246609</v>
+      </c>
+      <c r="B2537">
+        <v>1</v>
+      </c>
+      <c r="C2537">
+        <v>0</v>
+      </c>
+      <c r="D2537" s="2">
+        <v>45803.90694022291</v>
+      </c>
+      <c r="E2537">
+        <v>0</v>
+      </c>
+      <c r="G2537">
+        <v>0</v>
+      </c>
+      <c r="H2537" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizei os dados da bibi e add alem de fazer uns ajustes nas metricas de estoque para as duas e para bdxp
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2544" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2548" uniqueCount="10">
   <si>
     <t>id_produto</t>
   </si>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2537"/>
+  <dimension ref="A1:H2541"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -520,22 +520,22 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2">
-        <v>45803.64980324074</v>
+        <v>45804.71377314815</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -690,16 +690,16 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D12" s="2">
-        <v>45799.89534673509</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E12">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F12" s="2">
-        <v>45796.49008101852</v>
+        <v>45804.47773148148</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1194,22 +1194,22 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>1072</v>
+        <v>1062</v>
       </c>
       <c r="D33" s="2">
-        <v>45803.90692203668</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E33">
-        <v>1174</v>
+        <v>1062</v>
       </c>
       <c r="F33" s="2">
-        <v>45803.49555555556</v>
+        <v>45804.46582175926</v>
       </c>
       <c r="G33">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1563,16 +1563,16 @@
         <v>1</v>
       </c>
       <c r="C48">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D48" s="2">
-        <v>45799.8954510958</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E48">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F48" s="2">
-        <v>45797.99737268518</v>
+        <v>45804.69865740741</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1595,16 +1595,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E49">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F49" s="2">
-        <v>45803.64673611111</v>
+        <v>45803.77322916667</v>
       </c>
       <c r="G49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1765,22 +1765,22 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D56" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E56">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="F56" s="2">
-        <v>45803.5318287037</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G56">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1823,16 +1823,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E58">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F58" s="2">
-        <v>45803.5318287037</v>
+        <v>45803.75170138889</v>
       </c>
       <c r="G58">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1941,16 +1941,16 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D63" s="2">
-        <v>45800.93194931293</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E63">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F63" s="2">
-        <v>45800.68467592593</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2120,16 +2120,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E70">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F70" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G70">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2382,16 +2382,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E81">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F81" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G81">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2402,22 +2402,22 @@
         <v>1</v>
       </c>
       <c r="C82">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D82" s="2">
-        <v>45803.90692203668</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E82">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F82" s="2">
-        <v>45798.43265046296</v>
+        <v>45804.76886574074</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2437,7 +2437,7 @@
         <v>139</v>
       </c>
       <c r="F83" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -2477,16 +2477,16 @@
         <v>1</v>
       </c>
       <c r="C85">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D85" s="2">
-        <v>45803.62109434994</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E85">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F85" s="2">
-        <v>45803.62967592593</v>
+        <v>45804.42633101852</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -2509,16 +2509,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E86">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F86" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G86">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2529,22 +2529,22 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>12</v>
+        <v>-2</v>
       </c>
       <c r="D87" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E87">
-        <v>15</v>
+        <v>-2</v>
       </c>
       <c r="F87" s="2">
-        <v>45800.6955787037</v>
+        <v>45804.76971064815</v>
       </c>
       <c r="G87">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H87" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2630,22 +2630,22 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D91" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E91">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F91" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G91">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H91" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2702,22 +2702,22 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D94" s="2">
-        <v>45803.90694022291</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E94">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F94" s="2">
-        <v>45803.62967592593</v>
+        <v>45804.76993055556</v>
       </c>
       <c r="G94">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H94" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2751,22 +2751,22 @@
         <v>1</v>
       </c>
       <c r="C96">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="D96" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E96">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F96" s="2">
-        <v>45791.69931712963</v>
+        <v>45804.42633101852</v>
       </c>
       <c r="G96">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H96" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2872,22 +2872,22 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>1856</v>
+        <v>1791</v>
       </c>
       <c r="D101" s="2">
-        <v>45803.90694022291</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E101">
-        <v>2123</v>
+        <v>1791</v>
       </c>
       <c r="F101" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.46582175926</v>
       </c>
       <c r="G101">
-        <v>267</v>
+        <v>0</v>
       </c>
       <c r="H101" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -2927,16 +2927,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E103">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F103" s="2">
-        <v>45793.38017361111</v>
+        <v>45803.74128472222</v>
       </c>
       <c r="G103">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H103" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -2993,22 +2993,22 @@
         <v>1</v>
       </c>
       <c r="C106">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="D106" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E106">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="F106" s="2">
-        <v>45799.64056712963</v>
+        <v>45804.77440972222</v>
       </c>
       <c r="G106">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H106" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3267,7 +3267,7 @@
         <v>1202</v>
       </c>
       <c r="F117" s="2">
-        <v>45802.99459490741</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -3339,16 +3339,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E120">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F120" s="2">
-        <v>45796.72284722222</v>
+        <v>45803.73960648148</v>
       </c>
       <c r="G120">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H120" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -3368,7 +3368,7 @@
         <v>52</v>
       </c>
       <c r="F121" s="2">
-        <v>45803.64673611111</v>
+        <v>45803.70542824074</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -3408,22 +3408,22 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D123" s="2">
-        <v>45803.90694022291</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E123">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F123" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G123">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H123" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -3797,16 +3797,16 @@
         <v>1</v>
       </c>
       <c r="C139">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="D139" s="2">
-        <v>45799.89542737551</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E139">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="F139" s="2">
-        <v>45799.64041666667</v>
+        <v>45804.52372685185</v>
       </c>
       <c r="G139">
         <v>0</v>
@@ -3852,16 +3852,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E141">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="F141" s="2">
-        <v>45800.50141203704</v>
+        <v>45803.72625</v>
       </c>
       <c r="G141">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H141" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -4074,22 +4074,22 @@
         <v>1</v>
       </c>
       <c r="C150">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D150" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E150">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F150" s="2">
-        <v>45792.73215277777</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H150" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -4942,16 +4942,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E185">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F185" s="2">
-        <v>45799.54621527778</v>
+        <v>45803.73960648148</v>
       </c>
       <c r="G185">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H185" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5083,16 +5083,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E191">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="F191" s="2">
-        <v>45802.99361111111</v>
+        <v>45803.7415625</v>
       </c>
       <c r="G191">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H191" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -5103,16 +5103,16 @@
         <v>1</v>
       </c>
       <c r="C192">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D192" s="2">
-        <v>45799.89534672352</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E192">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F192" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.42633101852</v>
       </c>
       <c r="G192">
         <v>0</v>
@@ -5190,7 +5190,7 @@
         <v>13</v>
       </c>
       <c r="F195" s="2">
-        <v>45800.6955787037</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G195">
         <v>0</v>
@@ -5302,16 +5302,16 @@
         <v>1</v>
       </c>
       <c r="C200">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="D200" s="2">
-        <v>45799.89534672352</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E200">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="F200" s="2">
-        <v>45793.53142361111</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G200">
         <v>0</v>
@@ -5328,16 +5328,16 @@
         <v>1</v>
       </c>
       <c r="C201">
-        <v>1110</v>
+        <v>1104</v>
       </c>
       <c r="D201" s="2">
-        <v>45799.89534673509</v>
+        <v>45804.91952539605</v>
       </c>
       <c r="E201">
-        <v>1110</v>
+        <v>1104</v>
       </c>
       <c r="F201" s="2">
-        <v>45796.43337962963</v>
+        <v>45804.39973379629</v>
       </c>
       <c r="G201">
         <v>0</v>
@@ -5455,16 +5455,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E206">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F206" s="2">
-        <v>45792.73215277777</v>
+        <v>45803.74012731481</v>
       </c>
       <c r="G206">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H206" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -5711,22 +5711,22 @@
         <v>1</v>
       </c>
       <c r="C217">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D217" s="2">
-        <v>45803.90692203668</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E217">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F217" s="2">
-        <v>45798.62037037037</v>
+        <v>45804.49947916667</v>
       </c>
       <c r="G217">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H217" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -5743,16 +5743,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E218">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F218" s="2">
-        <v>45793.71568287037</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G218">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H218" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -6175,22 +6175,22 @@
         <v>1</v>
       </c>
       <c r="C236">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="D236" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E236">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="F236" s="2">
-        <v>45800.75763888889</v>
+        <v>45804.67836805555</v>
       </c>
       <c r="G236">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H236" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -6627,22 +6627,22 @@
         <v>1</v>
       </c>
       <c r="C255">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D255" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E255">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="F255" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.67107638889</v>
       </c>
       <c r="G255">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H255" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -6702,16 +6702,16 @@
         <v>1</v>
       </c>
       <c r="C258">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D258" s="2">
-        <v>45795.04208095842</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E258">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F258" s="2">
-        <v>45772.4734837963</v>
+        <v>45804.67836805555</v>
       </c>
       <c r="G258">
         <v>0</v>
@@ -6996,22 +6996,22 @@
         <v>1</v>
       </c>
       <c r="C270">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D270" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E270">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F270" s="2">
-        <v>45803.53376157407</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G270">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H270" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="271" spans="1:8">
@@ -7310,22 +7310,22 @@
         <v>1</v>
       </c>
       <c r="C283">
-        <v>-13</v>
+        <v>29</v>
       </c>
       <c r="D283" s="2">
-        <v>45803.90692203668</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E283">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F283" s="2">
-        <v>45800.47983796296</v>
+        <v>45804.59197916667</v>
       </c>
       <c r="G283">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H283" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="284" spans="1:8">
@@ -7408,22 +7408,22 @@
         <v>1</v>
       </c>
       <c r="C287">
-        <v>824</v>
+        <v>776</v>
       </c>
       <c r="D287" s="2">
-        <v>45803.90694022291</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E287">
-        <v>837</v>
+        <v>776</v>
       </c>
       <c r="F287" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.43545138889</v>
       </c>
       <c r="G287">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="H287" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="288" spans="1:8">
@@ -7509,16 +7509,16 @@
         <v>1</v>
       </c>
       <c r="C291">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="D291" s="2">
-        <v>45800.93204011993</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E291">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="F291" s="2">
-        <v>45800.77331018518</v>
+        <v>45804.51150462963</v>
       </c>
       <c r="G291">
         <v>0</v>
@@ -7610,16 +7610,16 @@
         <v>1</v>
       </c>
       <c r="C295">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D295" s="2">
-        <v>45800.93197718772</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E295">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F295" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.45849537037</v>
       </c>
       <c r="G295">
         <v>0</v>
@@ -7887,7 +7887,7 @@
         <v>1</v>
       </c>
       <c r="F306" s="2">
-        <v>45803.64673611111</v>
+        <v>45803.70542824074</v>
       </c>
       <c r="G306">
         <v>0</v>
@@ -7959,16 +7959,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E309">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="F309" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G309">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H309" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="310" spans="1:8">
@@ -8169,16 +8169,16 @@
         <v>1</v>
       </c>
       <c r="C318">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="D318" s="2">
-        <v>45800.93204011993</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E318">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F318" s="2">
-        <v>45803.61013888889</v>
+        <v>45804.43686342592</v>
       </c>
       <c r="G318">
         <v>0</v>
@@ -8201,16 +8201,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E319">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F319" s="2">
-        <v>45803.61216435185</v>
+        <v>45803.72883101852</v>
       </c>
       <c r="G319">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H319" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="320" spans="1:8">
@@ -8380,16 +8380,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E326">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F326" s="2">
-        <v>45796.65443287037</v>
+        <v>45803.7415625</v>
       </c>
       <c r="G326">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H326" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="327" spans="1:8">
@@ -8426,16 +8426,16 @@
         <v>1</v>
       </c>
       <c r="C328">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D328" s="2">
-        <v>45798.96533509644</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E328">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F328" s="2">
-        <v>45798.44711805556</v>
+        <v>45804.49947916667</v>
       </c>
       <c r="G328">
         <v>0</v>
@@ -8876,16 +8876,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E346">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F346" s="2">
-        <v>45800.40415509259</v>
+        <v>45803.72625</v>
       </c>
       <c r="G346">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H346" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="347" spans="1:8">
@@ -8965,16 +8965,16 @@
         <v>1</v>
       </c>
       <c r="C350">
-        <v>102</v>
+        <v>-30</v>
       </c>
       <c r="D350" s="2">
-        <v>45800.93188814504</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E350">
-        <v>102</v>
+        <v>-30</v>
       </c>
       <c r="F350" s="2">
-        <v>45800.62443287037</v>
+        <v>45804.51150462963</v>
       </c>
       <c r="G350">
         <v>0</v>
@@ -9072,16 +9072,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E354">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F354" s="2">
-        <v>45798.62037037037</v>
+        <v>45803.72625</v>
       </c>
       <c r="G354">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H354" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="355" spans="1:8">
@@ -9170,16 +9170,16 @@
         <v>45803.90694023441</v>
       </c>
       <c r="E358">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F358" s="2">
-        <v>45800.68569444444</v>
+        <v>45803.77322916667</v>
       </c>
       <c r="G358">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H358" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="359" spans="1:8">
@@ -9251,7 +9251,7 @@
         <v>130</v>
       </c>
       <c r="F361" s="2">
-        <v>45803.57027777778</v>
+        <v>45803.73357638889</v>
       </c>
       <c r="G361">
         <v>0</v>
@@ -9297,16 +9297,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E363">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="F363" s="2">
-        <v>45803.62967592593</v>
+        <v>45803.74128472222</v>
       </c>
       <c r="G363">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H363" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="364" spans="1:8">
@@ -9874,7 +9874,7 @@
         <v>0</v>
       </c>
       <c r="F386" s="2">
-        <v>45789.39277777778</v>
+        <v>45803.72883101852</v>
       </c>
       <c r="G386">
         <v>0</v>
@@ -9891,16 +9891,16 @@
         <v>1</v>
       </c>
       <c r="C387">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D387" s="2">
-        <v>45799.89532164588</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E387">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F387" s="2">
-        <v>45786.46773148148</v>
+        <v>45804.44082175926</v>
       </c>
       <c r="G387">
         <v>0</v>
@@ -9917,16 +9917,16 @@
         <v>1</v>
       </c>
       <c r="C388">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D388" s="2">
-        <v>45799.8954032937</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E388">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F388" s="2">
-        <v>45799.40561342592</v>
+        <v>45804.74640046297</v>
       </c>
       <c r="G388">
         <v>0</v>
@@ -9943,16 +9943,16 @@
         <v>1</v>
       </c>
       <c r="C389">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D389" s="2">
-        <v>45799.8954032937</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E389">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F389" s="2">
-        <v>45799.40561342592</v>
+        <v>45804.74640046297</v>
       </c>
       <c r="G389">
         <v>0</v>
@@ -9978,7 +9978,7 @@
         <v>29</v>
       </c>
       <c r="F390" s="2">
-        <v>45803.64673611111</v>
+        <v>45803.77322916667</v>
       </c>
       <c r="G390">
         <v>0</v>
@@ -10070,22 +10070,22 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D394" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E394">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="F394" s="2">
-        <v>45803.50018518518</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G394">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H394" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="395" spans="1:8">
@@ -10122,16 +10122,16 @@
         <v>1</v>
       </c>
       <c r="C396">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D396" s="2">
-        <v>45799.89532164588</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E396">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F396" s="2">
-        <v>45786.47606481481</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G396">
         <v>0</v>
@@ -10278,7 +10278,7 @@
         <v>212</v>
       </c>
       <c r="F402" s="2">
-        <v>45803.64673611111</v>
+        <v>45803.70542824074</v>
       </c>
       <c r="G402">
         <v>0</v>
@@ -10330,7 +10330,7 @@
         <v>263</v>
       </c>
       <c r="F404" s="2">
-        <v>45803.61216435185</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G404">
         <v>0</v>
@@ -10428,7 +10428,7 @@
         <v>83</v>
       </c>
       <c r="F408" s="2">
-        <v>45803.62967592593</v>
+        <v>45803.77025462963</v>
       </c>
       <c r="G408">
         <v>0</v>
@@ -10471,16 +10471,16 @@
         <v>1</v>
       </c>
       <c r="C410">
-        <v>658</v>
+        <v>608</v>
       </c>
       <c r="D410" s="2">
-        <v>45800.93188814504</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E410">
-        <v>658</v>
+        <v>608</v>
       </c>
       <c r="F410" s="2">
-        <v>45800.62752314815</v>
+        <v>45804.46663194444</v>
       </c>
       <c r="G410">
         <v>0</v>
@@ -10549,16 +10549,16 @@
         <v>1</v>
       </c>
       <c r="C413">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D413" s="2">
-        <v>45799.89534673509</v>
+        <v>45804.91952539605</v>
       </c>
       <c r="E413">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="F413" s="2">
-        <v>45796.43142361111</v>
+        <v>45804.39973379629</v>
       </c>
       <c r="G413">
         <v>0</v>
@@ -10673,22 +10673,22 @@
         <v>1</v>
       </c>
       <c r="C418">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="D418" s="2">
-        <v>45803.90692203668</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E418">
-        <v>350</v>
+        <v>303</v>
       </c>
       <c r="F418" s="2">
-        <v>45799.64056712963</v>
+        <v>45804.51150462963</v>
       </c>
       <c r="G418">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="H418" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="419" spans="1:8">
@@ -10771,16 +10771,16 @@
         <v>1</v>
       </c>
       <c r="C422">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D422" s="2">
-        <v>45799.89542737551</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E422">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F422" s="2">
-        <v>45799.64041666667</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G422">
         <v>0</v>
@@ -10843,16 +10843,16 @@
         <v>1</v>
       </c>
       <c r="C425">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D425" s="2">
-        <v>45800.93175383128</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E425">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F425" s="2">
-        <v>45800.47983796296</v>
+        <v>45804.42633101852</v>
       </c>
       <c r="G425">
         <v>0</v>
@@ -11013,16 +11013,16 @@
         <v>1</v>
       </c>
       <c r="C432">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D432" s="2">
-        <v>45800.93194931293</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E432">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F432" s="2">
-        <v>45800.68569444444</v>
+        <v>45804.42633101852</v>
       </c>
       <c r="G432">
         <v>0</v>
@@ -11114,16 +11114,16 @@
         <v>1</v>
       </c>
       <c r="C436">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D436" s="2">
-        <v>45799.89532165734</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E436">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F436" s="2">
-        <v>45789.51143518519</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G436">
         <v>0</v>
@@ -11832,16 +11832,16 @@
         <v>1</v>
       </c>
       <c r="C465">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D465" s="2">
-        <v>45798.96533511975</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E465">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F465" s="2">
-        <v>45798.64541666667</v>
+        <v>45804.42633101852</v>
       </c>
       <c r="G465">
         <v>0</v>
@@ -11930,16 +11930,16 @@
         <v>1</v>
       </c>
       <c r="C469">
-        <v>-48</v>
+        <v>0</v>
       </c>
       <c r="D469" s="2">
-        <v>45799.89540330523</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E469">
-        <v>-48</v>
+        <v>0</v>
       </c>
       <c r="F469" s="2">
-        <v>45799.54680555555</v>
+        <v>45804.43621527778</v>
       </c>
       <c r="G469">
         <v>0</v>
@@ -12207,22 +12207,22 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>14</v>
+        <v>-47</v>
       </c>
       <c r="D480" s="2">
-        <v>45803.90692203668</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E480">
-        <v>21</v>
+        <v>-47</v>
       </c>
       <c r="F480" s="2">
-        <v>45803.38509259259</v>
+        <v>45804.77440972222</v>
       </c>
       <c r="G480">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H480" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="481" spans="1:8">
@@ -12536,16 +12536,16 @@
         <v>1</v>
       </c>
       <c r="C493">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D493" s="2">
-        <v>45800.93204010786</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E493">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F493" s="2">
-        <v>45800.75802083333</v>
+        <v>45804.76993055556</v>
       </c>
       <c r="G493">
         <v>0</v>
@@ -12951,22 +12951,22 @@
         <v>1</v>
       </c>
       <c r="C510">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D510" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E510">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="F510" s="2">
-        <v>45803.50018518518</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G510">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H510" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="511" spans="1:8">
@@ -13366,16 +13366,16 @@
         <v>1</v>
       </c>
       <c r="C527">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D527" s="2">
-        <v>45799.89534672352</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E527">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F527" s="2">
-        <v>45792.65766203704</v>
+        <v>45804.49947916667</v>
       </c>
       <c r="G527">
         <v>0</v>
@@ -13476,7 +13476,7 @@
         <v>85</v>
       </c>
       <c r="F531" s="2">
-        <v>45798.62037037037</v>
+        <v>45804.66668981482</v>
       </c>
       <c r="G531">
         <v>0</v>
@@ -13643,16 +13643,16 @@
         <v>1</v>
       </c>
       <c r="C538">
-        <v>204</v>
+        <v>4</v>
       </c>
       <c r="D538" s="2">
-        <v>45799.89534674662</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E538">
-        <v>204</v>
+        <v>4</v>
       </c>
       <c r="F538" s="2">
-        <v>45796.62467592592</v>
+        <v>45804.45869212963</v>
       </c>
       <c r="G538">
         <v>0</v>
@@ -13675,16 +13675,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E539">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="F539" s="2">
-        <v>45784.73082175926</v>
+        <v>45803.71083333333</v>
       </c>
       <c r="G539">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H539" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="540" spans="1:8">
@@ -14415,16 +14415,16 @@
         <v>1</v>
       </c>
       <c r="C570">
-        <v>2760</v>
+        <v>2754</v>
       </c>
       <c r="D570" s="2">
-        <v>45803.62106753104</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E570">
-        <v>2760</v>
+        <v>2754</v>
       </c>
       <c r="F570" s="2">
-        <v>45803.49555555556</v>
+        <v>45804.76886574074</v>
       </c>
       <c r="G570">
         <v>0</v>
@@ -14510,16 +14510,16 @@
         <v>1</v>
       </c>
       <c r="C574">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D574" s="2">
-        <v>45799.89540330523</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E574">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F574" s="2">
-        <v>45799.54913194444</v>
+        <v>45804.53324074074</v>
       </c>
       <c r="G574">
         <v>0</v>
@@ -14677,16 +14677,16 @@
         <v>1</v>
       </c>
       <c r="C581">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D581" s="2">
-        <v>45799.89536723674</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E581">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F581" s="2">
-        <v>45797.74582175926</v>
+        <v>45804.76993055556</v>
       </c>
       <c r="G581">
         <v>0</v>
@@ -15884,16 +15884,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E631">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F631" s="2">
-        <v>45803.38153935185</v>
+        <v>45803.7415625</v>
       </c>
       <c r="G631">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H631" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="632" spans="1:8">
@@ -15962,16 +15962,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E634">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F634" s="2">
-        <v>45799.64056712963</v>
+        <v>45803.7415625</v>
       </c>
       <c r="G634">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H634" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="635" spans="1:8">
@@ -16509,16 +16509,16 @@
         <v>1</v>
       </c>
       <c r="C657">
-        <v>2383</v>
+        <v>2375</v>
       </c>
       <c r="D657" s="2">
-        <v>45800.93197722271</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E657">
-        <v>2383</v>
+        <v>2375</v>
       </c>
       <c r="F657" s="2">
-        <v>45800.6955787037</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G657">
         <v>0</v>
@@ -16541,16 +16541,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E658">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F658" s="2">
-        <v>45793.37982638889</v>
+        <v>45803.72575231481</v>
       </c>
       <c r="G658">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H658" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="659" spans="1:8">
@@ -17077,7 +17077,7 @@
         <v>6</v>
       </c>
       <c r="F680" s="2">
-        <v>45797.67186342592</v>
+        <v>45803.76681712963</v>
       </c>
       <c r="G680">
         <v>0</v>
@@ -17094,16 +17094,16 @@
         <v>1</v>
       </c>
       <c r="C681">
-        <v>-8</v>
+        <v>-12</v>
       </c>
       <c r="D681" s="2">
-        <v>45803.62106753104</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E681">
-        <v>-8</v>
+        <v>-12</v>
       </c>
       <c r="F681" s="2">
-        <v>45803.49592592593</v>
+        <v>45804.77440972222</v>
       </c>
       <c r="G681">
         <v>0</v>
@@ -17201,16 +17201,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E685">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F685" s="2">
-        <v>45800.40415509259</v>
+        <v>45803.7415625</v>
       </c>
       <c r="G685">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H685" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="686" spans="1:8">
@@ -17342,22 +17342,22 @@
         <v>1</v>
       </c>
       <c r="C691">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="D691" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E691">
-        <v>377</v>
+        <v>358</v>
       </c>
       <c r="F691" s="2">
-        <v>45796.65443287037</v>
+        <v>45804.67836805555</v>
       </c>
       <c r="G691">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H691" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="692" spans="1:8">
@@ -17599,16 +17599,16 @@
         <v>1</v>
       </c>
       <c r="C701">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D701" s="2">
-        <v>45803.62109434994</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E701">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F701" s="2">
-        <v>45803.62967592593</v>
+        <v>45804.45869212963</v>
       </c>
       <c r="G701">
         <v>0</v>
@@ -17755,7 +17755,7 @@
         <v>133</v>
       </c>
       <c r="F707" s="2">
-        <v>45782.6296875</v>
+        <v>45803.77025462963</v>
       </c>
       <c r="G707">
         <v>0</v>
@@ -18072,22 +18072,22 @@
         <v>1</v>
       </c>
       <c r="C720">
-        <v>775</v>
+        <v>765</v>
       </c>
       <c r="D720" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E720">
-        <v>786</v>
+        <v>765</v>
       </c>
       <c r="F720" s="2">
-        <v>45803.49555555556</v>
+        <v>45804.76993055556</v>
       </c>
       <c r="G720">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H720" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="721" spans="1:8">
@@ -18381,22 +18381,22 @@
         <v>1</v>
       </c>
       <c r="C732">
-        <v>442</v>
+        <v>424</v>
       </c>
       <c r="D732" s="2">
-        <v>45803.90692203668</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E732">
-        <v>444</v>
+        <v>424</v>
       </c>
       <c r="F732" s="2">
-        <v>45800.62752314815</v>
+        <v>45804.51150462963</v>
       </c>
       <c r="G732">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H732" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="733" spans="1:8">
@@ -18612,16 +18612,16 @@
         <v>1</v>
       </c>
       <c r="C741">
-        <v>14</v>
+        <v>-8</v>
       </c>
       <c r="D741" s="2">
-        <v>45800.93188814504</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E741">
-        <v>14</v>
+        <v>-8</v>
       </c>
       <c r="F741" s="2">
-        <v>45800.62018518519</v>
+        <v>45804.77462962963</v>
       </c>
       <c r="G741">
         <v>0</v>
@@ -19154,16 +19154,16 @@
         <v>1</v>
       </c>
       <c r="C763">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D763" s="2">
-        <v>45803.62106753104</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E763">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F763" s="2">
-        <v>45803.40251157407</v>
+        <v>45804.67107638889</v>
       </c>
       <c r="G763">
         <v>0</v>
@@ -19241,7 +19241,7 @@
         <v>7</v>
       </c>
       <c r="F766" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G766">
         <v>0</v>
@@ -19379,16 +19379,16 @@
         <v>1</v>
       </c>
       <c r="C772">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D772" s="2">
-        <v>45803.62106753104</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E772">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F772" s="2">
-        <v>45803.57027777778</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G772">
         <v>0</v>
@@ -19483,22 +19483,22 @@
         <v>1</v>
       </c>
       <c r="C776">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D776" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E776">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="F776" s="2">
-        <v>45800.62752314815</v>
+        <v>45804.76971064815</v>
       </c>
       <c r="G776">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="H776" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="777" spans="1:8">
@@ -19985,16 +19985,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E796">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F796" s="2">
-        <v>45797.63394675926</v>
+        <v>45803.71083333333</v>
       </c>
       <c r="G796">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H796" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="797" spans="1:8">
@@ -20005,16 +20005,16 @@
         <v>1</v>
       </c>
       <c r="C797">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D797" s="2">
-        <v>45799.895451121</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E797">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F797" s="2">
-        <v>45799.64056712963</v>
+        <v>45804.51150462963</v>
       </c>
       <c r="G797">
         <v>0</v>
@@ -20732,22 +20732,22 @@
         <v>1</v>
       </c>
       <c r="C826">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D826" s="2">
-        <v>45803.90694023441</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E826">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F826" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.42633101852</v>
       </c>
       <c r="G826">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H826" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="827" spans="1:8">
@@ -20862,7 +20862,7 @@
         <v>251</v>
       </c>
       <c r="F831" s="2">
-        <v>45793.37892361111</v>
+        <v>45803.76681712963</v>
       </c>
       <c r="G831">
         <v>0</v>
@@ -21343,16 +21343,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E851">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F851" s="2">
-        <v>45791.75405092593</v>
+        <v>45803.7415625</v>
       </c>
       <c r="G851">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H851" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="852" spans="1:8">
@@ -21395,16 +21395,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E853">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F853" s="2">
-        <v>45803.38509259259</v>
+        <v>45803.74012731481</v>
       </c>
       <c r="G853">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H853" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="854" spans="1:8">
@@ -21868,22 +21868,22 @@
         <v>1</v>
       </c>
       <c r="C872">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D872" s="2">
-        <v>45803.90694023441</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E872">
-        <v>748</v>
+        <v>717</v>
       </c>
       <c r="F872" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G872">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H872" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="873" spans="1:8">
@@ -22024,16 +22024,16 @@
         <v>1</v>
       </c>
       <c r="C878">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D878" s="2">
-        <v>45795.04210567895</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E878">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F878" s="2">
-        <v>45777.5341550926</v>
+        <v>45804.76886574074</v>
       </c>
       <c r="G878">
         <v>0</v>
@@ -22145,22 +22145,22 @@
         <v>1</v>
       </c>
       <c r="C883">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="D883" s="2">
-        <v>45803.90692203668</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E883">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="F883" s="2">
-        <v>45803.62967592593</v>
+        <v>45804.76886574074</v>
       </c>
       <c r="G883">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H883" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="884" spans="1:8">
@@ -22272,16 +22272,16 @@
         <v>1</v>
       </c>
       <c r="C888">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D888" s="2">
-        <v>45803.62106753104</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E888">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F888" s="2">
-        <v>45803.57027777778</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G888">
         <v>0</v>
@@ -22298,16 +22298,16 @@
         <v>1</v>
       </c>
       <c r="C889">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D889" s="2">
-        <v>45795.04208095842</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E889">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F889" s="2">
-        <v>45770.65818287037</v>
+        <v>45804.44082175926</v>
       </c>
       <c r="G889">
         <v>0</v>
@@ -23193,16 +23193,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E924">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F924" s="2">
-        <v>45803.50018518518</v>
+        <v>45803.74012731481</v>
       </c>
       <c r="G924">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H924" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="925" spans="1:8">
@@ -23545,16 +23545,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E938">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F938" s="2">
-        <v>45796.65907407407</v>
+        <v>45803.7415625</v>
       </c>
       <c r="G938">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H938" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="939" spans="1:8">
@@ -24142,16 +24142,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E962">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="F962" s="2">
-        <v>45803.38509259259</v>
+        <v>45803.74012731481</v>
       </c>
       <c r="G962">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H962" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="963" spans="1:8">
@@ -24168,16 +24168,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E963">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="F963" s="2">
-        <v>45798.64541666667</v>
+        <v>45803.72625</v>
       </c>
       <c r="G963">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H963" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="964" spans="1:8">
@@ -24924,16 +24924,16 @@
         <v>1</v>
       </c>
       <c r="C993">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D993" s="2">
-        <v>45799.89532166889</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E993">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F993" s="2">
-        <v>45791.64983796296</v>
+        <v>45804.60759259259</v>
       </c>
       <c r="G993">
         <v>0</v>
@@ -25155,16 +25155,16 @@
         <v>1</v>
       </c>
       <c r="C1002">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D1002" s="2">
-        <v>45803.62106753104</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E1002">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F1002" s="2">
-        <v>45803.38153935185</v>
+        <v>45804.76886574074</v>
       </c>
       <c r="G1002">
         <v>0</v>
@@ -25533,16 +25533,16 @@
         <v>1</v>
       </c>
       <c r="C1017">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="D1017" s="2">
-        <v>45803.62106753104</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1017">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="F1017" s="2">
-        <v>45803.57027777778</v>
+        <v>45804.71377314815</v>
       </c>
       <c r="G1017">
         <v>0</v>
@@ -26682,16 +26682,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E1062">
-        <v>840</v>
+        <v>804</v>
       </c>
       <c r="F1062" s="2">
-        <v>45803.41005787037</v>
+        <v>45803.73960648148</v>
       </c>
       <c r="G1062">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="H1062" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1063" spans="1:8">
@@ -27873,16 +27873,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E1110">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F1110" s="2">
-        <v>45799.64041666667</v>
+        <v>45803.7415625</v>
       </c>
       <c r="G1110">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H1110" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1111" spans="1:8">
@@ -28173,16 +28173,16 @@
         <v>1</v>
       </c>
       <c r="C1122">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D1122" s="2">
-        <v>45799.895427387</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E1122">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F1122" s="2">
-        <v>45799.64056712963</v>
+        <v>45804.77440972222</v>
       </c>
       <c r="G1122">
         <v>0</v>
@@ -28805,16 +28805,16 @@
         <v>1</v>
       </c>
       <c r="C1147">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1147" s="2">
-        <v>45800.93197718772</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E1147">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F1147" s="2">
-        <v>45800.6859837963</v>
+        <v>45804.76971064815</v>
       </c>
       <c r="G1147">
         <v>0</v>
@@ -28857,16 +28857,16 @@
         <v>1</v>
       </c>
       <c r="C1149">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D1149" s="2">
-        <v>45800.93192368435</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1149">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F1149" s="2">
-        <v>45800.40415509259</v>
+        <v>45804.71377314815</v>
       </c>
       <c r="G1149">
         <v>0</v>
@@ -29013,16 +29013,16 @@
         <v>1</v>
       </c>
       <c r="C1155">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1155" s="2">
-        <v>45799.89534672352</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E1155">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1155" s="2">
-        <v>45792.68052083333</v>
+        <v>45804.76993055556</v>
       </c>
       <c r="G1155">
         <v>0</v>
@@ -29839,7 +29839,7 @@
         <v>164</v>
       </c>
       <c r="F1187" s="2">
-        <v>45800.6955787037</v>
+        <v>45804.53158564815</v>
       </c>
       <c r="G1187">
         <v>0</v>
@@ -29934,16 +29934,16 @@
         <v>1</v>
       </c>
       <c r="C1191">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D1191" s="2">
-        <v>45799.89528858563</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1191">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F1191" s="2">
-        <v>45783.64329861111</v>
+        <v>45804.69865740741</v>
       </c>
       <c r="G1191">
         <v>0</v>
@@ -30142,16 +30142,16 @@
         <v>1</v>
       </c>
       <c r="C1199">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D1199" s="2">
-        <v>45799.89540330523</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1199">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F1199" s="2">
-        <v>45799.54651620371</v>
+        <v>45804.46582175926</v>
       </c>
       <c r="G1199">
         <v>0</v>
@@ -31372,22 +31372,22 @@
         <v>1</v>
       </c>
       <c r="C1247">
-        <v>-18</v>
+        <v>115</v>
       </c>
       <c r="D1247" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1247">
-        <v>4</v>
+        <v>115</v>
       </c>
       <c r="F1247" s="2">
-        <v>45796.72284722222</v>
+        <v>45804.60414351852</v>
       </c>
       <c r="G1247">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="H1247" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1248" spans="1:8">
@@ -31456,16 +31456,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E1250">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="F1250" s="2">
-        <v>45776.51189814815</v>
+        <v>45803.72575231481</v>
       </c>
       <c r="G1250">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H1250" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1251" spans="1:8">
@@ -31528,22 +31528,22 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>695</v>
+        <v>672</v>
       </c>
       <c r="D1253" s="2">
-        <v>45803.9069220483</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1253">
-        <v>749</v>
+        <v>672</v>
       </c>
       <c r="F1253" s="2">
-        <v>45803.49555555556</v>
+        <v>45804.51150462963</v>
       </c>
       <c r="G1253">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="H1253" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1254" spans="1:8">
@@ -33462,16 +33462,16 @@
         <v>1</v>
       </c>
       <c r="C1329">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D1329" s="2">
-        <v>45800.93194931293</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E1329">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F1329" s="2">
-        <v>45800.68467592593</v>
+        <v>45804.72743055555</v>
       </c>
       <c r="G1329">
         <v>0</v>
@@ -33797,16 +33797,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E1342">
-        <v>1771</v>
+        <v>1619</v>
       </c>
       <c r="F1342" s="2">
-        <v>45803.50018518518</v>
+        <v>45803.74128472222</v>
       </c>
       <c r="G1342">
-        <v>152</v>
+        <v>0</v>
       </c>
       <c r="H1342" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1343" spans="1:8">
@@ -35015,16 +35015,16 @@
         <v>1</v>
       </c>
       <c r="C1390">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D1390" s="2">
-        <v>45800.93175380815</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E1390">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F1390" s="2">
-        <v>45800.46056712963</v>
+        <v>45804.76886574074</v>
       </c>
       <c r="G1390">
         <v>0</v>
@@ -35047,16 +35047,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E1391">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F1391" s="2">
-        <v>45792.45592592593</v>
+        <v>45803.74012731481</v>
       </c>
       <c r="G1391">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H1391" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1392" spans="1:8">
@@ -35073,16 +35073,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E1392">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F1392" s="2">
-        <v>45784.64537037037</v>
+        <v>45803.7415625</v>
       </c>
       <c r="G1392">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H1392" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1393" spans="1:8">
@@ -35093,16 +35093,16 @@
         <v>1</v>
       </c>
       <c r="C1393">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D1393" s="2">
-        <v>45799.89536723674</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1393">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F1393" s="2">
-        <v>45797.76010416666</v>
+        <v>45804.42633101852</v>
       </c>
       <c r="G1393">
         <v>0</v>
@@ -35584,16 +35584,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E1412">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F1412" s="2">
-        <v>45803.4153125</v>
+        <v>45803.74012731481</v>
       </c>
       <c r="G1412">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1412" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1413" spans="1:8">
@@ -35604,16 +35604,16 @@
         <v>1</v>
       </c>
       <c r="C1413">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="D1413" s="2">
-        <v>45800.93204011993</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1413">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="F1413" s="2">
-        <v>45800.77331018518</v>
+        <v>45804.59533564815</v>
       </c>
       <c r="G1413">
         <v>0</v>
@@ -35806,16 +35806,16 @@
         <v>1</v>
       </c>
       <c r="C1421">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D1421" s="2">
-        <v>45800.93201923946</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E1421">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F1421" s="2">
-        <v>45800.40415509259</v>
+        <v>45804.76993055556</v>
       </c>
       <c r="G1421">
         <v>0</v>
@@ -35864,16 +35864,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E1423">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F1423" s="2">
-        <v>45792.65011574074</v>
+        <v>45803.72625</v>
       </c>
       <c r="G1423">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H1423" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1424" spans="1:8">
@@ -36447,16 +36447,16 @@
         <v>1</v>
       </c>
       <c r="C1446">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D1446" s="2">
-        <v>45799.89536724822</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1446">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F1446" s="2">
-        <v>45797.80143518518</v>
+        <v>45804.71377314815</v>
       </c>
       <c r="G1446">
         <v>0</v>
@@ -37376,16 +37376,16 @@
         <v>1</v>
       </c>
       <c r="C1483">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D1483" s="2">
-        <v>45798.9653592312</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E1483">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F1483" s="2">
-        <v>45798.71837962963</v>
+        <v>45804.76993055556</v>
       </c>
       <c r="G1483">
         <v>0</v>
@@ -38037,16 +38037,16 @@
         <v>1</v>
       </c>
       <c r="C1509">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1509" s="2">
-        <v>45799.89534674662</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E1509">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1509" s="2">
-        <v>45796.61327546297</v>
+        <v>45804.76886574074</v>
       </c>
       <c r="G1509">
         <v>0</v>
@@ -40151,7 +40151,7 @@
         <v>69</v>
       </c>
       <c r="F1594" s="2">
-        <v>45803.64673611111</v>
+        <v>45804.41571759259</v>
       </c>
       <c r="G1594">
         <v>0</v>
@@ -40220,22 +40220,22 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>7361</v>
+        <v>7347</v>
       </c>
       <c r="D1597" s="2">
-        <v>45803.90694023441</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E1597">
-        <v>7405</v>
+        <v>7347</v>
       </c>
       <c r="F1597" s="2">
-        <v>45803.49555555556</v>
+        <v>45804.76886574074</v>
       </c>
       <c r="G1597">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="H1597" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1598" spans="1:8">
@@ -41005,16 +41005,16 @@
         <v>1</v>
       </c>
       <c r="C1628">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1628" s="2">
-        <v>45799.89547823331</v>
+        <v>45804.91952539605</v>
       </c>
       <c r="E1628">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F1628" s="2">
-        <v>45793.66384259259</v>
+        <v>45804.39973379629</v>
       </c>
       <c r="G1628">
         <v>0</v>
@@ -41193,16 +41193,16 @@
         <v>45803.90692203668</v>
       </c>
       <c r="E1635">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F1635" s="2">
-        <v>45803.50018518518</v>
+        <v>45803.72625</v>
       </c>
       <c r="G1635">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H1635" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1636" spans="1:8">
@@ -42724,16 +42724,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E1697">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F1697" s="2">
-        <v>45792.65133101852</v>
+        <v>45803.7415625</v>
       </c>
       <c r="G1697">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H1697" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1698" spans="1:8">
@@ -43528,16 +43528,16 @@
         <v>1</v>
       </c>
       <c r="C1730">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D1730" s="2">
-        <v>45803.62109434994</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E1730">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F1730" s="2">
-        <v>45803.6213425926</v>
+        <v>45804.76993055556</v>
       </c>
       <c r="G1730">
         <v>0</v>
@@ -46696,16 +46696,16 @@
         <v>1</v>
       </c>
       <c r="C1856">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1856" s="2">
-        <v>45800.93175383128</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1856">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1856" s="2">
-        <v>45800.47983796296</v>
+        <v>45804.42633101852</v>
       </c>
       <c r="G1856">
         <v>0</v>
@@ -47060,16 +47060,16 @@
         <v>1</v>
       </c>
       <c r="C1870">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1870" s="2">
-        <v>45799.89528857399</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1870">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1870" s="2">
-        <v>45782.39422453703</v>
+        <v>45804.49641203704</v>
       </c>
       <c r="G1870">
         <v>0</v>
@@ -47317,16 +47317,16 @@
         <v>1</v>
       </c>
       <c r="C1880">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1880" s="2">
-        <v>45795.04208095842</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1880">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1880" s="2">
-        <v>45762.76935185185</v>
+        <v>45804.49947916667</v>
       </c>
       <c r="G1880">
         <v>0</v>
@@ -47891,16 +47891,16 @@
         <v>45803.9069220483</v>
       </c>
       <c r="E1903">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F1903" s="2">
-        <v>45797.67800925926</v>
+        <v>45803.74012731481</v>
       </c>
       <c r="G1903">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H1903" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="1904" spans="1:8">
@@ -48015,16 +48015,16 @@
         <v>1</v>
       </c>
       <c r="C1908">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1908" s="2">
-        <v>45795.04199234088</v>
+        <v>45804.91952539605</v>
       </c>
       <c r="E1908">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1908" s="2">
-        <v>45701.75829861111</v>
+        <v>45804.39973379629</v>
       </c>
       <c r="G1908">
         <v>0</v>
@@ -48119,16 +48119,16 @@
         <v>1</v>
       </c>
       <c r="C1912">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D1912" s="2">
-        <v>45799.89528858563</v>
+        <v>45804.91952539605</v>
       </c>
       <c r="E1912">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F1912" s="2">
-        <v>45783.66646990741</v>
+        <v>45804.39973379629</v>
       </c>
       <c r="G1912">
         <v>0</v>
@@ -48685,16 +48685,16 @@
         <v>1</v>
       </c>
       <c r="C1934">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1934" s="2">
-        <v>45795.04210567895</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E1934">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F1934" s="2">
-        <v>45777.61028935185</v>
+        <v>45804.42633101852</v>
       </c>
       <c r="G1934">
         <v>0</v>
@@ -51388,16 +51388,16 @@
         <v>1</v>
       </c>
       <c r="C2042">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2042" s="2">
-        <v>45799.89534672352</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E2042">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F2042" s="2">
-        <v>45792.72081018519</v>
+        <v>45804.76886574074</v>
       </c>
       <c r="G2042">
         <v>0</v>
@@ -54714,13 +54714,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E2175">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="F2175" s="2">
+        <v>45803.75266203703</v>
       </c>
       <c r="G2175">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H2175" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2176" spans="1:8">
@@ -54841,16 +54844,16 @@
         <v>45803.90694022291</v>
       </c>
       <c r="E2180">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F2180" s="2">
-        <v>45803.38509259259</v>
+        <v>45803.7415625</v>
       </c>
       <c r="G2180">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H2180" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2181" spans="1:8">
@@ -56232,16 +56235,16 @@
         <v>1</v>
       </c>
       <c r="C2235">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D2235" s="2">
-        <v>45799.89536724822</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E2235">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F2235" s="2">
-        <v>45798.63212962963</v>
+        <v>45804.59697916666</v>
       </c>
       <c r="G2235">
         <v>0</v>
@@ -58462,16 +58465,16 @@
         <v>1</v>
       </c>
       <c r="C2324">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D2324" s="2">
-        <v>45795.04190003897</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E2324">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F2324" s="2">
-        <v>45646.63540509259</v>
+        <v>45804.59592592593</v>
       </c>
       <c r="G2324">
         <v>0</v>
@@ -60749,22 +60752,22 @@
         <v>1</v>
       </c>
       <c r="C2416">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="D2416" s="2">
-        <v>45803.90694023441</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E2416">
-        <v>412</v>
+        <v>392</v>
       </c>
       <c r="F2416" s="2">
-        <v>45800.40415509259</v>
+        <v>45804.71377314815</v>
       </c>
       <c r="G2416">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H2416" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2417" spans="1:8">
@@ -62395,16 +62398,16 @@
         <v>1</v>
       </c>
       <c r="C2483">
-        <v>1013</v>
+        <v>1007</v>
       </c>
       <c r="D2483" s="2">
-        <v>45803.62106753104</v>
+        <v>45804.91952539605</v>
       </c>
       <c r="E2483">
-        <v>1013</v>
+        <v>1007</v>
       </c>
       <c r="F2483" s="2">
-        <v>45803.61216435185</v>
+        <v>45804.39973379629</v>
       </c>
       <c r="G2483">
         <v>0</v>
@@ -62421,16 +62424,16 @@
         <v>1</v>
       </c>
       <c r="C2484">
-        <v>1286</v>
+        <v>1086</v>
       </c>
       <c r="D2484" s="2">
-        <v>45800.93179064643</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E2484">
-        <v>1286</v>
+        <v>1086</v>
       </c>
       <c r="F2484" s="2">
-        <v>45800.48438657408</v>
+        <v>45804.57047453704</v>
       </c>
       <c r="G2484">
         <v>0</v>
@@ -62689,13 +62692,16 @@
         <v>1</v>
       </c>
       <c r="C2495">
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="D2495" s="2">
-        <v>45799.89532165734</v>
+        <v>45804.91952554927</v>
       </c>
       <c r="E2495">
-        <v>0</v>
+        <v>-200</v>
+      </c>
+      <c r="F2495" s="2">
+        <v>45804.71247685186</v>
       </c>
       <c r="G2495">
         <v>0</v>
@@ -63665,13 +63671,16 @@
         <v>1</v>
       </c>
       <c r="C2536">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="D2536" s="2">
-        <v>45803.62109434994</v>
+        <v>45804.91954472794</v>
       </c>
       <c r="E2536">
-        <v>0</v>
+        <v>-4</v>
+      </c>
+      <c r="F2536" s="2">
+        <v>45804.76993055556</v>
       </c>
       <c r="G2536">
         <v>0</v>
@@ -63700,6 +63709,101 @@
         <v>0</v>
       </c>
       <c r="H2537" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2538" spans="1:8">
+      <c r="A2538">
+        <v>43256930</v>
+      </c>
+      <c r="B2538">
+        <v>1</v>
+      </c>
+      <c r="C2538">
+        <v>0</v>
+      </c>
+      <c r="D2538" s="2">
+        <v>45804.91952554927</v>
+      </c>
+      <c r="E2538">
+        <v>0</v>
+      </c>
+      <c r="G2538">
+        <v>0</v>
+      </c>
+      <c r="H2538" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2539" spans="1:8">
+      <c r="A2539">
+        <v>43256945</v>
+      </c>
+      <c r="B2539">
+        <v>1</v>
+      </c>
+      <c r="C2539">
+        <v>0</v>
+      </c>
+      <c r="D2539" s="2">
+        <v>45804.91952554927</v>
+      </c>
+      <c r="E2539">
+        <v>0</v>
+      </c>
+      <c r="G2539">
+        <v>0</v>
+      </c>
+      <c r="H2539" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2540" spans="1:8">
+      <c r="A2540">
+        <v>43257727</v>
+      </c>
+      <c r="B2540">
+        <v>1</v>
+      </c>
+      <c r="C2540">
+        <v>0</v>
+      </c>
+      <c r="D2540" s="2">
+        <v>45804.91952554927</v>
+      </c>
+      <c r="E2540">
+        <v>0</v>
+      </c>
+      <c r="G2540">
+        <v>0</v>
+      </c>
+      <c r="H2540" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2541" spans="1:8">
+      <c r="A2541">
+        <v>43257788</v>
+      </c>
+      <c r="B2541">
+        <v>1</v>
+      </c>
+      <c r="C2541">
+        <v>-3</v>
+      </c>
+      <c r="D2541" s="2">
+        <v>45804.91952554927</v>
+      </c>
+      <c r="E2541">
+        <v>-3</v>
+      </c>
+      <c r="F2541" s="2">
+        <v>45804.53659722222</v>
+      </c>
+      <c r="G2541">
+        <v>0</v>
+      </c>
+      <c r="H2541" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ataulizacao dos dados da bibi e add
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2548" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2556" uniqueCount="10">
   <si>
     <t>id_produto</t>
   </si>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2541"/>
+  <dimension ref="A1:H2549"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,16 +494,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>45800.93194931293</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>45800.68467592593</v>
+        <v>45805.71751157408</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -520,16 +520,16 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2">
-        <v>45804.71377314815</v>
+        <v>45805.42017361111</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -952,16 +952,16 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="2">
-        <v>45803.62106753104</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E23">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23" s="2">
-        <v>45803.61216435185</v>
+        <v>45805.67193287037</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -978,16 +978,16 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D24" s="2">
-        <v>45803.62109434994</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F24" s="2">
-        <v>45803.62967592593</v>
+        <v>45805.69929398148</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1194,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>1062</v>
+        <v>1005</v>
       </c>
       <c r="D33" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E33">
-        <v>1062</v>
+        <v>1005</v>
       </c>
       <c r="F33" s="2">
-        <v>45804.46582175926</v>
+        <v>45805.76121527778</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1589,16 +1589,16 @@
         <v>1</v>
       </c>
       <c r="C49">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="D49" s="2">
-        <v>45803.90694022291</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E49">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F49" s="2">
-        <v>45803.77322916667</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -1765,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D56" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E56">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F56" s="2">
-        <v>45804.72743055555</v>
+        <v>45805.42017361111</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -1817,16 +1817,16 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D58" s="2">
-        <v>45803.90694022291</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E58">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F58" s="2">
-        <v>45803.75170138889</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -1892,16 +1892,16 @@
         <v>1</v>
       </c>
       <c r="C61">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D61" s="2">
-        <v>45798.96533509644</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E61">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F61" s="2">
-        <v>45798.43516203704</v>
+        <v>45805.76144675926</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -1941,16 +1941,16 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D63" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E63">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="F63" s="2">
-        <v>45804.72743055555</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2088,16 +2088,16 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D69" s="2">
-        <v>45799.89534672352</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E69">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F69" s="2">
-        <v>45792.72081018519</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -2114,16 +2114,16 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D70" s="2">
-        <v>45803.90694022291</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E70">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F70" s="2">
-        <v>45804.41571759259</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2376,16 +2376,16 @@
         <v>1</v>
       </c>
       <c r="C81">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D81" s="2">
-        <v>45803.90694022291</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E81">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F81" s="2">
-        <v>45804.41571759259</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -2428,16 +2428,16 @@
         <v>1</v>
       </c>
       <c r="C83">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D83" s="2">
-        <v>45803.62109434994</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E83">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F83" s="2">
-        <v>45804.41571759259</v>
+        <v>45805.65172453703</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -2503,16 +2503,16 @@
         <v>1</v>
       </c>
       <c r="C86">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D86" s="2">
-        <v>45803.90694022291</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E86">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F86" s="2">
-        <v>45804.41571759259</v>
+        <v>45805.76913194444</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -2529,16 +2529,16 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>-2</v>
+        <v>-8</v>
       </c>
       <c r="D87" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E87">
-        <v>-2</v>
+        <v>-8</v>
       </c>
       <c r="F87" s="2">
-        <v>45804.76971064815</v>
+        <v>45805.75204861111</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -2630,16 +2630,16 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="D91" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E91">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="F91" s="2">
-        <v>45804.72743055555</v>
+        <v>45805.74873842593</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -2702,16 +2702,16 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D94" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E94">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F94" s="2">
-        <v>45804.76993055556</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -2872,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>1791</v>
+        <v>1600</v>
       </c>
       <c r="D101" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E101">
-        <v>1791</v>
+        <v>1600</v>
       </c>
       <c r="F101" s="2">
-        <v>45804.46582175926</v>
+        <v>45805.76913194444</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -3160,16 +3160,16 @@
         <v>1</v>
       </c>
       <c r="C113">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D113" s="2">
-        <v>45799.89536723674</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E113">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="F113" s="2">
-        <v>45797.76186342593</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -3258,16 +3258,16 @@
         <v>1</v>
       </c>
       <c r="C117">
-        <v>1202</v>
+        <v>1194</v>
       </c>
       <c r="D117" s="2">
-        <v>45803.62106753104</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E117">
-        <v>1202</v>
+        <v>1194</v>
       </c>
       <c r="F117" s="2">
-        <v>45804.41571759259</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -3359,16 +3359,16 @@
         <v>1</v>
       </c>
       <c r="C121">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D121" s="2">
-        <v>45800.93197721101</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E121">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="F121" s="2">
-        <v>45803.70542824074</v>
+        <v>45805.76121527778</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -3408,16 +3408,16 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D123" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E123">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F123" s="2">
-        <v>45804.72743055555</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -3434,16 +3434,16 @@
         <v>1</v>
       </c>
       <c r="C124">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D124" s="2">
-        <v>45799.89536723674</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E124">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F124" s="2">
-        <v>45797.50270833333</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -3460,16 +3460,16 @@
         <v>1</v>
       </c>
       <c r="C125">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="D125" s="2">
-        <v>45799.89536723674</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E125">
-        <v>386</v>
+        <v>367</v>
       </c>
       <c r="F125" s="2">
-        <v>45797.63975694445</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -3486,16 +3486,16 @@
         <v>1</v>
       </c>
       <c r="C126">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D126" s="2">
-        <v>45798.96533511975</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E126">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F126" s="2">
-        <v>45798.69538194445</v>
+        <v>45805.76144675926</v>
       </c>
       <c r="G126">
         <v>0</v>
@@ -3846,16 +3846,16 @@
         <v>1</v>
       </c>
       <c r="C141">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="D141" s="2">
-        <v>45803.90692203668</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E141">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="F141" s="2">
-        <v>45803.72625</v>
+        <v>45805.70947916667</v>
       </c>
       <c r="G141">
         <v>0</v>
@@ -4936,16 +4936,16 @@
         <v>1</v>
       </c>
       <c r="C185">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D185" s="2">
-        <v>45803.90692203668</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E185">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F185" s="2">
-        <v>45803.73960648148</v>
+        <v>45805.70012731481</v>
       </c>
       <c r="G185">
         <v>0</v>
@@ -5253,16 +5253,16 @@
         <v>1</v>
       </c>
       <c r="C198">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D198" s="2">
-        <v>45795.04208095842</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E198">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F198" s="2">
-        <v>45770.695625</v>
+        <v>45805.62515046296</v>
       </c>
       <c r="G198">
         <v>0</v>
@@ -5302,16 +5302,16 @@
         <v>1</v>
       </c>
       <c r="C200">
-        <v>594</v>
+        <v>569</v>
       </c>
       <c r="D200" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E200">
-        <v>594</v>
+        <v>569</v>
       </c>
       <c r="F200" s="2">
-        <v>45804.72743055555</v>
+        <v>45805.70947916667</v>
       </c>
       <c r="G200">
         <v>0</v>
@@ -5328,16 +5328,16 @@
         <v>1</v>
       </c>
       <c r="C201">
-        <v>1104</v>
+        <v>1066</v>
       </c>
       <c r="D201" s="2">
-        <v>45804.91952539605</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E201">
-        <v>1104</v>
+        <v>1066</v>
       </c>
       <c r="F201" s="2">
-        <v>45804.39973379629</v>
+        <v>45805.70947916667</v>
       </c>
       <c r="G201">
         <v>0</v>
@@ -5521,16 +5521,16 @@
         <v>1</v>
       </c>
       <c r="C209">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D209" s="2">
-        <v>45803.62109434994</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E209">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F209" s="2">
-        <v>45803.62967592593</v>
+        <v>45805.76913194444</v>
       </c>
       <c r="G209">
         <v>0</v>
@@ -5737,16 +5737,16 @@
         <v>1</v>
       </c>
       <c r="C218">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D218" s="2">
-        <v>45803.90694022291</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E218">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F218" s="2">
-        <v>45804.41571759259</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G218">
         <v>0</v>
@@ -5835,16 +5835,16 @@
         <v>1</v>
       </c>
       <c r="C222">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D222" s="2">
-        <v>45800.93188814504</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E222">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F222" s="2">
-        <v>45800.61884259259</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G222">
         <v>0</v>
@@ -6175,16 +6175,16 @@
         <v>1</v>
       </c>
       <c r="C236">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="D236" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E236">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F236" s="2">
-        <v>45804.67836805555</v>
+        <v>45805.70140046296</v>
       </c>
       <c r="G236">
         <v>0</v>
@@ -6437,16 +6437,16 @@
         <v>1</v>
       </c>
       <c r="C247">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D247" s="2">
-        <v>45799.895427387</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E247">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F247" s="2">
-        <v>45799.67892361111</v>
+        <v>45805.65172453703</v>
       </c>
       <c r="G247">
         <v>0</v>
@@ -6627,16 +6627,16 @@
         <v>1</v>
       </c>
       <c r="C255">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="D255" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E255">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="F255" s="2">
-        <v>45804.67107638889</v>
+        <v>45805.69929398148</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -6996,16 +6996,16 @@
         <v>1</v>
       </c>
       <c r="C270">
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="D270" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E270">
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="F270" s="2">
-        <v>45804.72743055555</v>
+        <v>45805.40565972222</v>
       </c>
       <c r="G270">
         <v>0</v>
@@ -7071,16 +7071,16 @@
         <v>1</v>
       </c>
       <c r="C273">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D273" s="2">
-        <v>45799.895451121</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E273">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F273" s="2">
-        <v>45792.44024305556</v>
+        <v>45805.70140046296</v>
       </c>
       <c r="G273">
         <v>0</v>
@@ -7097,16 +7097,16 @@
         <v>1</v>
       </c>
       <c r="C274">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D274" s="2">
-        <v>45800.93201925102</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E274">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F274" s="2">
-        <v>45800.75802083333</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G274">
         <v>0</v>
@@ -7610,16 +7610,16 @@
         <v>1</v>
       </c>
       <c r="C295">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D295" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E295">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="F295" s="2">
-        <v>45804.45849537037</v>
+        <v>45805.70947916667</v>
       </c>
       <c r="G295">
         <v>0</v>
@@ -7953,16 +7953,16 @@
         <v>1</v>
       </c>
       <c r="C309">
-        <v>1237</v>
+        <v>1218</v>
       </c>
       <c r="D309" s="2">
-        <v>45803.90694022291</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E309">
-        <v>1237</v>
+        <v>1218</v>
       </c>
       <c r="F309" s="2">
-        <v>45804.41571759259</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G309">
         <v>0</v>
@@ -8071,16 +8071,16 @@
         <v>1</v>
       </c>
       <c r="C314">
-        <v>12</v>
+        <v>-3</v>
       </c>
       <c r="D314" s="2">
-        <v>45803.62109434994</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E314">
-        <v>12</v>
+        <v>-3</v>
       </c>
       <c r="F314" s="2">
-        <v>45803.64980324074</v>
+        <v>45805.74873842593</v>
       </c>
       <c r="G314">
         <v>0</v>
@@ -8169,16 +8169,16 @@
         <v>1</v>
       </c>
       <c r="C318">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D318" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E318">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F318" s="2">
-        <v>45804.43686342592</v>
+        <v>45805.76313657407</v>
       </c>
       <c r="G318">
         <v>0</v>
@@ -8374,16 +8374,16 @@
         <v>1</v>
       </c>
       <c r="C326">
-        <v>3</v>
+        <v>-27</v>
       </c>
       <c r="D326" s="2">
-        <v>45803.9069220483</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E326">
-        <v>3</v>
+        <v>-27</v>
       </c>
       <c r="F326" s="2">
-        <v>45803.7415625</v>
+        <v>45805.65172453703</v>
       </c>
       <c r="G326">
         <v>0</v>
@@ -8426,16 +8426,16 @@
         <v>1</v>
       </c>
       <c r="C328">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D328" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E328">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F328" s="2">
-        <v>45804.49947916667</v>
+        <v>45805.69929398148</v>
       </c>
       <c r="G328">
         <v>0</v>
@@ -8870,16 +8870,16 @@
         <v>1</v>
       </c>
       <c r="C346">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D346" s="2">
-        <v>45803.90692203668</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E346">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F346" s="2">
-        <v>45803.72625</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G346">
         <v>0</v>
@@ -8965,16 +8965,16 @@
         <v>1</v>
       </c>
       <c r="C350">
-        <v>-30</v>
+        <v>290</v>
       </c>
       <c r="D350" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E350">
-        <v>-30</v>
+        <v>290</v>
       </c>
       <c r="F350" s="2">
-        <v>45804.51150462963</v>
+        <v>45805.66680555556</v>
       </c>
       <c r="G350">
         <v>0</v>
@@ -8991,16 +8991,16 @@
         <v>1</v>
       </c>
       <c r="C351">
-        <v>353</v>
+        <v>283</v>
       </c>
       <c r="D351" s="2">
-        <v>45800.93188814504</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E351">
-        <v>353</v>
+        <v>283</v>
       </c>
       <c r="F351" s="2">
-        <v>45800.62752314815</v>
+        <v>45805.70947916667</v>
       </c>
       <c r="G351">
         <v>0</v>
@@ -9017,16 +9017,16 @@
         <v>1</v>
       </c>
       <c r="C352">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="D352" s="2">
-        <v>45799.89532164588</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E352">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="F352" s="2">
-        <v>45786.43359953703</v>
+        <v>45805.67193287037</v>
       </c>
       <c r="G352">
         <v>0</v>
@@ -9066,16 +9066,16 @@
         <v>1</v>
       </c>
       <c r="C354">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D354" s="2">
-        <v>45803.90692203668</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E354">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F354" s="2">
-        <v>45803.72625</v>
+        <v>45805.74226851852</v>
       </c>
       <c r="G354">
         <v>0</v>
@@ -9291,16 +9291,16 @@
         <v>1</v>
       </c>
       <c r="C363">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="D363" s="2">
-        <v>45803.9069220483</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E363">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="F363" s="2">
-        <v>45803.74128472222</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G363">
         <v>0</v>
@@ -9487,16 +9487,16 @@
         <v>1</v>
       </c>
       <c r="C371">
-        <v>230</v>
+        <v>190</v>
       </c>
       <c r="D371" s="2">
-        <v>45799.89536722513</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E371">
-        <v>230</v>
+        <v>190</v>
       </c>
       <c r="F371" s="2">
-        <v>45796.76049768519</v>
+        <v>45805.76121527778</v>
       </c>
       <c r="G371">
         <v>0</v>
@@ -9943,16 +9943,16 @@
         <v>1</v>
       </c>
       <c r="C389">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D389" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E389">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="F389" s="2">
-        <v>45804.74640046297</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G389">
         <v>0</v>
@@ -9969,16 +9969,16 @@
         <v>1</v>
       </c>
       <c r="C390">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D390" s="2">
-        <v>45800.93197718772</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E390">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F390" s="2">
-        <v>45803.77322916667</v>
+        <v>45805.70947916667</v>
       </c>
       <c r="G390">
         <v>0</v>
@@ -10070,16 +10070,16 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D394" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E394">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F394" s="2">
-        <v>45804.72743055555</v>
+        <v>45805.74280092592</v>
       </c>
       <c r="G394">
         <v>0</v>
@@ -10549,16 +10549,16 @@
         <v>1</v>
       </c>
       <c r="C413">
-        <v>300</v>
+        <v>258</v>
       </c>
       <c r="D413" s="2">
-        <v>45804.91952539605</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E413">
-        <v>300</v>
+        <v>258</v>
       </c>
       <c r="F413" s="2">
-        <v>45804.39973379629</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G413">
         <v>0</v>
@@ -10771,16 +10771,16 @@
         <v>1</v>
       </c>
       <c r="C422">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="D422" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E422">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="F422" s="2">
-        <v>45804.72743055555</v>
+        <v>45805.76913194444</v>
       </c>
       <c r="G422">
         <v>0</v>
@@ -12207,16 +12207,16 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>-47</v>
+        <v>-59</v>
       </c>
       <c r="D480" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E480">
-        <v>-47</v>
+        <v>-59</v>
       </c>
       <c r="F480" s="2">
-        <v>45804.77440972222</v>
+        <v>45805.76121527778</v>
       </c>
       <c r="G480">
         <v>0</v>
@@ -12951,16 +12951,16 @@
         <v>1</v>
       </c>
       <c r="C510">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D510" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E510">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="F510" s="2">
-        <v>45804.72743055555</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G510">
         <v>0</v>
@@ -13643,16 +13643,16 @@
         <v>1</v>
       </c>
       <c r="C538">
-        <v>4</v>
+        <v>-6</v>
       </c>
       <c r="D538" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E538">
-        <v>4</v>
+        <v>-6</v>
       </c>
       <c r="F538" s="2">
-        <v>45804.45869212963</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G538">
         <v>0</v>
@@ -14415,16 +14415,16 @@
         <v>1</v>
       </c>
       <c r="C570">
-        <v>2754</v>
+        <v>2729</v>
       </c>
       <c r="D570" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E570">
-        <v>2754</v>
+        <v>2729</v>
       </c>
       <c r="F570" s="2">
-        <v>45804.76886574074</v>
+        <v>45805.74873842593</v>
       </c>
       <c r="G570">
         <v>0</v>
@@ -14510,16 +14510,16 @@
         <v>1</v>
       </c>
       <c r="C574">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D574" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E574">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F574" s="2">
-        <v>45804.53324074074</v>
+        <v>45805.46181712963</v>
       </c>
       <c r="G574">
         <v>0</v>
@@ -15495,16 +15495,16 @@
         <v>1</v>
       </c>
       <c r="C615">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="D615" s="2">
-        <v>45799.89532164588</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E615">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="F615" s="2">
-        <v>45786.46802083333</v>
+        <v>45805.76121527778</v>
       </c>
       <c r="G615">
         <v>0</v>
@@ -15930,16 +15930,16 @@
         <v>1</v>
       </c>
       <c r="C633">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D633" s="2">
-        <v>45799.89532163485</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E633">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F633" s="2">
-        <v>45785.42679398148</v>
+        <v>45805.74226851852</v>
       </c>
       <c r="G633">
         <v>0</v>
@@ -16509,16 +16509,16 @@
         <v>1</v>
       </c>
       <c r="C657">
-        <v>2375</v>
+        <v>2367</v>
       </c>
       <c r="D657" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E657">
-        <v>2375</v>
+        <v>2367</v>
       </c>
       <c r="F657" s="2">
-        <v>45804.72743055555</v>
+        <v>45805.70140046296</v>
       </c>
       <c r="G657">
         <v>0</v>
@@ -17094,16 +17094,16 @@
         <v>1</v>
       </c>
       <c r="C681">
-        <v>-12</v>
+        <v>12</v>
       </c>
       <c r="D681" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E681">
-        <v>-12</v>
+        <v>12</v>
       </c>
       <c r="F681" s="2">
-        <v>45804.77440972222</v>
+        <v>45805.6750925926</v>
       </c>
       <c r="G681">
         <v>0</v>
@@ -17290,16 +17290,16 @@
         <v>1</v>
       </c>
       <c r="C689">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="D689" s="2">
-        <v>45799.89532165734</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E689">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="F689" s="2">
-        <v>45790.3869212963</v>
+        <v>45805.62515046296</v>
       </c>
       <c r="G689">
         <v>0</v>
@@ -17342,16 +17342,16 @@
         <v>1</v>
       </c>
       <c r="C691">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D691" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E691">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="F691" s="2">
-        <v>45804.67836805555</v>
+        <v>45805.76913194444</v>
       </c>
       <c r="G691">
         <v>0</v>
@@ -17599,16 +17599,16 @@
         <v>1</v>
       </c>
       <c r="C701">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D701" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E701">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F701" s="2">
-        <v>45804.45869212963</v>
+        <v>45805.42017361111</v>
       </c>
       <c r="G701">
         <v>0</v>
@@ -17648,16 +17648,16 @@
         <v>1</v>
       </c>
       <c r="C703">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="D703" s="2">
-        <v>45799.89536722513</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E703">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="F703" s="2">
-        <v>45796.76049768519</v>
+        <v>45805.74873842593</v>
       </c>
       <c r="G703">
         <v>0</v>
@@ -17746,16 +17746,16 @@
         <v>1</v>
       </c>
       <c r="C707">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="D707" s="2">
-        <v>45799.89528858563</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E707">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="F707" s="2">
-        <v>45803.77025462963</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G707">
         <v>0</v>
@@ -18072,16 +18072,16 @@
         <v>1</v>
       </c>
       <c r="C720">
-        <v>765</v>
+        <v>750</v>
       </c>
       <c r="D720" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E720">
-        <v>765</v>
+        <v>750</v>
       </c>
       <c r="F720" s="2">
-        <v>45804.76993055556</v>
+        <v>45805.76121527778</v>
       </c>
       <c r="G720">
         <v>0</v>
@@ -18228,16 +18228,16 @@
         <v>1</v>
       </c>
       <c r="C726">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="D726" s="2">
-        <v>45799.89534673509</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E726">
-        <v>355</v>
+        <v>335</v>
       </c>
       <c r="F726" s="2">
-        <v>45796.49008101852</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G726">
         <v>0</v>
@@ -18560,16 +18560,16 @@
         <v>1</v>
       </c>
       <c r="C739">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D739" s="2">
-        <v>45799.89532165734</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E739">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F739" s="2">
-        <v>45789.63391203704</v>
+        <v>45805.76938657407</v>
       </c>
       <c r="G739">
         <v>0</v>
@@ -19206,16 +19206,16 @@
         <v>1</v>
       </c>
       <c r="C765">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D765" s="2">
-        <v>45795.04208095842</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E765">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F765" s="2">
-        <v>45764.54935185185</v>
+        <v>45805.62515046296</v>
       </c>
       <c r="G765">
         <v>0</v>
@@ -19535,16 +19535,16 @@
         <v>1</v>
       </c>
       <c r="C778">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D778" s="2">
-        <v>45800.93197722271</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E778">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F778" s="2">
-        <v>45800.6955787037</v>
+        <v>45805.42017361111</v>
       </c>
       <c r="G778">
         <v>0</v>
@@ -19587,16 +19587,16 @@
         <v>1</v>
       </c>
       <c r="C780">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D780" s="2">
-        <v>45795.04204563411</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E780">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F780" s="2">
-        <v>45754.49483796296</v>
+        <v>45805.65172453703</v>
       </c>
       <c r="G780">
         <v>0</v>
@@ -20732,16 +20732,16 @@
         <v>1</v>
       </c>
       <c r="C826">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D826" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E826">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F826" s="2">
-        <v>45804.42633101852</v>
+        <v>45805.74873842593</v>
       </c>
       <c r="G826">
         <v>0</v>
@@ -21389,16 +21389,16 @@
         <v>1</v>
       </c>
       <c r="C853">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D853" s="2">
-        <v>45803.9069220483</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E853">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F853" s="2">
-        <v>45803.74012731481</v>
+        <v>45805.70947916667</v>
       </c>
       <c r="G853">
         <v>0</v>
@@ -21415,16 +21415,16 @@
         <v>1</v>
       </c>
       <c r="C854">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D854" s="2">
-        <v>45799.89542739857</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E854">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F854" s="2">
-        <v>45796.61327546297</v>
+        <v>45805.67193287037</v>
       </c>
       <c r="G854">
         <v>0</v>
@@ -21689,16 +21689,16 @@
         <v>1</v>
       </c>
       <c r="C865">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D865" s="2">
-        <v>45799.89528858563</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E865">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F865" s="2">
-        <v>45782.65074074074</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G865">
         <v>0</v>
@@ -22145,16 +22145,16 @@
         <v>1</v>
       </c>
       <c r="C883">
-        <v>321</v>
+        <v>292</v>
       </c>
       <c r="D883" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E883">
-        <v>321</v>
+        <v>292</v>
       </c>
       <c r="F883" s="2">
-        <v>45804.76886574074</v>
+        <v>45805.70012731481</v>
       </c>
       <c r="G883">
         <v>0</v>
@@ -22272,16 +22272,16 @@
         <v>1</v>
       </c>
       <c r="C888">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D888" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E888">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F888" s="2">
-        <v>45804.72743055555</v>
+        <v>45805.62515046296</v>
       </c>
       <c r="G888">
         <v>0</v>
@@ -22627,16 +22627,16 @@
         <v>1</v>
       </c>
       <c r="C902">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D902" s="2">
-        <v>45798.96533509644</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E902">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F902" s="2">
-        <v>45798.64170138889</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G902">
         <v>0</v>
@@ -22679,16 +22679,16 @@
         <v>1</v>
       </c>
       <c r="C904">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="D904" s="2">
-        <v>45795.04210567895</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E904">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="F904" s="2">
-        <v>45777.60503472222</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G904">
         <v>0</v>
@@ -23187,16 +23187,16 @@
         <v>1</v>
       </c>
       <c r="C924">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D924" s="2">
-        <v>45803.9069220483</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E924">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="F924" s="2">
-        <v>45803.74012731481</v>
+        <v>45805.42017361111</v>
       </c>
       <c r="G924">
         <v>0</v>
@@ -23848,16 +23848,16 @@
         <v>1</v>
       </c>
       <c r="C950">
-        <v>6</v>
+        <v>-4</v>
       </c>
       <c r="D950" s="2">
-        <v>45800.93204010786</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E950">
-        <v>6</v>
+        <v>-4</v>
       </c>
       <c r="F950" s="2">
-        <v>45800.75802083333</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G950">
         <v>0</v>
@@ -24110,16 +24110,16 @@
         <v>1</v>
       </c>
       <c r="C961">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D961" s="2">
-        <v>45799.89532164588</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E961">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F961" s="2">
-        <v>45786.61480324074</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G961">
         <v>0</v>
@@ -24136,16 +24136,16 @@
         <v>1</v>
       </c>
       <c r="C962">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="D962" s="2">
-        <v>45803.9069220483</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E962">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="F962" s="2">
-        <v>45803.74012731481</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G962">
         <v>0</v>
@@ -24162,16 +24162,16 @@
         <v>1</v>
       </c>
       <c r="C963">
-        <v>915</v>
+        <v>875</v>
       </c>
       <c r="D963" s="2">
-        <v>45803.90692203668</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E963">
-        <v>915</v>
+        <v>875</v>
       </c>
       <c r="F963" s="2">
-        <v>45803.72625</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G963">
         <v>0</v>
@@ -24999,16 +24999,16 @@
         <v>1</v>
       </c>
       <c r="C996">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D996" s="2">
-        <v>45795.04210567895</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E996">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F996" s="2">
-        <v>45777.66376157408</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G996">
         <v>0</v>
@@ -26116,16 +26116,16 @@
         <v>1</v>
       </c>
       <c r="C1040">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1040" s="2">
-        <v>45795.04204563411</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1040">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1040" s="2">
-        <v>45751.45496527778</v>
+        <v>45805.74280092592</v>
       </c>
       <c r="G1040">
         <v>0</v>
@@ -26598,16 +26598,16 @@
         <v>1</v>
       </c>
       <c r="C1059">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1059" s="2">
-        <v>45795.04210567895</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E1059">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F1059" s="2">
-        <v>45776.64395833333</v>
+        <v>45805.70012731481</v>
       </c>
       <c r="G1059">
         <v>0</v>
@@ -27492,16 +27492,16 @@
         <v>1</v>
       </c>
       <c r="C1095">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="D1095" s="2">
-        <v>45795.04199234088</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1095">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="F1095" s="2">
-        <v>45702.38758101852</v>
+        <v>45805.62515046296</v>
       </c>
       <c r="G1095">
         <v>0</v>
@@ -27564,16 +27564,16 @@
         <v>1</v>
       </c>
       <c r="C1098">
-        <v>8</v>
+        <v>-32</v>
       </c>
       <c r="D1098" s="2">
-        <v>45799.89534674662</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1098">
-        <v>8</v>
+        <v>-32</v>
       </c>
       <c r="F1098" s="2">
-        <v>45796.49008101852</v>
+        <v>45805.76121527778</v>
       </c>
       <c r="G1098">
         <v>0</v>
@@ -27674,7 +27674,7 @@
         <v>59</v>
       </c>
       <c r="F1102" s="2">
-        <v>45770.74755787037</v>
+        <v>45805.76913194444</v>
       </c>
       <c r="G1102">
         <v>0</v>
@@ -27867,16 +27867,16 @@
         <v>1</v>
       </c>
       <c r="C1110">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D1110" s="2">
-        <v>45803.90694022291</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E1110">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F1110" s="2">
-        <v>45803.7415625</v>
+        <v>45805.70140046296</v>
       </c>
       <c r="G1110">
         <v>0</v>
@@ -27942,16 +27942,16 @@
         <v>1</v>
       </c>
       <c r="C1113">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1113" s="2">
-        <v>45799.89528857399</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E1113">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F1113" s="2">
-        <v>45779.72231481481</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G1113">
         <v>0</v>
@@ -28805,16 +28805,16 @@
         <v>1</v>
       </c>
       <c r="C1147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1147" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E1147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1147" s="2">
-        <v>45804.76971064815</v>
+        <v>45805.42017361111</v>
       </c>
       <c r="G1147">
         <v>0</v>
@@ -28909,16 +28909,16 @@
         <v>1</v>
       </c>
       <c r="C1151">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D1151" s="2">
-        <v>45799.89534673509</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E1151">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F1151" s="2">
-        <v>45793.60556712963</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G1151">
         <v>0</v>
@@ -28987,16 +28987,16 @@
         <v>1</v>
       </c>
       <c r="C1154">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D1154" s="2">
-        <v>45799.89528857399</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E1154">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F1154" s="2">
-        <v>45782.5897800926</v>
+        <v>45805.67193287037</v>
       </c>
       <c r="G1154">
         <v>0</v>
@@ -29013,16 +29013,16 @@
         <v>1</v>
       </c>
       <c r="C1155">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D1155" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E1155">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F1155" s="2">
-        <v>45804.76993055556</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G1155">
         <v>0</v>
@@ -29521,16 +29521,16 @@
         <v>1</v>
       </c>
       <c r="C1175">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D1175" s="2">
-        <v>45799.89532166889</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E1175">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F1175" s="2">
-        <v>45790.66951388889</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G1175">
         <v>0</v>
@@ -29573,16 +29573,16 @@
         <v>1</v>
       </c>
       <c r="C1177">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D1177" s="2">
-        <v>45803.62106753104</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E1177">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F1177" s="2">
-        <v>45803.51891203703</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G1177">
         <v>0</v>
@@ -29726,16 +29726,16 @@
         <v>1</v>
       </c>
       <c r="C1183">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D1183" s="2">
-        <v>45798.96533511975</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E1183">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F1183" s="2">
-        <v>45798.64541666667</v>
+        <v>45805.70140046296</v>
       </c>
       <c r="G1183">
         <v>0</v>
@@ -29830,16 +29830,16 @@
         <v>1</v>
       </c>
       <c r="C1187">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D1187" s="2">
-        <v>45800.93197722271</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1187">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F1187" s="2">
-        <v>45804.53158564815</v>
+        <v>45805.74873842593</v>
       </c>
       <c r="G1187">
         <v>0</v>
@@ -29934,16 +29934,16 @@
         <v>1</v>
       </c>
       <c r="C1191">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D1191" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E1191">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F1191" s="2">
-        <v>45804.69865740741</v>
+        <v>45805.67751157407</v>
       </c>
       <c r="G1191">
         <v>0</v>
@@ -30734,16 +30734,16 @@
         <v>1</v>
       </c>
       <c r="C1222">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1222" s="2">
-        <v>45799.89528858563</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1222">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F1222" s="2">
-        <v>45782.63818287037</v>
+        <v>45805.76913194444</v>
       </c>
       <c r="G1222">
         <v>0</v>
@@ -31528,16 +31528,16 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>672</v>
+        <v>619</v>
       </c>
       <c r="D1253" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1253">
-        <v>672</v>
+        <v>619</v>
       </c>
       <c r="F1253" s="2">
-        <v>45804.51150462963</v>
+        <v>45805.76121527778</v>
       </c>
       <c r="G1253">
         <v>0</v>
@@ -31863,16 +31863,16 @@
         <v>1</v>
       </c>
       <c r="C1266">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D1266" s="2">
-        <v>45795.04204563411</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E1266">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F1266" s="2">
-        <v>45747.75686342592</v>
+        <v>45805.65172453703</v>
       </c>
       <c r="G1266">
         <v>0</v>
@@ -32097,16 +32097,16 @@
         <v>1</v>
       </c>
       <c r="C1275">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1275" s="2">
-        <v>45795.04210567895</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E1275">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F1275" s="2">
-        <v>45776.6746875</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G1275">
         <v>0</v>
@@ -33488,16 +33488,16 @@
         <v>1</v>
       </c>
       <c r="C1330">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D1330" s="2">
-        <v>45798.96533509644</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E1330">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F1330" s="2">
-        <v>45798.44859953703</v>
+        <v>45805.69929398148</v>
       </c>
       <c r="G1330">
         <v>0</v>
@@ -33540,16 +33540,16 @@
         <v>1</v>
       </c>
       <c r="C1332">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D1332" s="2">
-        <v>45800.93197719934</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E1332">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F1332" s="2">
-        <v>45800.686875</v>
+        <v>45805.67422453704</v>
       </c>
       <c r="G1332">
         <v>0</v>
@@ -33791,16 +33791,16 @@
         <v>1</v>
       </c>
       <c r="C1342">
-        <v>1619</v>
+        <v>1563</v>
       </c>
       <c r="D1342" s="2">
-        <v>45803.9069220483</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E1342">
-        <v>1619</v>
+        <v>1563</v>
       </c>
       <c r="F1342" s="2">
-        <v>45803.74128472222</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G1342">
         <v>0</v>
@@ -34478,16 +34478,16 @@
         <v>1</v>
       </c>
       <c r="C1369">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="D1369" s="2">
-        <v>45799.89542739857</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E1369">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="F1369" s="2">
-        <v>45786.62262731481</v>
+        <v>45805.67193287037</v>
       </c>
       <c r="G1369">
         <v>0</v>
@@ -34963,16 +34963,16 @@
         <v>1</v>
       </c>
       <c r="C1388">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="D1388" s="2">
-        <v>45803.62106753104</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1388">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="F1388" s="2">
-        <v>45803.50018518518</v>
+        <v>45805.76121527778</v>
       </c>
       <c r="G1388">
         <v>0</v>
@@ -35041,16 +35041,16 @@
         <v>1</v>
       </c>
       <c r="C1391">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="D1391" s="2">
-        <v>45803.9069220483</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1391">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="F1391" s="2">
-        <v>45803.74012731481</v>
+        <v>45805.76913194444</v>
       </c>
       <c r="G1391">
         <v>0</v>
@@ -35832,16 +35832,16 @@
         <v>1</v>
       </c>
       <c r="C1422">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1422" s="2">
-        <v>45803.62106753104</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E1422">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F1422" s="2">
-        <v>45803.50018518518</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G1422">
         <v>0</v>
@@ -35858,16 +35858,16 @@
         <v>1</v>
       </c>
       <c r="C1423">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1423" s="2">
-        <v>45803.90692203668</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E1423">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1423" s="2">
-        <v>45803.72625</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G1423">
         <v>0</v>
@@ -36219,16 +36219,16 @@
         <v>1</v>
       </c>
       <c r="C1437">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1437" s="2">
-        <v>45795.0420164208</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E1437">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F1437" s="2">
-        <v>45727.40094907407</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G1437">
         <v>0</v>
@@ -38063,16 +38063,16 @@
         <v>1</v>
       </c>
       <c r="C1510">
-        <v>3</v>
+        <v>-7</v>
       </c>
       <c r="D1510" s="2">
-        <v>45799.89532163485</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E1510">
-        <v>3</v>
+        <v>-7</v>
       </c>
       <c r="F1510" s="2">
-        <v>45785.46993055556</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G1510">
         <v>0</v>
@@ -38328,16 +38328,16 @@
         <v>1</v>
       </c>
       <c r="C1521">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D1521" s="2">
-        <v>45795.04210567895</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1521">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F1521" s="2">
-        <v>45777.50487268518</v>
+        <v>45805.74226851852</v>
       </c>
       <c r="G1521">
         <v>0</v>
@@ -39467,16 +39467,16 @@
         <v>1</v>
       </c>
       <c r="C1567">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="D1567" s="2">
-        <v>45799.89540331678</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E1567">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="F1567" s="2">
-        <v>45799.61177083333</v>
+        <v>45805.69929398148</v>
       </c>
       <c r="G1567">
         <v>0</v>
@@ -39698,16 +39698,16 @@
         <v>1</v>
       </c>
       <c r="C1576">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D1576" s="2">
-        <v>45799.89532164588</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E1576">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="F1576" s="2">
-        <v>45786.62262731481</v>
+        <v>45805.67193287037</v>
       </c>
       <c r="G1576">
         <v>0</v>
@@ -40099,7 +40099,7 @@
         <v>0</v>
       </c>
       <c r="D1592" s="2">
-        <v>45795.04169367771</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E1592">
         <v>0</v>
@@ -40142,16 +40142,16 @@
         <v>1</v>
       </c>
       <c r="C1594">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D1594" s="2">
-        <v>45800.93204010786</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1594">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F1594" s="2">
-        <v>45804.41571759259</v>
+        <v>45805.74873842593</v>
       </c>
       <c r="G1594">
         <v>0</v>
@@ -40220,16 +40220,16 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>7347</v>
+        <v>7322</v>
       </c>
       <c r="D1597" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E1597">
-        <v>7347</v>
+        <v>7322</v>
       </c>
       <c r="F1597" s="2">
-        <v>45804.76886574074</v>
+        <v>45805.65172453703</v>
       </c>
       <c r="G1597">
         <v>0</v>
@@ -40295,16 +40295,16 @@
         <v>1</v>
       </c>
       <c r="C1600">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D1600" s="2">
-        <v>45799.89528859723</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1600">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="F1600" s="2">
-        <v>45784.6205787037</v>
+        <v>45805.74226851852</v>
       </c>
       <c r="G1600">
         <v>0</v>
@@ -41674,16 +41674,16 @@
         <v>1</v>
       </c>
       <c r="C1655">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D1655" s="2">
-        <v>45795.04204563411</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1655">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="F1655" s="2">
-        <v>45749.76723379629</v>
+        <v>45805.75204861111</v>
       </c>
       <c r="G1655">
         <v>0</v>
@@ -42986,16 +42986,16 @@
         <v>1</v>
       </c>
       <c r="C1708">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="D1708" s="2">
-        <v>45795.04169367771</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1708">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="F1708" s="2">
-        <v>45400.71608796297</v>
+        <v>45805.76121527778</v>
       </c>
       <c r="G1708">
         <v>0</v>
@@ -43724,16 +43724,16 @@
         <v>1</v>
       </c>
       <c r="C1738">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1738" s="2">
-        <v>45795.04210567895</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E1738">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1738" s="2">
-        <v>45776.70671296296</v>
+        <v>45805.76913194444</v>
       </c>
       <c r="G1738">
         <v>0</v>
@@ -45175,16 +45175,16 @@
         <v>1</v>
       </c>
       <c r="C1796">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D1796" s="2">
-        <v>45799.89542739857</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E1796">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F1796" s="2">
-        <v>45790.52543981482</v>
+        <v>45805.65278935185</v>
       </c>
       <c r="G1796">
         <v>0</v>
@@ -47060,16 +47060,16 @@
         <v>1</v>
       </c>
       <c r="C1870">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1870" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E1870">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F1870" s="2">
-        <v>45804.49641203704</v>
+        <v>45805.66414351852</v>
       </c>
       <c r="G1870">
         <v>0</v>
@@ -47274,7 +47274,7 @@
         <v>10</v>
       </c>
       <c r="F1878" s="2">
-        <v>45797.53369212963</v>
+        <v>45805.67422453704</v>
       </c>
       <c r="G1878">
         <v>0</v>
@@ -49856,7 +49856,7 @@
         <v>0</v>
       </c>
       <c r="D1981" s="2">
-        <v>45795.04186106093</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E1981">
         <v>0</v>
@@ -51206,16 +51206,16 @@
         <v>1</v>
       </c>
       <c r="C2035">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D2035" s="2">
-        <v>45795.04210567895</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E2035">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F2035" s="2">
-        <v>45777.66869212963</v>
+        <v>45805.65172453703</v>
       </c>
       <c r="G2035">
         <v>0</v>
@@ -51867,16 +51867,16 @@
         <v>1</v>
       </c>
       <c r="C2061">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2061" s="2">
-        <v>45795.04190003897</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E2061">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2061" s="2">
-        <v>45659.72938657407</v>
+        <v>45805.70869212963</v>
       </c>
       <c r="G2061">
         <v>0</v>
@@ -52822,16 +52822,16 @@
         <v>1</v>
       </c>
       <c r="C2099">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D2099" s="2">
-        <v>45798.96533509644</v>
+        <v>45805.91875150988</v>
       </c>
       <c r="E2099">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F2099" s="2">
-        <v>45798.44711805556</v>
+        <v>45805.62515046296</v>
       </c>
       <c r="G2099">
         <v>0</v>
@@ -55479,7 +55479,7 @@
         <v>0</v>
       </c>
       <c r="D2205" s="2">
-        <v>45795.0418106143</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E2205">
         <v>0</v>
@@ -56365,16 +56365,16 @@
         <v>1</v>
       </c>
       <c r="C2240">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="D2240" s="2">
-        <v>45803.62106753104</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E2240">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="F2240" s="2">
-        <v>45803.38153935185</v>
+        <v>45805.70947916667</v>
       </c>
       <c r="G2240">
         <v>0</v>
@@ -56391,16 +56391,16 @@
         <v>1</v>
       </c>
       <c r="C2241">
-        <v>386</v>
+        <v>330</v>
       </c>
       <c r="D2241" s="2">
-        <v>45799.89534671205</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E2241">
-        <v>386</v>
+        <v>330</v>
       </c>
       <c r="F2241" s="2">
-        <v>45792.52895833334</v>
+        <v>45805.70947916667</v>
       </c>
       <c r="G2241">
         <v>0</v>
@@ -57294,7 +57294,7 @@
         <v>0</v>
       </c>
       <c r="D2277" s="2">
-        <v>45795.04190003897</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E2277">
         <v>0</v>
@@ -58269,16 +58269,16 @@
         <v>1</v>
       </c>
       <c r="C2316">
-        <v>0</v>
+        <v>-30</v>
       </c>
       <c r="D2316" s="2">
-        <v>45799.89536722513</v>
+        <v>45805.91875154599</v>
       </c>
       <c r="E2316">
-        <v>0</v>
+        <v>-30</v>
       </c>
       <c r="F2316" s="2">
-        <v>45796.76170138889</v>
+        <v>45805.70905092593</v>
       </c>
       <c r="G2316">
         <v>0</v>
@@ -58728,7 +58728,7 @@
         <v>0</v>
       </c>
       <c r="D2334" s="2">
-        <v>45795.04190003897</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E2334">
         <v>0</v>
@@ -58754,7 +58754,7 @@
         <v>0</v>
       </c>
       <c r="D2335" s="2">
-        <v>45795.04190003897</v>
+        <v>45805.91872982616</v>
       </c>
       <c r="E2335">
         <v>0</v>
@@ -59097,16 +59097,16 @@
         <v>1</v>
       </c>
       <c r="C2349">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D2349" s="2">
-        <v>45795.04199224871</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E2349">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="F2349" s="2">
-        <v>45688.74428240741</v>
+        <v>45805.75204861111</v>
       </c>
       <c r="G2349">
         <v>0</v>
@@ -59198,16 +59198,16 @@
         <v>1</v>
       </c>
       <c r="C2353">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2353" s="2">
-        <v>45795.04193352044</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E2353">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2353" s="2">
-        <v>45660.45560185185</v>
+        <v>45805.76913194444</v>
       </c>
       <c r="G2353">
         <v>0</v>
@@ -61372,16 +61372,16 @@
         <v>1</v>
       </c>
       <c r="C2441">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D2441" s="2">
-        <v>45795.0420164208</v>
+        <v>45805.9187731686</v>
       </c>
       <c r="E2441">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F2441" s="2">
-        <v>45733.74019675926</v>
+        <v>45805.75204861111</v>
       </c>
       <c r="G2441">
         <v>0</v>
@@ -62692,16 +62692,16 @@
         <v>1</v>
       </c>
       <c r="C2495">
-        <v>-200</v>
+        <v>4</v>
       </c>
       <c r="D2495" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E2495">
-        <v>-200</v>
+        <v>4</v>
       </c>
       <c r="F2495" s="2">
-        <v>45804.71247685186</v>
+        <v>45805.6706712963</v>
       </c>
       <c r="G2495">
         <v>0</v>
@@ -63300,13 +63300,16 @@
         <v>1</v>
       </c>
       <c r="C2520">
-        <v>0</v>
+        <v>-300</v>
       </c>
       <c r="D2520" s="2">
-        <v>45800.93192368435</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E2520">
-        <v>0</v>
+        <v>-300</v>
+      </c>
+      <c r="F2520" s="2">
+        <v>45805.6905787037</v>
       </c>
       <c r="G2520">
         <v>0</v>
@@ -63323,13 +63326,16 @@
         <v>1</v>
       </c>
       <c r="C2521">
-        <v>0</v>
+        <v>-300</v>
       </c>
       <c r="D2521" s="2">
-        <v>45799.895451121</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E2521">
-        <v>0</v>
+        <v>-300</v>
+      </c>
+      <c r="F2521" s="2">
+        <v>45805.6905787037</v>
       </c>
       <c r="G2521">
         <v>0</v>
@@ -63671,16 +63677,16 @@
         <v>1</v>
       </c>
       <c r="C2536">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="D2536" s="2">
-        <v>45804.91954472794</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E2536">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="F2536" s="2">
-        <v>45804.76993055556</v>
+        <v>45805.67351851852</v>
       </c>
       <c r="G2536">
         <v>0</v>
@@ -63766,13 +63772,16 @@
         <v>1</v>
       </c>
       <c r="C2540">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D2540" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.91875152234</v>
       </c>
       <c r="E2540">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="F2540" s="2">
+        <v>45805.65278935185</v>
       </c>
       <c r="G2540">
         <v>0</v>
@@ -63789,21 +63798,205 @@
         <v>1</v>
       </c>
       <c r="C2541">
-        <v>-3</v>
+        <v>9</v>
       </c>
       <c r="D2541" s="2">
-        <v>45804.91952554927</v>
+        <v>45805.918751534</v>
       </c>
       <c r="E2541">
-        <v>-3</v>
+        <v>9</v>
       </c>
       <c r="F2541" s="2">
-        <v>45804.53659722222</v>
+        <v>45805.67633101852</v>
       </c>
       <c r="G2541">
         <v>0</v>
       </c>
       <c r="H2541" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2542" spans="1:8">
+      <c r="A2542">
+        <v>43279902</v>
+      </c>
+      <c r="B2542">
+        <v>1</v>
+      </c>
+      <c r="C2542">
+        <v>0</v>
+      </c>
+      <c r="D2542" s="2">
+        <v>45805.91872982616</v>
+      </c>
+      <c r="E2542">
+        <v>0</v>
+      </c>
+      <c r="G2542">
+        <v>0</v>
+      </c>
+      <c r="H2542" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2543" spans="1:8">
+      <c r="A2543">
+        <v>43279956</v>
+      </c>
+      <c r="B2543">
+        <v>1</v>
+      </c>
+      <c r="C2543">
+        <v>0</v>
+      </c>
+      <c r="D2543" s="2">
+        <v>45805.91872982616</v>
+      </c>
+      <c r="E2543">
+        <v>0</v>
+      </c>
+      <c r="G2543">
+        <v>0</v>
+      </c>
+      <c r="H2543" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2544" spans="1:8">
+      <c r="A2544">
+        <v>43279959</v>
+      </c>
+      <c r="B2544">
+        <v>1</v>
+      </c>
+      <c r="C2544">
+        <v>0</v>
+      </c>
+      <c r="D2544" s="2">
+        <v>45805.91872982616</v>
+      </c>
+      <c r="E2544">
+        <v>0</v>
+      </c>
+      <c r="G2544">
+        <v>0</v>
+      </c>
+      <c r="H2544" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2545" spans="1:8">
+      <c r="A2545">
+        <v>43279975</v>
+      </c>
+      <c r="B2545">
+        <v>1</v>
+      </c>
+      <c r="C2545">
+        <v>0</v>
+      </c>
+      <c r="D2545" s="2">
+        <v>45805.91875150988</v>
+      </c>
+      <c r="E2545">
+        <v>0</v>
+      </c>
+      <c r="G2545">
+        <v>0</v>
+      </c>
+      <c r="H2545" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2546" spans="1:8">
+      <c r="A2546">
+        <v>43279982</v>
+      </c>
+      <c r="B2546">
+        <v>1</v>
+      </c>
+      <c r="C2546">
+        <v>0</v>
+      </c>
+      <c r="D2546" s="2">
+        <v>45805.91875150988</v>
+      </c>
+      <c r="E2546">
+        <v>0</v>
+      </c>
+      <c r="G2546">
+        <v>0</v>
+      </c>
+      <c r="H2546" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2547" spans="1:8">
+      <c r="A2547">
+        <v>43280159</v>
+      </c>
+      <c r="B2547">
+        <v>1</v>
+      </c>
+      <c r="C2547">
+        <v>0</v>
+      </c>
+      <c r="D2547" s="2">
+        <v>45805.91875150988</v>
+      </c>
+      <c r="E2547">
+        <v>0</v>
+      </c>
+      <c r="G2547">
+        <v>0</v>
+      </c>
+      <c r="H2547" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2548" spans="1:8">
+      <c r="A2548">
+        <v>43280202</v>
+      </c>
+      <c r="B2548">
+        <v>1</v>
+      </c>
+      <c r="C2548">
+        <v>0</v>
+      </c>
+      <c r="D2548" s="2">
+        <v>45805.91875150988</v>
+      </c>
+      <c r="E2548">
+        <v>0</v>
+      </c>
+      <c r="G2548">
+        <v>0</v>
+      </c>
+      <c r="H2548" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2549" spans="1:8">
+      <c r="A2549">
+        <v>43283496</v>
+      </c>
+      <c r="B2549">
+        <v>1</v>
+      </c>
+      <c r="C2549">
+        <v>0</v>
+      </c>
+      <c r="D2549" s="2">
+        <v>45805.91875152234</v>
+      </c>
+      <c r="E2549">
+        <v>0</v>
+      </c>
+      <c r="G2549">
+        <v>0</v>
+      </c>
+      <c r="H2549" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizacao dos dados bibi e add
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2558" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2561" uniqueCount="10">
   <si>
     <t>id_produto</t>
   </si>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2551"/>
+  <dimension ref="A1:H2554"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,10 +494,10 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
-        <v>45805.9187731686</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -506,10 +506,10 @@
         <v>45805.71751157408</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -520,10 +520,10 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72559947376</v>
       </c>
       <c r="E5">
         <v>37</v>
@@ -532,10 +532,10 @@
         <v>45807.78447916666</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -690,10 +690,10 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D12" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E12">
         <v>49</v>
@@ -702,10 +702,10 @@
         <v>45807.62427083333</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -952,10 +952,10 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D23" s="2">
-        <v>45806.77603763194</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E23">
         <v>56</v>
@@ -964,10 +964,10 @@
         <v>45806.68203703704</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1194,10 +1194,10 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>1704</v>
+        <v>1660</v>
       </c>
       <c r="D33" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E33">
         <v>1704</v>
@@ -1206,10 +1206,10 @@
         <v>45807.78542824074</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="H33" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1312,10 +1312,10 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D38" s="2">
-        <v>45799.89528858563</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E38">
         <v>79</v>
@@ -1324,10 +1324,10 @@
         <v>45782.69275462963</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1589,10 +1589,10 @@
         <v>1</v>
       </c>
       <c r="C49">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D49" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E49">
         <v>88</v>
@@ -1601,10 +1601,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H49" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1765,10 +1765,10 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D56" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E56">
         <v>181</v>
@@ -1777,10 +1777,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1817,10 +1817,10 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D58" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E58">
         <v>116</v>
@@ -1829,10 +1829,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1941,10 +1941,10 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="D63" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E63">
         <v>101</v>
@@ -1953,10 +1953,10 @@
         <v>45807.6128125</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="H63" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2088,10 +2088,10 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D69" s="2">
-        <v>45805.91875152234</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E69">
         <v>42</v>
@@ -2100,10 +2100,10 @@
         <v>45805.65278935185</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2114,10 +2114,10 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D70" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E70">
         <v>61</v>
@@ -2126,10 +2126,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H70" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2140,10 +2140,10 @@
         <v>1</v>
       </c>
       <c r="C71">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D71" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E71">
         <v>52</v>
@@ -2152,10 +2152,10 @@
         <v>45807.69802083333</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H71" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2376,10 +2376,10 @@
         <v>1</v>
       </c>
       <c r="C81">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D81" s="2">
-        <v>45807.78638608912</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E81">
         <v>36</v>
@@ -2388,10 +2388,10 @@
         <v>45807.43640046296</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H81" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2402,10 +2402,10 @@
         <v>1</v>
       </c>
       <c r="C82">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D82" s="2">
-        <v>45806.77603763194</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E82">
         <v>48</v>
@@ -2414,10 +2414,10 @@
         <v>45806.69827546296</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H82" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2428,10 +2428,10 @@
         <v>1</v>
       </c>
       <c r="C83">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D83" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E83">
         <v>101</v>
@@ -2440,10 +2440,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H83" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2477,10 +2477,10 @@
         <v>1</v>
       </c>
       <c r="C85">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D85" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E85">
         <v>17</v>
@@ -2489,10 +2489,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H85" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2503,10 +2503,10 @@
         <v>1</v>
       </c>
       <c r="C86">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D86" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E86">
         <v>33</v>
@@ -2515,10 +2515,10 @@
         <v>45807.6128125</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H86" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2529,10 +2529,10 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="D87" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E87">
         <v>120</v>
@@ -2541,10 +2541,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H87" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2630,10 +2630,10 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="D91" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E91">
         <v>136</v>
@@ -2642,10 +2642,10 @@
         <v>45807.78510416667</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="H91" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2702,10 +2702,10 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D94" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559943295</v>
       </c>
       <c r="E94">
         <v>108</v>
@@ -2714,10 +2714,10 @@
         <v>45807.69886574074</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H94" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2872,10 +2872,10 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>1481</v>
+        <v>1379</v>
       </c>
       <c r="D101" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E101">
         <v>1481</v>
@@ -2884,10 +2884,10 @@
         <v>45807.78510416667</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="H101" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -2921,10 +2921,10 @@
         <v>1</v>
       </c>
       <c r="C103">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D103" s="2">
-        <v>45803.9069220483</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E103">
         <v>33</v>
@@ -2933,10 +2933,10 @@
         <v>45803.74128472222</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H103" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -2993,10 +2993,10 @@
         <v>1</v>
       </c>
       <c r="C106">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D106" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E106">
         <v>58</v>
@@ -3005,10 +3005,10 @@
         <v>45807.74045138889</v>
       </c>
       <c r="G106">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H106" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3258,10 +3258,10 @@
         <v>1</v>
       </c>
       <c r="C117">
-        <v>1192</v>
+        <v>1187</v>
       </c>
       <c r="D117" s="2">
-        <v>45806.77600903736</v>
+        <v>45810.72559943295</v>
       </c>
       <c r="E117">
         <v>1192</v>
@@ -3270,10 +3270,10 @@
         <v>45806.44605324074</v>
       </c>
       <c r="G117">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H117" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -3310,7 +3310,7 @@
         <v>0</v>
       </c>
       <c r="D119" s="2">
-        <v>45795.04163815061</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E119">
         <v>0</v>
@@ -3333,10 +3333,10 @@
         <v>1</v>
       </c>
       <c r="C120">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D120" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E120">
         <v>53</v>
@@ -3345,10 +3345,10 @@
         <v>45807.70125</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H120" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -3359,10 +3359,10 @@
         <v>1</v>
       </c>
       <c r="C121">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D121" s="2">
-        <v>45805.9187731686</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E121">
         <v>32</v>
@@ -3371,10 +3371,10 @@
         <v>45805.76121527778</v>
       </c>
       <c r="G121">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H121" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -3408,10 +3408,10 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="D123" s="2">
-        <v>45806.77603763194</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E123">
         <v>83</v>
@@ -3420,10 +3420,10 @@
         <v>45806.74983796296</v>
       </c>
       <c r="G123">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H123" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -3460,10 +3460,10 @@
         <v>1</v>
       </c>
       <c r="C125">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D125" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E125">
         <v>322</v>
@@ -3472,10 +3472,10 @@
         <v>45807.6128125</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H125" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -3486,10 +3486,10 @@
         <v>1</v>
       </c>
       <c r="C126">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D126" s="2">
-        <v>45805.9187731686</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E126">
         <v>20</v>
@@ -3498,10 +3498,10 @@
         <v>45805.76144675926</v>
       </c>
       <c r="G126">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H126" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -3535,10 +3535,10 @@
         <v>1</v>
       </c>
       <c r="C128">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D128" s="2">
-        <v>45799.89532165734</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E128">
         <v>77</v>
@@ -3547,10 +3547,10 @@
         <v>45789.51143518519</v>
       </c>
       <c r="G128">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H128" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -3846,10 +3846,10 @@
         <v>1</v>
       </c>
       <c r="C141">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D141" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559947376</v>
       </c>
       <c r="E141">
         <v>590</v>
@@ -3858,10 +3858,10 @@
         <v>45807.69886574074</v>
       </c>
       <c r="G141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H141" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -4149,10 +4149,10 @@
         <v>1</v>
       </c>
       <c r="C153">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D153" s="2">
-        <v>45807.78640665015</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E153">
         <v>9</v>
@@ -4161,10 +4161,10 @@
         <v>45807.43805555555</v>
       </c>
       <c r="G153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H153" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -4691,10 +4691,10 @@
         <v>1</v>
       </c>
       <c r="C175">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D175" s="2">
-        <v>45806.77600903736</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E175">
         <v>103</v>
@@ -4703,10 +4703,10 @@
         <v>45806.41142361111</v>
       </c>
       <c r="G175">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H175" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -4936,10 +4936,10 @@
         <v>1</v>
       </c>
       <c r="C185">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D185" s="2">
-        <v>45805.918751534</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E185">
         <v>85</v>
@@ -4948,10 +4948,10 @@
         <v>45805.70012731481</v>
       </c>
       <c r="G185">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H185" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5103,10 +5103,10 @@
         <v>1</v>
       </c>
       <c r="C192">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D192" s="2">
-        <v>45807.78640665015</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E192">
         <v>29</v>
@@ -5115,10 +5115,10 @@
         <v>45807.43805555555</v>
       </c>
       <c r="G192">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H192" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -5181,10 +5181,10 @@
         <v>1</v>
       </c>
       <c r="C195">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D195" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E195">
         <v>0</v>
@@ -5193,10 +5193,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G195">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H195" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -5302,10 +5302,10 @@
         <v>1</v>
       </c>
       <c r="C200">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="D200" s="2">
-        <v>45806.77603763194</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E200">
         <v>564</v>
@@ -5314,10 +5314,10 @@
         <v>45806.74347222222</v>
       </c>
       <c r="G200">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H200" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -5521,10 +5521,10 @@
         <v>1</v>
       </c>
       <c r="C209">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="D209" s="2">
-        <v>45805.9187731686</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E209">
         <v>31</v>
@@ -5533,10 +5533,10 @@
         <v>45805.76913194444</v>
       </c>
       <c r="G209">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H209" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -5711,10 +5711,10 @@
         <v>1</v>
       </c>
       <c r="C217">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D217" s="2">
-        <v>45806.77603756409</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E217">
         <v>119</v>
@@ -5723,10 +5723,10 @@
         <v>45806.67587962963</v>
       </c>
       <c r="G217">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H217" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -5933,10 +5933,10 @@
         <v>1</v>
       </c>
       <c r="C226">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D226" s="2">
-        <v>45800.93201925102</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E226">
         <v>123</v>
@@ -5945,10 +5945,10 @@
         <v>45800.75763888889</v>
       </c>
       <c r="G226">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H226" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -6149,10 +6149,10 @@
         <v>1</v>
       </c>
       <c r="C235">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D235" s="2">
-        <v>45807.78643074667</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E235">
         <v>48</v>
@@ -6161,10 +6161,10 @@
         <v>45807.72325231481</v>
       </c>
       <c r="G235">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H235" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -6437,10 +6437,10 @@
         <v>1</v>
       </c>
       <c r="C247">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="D247" s="2">
-        <v>45805.91875150988</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E247">
         <v>529</v>
@@ -6449,10 +6449,10 @@
         <v>45805.65172453703</v>
       </c>
       <c r="G247">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H247" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -6627,10 +6627,10 @@
         <v>1</v>
       </c>
       <c r="C255">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D255" s="2">
-        <v>45807.78638608912</v>
+        <v>45810.72559947376</v>
       </c>
       <c r="E255">
         <v>54</v>
@@ -6639,10 +6639,10 @@
         <v>45807.43640046296</v>
       </c>
       <c r="G255">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H255" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="256" spans="1:8">
@@ -6996,10 +6996,10 @@
         <v>1</v>
       </c>
       <c r="C270">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D270" s="2">
-        <v>45807.78638608912</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E270">
         <v>2</v>
@@ -7008,10 +7008,10 @@
         <v>45807.43640046296</v>
       </c>
       <c r="G270">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H270" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="271" spans="1:8">
@@ -7097,10 +7097,10 @@
         <v>1</v>
       </c>
       <c r="C274">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D274" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E274">
         <v>245</v>
@@ -7109,10 +7109,10 @@
         <v>45807.74045138889</v>
       </c>
       <c r="G274">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H274" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="275" spans="1:8">
@@ -7310,10 +7310,10 @@
         <v>1</v>
       </c>
       <c r="C283">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="D283" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E283">
         <v>252</v>
@@ -7322,10 +7322,10 @@
         <v>45807.78510416667</v>
       </c>
       <c r="G283">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H283" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="284" spans="1:8">
@@ -7408,10 +7408,10 @@
         <v>1</v>
       </c>
       <c r="C287">
-        <v>746</v>
+        <v>701</v>
       </c>
       <c r="D287" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E287">
         <v>746</v>
@@ -7420,10 +7420,10 @@
         <v>45807.55438657408</v>
       </c>
       <c r="G287">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H287" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="288" spans="1:8">
@@ -7509,10 +7509,10 @@
         <v>1</v>
       </c>
       <c r="C291">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D291" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E291">
         <v>31</v>
@@ -7521,10 +7521,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G291">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H291" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="292" spans="1:8">
@@ -7535,10 +7535,10 @@
         <v>1</v>
       </c>
       <c r="C292">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D292" s="2">
-        <v>45806.77600903736</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E292">
         <v>26</v>
@@ -7547,10 +7547,10 @@
         <v>45806.44605324074</v>
       </c>
       <c r="G292">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H292" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="293" spans="1:8">
@@ -7610,10 +7610,10 @@
         <v>1</v>
       </c>
       <c r="C295">
-        <v>608</v>
+        <v>582</v>
       </c>
       <c r="D295" s="2">
-        <v>45807.78643074667</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E295">
         <v>608</v>
@@ -7622,10 +7622,10 @@
         <v>45807.72819444445</v>
       </c>
       <c r="G295">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H295" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="296" spans="1:8">
@@ -7904,10 +7904,10 @@
         <v>1</v>
       </c>
       <c r="C307">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D307" s="2">
-        <v>45799.89532165734</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E307">
         <v>1</v>
@@ -7916,10 +7916,10 @@
         <v>45789.61173611111</v>
       </c>
       <c r="G307">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H307" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="308" spans="1:8">
@@ -7953,10 +7953,10 @@
         <v>1</v>
       </c>
       <c r="C309">
-        <v>1196</v>
+        <v>1179</v>
       </c>
       <c r="D309" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E309">
         <v>1196</v>
@@ -7965,10 +7965,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G309">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H309" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="310" spans="1:8">
@@ -8374,10 +8374,10 @@
         <v>1</v>
       </c>
       <c r="C326">
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="D326" s="2">
-        <v>45807.78640657826</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E326">
         <v>10</v>
@@ -8386,10 +8386,10 @@
         <v>45807.43640046296</v>
       </c>
       <c r="G326">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H326" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="327" spans="1:8">
@@ -8870,10 +8870,10 @@
         <v>1</v>
       </c>
       <c r="C346">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D346" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559943295</v>
       </c>
       <c r="E346">
         <v>38</v>
@@ -8882,10 +8882,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G346">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H346" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="347" spans="1:8">
@@ -8991,10 +8991,10 @@
         <v>1</v>
       </c>
       <c r="C351">
-        <v>278</v>
+        <v>206</v>
       </c>
       <c r="D351" s="2">
-        <v>45807.78643074667</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E351">
         <v>278</v>
@@ -9003,10 +9003,10 @@
         <v>45807.72325231481</v>
       </c>
       <c r="G351">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="H351" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="352" spans="1:8">
@@ -9017,10 +9017,10 @@
         <v>1</v>
       </c>
       <c r="C352">
-        <v>635</v>
+        <v>563</v>
       </c>
       <c r="D352" s="2">
-        <v>45805.91875152234</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E352">
         <v>635</v>
@@ -9029,10 +9029,10 @@
         <v>45805.67193287037</v>
       </c>
       <c r="G352">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="H352" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="353" spans="1:8">
@@ -9115,10 +9115,10 @@
         <v>1</v>
       </c>
       <c r="C356">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D356" s="2">
-        <v>45800.93197718772</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E356">
         <v>26</v>
@@ -9127,10 +9127,10 @@
         <v>45800.68631944444</v>
       </c>
       <c r="G356">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H356" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="357" spans="1:8">
@@ -9164,10 +9164,10 @@
         <v>1</v>
       </c>
       <c r="C358">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D358" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E358">
         <v>64</v>
@@ -9176,10 +9176,10 @@
         <v>45807.69886574074</v>
       </c>
       <c r="G358">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H358" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="359" spans="1:8">
@@ -9291,10 +9291,10 @@
         <v>1</v>
       </c>
       <c r="C363">
-        <v>826</v>
+        <v>803</v>
       </c>
       <c r="D363" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E363">
         <v>826</v>
@@ -9303,10 +9303,10 @@
         <v>45807.78510416667</v>
       </c>
       <c r="G363">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H363" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="364" spans="1:8">
@@ -9943,10 +9943,10 @@
         <v>1</v>
       </c>
       <c r="C389">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D389" s="2">
-        <v>45807.78640657826</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E389">
         <v>17</v>
@@ -9955,10 +9955,10 @@
         <v>45807.43640046296</v>
       </c>
       <c r="G389">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H389" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="390" spans="1:8">
@@ -9969,10 +9969,10 @@
         <v>1</v>
       </c>
       <c r="C390">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D390" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72559947376</v>
       </c>
       <c r="E390">
         <v>16</v>
@@ -9981,10 +9981,10 @@
         <v>45807.78542824074</v>
       </c>
       <c r="G390">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H390" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="391" spans="1:8">
@@ -10021,10 +10021,10 @@
         <v>1</v>
       </c>
       <c r="C392">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D392" s="2">
-        <v>45799.89532164588</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E392">
         <v>28</v>
@@ -10033,10 +10033,10 @@
         <v>45786.60901620371</v>
       </c>
       <c r="G392">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H392" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="393" spans="1:8">
@@ -10070,10 +10070,10 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="D394" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E394">
         <v>125</v>
@@ -10082,10 +10082,10 @@
         <v>45807.74167824074</v>
       </c>
       <c r="G394">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H394" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="395" spans="1:8">
@@ -10295,10 +10295,10 @@
         <v>1</v>
       </c>
       <c r="C403">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="D403" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E403">
         <v>0</v>
@@ -10307,10 +10307,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G403">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H403" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="404" spans="1:8">
@@ -10321,10 +10321,10 @@
         <v>1</v>
       </c>
       <c r="C404">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="D404" s="2">
-        <v>45806.77600903736</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E404">
         <v>163</v>
@@ -10333,10 +10333,10 @@
         <v>45806.38988425926</v>
       </c>
       <c r="G404">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H404" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="405" spans="1:8">
@@ -10471,10 +10471,10 @@
         <v>1</v>
       </c>
       <c r="C410">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="D410" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72559943295</v>
       </c>
       <c r="E410">
         <v>458</v>
@@ -10483,10 +10483,10 @@
         <v>45807.74045138889</v>
       </c>
       <c r="G410">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H410" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="411" spans="1:8">
@@ -10673,10 +10673,10 @@
         <v>1</v>
       </c>
       <c r="C418">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="D418" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E418">
         <v>253</v>
@@ -10685,10 +10685,10 @@
         <v>45807.74045138889</v>
       </c>
       <c r="G418">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H418" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="419" spans="1:8">
@@ -10771,10 +10771,10 @@
         <v>1</v>
       </c>
       <c r="C422">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D422" s="2">
-        <v>45805.9187731686</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E422">
         <v>160</v>
@@ -10783,10 +10783,10 @@
         <v>45805.76913194444</v>
       </c>
       <c r="G422">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H422" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="423" spans="1:8">
@@ -10843,10 +10843,10 @@
         <v>1</v>
       </c>
       <c r="C425">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D425" s="2">
-        <v>45806.77600903736</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E425">
         <v>205</v>
@@ -10855,10 +10855,10 @@
         <v>45806.47244212963</v>
       </c>
       <c r="G425">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H425" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="426" spans="1:8">
@@ -11088,10 +11088,10 @@
         <v>1</v>
       </c>
       <c r="C435">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D435" s="2">
-        <v>45799.89540330523</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E435">
         <v>122</v>
@@ -11100,10 +11100,10 @@
         <v>45799.54719907408</v>
       </c>
       <c r="G435">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H435" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="436" spans="1:8">
@@ -11192,10 +11192,10 @@
         <v>1</v>
       </c>
       <c r="C439">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D439" s="2">
-        <v>45800.93197721101</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E439">
         <v>17</v>
@@ -11204,10 +11204,10 @@
         <v>45800.6955787037</v>
       </c>
       <c r="G439">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H439" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="440" spans="1:8">
@@ -12005,10 +12005,10 @@
         <v>1</v>
       </c>
       <c r="C472">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D472" s="2">
-        <v>45806.77603763194</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E472">
         <v>66</v>
@@ -12017,10 +12017,10 @@
         <v>45806.74347222222</v>
       </c>
       <c r="G472">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H472" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="473" spans="1:8">
@@ -12207,10 +12207,10 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D480" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E480">
         <v>183</v>
@@ -12219,10 +12219,10 @@
         <v>45807.74045138889</v>
       </c>
       <c r="G480">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H480" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="481" spans="1:8">
@@ -13467,10 +13467,10 @@
         <v>1</v>
       </c>
       <c r="C531">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D531" s="2">
-        <v>45806.77603765521</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E531">
         <v>74</v>
@@ -13479,10 +13479,10 @@
         <v>45806.74983796296</v>
       </c>
       <c r="G531">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H531" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="532" spans="1:8">
@@ -13643,10 +13643,10 @@
         <v>1</v>
       </c>
       <c r="C538">
-        <v>-85</v>
+        <v>635</v>
       </c>
       <c r="D538" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E538">
         <v>-85</v>
@@ -13655,10 +13655,10 @@
         <v>45807.71612268518</v>
       </c>
       <c r="G538">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="H538" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="539" spans="1:8">
@@ -13718,10 +13718,10 @@
         <v>1</v>
       </c>
       <c r="C541">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D541" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E541">
         <v>-1</v>
@@ -13730,10 +13730,10 @@
         <v>45807.69802083333</v>
       </c>
       <c r="G541">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H541" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="542" spans="1:8">
@@ -14389,10 +14389,10 @@
         <v>1</v>
       </c>
       <c r="C569">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D569" s="2">
-        <v>45798.96533509644</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E569">
         <v>8</v>
@@ -14401,10 +14401,10 @@
         <v>45798.63483796296</v>
       </c>
       <c r="G569">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H569" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="570" spans="1:8">
@@ -14415,10 +14415,10 @@
         <v>1</v>
       </c>
       <c r="C570">
-        <v>2691</v>
+        <v>2689</v>
       </c>
       <c r="D570" s="2">
-        <v>45807.78640665015</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E570">
         <v>2691</v>
@@ -14427,10 +14427,10 @@
         <v>45807.43805555555</v>
       </c>
       <c r="G570">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H570" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="571" spans="1:8">
@@ -14510,10 +14510,10 @@
         <v>1</v>
       </c>
       <c r="C574">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D574" s="2">
-        <v>45805.91872982616</v>
+        <v>45810.72559943295</v>
       </c>
       <c r="E574">
         <v>26</v>
@@ -14522,10 +14522,10 @@
         <v>45805.46181712963</v>
       </c>
       <c r="G574">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H574" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="575" spans="1:8">
@@ -14536,10 +14536,10 @@
         <v>1</v>
       </c>
       <c r="C575">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D575" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E575">
         <v>7</v>
@@ -14548,10 +14548,10 @@
         <v>45807.55438657408</v>
       </c>
       <c r="G575">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H575" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="576" spans="1:8">
@@ -15158,10 +15158,10 @@
         <v>1</v>
       </c>
       <c r="C601">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D601" s="2">
-        <v>45807.78643074667</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E601">
         <v>1</v>
@@ -15170,10 +15170,10 @@
         <v>45807.71612268518</v>
       </c>
       <c r="G601">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H601" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="602" spans="1:8">
@@ -15495,10 +15495,10 @@
         <v>1</v>
       </c>
       <c r="C615">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D615" s="2">
-        <v>45806.77600903736</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E615">
         <v>29</v>
@@ -15507,10 +15507,10 @@
         <v>45806.41142361111</v>
       </c>
       <c r="G615">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H615" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="616" spans="1:8">
@@ -15930,10 +15930,10 @@
         <v>1</v>
       </c>
       <c r="C633">
-        <v>8</v>
+        <v>-2</v>
       </c>
       <c r="D633" s="2">
-        <v>45806.77600903736</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E633">
         <v>8</v>
@@ -15942,10 +15942,10 @@
         <v>45806.44605324074</v>
       </c>
       <c r="G633">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H633" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="634" spans="1:8">
@@ -16385,10 +16385,10 @@
         <v>1</v>
       </c>
       <c r="C652">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D652" s="2">
-        <v>45799.89542737551</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E652">
         <v>22</v>
@@ -16397,10 +16397,10 @@
         <v>45799.64041666667</v>
       </c>
       <c r="G652">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H652" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="653" spans="1:8">
@@ -16509,10 +16509,10 @@
         <v>1</v>
       </c>
       <c r="C657">
-        <v>2271</v>
+        <v>2258</v>
       </c>
       <c r="D657" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E657">
         <v>2271</v>
@@ -16521,10 +16521,10 @@
         <v>45807.78542824074</v>
       </c>
       <c r="G657">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H657" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="658" spans="1:8">
@@ -16584,10 +16584,10 @@
         <v>1</v>
       </c>
       <c r="C660">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D660" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559947376</v>
       </c>
       <c r="E660">
         <v>458</v>
@@ -16596,10 +16596,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G660">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H660" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="661" spans="1:8">
@@ -17342,10 +17342,10 @@
         <v>1</v>
       </c>
       <c r="C691">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="D691" s="2">
-        <v>45806.77603765521</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E691">
         <v>295</v>
@@ -17354,10 +17354,10 @@
         <v>45806.74983796296</v>
       </c>
       <c r="G691">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H691" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="692" spans="1:8">
@@ -17417,10 +17417,10 @@
         <v>1</v>
       </c>
       <c r="C694">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="D694" s="2">
-        <v>45799.89542739857</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E694">
         <v>96</v>
@@ -17429,10 +17429,10 @@
         <v>45791.52667824074</v>
       </c>
       <c r="G694">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="H694" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="695" spans="1:8">
@@ -17599,10 +17599,10 @@
         <v>1</v>
       </c>
       <c r="C701">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D701" s="2">
-        <v>45805.91872982616</v>
+        <v>45810.72559947376</v>
       </c>
       <c r="E701">
         <v>169</v>
@@ -17611,10 +17611,10 @@
         <v>45805.42017361111</v>
       </c>
       <c r="G701">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H701" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="702" spans="1:8">
@@ -17648,10 +17648,10 @@
         <v>1</v>
       </c>
       <c r="C703">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D703" s="2">
-        <v>45806.77600903736</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E703">
         <v>11</v>
@@ -17660,10 +17660,10 @@
         <v>45806.66012731481</v>
       </c>
       <c r="G703">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H703" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="704" spans="1:8">
@@ -18228,10 +18228,10 @@
         <v>1</v>
       </c>
       <c r="C726">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="D726" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E726">
         <v>151</v>
@@ -18240,10 +18240,10 @@
         <v>45807.43805555555</v>
       </c>
       <c r="G726">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H726" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="727" spans="1:8">
@@ -19154,10 +19154,10 @@
         <v>1</v>
       </c>
       <c r="C763">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D763" s="2">
-        <v>45804.91952554927</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E763">
         <v>120</v>
@@ -19166,10 +19166,10 @@
         <v>45804.67107638889</v>
       </c>
       <c r="G763">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H763" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="764" spans="1:8">
@@ -19232,10 +19232,10 @@
         <v>1</v>
       </c>
       <c r="C766">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D766" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559947376</v>
       </c>
       <c r="E766">
         <v>4</v>
@@ -19244,10 +19244,10 @@
         <v>45807.43805555555</v>
       </c>
       <c r="G766">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H766" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="767" spans="1:8">
@@ -19327,10 +19327,10 @@
         <v>1</v>
       </c>
       <c r="C770">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D770" s="2">
-        <v>45799.89528857399</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E770">
         <v>3</v>
@@ -19339,10 +19339,10 @@
         <v>45779.60292824074</v>
       </c>
       <c r="G770">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H770" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="771" spans="1:8">
@@ -19379,10 +19379,10 @@
         <v>1</v>
       </c>
       <c r="C772">
-        <v>451</v>
+        <v>318</v>
       </c>
       <c r="D772" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E772">
         <v>451</v>
@@ -19391,10 +19391,10 @@
         <v>45807.78510416667</v>
       </c>
       <c r="G772">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="H772" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="773" spans="1:8">
@@ -19431,10 +19431,10 @@
         <v>1</v>
       </c>
       <c r="C774">
-        <v>-2</v>
+        <v>7</v>
       </c>
       <c r="D774" s="2">
-        <v>45807.78640657826</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E774">
         <v>-2</v>
@@ -19443,10 +19443,10 @@
         <v>45807.43640046296</v>
       </c>
       <c r="G774">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H774" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="775" spans="1:8">
@@ -19535,10 +19535,10 @@
         <v>1</v>
       </c>
       <c r="C778">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D778" s="2">
-        <v>45805.91872982616</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E778">
         <v>20</v>
@@ -19547,10 +19547,10 @@
         <v>45805.42017361111</v>
       </c>
       <c r="G778">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H778" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="779" spans="1:8">
@@ -20608,10 +20608,10 @@
         <v>1</v>
       </c>
       <c r="C821">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D821" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E821">
         <v>28</v>
@@ -20620,10 +20620,10 @@
         <v>45807.78510416667</v>
       </c>
       <c r="G821">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H821" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="822" spans="1:8">
@@ -20732,10 +20732,10 @@
         <v>1</v>
       </c>
       <c r="C826">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D826" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E826">
         <v>122</v>
@@ -20744,10 +20744,10 @@
         <v>45807.78447916666</v>
       </c>
       <c r="G826">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H826" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="827" spans="1:8">
@@ -21337,10 +21337,10 @@
         <v>1</v>
       </c>
       <c r="C851">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D851" s="2">
-        <v>45803.9069220483</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E851">
         <v>7</v>
@@ -21349,10 +21349,10 @@
         <v>45803.7415625</v>
       </c>
       <c r="G851">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H851" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="852" spans="1:8">
@@ -21363,10 +21363,10 @@
         <v>1</v>
       </c>
       <c r="C852">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="D852" s="2">
-        <v>45799.89528858563</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E852">
         <v>0</v>
@@ -21375,10 +21375,10 @@
         <v>45783.65251157407</v>
       </c>
       <c r="G852">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H852" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="853" spans="1:8">
@@ -21389,10 +21389,10 @@
         <v>1</v>
       </c>
       <c r="C853">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D853" s="2">
-        <v>45806.77603763194</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E853">
         <v>101</v>
@@ -21401,10 +21401,10 @@
         <v>45806.72784722222</v>
       </c>
       <c r="G853">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H853" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="854" spans="1:8">
@@ -21415,10 +21415,10 @@
         <v>1</v>
       </c>
       <c r="C854">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D854" s="2">
-        <v>45805.91875152234</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E854">
         <v>28</v>
@@ -21427,10 +21427,10 @@
         <v>45805.67193287037</v>
       </c>
       <c r="G854">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H854" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="855" spans="1:8">
@@ -21689,10 +21689,10 @@
         <v>1</v>
       </c>
       <c r="C865">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D865" s="2">
-        <v>45805.91875152234</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E865">
         <v>24</v>
@@ -21701,10 +21701,10 @@
         <v>45805.65278935185</v>
       </c>
       <c r="G865">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H865" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="866" spans="1:8">
@@ -21972,10 +21972,10 @@
         <v>1</v>
       </c>
       <c r="C876">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="D876" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E876">
         <v>810</v>
@@ -21984,10 +21984,10 @@
         <v>45807.43805555555</v>
       </c>
       <c r="G876">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H876" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="877" spans="1:8">
@@ -22145,10 +22145,10 @@
         <v>1</v>
       </c>
       <c r="C883">
-        <v>178</v>
+        <v>130</v>
       </c>
       <c r="D883" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E883">
         <v>178</v>
@@ -22157,10 +22157,10 @@
         <v>45807.69886574074</v>
       </c>
       <c r="G883">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H883" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="884" spans="1:8">
@@ -22171,10 +22171,10 @@
         <v>1</v>
       </c>
       <c r="C884">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D884" s="2">
-        <v>45799.89540330523</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E884">
         <v>123</v>
@@ -22183,10 +22183,10 @@
         <v>45799.45596064815</v>
       </c>
       <c r="G884">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H884" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="885" spans="1:8">
@@ -22272,10 +22272,10 @@
         <v>1</v>
       </c>
       <c r="C888">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D888" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E888">
         <v>213</v>
@@ -22284,10 +22284,10 @@
         <v>45807.78542824074</v>
       </c>
       <c r="G888">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H888" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="889" spans="1:8">
@@ -22500,10 +22500,10 @@
         <v>1</v>
       </c>
       <c r="C897">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D897" s="2">
-        <v>45799.89528859723</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E897">
         <v>32</v>
@@ -22512,10 +22512,10 @@
         <v>45784.76087962963</v>
       </c>
       <c r="G897">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H897" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="898" spans="1:8">
@@ -22627,10 +22627,10 @@
         <v>1</v>
       </c>
       <c r="C902">
-        <v>7</v>
+        <v>-3</v>
       </c>
       <c r="D902" s="2">
-        <v>45805.918751534</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E902">
         <v>7</v>
@@ -22639,10 +22639,10 @@
         <v>45805.70869212963</v>
       </c>
       <c r="G902">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H902" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="903" spans="1:8">
@@ -23161,10 +23161,10 @@
         <v>1</v>
       </c>
       <c r="C923">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D923" s="2">
-        <v>45795.04204563411</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E923">
         <v>430</v>
@@ -23173,10 +23173,10 @@
         <v>45750.43479166667</v>
       </c>
       <c r="G923">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H923" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="924" spans="1:8">
@@ -23187,10 +23187,10 @@
         <v>1</v>
       </c>
       <c r="C924">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="D924" s="2">
-        <v>45806.77600903736</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E924">
         <v>137</v>
@@ -23199,10 +23199,10 @@
         <v>45806.65318287037</v>
       </c>
       <c r="G924">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H924" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="925" spans="1:8">
@@ -23539,10 +23539,10 @@
         <v>1</v>
       </c>
       <c r="C938">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D938" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E938">
         <v>13</v>
@@ -23551,10 +23551,10 @@
         <v>45807.69802083333</v>
       </c>
       <c r="G938">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H938" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="939" spans="1:8">
@@ -24110,10 +24110,10 @@
         <v>1</v>
       </c>
       <c r="C961">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D961" s="2">
-        <v>45806.77600903736</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E961">
         <v>51</v>
@@ -24122,10 +24122,10 @@
         <v>45806.44605324074</v>
       </c>
       <c r="G961">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H961" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="962" spans="1:8">
@@ -24136,10 +24136,10 @@
         <v>1</v>
       </c>
       <c r="C962">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D962" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E962">
         <v>83</v>
@@ -24148,10 +24148,10 @@
         <v>45807.55458333333</v>
       </c>
       <c r="G962">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H962" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="963" spans="1:8">
@@ -25937,10 +25937,10 @@
         <v>1</v>
       </c>
       <c r="C1033">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D1033" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E1033">
         <v>-1</v>
@@ -25949,10 +25949,10 @@
         <v>45807.69886574074</v>
       </c>
       <c r="G1033">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1033" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1034" spans="1:8">
@@ -26116,10 +26116,10 @@
         <v>1</v>
       </c>
       <c r="C1040">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1040" s="2">
-        <v>45805.9187731686</v>
+        <v>45810.72559943295</v>
       </c>
       <c r="E1040">
         <v>24</v>
@@ -26128,10 +26128,10 @@
         <v>45805.74280092592</v>
       </c>
       <c r="G1040">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H1040" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1041" spans="1:8">
@@ -26676,10 +26676,10 @@
         <v>1</v>
       </c>
       <c r="C1062">
-        <v>800</v>
+        <v>720</v>
       </c>
       <c r="D1062" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E1062">
         <v>800</v>
@@ -26688,10 +26688,10 @@
         <v>45807.78447916666</v>
       </c>
       <c r="G1062">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="H1062" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1063" spans="1:8">
@@ -27867,10 +27867,10 @@
         <v>1</v>
       </c>
       <c r="C1110">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D1110" s="2">
-        <v>45805.918751534</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E1110">
         <v>179</v>
@@ -27879,10 +27879,10 @@
         <v>45805.70140046296</v>
       </c>
       <c r="G1110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1110" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1111" spans="1:8">
@@ -28274,10 +28274,10 @@
         <v>1</v>
       </c>
       <c r="C1126">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D1126" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E1126">
         <v>171</v>
@@ -28286,10 +28286,10 @@
         <v>45807.78510416667</v>
       </c>
       <c r="G1126">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H1126" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1127" spans="1:8">
@@ -28805,10 +28805,10 @@
         <v>1</v>
       </c>
       <c r="C1147">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D1147" s="2">
-        <v>45806.77603763194</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E1147">
         <v>19</v>
@@ -28817,10 +28817,10 @@
         <v>45806.74347222222</v>
       </c>
       <c r="G1147">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H1147" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1148" spans="1:8">
@@ -29143,10 +29143,10 @@
         <v>1</v>
       </c>
       <c r="C1160">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1160" s="2">
-        <v>45799.89532166889</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E1160">
         <v>26</v>
@@ -29155,10 +29155,10 @@
         <v>45791.54950231482</v>
       </c>
       <c r="G1160">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1160" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1161" spans="1:8">
@@ -29495,10 +29495,10 @@
         <v>1</v>
       </c>
       <c r="C1174">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D1174" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E1174">
         <v>39</v>
@@ -29507,10 +29507,10 @@
         <v>45807.69747685185</v>
       </c>
       <c r="G1174">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H1174" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1175" spans="1:8">
@@ -29521,10 +29521,10 @@
         <v>1</v>
       </c>
       <c r="C1175">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D1175" s="2">
-        <v>45805.91875152234</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E1175">
         <v>10</v>
@@ -29533,10 +29533,10 @@
         <v>45805.65278935185</v>
       </c>
       <c r="G1175">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H1175" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1176" spans="1:8">
@@ -29986,10 +29986,10 @@
         <v>1</v>
       </c>
       <c r="C1193">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D1193" s="2">
-        <v>45799.89532166889</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E1193">
         <v>0</v>
@@ -29998,10 +29998,10 @@
         <v>45791.64023148148</v>
       </c>
       <c r="G1193">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1193" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1194" spans="1:8">
@@ -30038,10 +30038,10 @@
         <v>1</v>
       </c>
       <c r="C1195">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D1195" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E1195">
         <v>20</v>
@@ -30050,10 +30050,10 @@
         <v>45807.62085648148</v>
       </c>
       <c r="G1195">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H1195" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1196" spans="1:8">
@@ -30142,10 +30142,10 @@
         <v>1</v>
       </c>
       <c r="C1199">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D1199" s="2">
-        <v>45804.91952554927</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E1199">
         <v>84</v>
@@ -30154,10 +30154,10 @@
         <v>45804.46582175926</v>
       </c>
       <c r="G1199">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H1199" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1200" spans="1:8">
@@ -30734,10 +30734,10 @@
         <v>1</v>
       </c>
       <c r="C1222">
-        <v>2</v>
+        <v>-16</v>
       </c>
       <c r="D1222" s="2">
-        <v>45805.9187731686</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E1222">
         <v>2</v>
@@ -30746,10 +30746,10 @@
         <v>45805.76913194444</v>
       </c>
       <c r="G1222">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H1222" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1223" spans="1:8">
@@ -31372,10 +31372,10 @@
         <v>1</v>
       </c>
       <c r="C1247">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D1247" s="2">
-        <v>45804.91952554927</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E1247">
         <v>115</v>
@@ -31384,10 +31384,10 @@
         <v>45804.60414351852</v>
       </c>
       <c r="G1247">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H1247" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1248" spans="1:8">
@@ -31528,10 +31528,10 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>507</v>
+        <v>450</v>
       </c>
       <c r="D1253" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E1253">
         <v>507</v>
@@ -31540,10 +31540,10 @@
         <v>45807.70125</v>
       </c>
       <c r="G1253">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="H1253" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1254" spans="1:8">
@@ -33540,10 +33540,10 @@
         <v>1</v>
       </c>
       <c r="C1332">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D1332" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E1332">
         <v>41</v>
@@ -33552,10 +33552,10 @@
         <v>45807.78447916666</v>
       </c>
       <c r="G1332">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H1332" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1333" spans="1:8">
@@ -33791,10 +33791,10 @@
         <v>1</v>
       </c>
       <c r="C1342">
-        <v>1547</v>
+        <v>1286</v>
       </c>
       <c r="D1342" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E1342">
         <v>1547</v>
@@ -33803,10 +33803,10 @@
         <v>45807.70125</v>
       </c>
       <c r="G1342">
-        <v>0</v>
+        <v>261</v>
       </c>
       <c r="H1342" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1343" spans="1:8">
@@ -35041,10 +35041,10 @@
         <v>1</v>
       </c>
       <c r="C1391">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D1391" s="2">
-        <v>45806.77603763194</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E1391">
         <v>92</v>
@@ -35053,10 +35053,10 @@
         <v>45806.74347222222</v>
       </c>
       <c r="G1391">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H1391" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1392" spans="1:8">
@@ -35067,10 +35067,10 @@
         <v>1</v>
       </c>
       <c r="C1392">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1392" s="2">
-        <v>45803.90694022291</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E1392">
         <v>3</v>
@@ -35079,10 +35079,10 @@
         <v>45803.7415625</v>
       </c>
       <c r="G1392">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1392" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1393" spans="1:8">
@@ -35093,10 +35093,10 @@
         <v>1</v>
       </c>
       <c r="C1393">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D1393" s="2">
-        <v>45804.91952554927</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E1393">
         <v>18</v>
@@ -35105,10 +35105,10 @@
         <v>45804.42633101852</v>
       </c>
       <c r="G1393">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H1393" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1394" spans="1:8">
@@ -35578,10 +35578,10 @@
         <v>1</v>
       </c>
       <c r="C1412">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D1412" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E1412">
         <v>101</v>
@@ -35590,10 +35590,10 @@
         <v>45807.78542824074</v>
       </c>
       <c r="G1412">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H1412" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1413" spans="1:8">
@@ -35806,10 +35806,10 @@
         <v>1</v>
       </c>
       <c r="C1421">
-        <v>-8</v>
+        <v>192</v>
       </c>
       <c r="D1421" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E1421">
         <v>-8</v>
@@ -35818,10 +35818,10 @@
         <v>45807.69747685185</v>
       </c>
       <c r="G1421">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H1421" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1422" spans="1:8">
@@ -35832,10 +35832,10 @@
         <v>1</v>
       </c>
       <c r="C1422">
-        <v>-6</v>
+        <v>18</v>
       </c>
       <c r="D1422" s="2">
-        <v>45806.77605776805</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E1422">
         <v>-6</v>
@@ -35844,10 +35844,10 @@
         <v>45806.75375</v>
       </c>
       <c r="G1422">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H1422" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1423" spans="1:8">
@@ -37220,10 +37220,10 @@
         <v>1</v>
       </c>
       <c r="C1477">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1477" s="2">
-        <v>45799.89528858563</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E1477">
         <v>6</v>
@@ -37232,10 +37232,10 @@
         <v>45783.63425925926</v>
       </c>
       <c r="G1477">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H1477" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1478" spans="1:8">
@@ -37985,10 +37985,10 @@
         <v>1</v>
       </c>
       <c r="C1507">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="D1507" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E1507">
         <v>217</v>
@@ -37997,10 +37997,10 @@
         <v>45807.74045138889</v>
       </c>
       <c r="G1507">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H1507" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1508" spans="1:8">
@@ -38037,10 +38037,10 @@
         <v>1</v>
       </c>
       <c r="C1509">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="D1509" s="2">
-        <v>45804.91954472794</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E1509">
         <v>51</v>
@@ -38049,10 +38049,10 @@
         <v>45806.66423611111</v>
       </c>
       <c r="G1509">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H1509" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1510" spans="1:8">
@@ -39597,10 +39597,10 @@
         <v>1</v>
       </c>
       <c r="C1572">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1572" s="2">
-        <v>45807.78643074667</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E1572">
         <v>8</v>
@@ -39609,10 +39609,10 @@
         <v>45807.71956018519</v>
       </c>
       <c r="G1572">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1572" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1573" spans="1:8">
@@ -39672,10 +39672,10 @@
         <v>1</v>
       </c>
       <c r="C1575">
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="D1575" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72556744247</v>
       </c>
       <c r="E1575">
         <v>-4</v>
@@ -39684,10 +39684,10 @@
         <v>45807.46862268518</v>
       </c>
       <c r="G1575">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H1575" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1576" spans="1:8">
@@ -40220,10 +40220,10 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>7192</v>
+        <v>7114</v>
       </c>
       <c r="D1597" s="2">
-        <v>45807.78643077149</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E1597">
         <v>7192</v>
@@ -40232,10 +40232,10 @@
         <v>45807.78542824074</v>
       </c>
       <c r="G1597">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="H1597" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1598" spans="1:8">
@@ -40295,10 +40295,10 @@
         <v>1</v>
       </c>
       <c r="C1600">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D1600" s="2">
-        <v>45805.9187731686</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E1600">
         <v>49</v>
@@ -40307,10 +40307,10 @@
         <v>45805.74226851852</v>
       </c>
       <c r="G1600">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H1600" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1601" spans="1:8">
@@ -41187,10 +41187,10 @@
         <v>1</v>
       </c>
       <c r="C1635">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="D1635" s="2">
-        <v>45803.90692203668</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E1635">
         <v>279</v>
@@ -41199,10 +41199,10 @@
         <v>45803.72625</v>
       </c>
       <c r="G1635">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H1635" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1636" spans="1:8">
@@ -41573,10 +41573,10 @@
         <v>1</v>
       </c>
       <c r="C1651">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D1651" s="2">
-        <v>45807.78643074667</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E1651">
         <v>36</v>
@@ -41585,10 +41585,10 @@
         <v>45807.7375925926</v>
       </c>
       <c r="G1651">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H1651" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1652" spans="1:8">
@@ -41700,10 +41700,10 @@
         <v>1</v>
       </c>
       <c r="C1656">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D1656" s="2">
-        <v>45803.62106753104</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E1656">
         <v>12</v>
@@ -41712,10 +41712,10 @@
         <v>45803.49555555556</v>
       </c>
       <c r="G1656">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H1656" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1657" spans="1:8">
@@ -43851,10 +43851,10 @@
         <v>1</v>
       </c>
       <c r="C1743">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D1743" s="2">
-        <v>45807.78643074667</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E1743">
         <v>-1</v>
@@ -43863,10 +43863,10 @@
         <v>45807.71884259259</v>
       </c>
       <c r="G1743">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1743" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1744" spans="1:8">
@@ -44116,10 +44116,10 @@
         <v>1</v>
       </c>
       <c r="C1754">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D1754" s="2">
-        <v>45799.89545110933</v>
+        <v>45810.72559943295</v>
       </c>
       <c r="E1754">
         <v>28</v>
@@ -44128,10 +44128,10 @@
         <v>45790.63041666667</v>
       </c>
       <c r="G1754">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H1754" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1755" spans="1:8">
@@ -45888,10 +45888,10 @@
         <v>1</v>
       </c>
       <c r="C1824">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1824" s="2">
-        <v>45799.89534673509</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E1824">
         <v>15</v>
@@ -45900,10 +45900,10 @@
         <v>45796.43543981481</v>
       </c>
       <c r="G1824">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1824" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1825" spans="1:8">
@@ -46396,10 +46396,10 @@
         <v>1</v>
       </c>
       <c r="C1844">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D1844" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E1844">
         <v>448</v>
@@ -46408,10 +46408,10 @@
         <v>45807.69886574074</v>
       </c>
       <c r="G1844">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1844" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1845" spans="1:8">
@@ -46448,10 +46448,10 @@
         <v>1</v>
       </c>
       <c r="C1846">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1846" s="2">
-        <v>45799.89528858563</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E1846">
         <v>2</v>
@@ -46460,10 +46460,10 @@
         <v>45782.63818287037</v>
       </c>
       <c r="G1846">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1846" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1847" spans="1:8">
@@ -46670,10 +46670,10 @@
         <v>1</v>
       </c>
       <c r="C1855">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D1855" s="2">
-        <v>45806.77605776805</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E1855">
         <v>4</v>
@@ -46682,10 +46682,10 @@
         <v>45806.75375</v>
       </c>
       <c r="G1855">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H1855" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1856" spans="1:8">
@@ -47317,10 +47317,10 @@
         <v>1</v>
       </c>
       <c r="C1880">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D1880" s="2">
-        <v>45804.91952554927</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E1880">
         <v>15</v>
@@ -47329,10 +47329,10 @@
         <v>45804.49947916667</v>
       </c>
       <c r="G1880">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H1880" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1881" spans="1:8">
@@ -47441,10 +47441,10 @@
         <v>1</v>
       </c>
       <c r="C1885">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D1885" s="2">
-        <v>45799.89536723674</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E1885">
         <v>53</v>
@@ -47453,10 +47453,10 @@
         <v>45797.75920138889</v>
       </c>
       <c r="G1885">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H1885" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1886" spans="1:8">
@@ -48119,10 +48119,10 @@
         <v>1</v>
       </c>
       <c r="C1912">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D1912" s="2">
-        <v>45804.91952539605</v>
+        <v>45810.72559947376</v>
       </c>
       <c r="E1912">
         <v>135</v>
@@ -48131,10 +48131,10 @@
         <v>45804.39973379629</v>
       </c>
       <c r="G1912">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H1912" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1913" spans="1:8">
@@ -48852,10 +48852,10 @@
         <v>1</v>
       </c>
       <c r="C1941">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1941" s="2">
-        <v>45799.89532166889</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E1941">
         <v>2</v>
@@ -48864,10 +48864,10 @@
         <v>45790.67538194444</v>
       </c>
       <c r="G1941">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H1941" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1942" spans="1:8">
@@ -49830,7 +49830,7 @@
         <v>0</v>
       </c>
       <c r="D1980" s="2">
-        <v>45795.04171905605</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E1980">
         <v>0</v>
@@ -50903,10 +50903,10 @@
         <v>1</v>
       </c>
       <c r="C2023">
-        <v>10</v>
+        <v>-6</v>
       </c>
       <c r="D2023" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E2023">
         <v>10</v>
@@ -50915,10 +50915,10 @@
         <v>45807.43805555555</v>
       </c>
       <c r="G2023">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H2023" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2024" spans="1:8">
@@ -51388,10 +51388,10 @@
         <v>1</v>
       </c>
       <c r="C2042">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2042" s="2">
-        <v>45804.91954472794</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E2042">
         <v>2</v>
@@ -51400,10 +51400,10 @@
         <v>45804.76886574074</v>
       </c>
       <c r="G2042">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2042" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2043" spans="1:8">
@@ -53448,10 +53448,10 @@
         <v>1</v>
       </c>
       <c r="C2124">
-        <v>-69</v>
+        <v>291</v>
       </c>
       <c r="D2124" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E2124">
         <v>-69</v>
@@ -53460,10 +53460,10 @@
         <v>45807.55458333333</v>
       </c>
       <c r="G2124">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="H2124" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2125" spans="1:8">
@@ -54965,10 +54965,10 @@
         <v>1</v>
       </c>
       <c r="C2185">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D2185" s="2">
-        <v>45807.78643074667</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E2185">
         <v>-2</v>
@@ -54977,10 +54977,10 @@
         <v>45807.71784722222</v>
       </c>
       <c r="G2185">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H2185" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2186" spans="1:8">
@@ -56365,10 +56365,10 @@
         <v>1</v>
       </c>
       <c r="C2240">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D2240" s="2">
-        <v>45805.9187731686</v>
+        <v>45810.72559944464</v>
       </c>
       <c r="E2240">
         <v>281</v>
@@ -56377,10 +56377,10 @@
         <v>45805.70947916667</v>
       </c>
       <c r="G2240">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H2240" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2241" spans="1:8">
@@ -56391,10 +56391,10 @@
         <v>1</v>
       </c>
       <c r="C2241">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="D2241" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E2241">
         <v>308</v>
@@ -56403,10 +56403,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G2241">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H2241" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2242" spans="1:8">
@@ -58569,10 +58569,10 @@
         <v>1</v>
       </c>
       <c r="C2328">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2328" s="2">
-        <v>45799.89528859723</v>
+        <v>45810.72556745499</v>
       </c>
       <c r="E2328">
         <v>1</v>
@@ -58581,10 +58581,10 @@
         <v>45784.75885416667</v>
       </c>
       <c r="G2328">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2328" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2329" spans="1:8">
@@ -59273,10 +59273,10 @@
         <v>1</v>
       </c>
       <c r="C2356">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D2356" s="2">
-        <v>45807.78640657826</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E2356">
         <v>-1</v>
@@ -59285,10 +59285,10 @@
         <v>45807.43640046296</v>
       </c>
       <c r="G2356">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2356" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2357" spans="1:8">
@@ -60677,10 +60677,10 @@
         <v>1</v>
       </c>
       <c r="C2413">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D2413" s="2">
-        <v>45799.89528858563</v>
+        <v>45810.72559943295</v>
       </c>
       <c r="E2413">
         <v>0</v>
@@ -60689,10 +60689,10 @@
         <v>45782.69798611111</v>
       </c>
       <c r="G2413">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2413" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2414" spans="1:8">
@@ -60755,10 +60755,10 @@
         <v>1</v>
       </c>
       <c r="C2416">
-        <v>385</v>
+        <v>355</v>
       </c>
       <c r="D2416" s="2">
-        <v>45807.78640665444</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E2416">
         <v>385</v>
@@ -60767,10 +60767,10 @@
         <v>45807.69164351852</v>
       </c>
       <c r="G2416">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H2416" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2417" spans="1:8">
@@ -61960,10 +61960,10 @@
         <v>1</v>
       </c>
       <c r="C2465">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D2465" s="2">
-        <v>45803.62106753104</v>
+        <v>45810.72563720519</v>
       </c>
       <c r="E2465">
         <v>59</v>
@@ -61972,10 +61972,10 @@
         <v>45803.4153125</v>
       </c>
       <c r="G2465">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H2465" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2466" spans="1:8">
@@ -62375,10 +62375,10 @@
         <v>1</v>
       </c>
       <c r="C2482">
-        <v>581</v>
+        <v>559</v>
       </c>
       <c r="D2482" s="2">
-        <v>45806.77605776805</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E2482">
         <v>581</v>
@@ -62387,10 +62387,10 @@
         <v>45806.74983796296</v>
       </c>
       <c r="G2482">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H2482" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2483" spans="1:8">
@@ -62401,10 +62401,10 @@
         <v>1</v>
       </c>
       <c r="C2483">
-        <v>957</v>
+        <v>939</v>
       </c>
       <c r="D2483" s="2">
-        <v>45806.77605776805</v>
+        <v>45810.72559946219</v>
       </c>
       <c r="E2483">
         <v>957</v>
@@ -62413,10 +62413,10 @@
         <v>45806.74983796296</v>
       </c>
       <c r="G2483">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H2483" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2484" spans="1:8">
@@ -62427,10 +62427,10 @@
         <v>1</v>
       </c>
       <c r="C2484">
-        <v>1012</v>
+        <v>997</v>
       </c>
       <c r="D2484" s="2">
-        <v>45806.77605776805</v>
+        <v>45810.72559945051</v>
       </c>
       <c r="E2484">
         <v>1012</v>
@@ -62439,10 +62439,10 @@
         <v>45806.74983796296</v>
       </c>
       <c r="G2484">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H2484" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2485" spans="1:8">
@@ -64040,18 +64040,87 @@
         <v>1</v>
       </c>
       <c r="C2551">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D2551" s="2">
-        <v>45806.77603763194</v>
+        <v>45810.72563721648</v>
       </c>
       <c r="E2551">
         <v>0</v>
       </c>
       <c r="G2551">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H2551" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2552" spans="1:8">
+      <c r="A2552">
+        <v>43372191</v>
+      </c>
+      <c r="B2552">
+        <v>1</v>
+      </c>
+      <c r="C2552">
+        <v>-1</v>
+      </c>
+      <c r="D2552" s="2">
+        <v>45810.72559945051</v>
+      </c>
+      <c r="E2552">
+        <v>0</v>
+      </c>
+      <c r="G2552">
+        <v>1</v>
+      </c>
+      <c r="H2552" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2553" spans="1:8">
+      <c r="A2553">
+        <v>43372259</v>
+      </c>
+      <c r="B2553">
+        <v>1</v>
+      </c>
+      <c r="C2553">
+        <v>0</v>
+      </c>
+      <c r="D2553" s="2">
+        <v>45810.72556745499</v>
+      </c>
+      <c r="E2553">
+        <v>0</v>
+      </c>
+      <c r="G2553">
+        <v>0</v>
+      </c>
+      <c r="H2553" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2554" spans="1:8">
+      <c r="A2554">
+        <v>43372946</v>
+      </c>
+      <c r="B2554">
+        <v>1</v>
+      </c>
+      <c r="C2554">
+        <v>0</v>
+      </c>
+      <c r="D2554" s="2">
+        <v>45810.72556745499</v>
+      </c>
+      <c r="E2554">
+        <v>0</v>
+      </c>
+      <c r="G2554">
+        <v>0</v>
+      </c>
+      <c r="H2554" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizei dados da bibi e add
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="10">
   <si>
     <t>id_produto</t>
   </si>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2555"/>
+  <dimension ref="A1:H2557"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,16 +494,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="D4" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E4">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="F4" s="2">
-        <v>45811.68890046296</v>
+        <v>45812.78209490741</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -978,16 +978,16 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E24">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24" s="2">
-        <v>45811.54368055556</v>
+        <v>45812.70203703704</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1194,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>1570</v>
+        <v>1558</v>
       </c>
       <c r="D33" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E33">
-        <v>1570</v>
+        <v>1558</v>
       </c>
       <c r="F33" s="2">
-        <v>45811.72346064815</v>
+        <v>45812.63878472222</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1563,16 +1563,16 @@
         <v>1</v>
       </c>
       <c r="C48">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D48" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E48">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F48" s="2">
-        <v>45811.70625</v>
+        <v>45812.70203703704</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1589,16 +1589,16 @@
         <v>1</v>
       </c>
       <c r="C49">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D49" s="2">
-        <v>45811.92552606984</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E49">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F49" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -1765,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D56" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E56">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="F56" s="2">
-        <v>45811.6834837963</v>
+        <v>45812.65041666666</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -1817,16 +1817,16 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="D58" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E58">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="F58" s="2">
-        <v>45811.68890046296</v>
+        <v>45812.70203703704</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -1941,16 +1941,16 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D63" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E63">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F63" s="2">
-        <v>45811.72346064815</v>
+        <v>45812.70203703704</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2088,16 +2088,16 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D69" s="2">
-        <v>45811.92552605522</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E69">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F69" s="2">
-        <v>45811.74833333334</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -2114,16 +2114,16 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D70" s="2">
-        <v>45811.92552606984</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E70">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F70" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.5275925926</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2376,16 +2376,16 @@
         <v>1</v>
       </c>
       <c r="C81">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D81" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E81">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F81" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.65041666666</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -2402,16 +2402,16 @@
         <v>1</v>
       </c>
       <c r="C82">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D82" s="2">
-        <v>45810.72563720519</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E82">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F82" s="2">
-        <v>45810.68862268519</v>
+        <v>45812.48946759259</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -2428,16 +2428,16 @@
         <v>1</v>
       </c>
       <c r="C83">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D83" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E83">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F83" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.53496527778</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -2477,16 +2477,16 @@
         <v>1</v>
       </c>
       <c r="C85">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D85" s="2">
-        <v>45810.72559944464</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E85">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F85" s="2">
-        <v>45810.60861111111</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -2529,16 +2529,16 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D87" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E87">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F87" s="2">
-        <v>45811.50931712963</v>
+        <v>45812.6909837963</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -2613,7 +2613,7 @@
         <v>28</v>
       </c>
       <c r="F90" s="2">
-        <v>45807.43640046296</v>
+        <v>45812.5275925926</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -2630,16 +2630,16 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="D91" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E91">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="F91" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.69229166667</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -2702,16 +2702,16 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D94" s="2">
-        <v>45811.92552606984</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E94">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F94" s="2">
-        <v>45811.75518518518</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -2872,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>1087</v>
+        <v>1045</v>
       </c>
       <c r="D101" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E101">
-        <v>1087</v>
+        <v>1045</v>
       </c>
       <c r="F101" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -3408,16 +3408,16 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D123" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E123">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F123" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -3460,16 +3460,16 @@
         <v>1</v>
       </c>
       <c r="C125">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D125" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E125">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F125" s="2">
-        <v>45811.72704861111</v>
+        <v>45812.65041666666</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -3846,16 +3846,16 @@
         <v>1</v>
       </c>
       <c r="C141">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="D141" s="2">
-        <v>45811.92552606984</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E141">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="F141" s="2">
-        <v>45811.75518518518</v>
+        <v>45812.70203703704</v>
       </c>
       <c r="G141">
         <v>0</v>
@@ -4319,16 +4319,16 @@
         <v>1</v>
       </c>
       <c r="C160">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D160" s="2">
-        <v>45795.04204563411</v>
+        <v>45812.78306321269</v>
       </c>
       <c r="E160">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F160" s="2">
-        <v>45756.53471064815</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G160">
         <v>0</v>
@@ -4691,16 +4691,16 @@
         <v>1</v>
       </c>
       <c r="C175">
-        <v>19</v>
+        <v>199</v>
       </c>
       <c r="D175" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E175">
-        <v>19</v>
+        <v>199</v>
       </c>
       <c r="F175" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.6706712963</v>
       </c>
       <c r="G175">
         <v>0</v>
@@ -5077,16 +5077,16 @@
         <v>1</v>
       </c>
       <c r="C191">
-        <v>-244</v>
+        <v>356</v>
       </c>
       <c r="D191" s="2">
-        <v>45811.92544186871</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E191">
-        <v>-244</v>
+        <v>356</v>
       </c>
       <c r="F191" s="2">
-        <v>45810.76819444444</v>
+        <v>45812.31930555555</v>
       </c>
       <c r="G191">
         <v>0</v>
@@ -5103,16 +5103,16 @@
         <v>1</v>
       </c>
       <c r="C192">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D192" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E192">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F192" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.53496527778</v>
       </c>
       <c r="G192">
         <v>0</v>
@@ -5521,16 +5521,16 @@
         <v>1</v>
       </c>
       <c r="C209">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D209" s="2">
-        <v>45810.72556745499</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E209">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F209" s="2">
-        <v>45810.51450231481</v>
+        <v>45812.53496527778</v>
       </c>
       <c r="G209">
         <v>0</v>
@@ -6437,16 +6437,16 @@
         <v>1</v>
       </c>
       <c r="C247">
-        <v>469</v>
+        <v>1269</v>
       </c>
       <c r="D247" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78299904546</v>
       </c>
       <c r="E247">
-        <v>469</v>
+        <v>1269</v>
       </c>
       <c r="F247" s="2">
-        <v>45811.50664351852</v>
+        <v>45812.31732638889</v>
       </c>
       <c r="G247">
         <v>0</v>
@@ -6627,16 +6627,16 @@
         <v>1</v>
       </c>
       <c r="C255">
-        <v>32</v>
+        <v>-33</v>
       </c>
       <c r="D255" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E255">
-        <v>32</v>
+        <v>-33</v>
       </c>
       <c r="F255" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.63135416667</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -6898,16 +6898,16 @@
         <v>1</v>
       </c>
       <c r="C266">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D266" s="2">
-        <v>45795.04186106093</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E266">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F266" s="2">
-        <v>45607.63087962963</v>
+        <v>45812.47731481482</v>
       </c>
       <c r="G266">
         <v>0</v>
@@ -6996,16 +6996,16 @@
         <v>1</v>
       </c>
       <c r="C270">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="D270" s="2">
-        <v>45811.92552605522</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E270">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="F270" s="2">
-        <v>45811.74833333334</v>
+        <v>45812.47226851852</v>
       </c>
       <c r="G270">
         <v>0</v>
@@ -7408,16 +7408,16 @@
         <v>1</v>
       </c>
       <c r="C287">
-        <v>590</v>
+        <v>560</v>
       </c>
       <c r="D287" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E287">
-        <v>590</v>
+        <v>560</v>
       </c>
       <c r="F287" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.48946759259</v>
       </c>
       <c r="G287">
         <v>0</v>
@@ -7509,16 +7509,16 @@
         <v>1</v>
       </c>
       <c r="C291">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D291" s="2">
-        <v>45811.92552608132</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E291">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="F291" s="2">
-        <v>45811.78815972222</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G291">
         <v>0</v>
@@ -7610,16 +7610,16 @@
         <v>1</v>
       </c>
       <c r="C295">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="D295" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E295">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="F295" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.69229166667</v>
       </c>
       <c r="G295">
         <v>0</v>
@@ -8071,16 +8071,16 @@
         <v>1</v>
       </c>
       <c r="C314">
-        <v>-13</v>
+        <v>5</v>
       </c>
       <c r="D314" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E314">
-        <v>-13</v>
+        <v>5</v>
       </c>
       <c r="F314" s="2">
-        <v>45811.68634259259</v>
+        <v>45812.54806712963</v>
       </c>
       <c r="G314">
         <v>0</v>
@@ -8195,16 +8195,16 @@
         <v>1</v>
       </c>
       <c r="C319">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="D319" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E319">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="F319" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.66025462963</v>
       </c>
       <c r="G319">
         <v>0</v>
@@ -8247,16 +8247,16 @@
         <v>1</v>
       </c>
       <c r="C321">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D321" s="2">
-        <v>45799.895427387</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E321">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="F321" s="2">
-        <v>45799.69793981482</v>
+        <v>45812.5547337963</v>
       </c>
       <c r="G321">
         <v>0</v>
@@ -8374,16 +8374,16 @@
         <v>1</v>
       </c>
       <c r="C326">
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="D326" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E326">
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="F326" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.65549768518</v>
       </c>
       <c r="G326">
         <v>0</v>
@@ -8426,16 +8426,16 @@
         <v>1</v>
       </c>
       <c r="C328">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D328" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E328">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F328" s="2">
-        <v>45811.50076388889</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G328">
         <v>0</v>
@@ -9164,16 +9164,16 @@
         <v>1</v>
       </c>
       <c r="C358">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D358" s="2">
-        <v>45811.92552606984</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E358">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F358" s="2">
-        <v>45811.75627314814</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G358">
         <v>0</v>
@@ -9190,16 +9190,16 @@
         <v>1</v>
       </c>
       <c r="C359">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D359" s="2">
-        <v>45806.77603763194</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E359">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F359" s="2">
-        <v>45806.74983796296</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G359">
         <v>0</v>
@@ -9291,16 +9291,16 @@
         <v>1</v>
       </c>
       <c r="C363">
-        <v>740</v>
+        <v>730</v>
       </c>
       <c r="D363" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E363">
-        <v>740</v>
+        <v>730</v>
       </c>
       <c r="F363" s="2">
-        <v>45811.67811342593</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G363">
         <v>0</v>
@@ -9438,16 +9438,16 @@
         <v>1</v>
       </c>
       <c r="C369">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D369" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E369">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F369" s="2">
-        <v>45811.72704861111</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G369">
         <v>0</v>
@@ -9640,16 +9640,16 @@
         <v>1</v>
       </c>
       <c r="C377">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D377" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E377">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F377" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.47423611111</v>
       </c>
       <c r="G377">
         <v>0</v>
@@ -9764,16 +9764,16 @@
         <v>1</v>
       </c>
       <c r="C382">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D382" s="2">
-        <v>45807.78640665015</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E382">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F382" s="2">
-        <v>45807.43805555555</v>
+        <v>45812.43199074074</v>
       </c>
       <c r="G382">
         <v>0</v>
@@ -9839,16 +9839,16 @@
         <v>1</v>
       </c>
       <c r="C385">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D385" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E385">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="F385" s="2">
-        <v>45811.49467592593</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G385">
         <v>0</v>
@@ -9865,16 +9865,16 @@
         <v>1</v>
       </c>
       <c r="C386">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D386" s="2">
-        <v>45799.89532165734</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E386">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="F386" s="2">
-        <v>45803.72883101852</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G386">
         <v>0</v>
@@ -9891,16 +9891,16 @@
         <v>1</v>
       </c>
       <c r="C387">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D387" s="2">
-        <v>45806.77603763194</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E387">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F387" s="2">
-        <v>45806.74983796296</v>
+        <v>45812.63135416667</v>
       </c>
       <c r="G387">
         <v>0</v>
@@ -9969,16 +9969,16 @@
         <v>1</v>
       </c>
       <c r="C390">
-        <v>-52</v>
+        <v>-44</v>
       </c>
       <c r="D390" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E390">
-        <v>-52</v>
+        <v>-44</v>
       </c>
       <c r="F390" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.4777662037</v>
       </c>
       <c r="G390">
         <v>0</v>
@@ -10070,16 +10070,16 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D394" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E394">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="F394" s="2">
-        <v>45811.72346064815</v>
+        <v>45812.65041666666</v>
       </c>
       <c r="G394">
         <v>0</v>
@@ -10122,16 +10122,16 @@
         <v>1</v>
       </c>
       <c r="C396">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="D396" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E396">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="F396" s="2">
-        <v>45811.42236111111</v>
+        <v>45812.32835648148</v>
       </c>
       <c r="G396">
         <v>0</v>
@@ -10295,16 +10295,16 @@
         <v>1</v>
       </c>
       <c r="C403">
-        <v>-6</v>
+        <v>66</v>
       </c>
       <c r="D403" s="2">
-        <v>45810.72559945051</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E403">
-        <v>-6</v>
+        <v>66</v>
       </c>
       <c r="F403" s="2">
-        <v>45810.61395833334</v>
+        <v>45812.32231481482</v>
       </c>
       <c r="G403">
         <v>0</v>
@@ -10321,16 +10321,16 @@
         <v>1</v>
       </c>
       <c r="C404">
-        <v>69</v>
+        <v>229</v>
       </c>
       <c r="D404" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E404">
-        <v>69</v>
+        <v>229</v>
       </c>
       <c r="F404" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G404">
         <v>0</v>
@@ -10575,16 +10575,16 @@
         <v>1</v>
       </c>
       <c r="C414">
-        <v>-3</v>
+        <v>97</v>
       </c>
       <c r="D414" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E414">
-        <v>-3</v>
+        <v>97</v>
       </c>
       <c r="F414" s="2">
-        <v>45811.68890046296</v>
+        <v>45812.66328703704</v>
       </c>
       <c r="G414">
         <v>0</v>
@@ -10843,16 +10843,16 @@
         <v>1</v>
       </c>
       <c r="C425">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D425" s="2">
-        <v>45810.72563721648</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E425">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F425" s="2">
-        <v>45810.75585648148</v>
+        <v>45812.63878472222</v>
       </c>
       <c r="G425">
         <v>0</v>
@@ -11296,16 +11296,16 @@
         <v>1</v>
       </c>
       <c r="C443">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D443" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E443">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F443" s="2">
-        <v>45811.4736574074</v>
+        <v>45812.48946759259</v>
       </c>
       <c r="G443">
         <v>0</v>
@@ -11930,16 +11930,16 @@
         <v>1</v>
       </c>
       <c r="C469">
-        <v>-57</v>
+        <v>-87</v>
       </c>
       <c r="D469" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E469">
-        <v>-57</v>
+        <v>-87</v>
       </c>
       <c r="F469" s="2">
-        <v>45811.47556712963</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G469">
         <v>0</v>
@@ -12207,16 +12207,16 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>162</v>
+        <v>249</v>
       </c>
       <c r="D480" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E480">
-        <v>162</v>
+        <v>249</v>
       </c>
       <c r="F480" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G480">
         <v>0</v>
@@ -12285,16 +12285,16 @@
         <v>1</v>
       </c>
       <c r="C483">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D483" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E483">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F483" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.6531712963</v>
       </c>
       <c r="G483">
         <v>0</v>
@@ -12951,16 +12951,16 @@
         <v>1</v>
       </c>
       <c r="C510">
-        <v>69</v>
+        <v>315</v>
       </c>
       <c r="D510" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E510">
-        <v>69</v>
+        <v>315</v>
       </c>
       <c r="F510" s="2">
-        <v>45811.72346064815</v>
+        <v>45812.43105324074</v>
       </c>
       <c r="G510">
         <v>0</v>
@@ -13366,16 +13366,16 @@
         <v>1</v>
       </c>
       <c r="C527">
-        <v>8</v>
+        <v>-4</v>
       </c>
       <c r="D527" s="2">
-        <v>45807.78640657826</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E527">
-        <v>8</v>
+        <v>-4</v>
       </c>
       <c r="F527" s="2">
-        <v>45807.43640046296</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G527">
         <v>0</v>
@@ -14389,16 +14389,16 @@
         <v>1</v>
       </c>
       <c r="C569">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D569" s="2">
-        <v>45810.72559945051</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E569">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F569" s="2">
-        <v>45810.64912037037</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G569">
         <v>0</v>
@@ -14415,16 +14415,16 @@
         <v>1</v>
       </c>
       <c r="C570">
-        <v>2671</v>
+        <v>2645</v>
       </c>
       <c r="D570" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E570">
-        <v>2671</v>
+        <v>2645</v>
       </c>
       <c r="F570" s="2">
-        <v>45811.72704861111</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G570">
         <v>0</v>
@@ -15158,16 +15158,16 @@
         <v>1</v>
       </c>
       <c r="C601">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D601" s="2">
-        <v>45810.72559946219</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E601">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F601" s="2">
-        <v>45810.66146990741</v>
+        <v>45812.43105324074</v>
       </c>
       <c r="G601">
         <v>0</v>
@@ -15878,16 +15878,16 @@
         <v>1</v>
       </c>
       <c r="C631">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D631" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E631">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F631" s="2">
-        <v>45811.50252314815</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G631">
         <v>0</v>
@@ -15930,16 +15930,16 @@
         <v>1</v>
       </c>
       <c r="C633">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D633" s="2">
-        <v>45810.72556745499</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E633">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F633" s="2">
-        <v>45810.50998842593</v>
+        <v>45812.47270833333</v>
       </c>
       <c r="G633">
         <v>0</v>
@@ -16483,16 +16483,16 @@
         <v>1</v>
       </c>
       <c r="C656">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D656" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E656">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F656" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.70203703704</v>
       </c>
       <c r="G656">
         <v>0</v>
@@ -16509,16 +16509,16 @@
         <v>1</v>
       </c>
       <c r="C657">
-        <v>2172</v>
+        <v>2160</v>
       </c>
       <c r="D657" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E657">
-        <v>2172</v>
+        <v>2160</v>
       </c>
       <c r="F657" s="2">
-        <v>45811.73181712963</v>
+        <v>45812.63135416667</v>
       </c>
       <c r="G657">
         <v>0</v>
@@ -16535,16 +16535,16 @@
         <v>1</v>
       </c>
       <c r="C658">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D658" s="2">
-        <v>45803.90692203668</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E658">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F658" s="2">
-        <v>45803.72575231481</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G658">
         <v>0</v>
@@ -16584,16 +16584,16 @@
         <v>1</v>
       </c>
       <c r="C660">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="D660" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E660">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="F660" s="2">
-        <v>45811.70625</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G660">
         <v>0</v>
@@ -17068,16 +17068,16 @@
         <v>1</v>
       </c>
       <c r="C680">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D680" s="2">
-        <v>45799.89536723674</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E680">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F680" s="2">
-        <v>45803.76681712963</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G680">
         <v>0</v>
@@ -17094,16 +17094,16 @@
         <v>1</v>
       </c>
       <c r="C681">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D681" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E681">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F681" s="2">
-        <v>45811.68216435185</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G681">
         <v>0</v>
@@ -17342,16 +17342,16 @@
         <v>1</v>
       </c>
       <c r="C691">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="D691" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E691">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="F691" s="2">
-        <v>45811.68634259259</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G691">
         <v>0</v>
@@ -17599,16 +17599,16 @@
         <v>1</v>
       </c>
       <c r="C701">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="D701" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E701">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="F701" s="2">
-        <v>45811.72346064815</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G701">
         <v>0</v>
@@ -17648,16 +17648,16 @@
         <v>1</v>
       </c>
       <c r="C703">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D703" s="2">
-        <v>45810.72556744247</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E703">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F703" s="2">
-        <v>45810.44699074074</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G703">
         <v>0</v>
@@ -17994,16 +17994,16 @@
         <v>1</v>
       </c>
       <c r="C717">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D717" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E717">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F717" s="2">
-        <v>45811.48225694444</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G717">
         <v>0</v>
@@ -18072,16 +18072,16 @@
         <v>1</v>
       </c>
       <c r="C720">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="D720" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78306321269</v>
       </c>
       <c r="E720">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="F720" s="2">
-        <v>45811.50931712963</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G720">
         <v>0</v>
@@ -18098,16 +18098,16 @@
         <v>1</v>
       </c>
       <c r="C721">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="D721" s="2">
-        <v>45800.93192368435</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E721">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="F721" s="2">
-        <v>45800.64704861111</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G721">
         <v>0</v>
@@ -18228,16 +18228,16 @@
         <v>1</v>
       </c>
       <c r="C726">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D726" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E726">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F726" s="2">
-        <v>45811.72704861111</v>
+        <v>45812.47731481482</v>
       </c>
       <c r="G726">
         <v>0</v>
@@ -19379,16 +19379,16 @@
         <v>1</v>
       </c>
       <c r="C772">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D772" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E772">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F772" s="2">
-        <v>45811.66579861111</v>
+        <v>45812.6909837963</v>
       </c>
       <c r="G772">
         <v>0</v>
@@ -19535,16 +19535,16 @@
         <v>1</v>
       </c>
       <c r="C778">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D778" s="2">
-        <v>45810.72559945051</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E778">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F778" s="2">
-        <v>45810.64912037037</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G778">
         <v>0</v>
@@ -20556,16 +20556,16 @@
         <v>1</v>
       </c>
       <c r="C819">
-        <v>35</v>
+        <v>-1</v>
       </c>
       <c r="D819" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E819">
-        <v>35</v>
+        <v>-1</v>
       </c>
       <c r="F819" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.63878472222</v>
       </c>
       <c r="G819">
         <v>0</v>
@@ -20732,16 +20732,16 @@
         <v>1</v>
       </c>
       <c r="C826">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D826" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E826">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F826" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.47731481482</v>
       </c>
       <c r="G826">
         <v>0</v>
@@ -21337,16 +21337,16 @@
         <v>1</v>
       </c>
       <c r="C851">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D851" s="2">
-        <v>45810.72559944464</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E851">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F851" s="2">
-        <v>45810.54670138889</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G851">
         <v>0</v>
@@ -21363,16 +21363,16 @@
         <v>1</v>
       </c>
       <c r="C852">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="D852" s="2">
-        <v>45810.72563720519</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E852">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F852" s="2">
-        <v>45810.68862268519</v>
+        <v>45812.471875</v>
       </c>
       <c r="G852">
         <v>0</v>
@@ -21689,16 +21689,16 @@
         <v>1</v>
       </c>
       <c r="C865">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D865" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E865">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F865" s="2">
-        <v>45811.73181712963</v>
+        <v>45812.6909837963</v>
       </c>
       <c r="G865">
         <v>0</v>
@@ -21868,16 +21868,16 @@
         <v>1</v>
       </c>
       <c r="C872">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D872" s="2">
-        <v>45811.92552608132</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E872">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F872" s="2">
-        <v>45811.78815972222</v>
+        <v>45812.43199074074</v>
       </c>
       <c r="G872">
         <v>0</v>
@@ -21972,16 +21972,16 @@
         <v>1</v>
       </c>
       <c r="C876">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="D876" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E876">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="F876" s="2">
-        <v>45811.49375</v>
+        <v>45812.43199074074</v>
       </c>
       <c r="G876">
         <v>0</v>
@@ -22500,16 +22500,16 @@
         <v>1</v>
       </c>
       <c r="C897">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D897" s="2">
-        <v>45810.72559944464</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E897">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F897" s="2">
-        <v>45810.54670138889</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G897">
         <v>0</v>
@@ -22627,16 +22627,16 @@
         <v>1</v>
       </c>
       <c r="C902">
-        <v>7</v>
+        <v>-43</v>
       </c>
       <c r="D902" s="2">
-        <v>45811.92552608132</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E902">
-        <v>7</v>
+        <v>-43</v>
       </c>
       <c r="F902" s="2">
-        <v>45811.76508101852</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G902">
         <v>0</v>
@@ -23187,16 +23187,16 @@
         <v>1</v>
       </c>
       <c r="C924">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D924" s="2">
-        <v>45811.92552606984</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E924">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F924" s="2">
-        <v>45811.75681712963</v>
+        <v>45812.63878472222</v>
       </c>
       <c r="G924">
         <v>0</v>
@@ -23695,16 +23695,16 @@
         <v>1</v>
       </c>
       <c r="C944">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D944" s="2">
-        <v>45806.77605776805</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E944">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F944" s="2">
-        <v>45806.75375</v>
+        <v>45812.65958333333</v>
       </c>
       <c r="G944">
         <v>0</v>
@@ -24136,16 +24136,16 @@
         <v>1</v>
       </c>
       <c r="C962">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D962" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E962">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F962" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G962">
         <v>0</v>
@@ -25738,16 +25738,16 @@
         <v>1</v>
       </c>
       <c r="C1025">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D1025" s="2">
-        <v>45806.77605776805</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1025">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F1025" s="2">
-        <v>45806.74983796296</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G1025">
         <v>0</v>
@@ -26650,16 +26650,16 @@
         <v>1</v>
       </c>
       <c r="C1061">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D1061" s="2">
-        <v>45798.9653592312</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E1061">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F1061" s="2">
-        <v>45798.71837962963</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G1061">
         <v>0</v>
@@ -26676,16 +26676,16 @@
         <v>1</v>
       </c>
       <c r="C1062">
-        <v>691</v>
+        <v>681</v>
       </c>
       <c r="D1062" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E1062">
-        <v>691</v>
+        <v>681</v>
       </c>
       <c r="F1062" s="2">
-        <v>45811.50931712963</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G1062">
         <v>0</v>
@@ -28017,16 +28017,16 @@
         <v>1</v>
       </c>
       <c r="C1116">
-        <v>33</v>
+        <v>-87</v>
       </c>
       <c r="D1116" s="2">
-        <v>45795.04204563411</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E1116">
-        <v>33</v>
+        <v>-87</v>
       </c>
       <c r="F1116" s="2">
-        <v>45749.69678240741</v>
+        <v>45812.69229166667</v>
       </c>
       <c r="G1116">
         <v>0</v>
@@ -28173,16 +28173,16 @@
         <v>1</v>
       </c>
       <c r="C1122">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1122" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E1122">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1122" s="2">
-        <v>45811.65459490741</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G1122">
         <v>0</v>
@@ -28479,16 +28479,16 @@
         <v>1</v>
       </c>
       <c r="C1134">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D1134" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E1134">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F1134" s="2">
-        <v>45811.69771990741</v>
+        <v>45812.68138888889</v>
       </c>
       <c r="G1134">
         <v>0</v>
@@ -28805,16 +28805,16 @@
         <v>1</v>
       </c>
       <c r="C1147">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1147" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1147">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F1147" s="2">
-        <v>45811.50252314815</v>
+        <v>45812.43199074074</v>
       </c>
       <c r="G1147">
         <v>0</v>
@@ -29521,16 +29521,16 @@
         <v>1</v>
       </c>
       <c r="C1175">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1175" s="2">
-        <v>45810.72559945051</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1175">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F1175" s="2">
-        <v>45810.60861111111</v>
+        <v>45812.43199074074</v>
       </c>
       <c r="G1175">
         <v>0</v>
@@ -29573,16 +29573,16 @@
         <v>1</v>
       </c>
       <c r="C1177">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D1177" s="2">
-        <v>45806.77600903736</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1177">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F1177" s="2">
-        <v>45806.44422453704</v>
+        <v>45812.43105324074</v>
       </c>
       <c r="G1177">
         <v>0</v>
@@ -29943,7 +29943,7 @@
         <v>0</v>
       </c>
       <c r="F1191" s="2">
-        <v>45805.67751157407</v>
+        <v>45812.78693287037</v>
       </c>
       <c r="G1191">
         <v>0</v>
@@ -30064,16 +30064,16 @@
         <v>1</v>
       </c>
       <c r="C1196">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1196" s="2">
-        <v>45795.04199224871</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E1196">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1196" s="2">
-        <v>45694.52438657408</v>
+        <v>45812.70203703704</v>
       </c>
       <c r="G1196">
         <v>0</v>
@@ -30760,16 +30760,16 @@
         <v>1</v>
       </c>
       <c r="C1223">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D1223" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E1223">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F1223" s="2">
-        <v>45811.6834837963</v>
+        <v>45812.5547337963</v>
       </c>
       <c r="G1223">
         <v>0</v>
@@ -31528,16 +31528,16 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>269</v>
+        <v>235</v>
       </c>
       <c r="D1253" s="2">
-        <v>45811.92552608132</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E1253">
-        <v>269</v>
+        <v>235</v>
       </c>
       <c r="F1253" s="2">
-        <v>45811.78815972222</v>
+        <v>45812.65041666666</v>
       </c>
       <c r="G1253">
         <v>0</v>
@@ -31733,16 +31733,16 @@
         <v>1</v>
       </c>
       <c r="C1261">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D1261" s="2">
-        <v>45806.77600903736</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1261">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F1261" s="2">
-        <v>45806.66086805556</v>
+        <v>45812.47731481482</v>
       </c>
       <c r="G1261">
         <v>0</v>
@@ -31759,16 +31759,16 @@
         <v>1</v>
       </c>
       <c r="C1262">
-        <v>-5</v>
+        <v>7</v>
       </c>
       <c r="D1262" s="2">
-        <v>45811.92544186871</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1262">
-        <v>-5</v>
+        <v>7</v>
       </c>
       <c r="F1262" s="2">
-        <v>45811.40424768518</v>
+        <v>45812.32332175926</v>
       </c>
       <c r="G1262">
         <v>0</v>
@@ -33791,16 +33791,16 @@
         <v>1</v>
       </c>
       <c r="C1342">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="D1342" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78306321269</v>
       </c>
       <c r="E1342">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="F1342" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.70203703704</v>
       </c>
       <c r="G1342">
         <v>0</v>
@@ -34478,16 +34478,16 @@
         <v>1</v>
       </c>
       <c r="C1369">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D1369" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1369">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F1369" s="2">
-        <v>45811.68634259259</v>
+        <v>45812.47731481482</v>
       </c>
       <c r="G1369">
         <v>0</v>
@@ -35067,16 +35067,16 @@
         <v>1</v>
       </c>
       <c r="C1392">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="D1392" s="2">
-        <v>45810.72559944464</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1392">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="F1392" s="2">
-        <v>45810.54670138889</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G1392">
         <v>0</v>
@@ -36450,16 +36450,16 @@
         <v>1</v>
       </c>
       <c r="C1446">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D1446" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E1446">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F1446" s="2">
-        <v>45811.72346064815</v>
+        <v>45812.65041666666</v>
       </c>
       <c r="G1446">
         <v>0</v>
@@ -37962,16 +37962,16 @@
         <v>1</v>
       </c>
       <c r="C1506">
-        <v>-3</v>
+        <v>6</v>
       </c>
       <c r="D1506" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1506">
-        <v>-3</v>
+        <v>6</v>
       </c>
       <c r="F1506" s="2">
-        <v>45811.45587962963</v>
+        <v>45812.32796296296</v>
       </c>
       <c r="G1506">
         <v>0</v>
@@ -37988,16 +37988,16 @@
         <v>1</v>
       </c>
       <c r="C1507">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D1507" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E1507">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="F1507" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G1507">
         <v>0</v>
@@ -40145,16 +40145,16 @@
         <v>1</v>
       </c>
       <c r="C1594">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D1594" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E1594">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F1594" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.65041666666</v>
       </c>
       <c r="G1594">
         <v>0</v>
@@ -40223,16 +40223,16 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>6649</v>
+        <v>6092</v>
       </c>
       <c r="D1597" s="2">
-        <v>45811.92552608132</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E1597">
-        <v>6649</v>
+        <v>6092</v>
       </c>
       <c r="F1597" s="2">
-        <v>45811.78815972222</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G1597">
         <v>0</v>
@@ -41190,16 +41190,16 @@
         <v>1</v>
       </c>
       <c r="C1635">
-        <v>186</v>
+        <v>2773</v>
       </c>
       <c r="D1635" s="2">
-        <v>45811.92552608132</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E1635">
-        <v>186</v>
+        <v>2773</v>
       </c>
       <c r="F1635" s="2">
-        <v>45811.78815972222</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G1635">
         <v>0</v>
@@ -41576,16 +41576,16 @@
         <v>1</v>
       </c>
       <c r="C1651">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D1651" s="2">
-        <v>45810.72563720519</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1651">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F1651" s="2">
-        <v>45810.68862268519</v>
+        <v>45812.47731481482</v>
       </c>
       <c r="G1651">
         <v>0</v>
@@ -41703,16 +41703,16 @@
         <v>1</v>
       </c>
       <c r="C1656">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1656" s="2">
-        <v>45810.72559945051</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1656">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F1656" s="2">
-        <v>45810.61395833334</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G1656">
         <v>0</v>
@@ -43805,16 +43805,16 @@
         <v>1</v>
       </c>
       <c r="C1741">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1741" s="2">
-        <v>45798.96533509644</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1741">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F1741" s="2">
-        <v>45798.64270833333</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G1741">
         <v>0</v>
@@ -45533,16 +45533,16 @@
         <v>1</v>
       </c>
       <c r="C1810">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D1810" s="2">
-        <v>45800.9317538197</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E1810">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F1810" s="2">
-        <v>45800.46056712963</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G1810">
         <v>0</v>
@@ -45943,16 +45943,16 @@
         <v>1</v>
       </c>
       <c r="C1826">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1826" s="2">
-        <v>45795.04204563411</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1826">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F1826" s="2">
-        <v>45747.70436342592</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G1826">
         <v>0</v>
@@ -46855,16 +46855,16 @@
         <v>1</v>
       </c>
       <c r="C1862">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D1862" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E1862">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F1862" s="2">
-        <v>45811.72346064815</v>
+        <v>45812.32642361111</v>
       </c>
       <c r="G1862">
         <v>0</v>
@@ -47037,16 +47037,16 @@
         <v>1</v>
       </c>
       <c r="C1869">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D1869" s="2">
-        <v>45799.89536722513</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E1869">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="F1869" s="2">
-        <v>45796.76049768519</v>
+        <v>45812.63878472222</v>
       </c>
       <c r="G1869">
         <v>0</v>
@@ -47444,16 +47444,16 @@
         <v>1</v>
       </c>
       <c r="C1885">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D1885" s="2">
-        <v>45810.72556745499</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1885">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F1885" s="2">
-        <v>45810.44699074074</v>
+        <v>45812.43199074074</v>
       </c>
       <c r="G1885">
         <v>0</v>
@@ -47888,16 +47888,16 @@
         <v>1</v>
       </c>
       <c r="C1903">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="D1903" s="2">
-        <v>45806.77600903736</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E1903">
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="F1903" s="2">
-        <v>45806.44605324074</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G1903">
         <v>0</v>
@@ -48122,16 +48122,16 @@
         <v>1</v>
       </c>
       <c r="C1912">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D1912" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E1912">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="F1912" s="2">
-        <v>45811.42484953703</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G1912">
         <v>0</v>
@@ -48832,16 +48832,16 @@
         <v>1</v>
       </c>
       <c r="C1940">
-        <v>-9</v>
+        <v>91</v>
       </c>
       <c r="D1940" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E1940">
-        <v>-9</v>
+        <v>91</v>
       </c>
       <c r="F1940" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.66930555556</v>
       </c>
       <c r="G1940">
         <v>0</v>
@@ -49833,16 +49833,16 @@
         <v>1</v>
       </c>
       <c r="C1980">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D1980" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1980">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F1980" s="2">
-        <v>45811.64200231482</v>
+        <v>45812.32672453704</v>
       </c>
       <c r="G1980">
         <v>0</v>
@@ -50032,16 +50032,16 @@
         <v>1</v>
       </c>
       <c r="C1988">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="D1988" s="2">
-        <v>45795.04186106093</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E1988">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="F1988" s="2">
-        <v>45587.3391087963</v>
+        <v>45812.44633101852</v>
       </c>
       <c r="G1988">
         <v>0</v>
@@ -50918,7 +50918,7 @@
         <v>24</v>
       </c>
       <c r="F2023" s="2">
-        <v>45811.67199074074</v>
+        <v>45812.67899305555</v>
       </c>
       <c r="G2023">
         <v>0</v>
@@ -50935,16 +50935,16 @@
         <v>1</v>
       </c>
       <c r="C2024">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2024" s="2">
-        <v>45811.92552608132</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E2024">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2024" s="2">
-        <v>45811.78815972222</v>
+        <v>45812.67899305555</v>
       </c>
       <c r="G2024">
         <v>0</v>
@@ -51059,16 +51059,16 @@
         <v>1</v>
       </c>
       <c r="C2029">
-        <v>14</v>
+        <v>-9</v>
       </c>
       <c r="D2029" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E2029">
-        <v>14</v>
+        <v>-9</v>
       </c>
       <c r="F2029" s="2">
-        <v>45811.54019675926</v>
+        <v>45812.54806712963</v>
       </c>
       <c r="G2029">
         <v>0</v>
@@ -51394,16 +51394,16 @@
         <v>1</v>
       </c>
       <c r="C2042">
-        <v>-4</v>
+        <v>11</v>
       </c>
       <c r="D2042" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E2042">
-        <v>-4</v>
+        <v>11</v>
       </c>
       <c r="F2042" s="2">
-        <v>45811.6834837963</v>
+        <v>45812.64480324074</v>
       </c>
       <c r="G2042">
         <v>0</v>
@@ -51746,16 +51746,16 @@
         <v>1</v>
       </c>
       <c r="C2056">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D2056" s="2">
-        <v>45811.92552606984</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E2056">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F2056" s="2">
-        <v>45811.75439814815</v>
+        <v>45812.53496527778</v>
       </c>
       <c r="G2056">
         <v>0</v>
@@ -53682,16 +53682,16 @@
         <v>1</v>
       </c>
       <c r="C2133">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D2133" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E2133">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F2133" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.66236111111</v>
       </c>
       <c r="G2133">
         <v>0</v>
@@ -56660,16 +56660,16 @@
         <v>1</v>
       </c>
       <c r="C2251">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D2251" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78303939045</v>
       </c>
       <c r="E2251">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F2251" s="2">
-        <v>45811.50252314815</v>
+        <v>45812.32579861111</v>
       </c>
       <c r="G2251">
         <v>0</v>
@@ -57944,10 +57944,13 @@
         <v>0</v>
       </c>
       <c r="D2302" s="2">
-        <v>45795.04186106093</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E2302">
         <v>0</v>
+      </c>
+      <c r="F2302" s="2">
+        <v>45812.65283564815</v>
       </c>
       <c r="G2302">
         <v>0</v>
@@ -58252,16 +58255,16 @@
         <v>1</v>
       </c>
       <c r="C2315">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D2315" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E2315">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F2315" s="2">
-        <v>45811.69520833333</v>
+        <v>45812.66177083334</v>
       </c>
       <c r="G2315">
         <v>0</v>
@@ -60764,16 +60767,16 @@
         <v>1</v>
       </c>
       <c r="C2416">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="D2416" s="2">
-        <v>45811.92552607598</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E2416">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="F2416" s="2">
-        <v>45811.76255787037</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G2416">
         <v>0</v>
@@ -60992,16 +60995,16 @@
         <v>1</v>
       </c>
       <c r="C2425">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="D2425" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301983239</v>
       </c>
       <c r="E2425">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="F2425" s="2">
-        <v>45811.6834837963</v>
+        <v>45812.32371527778</v>
       </c>
       <c r="G2425">
         <v>0</v>
@@ -61159,16 +61162,16 @@
         <v>1</v>
       </c>
       <c r="C2432">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D2432" s="2">
-        <v>45811.92546678011</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E2432">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F2432" s="2">
-        <v>45811.64716435185</v>
+        <v>45812.65634259259</v>
       </c>
       <c r="G2432">
         <v>0</v>
@@ -62358,16 +62361,16 @@
         <v>1</v>
       </c>
       <c r="C2481">
-        <v>193</v>
+        <v>138</v>
       </c>
       <c r="D2481" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E2481">
-        <v>193</v>
+        <v>138</v>
       </c>
       <c r="F2481" s="2">
-        <v>45811.73097222222</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G2481">
         <v>0</v>
@@ -62384,16 +62387,16 @@
         <v>1</v>
       </c>
       <c r="C2482">
-        <v>468</v>
+        <v>398</v>
       </c>
       <c r="D2482" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E2482">
-        <v>468</v>
+        <v>398</v>
       </c>
       <c r="F2482" s="2">
-        <v>45811.72704861111</v>
+        <v>45812.53040509259</v>
       </c>
       <c r="G2482">
         <v>0</v>
@@ -62410,16 +62413,16 @@
         <v>1</v>
       </c>
       <c r="C2483">
-        <v>826</v>
+        <v>821</v>
       </c>
       <c r="D2483" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78306321269</v>
       </c>
       <c r="E2483">
-        <v>826</v>
+        <v>821</v>
       </c>
       <c r="F2483" s="2">
-        <v>45811.73097222222</v>
+        <v>45812.70203703704</v>
       </c>
       <c r="G2483">
         <v>0</v>
@@ -62436,16 +62439,16 @@
         <v>1</v>
       </c>
       <c r="C2484">
-        <v>891</v>
+        <v>841</v>
       </c>
       <c r="D2484" s="2">
-        <v>45811.92549991595</v>
+        <v>45812.78306321269</v>
       </c>
       <c r="E2484">
-        <v>891</v>
+        <v>841</v>
       </c>
       <c r="F2484" s="2">
-        <v>45811.73097222222</v>
+        <v>45812.70203703704</v>
       </c>
       <c r="G2484">
         <v>0</v>
@@ -62514,16 +62517,16 @@
         <v>1</v>
       </c>
       <c r="C2487">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2487" s="2">
-        <v>45799.89536722513</v>
+        <v>45812.78301989438</v>
       </c>
       <c r="E2487">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2487" s="2">
-        <v>45796.65907407407</v>
+        <v>45812.65958333333</v>
       </c>
       <c r="G2487">
         <v>0</v>
@@ -63790,16 +63793,16 @@
         <v>1</v>
       </c>
       <c r="C2540">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2540" s="2">
-        <v>45807.78643074667</v>
+        <v>45812.78306322403</v>
       </c>
       <c r="E2540">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F2540" s="2">
-        <v>45807.72137731482</v>
+        <v>45812.70449074074</v>
       </c>
       <c r="G2540">
         <v>0</v>
@@ -64168,6 +64171,52 @@
         <v>0</v>
       </c>
       <c r="H2555" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2556" spans="1:8">
+      <c r="A2556">
+        <v>43435093</v>
+      </c>
+      <c r="B2556">
+        <v>1</v>
+      </c>
+      <c r="C2556">
+        <v>0</v>
+      </c>
+      <c r="D2556" s="2">
+        <v>45812.78301983239</v>
+      </c>
+      <c r="E2556">
+        <v>0</v>
+      </c>
+      <c r="G2556">
+        <v>0</v>
+      </c>
+      <c r="H2556" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:8">
+      <c r="A2557">
+        <v>43445008</v>
+      </c>
+      <c r="B2557">
+        <v>1</v>
+      </c>
+      <c r="C2557">
+        <v>0</v>
+      </c>
+      <c r="D2557" s="2">
+        <v>45812.78306321269</v>
+      </c>
+      <c r="E2557">
+        <v>0</v>
+      </c>
+      <c r="G2557">
+        <v>0</v>
+      </c>
+      <c r="H2557" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizacao dos dados da add
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="10">
   <si>
     <t>id_produto</t>
   </si>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2557"/>
+  <dimension ref="A1:H2558"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,16 +494,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95782005877</v>
       </c>
       <c r="E4">
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2">
-        <v>45812.78209490741</v>
+        <v>45813.426875</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -529,7 +529,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>45811.69234953704</v>
+        <v>45813.68033564815</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -690,16 +690,16 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95785145537</v>
       </c>
       <c r="E12">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="2">
-        <v>45811.68651620371</v>
+        <v>45813.46407407407</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -978,16 +978,16 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D24" s="2">
-        <v>45812.78303939045</v>
+        <v>45813.95782007044</v>
       </c>
       <c r="E24">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F24" s="2">
-        <v>45812.70203703704</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1194,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>1558</v>
+        <v>3172</v>
       </c>
       <c r="D33" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95788194679</v>
       </c>
       <c r="E33">
-        <v>1558</v>
+        <v>3172</v>
       </c>
       <c r="F33" s="2">
-        <v>45812.63878472222</v>
+        <v>45813.67818287037</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1563,16 +1563,16 @@
         <v>1</v>
       </c>
       <c r="C48">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D48" s="2">
-        <v>45812.78303939045</v>
+        <v>45813.95788194679</v>
       </c>
       <c r="E48">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F48" s="2">
-        <v>45812.70203703704</v>
+        <v>45813.67818287037</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1589,16 +1589,16 @@
         <v>1</v>
       </c>
       <c r="C49">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D49" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E49">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F49" s="2">
-        <v>45812.53040509259</v>
+        <v>45813.60496527778</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -1765,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D56" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95795447831</v>
       </c>
       <c r="E56">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="F56" s="2">
-        <v>45812.65041666666</v>
+        <v>45813.60496527778</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -1817,16 +1817,16 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D58" s="2">
-        <v>45812.78303939045</v>
+        <v>45813.95795446759</v>
       </c>
       <c r="E58">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F58" s="2">
-        <v>45812.70203703704</v>
+        <v>45813.57855324074</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -1843,16 +1843,16 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D59" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95795446759</v>
       </c>
       <c r="E59">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F59" s="2">
-        <v>45811.6834837963</v>
+        <v>45813.57359953703</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -1941,16 +1941,16 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D63" s="2">
-        <v>45812.78303939045</v>
+        <v>45813.95795446759</v>
       </c>
       <c r="E63">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F63" s="2">
-        <v>45812.70203703704</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2114,16 +2114,16 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D70" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E70">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F70" s="2">
-        <v>45812.5275925926</v>
+        <v>45813.65289351852</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2503,16 +2503,16 @@
         <v>1</v>
       </c>
       <c r="C86">
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="D86" s="2">
-        <v>45811.92552607598</v>
+        <v>45813.95788194679</v>
       </c>
       <c r="E86">
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="F86" s="2">
-        <v>45811.76255787037</v>
+        <v>45813.67818287037</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -2529,16 +2529,16 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D87" s="2">
-        <v>45812.78303939045</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E87">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="F87" s="2">
-        <v>45812.6909837963</v>
+        <v>45813.58277777778</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -2630,16 +2630,16 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D91" s="2">
-        <v>45812.78303939045</v>
+        <v>45813.95782007044</v>
       </c>
       <c r="E91">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F91" s="2">
-        <v>45812.69229166667</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -2702,16 +2702,16 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D94" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E94">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F94" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.65432870371</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -2872,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>1045</v>
+        <v>875</v>
       </c>
       <c r="D101" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95793318399</v>
       </c>
       <c r="E101">
-        <v>1045</v>
+        <v>875</v>
       </c>
       <c r="F101" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -2993,16 +2993,16 @@
         <v>1</v>
       </c>
       <c r="C106">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="D106" s="2">
-        <v>45811.92552608132</v>
+        <v>45813.95793319555</v>
       </c>
       <c r="E106">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="F106" s="2">
-        <v>45811.7677662037</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -3209,16 +3209,16 @@
         <v>1</v>
       </c>
       <c r="C115">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D115" s="2">
-        <v>45807.78643077149</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E115">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="F115" s="2">
-        <v>45807.78542824074</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -3267,7 +3267,7 @@
         <v>1131</v>
       </c>
       <c r="F117" s="2">
-        <v>45811.75119212963</v>
+        <v>45813.51170138889</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -3408,16 +3408,16 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>2</v>
+        <v>-13</v>
       </c>
       <c r="D123" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E123">
-        <v>2</v>
+        <v>-13</v>
       </c>
       <c r="F123" s="2">
-        <v>45812.44633101852</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -3460,16 +3460,16 @@
         <v>1</v>
       </c>
       <c r="C125">
-        <v>289</v>
+        <v>202</v>
       </c>
       <c r="D125" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95788194679</v>
       </c>
       <c r="E125">
-        <v>289</v>
+        <v>202</v>
       </c>
       <c r="F125" s="2">
-        <v>45812.65041666666</v>
+        <v>45813.67818287037</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -3797,16 +3797,16 @@
         <v>1</v>
       </c>
       <c r="C139">
-        <v>-4</v>
+        <v>57</v>
       </c>
       <c r="D139" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95788193521</v>
       </c>
       <c r="E139">
-        <v>-4</v>
+        <v>57</v>
       </c>
       <c r="F139" s="2">
-        <v>45811.50664351852</v>
+        <v>45813.67089120371</v>
       </c>
       <c r="G139">
         <v>0</v>
@@ -3846,16 +3846,16 @@
         <v>1</v>
       </c>
       <c r="C141">
-        <v>580</v>
+        <v>556</v>
       </c>
       <c r="D141" s="2">
-        <v>45812.78303939045</v>
+        <v>45813.95785145537</v>
       </c>
       <c r="E141">
-        <v>580</v>
+        <v>556</v>
       </c>
       <c r="F141" s="2">
-        <v>45812.70203703704</v>
+        <v>45813.51621527778</v>
       </c>
       <c r="G141">
         <v>0</v>
@@ -4109,7 +4109,7 @@
         <v>0</v>
       </c>
       <c r="F151" s="2">
-        <v>45807.70732638889</v>
+        <v>45813.63825231481</v>
       </c>
       <c r="G151">
         <v>0</v>
@@ -4230,7 +4230,7 @@
         <v>0</v>
       </c>
       <c r="F156" s="2">
-        <v>45811.52616898148</v>
+        <v>45813.65226851852</v>
       </c>
       <c r="G156">
         <v>0</v>
@@ -4319,16 +4319,16 @@
         <v>1</v>
       </c>
       <c r="C160">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="D160" s="2">
-        <v>45812.78306321269</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E160">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="F160" s="2">
-        <v>45812.44633101852</v>
+        <v>45813.6289699074</v>
       </c>
       <c r="G160">
         <v>0</v>
@@ -4936,16 +4936,16 @@
         <v>1</v>
       </c>
       <c r="C185">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="D185" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95788193521</v>
       </c>
       <c r="E185">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="F185" s="2">
-        <v>45811.48847222222</v>
+        <v>45813.66761574074</v>
       </c>
       <c r="G185">
         <v>0</v>
@@ -5077,16 +5077,16 @@
         <v>1</v>
       </c>
       <c r="C191">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D191" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E191">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F191" s="2">
-        <v>45812.31930555555</v>
+        <v>45813.57680555555</v>
       </c>
       <c r="G191">
         <v>0</v>
@@ -5181,16 +5181,16 @@
         <v>1</v>
       </c>
       <c r="C195">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D195" s="2">
-        <v>45811.92552606984</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E195">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F195" s="2">
-        <v>45811.75335648148</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G195">
         <v>0</v>
@@ -5302,16 +5302,16 @@
         <v>1</v>
       </c>
       <c r="C200">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="D200" s="2">
-        <v>45810.72563721648</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E200">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="F200" s="2">
-        <v>45810.75585648148</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G200">
         <v>0</v>
@@ -5328,16 +5328,16 @@
         <v>1</v>
       </c>
       <c r="C201">
-        <v>1066</v>
+        <v>1056</v>
       </c>
       <c r="D201" s="2">
-        <v>45805.91875154599</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E201">
-        <v>1066</v>
+        <v>1056</v>
       </c>
       <c r="F201" s="2">
-        <v>45805.70947916667</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G201">
         <v>0</v>
@@ -6175,16 +6175,16 @@
         <v>1</v>
       </c>
       <c r="C236">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D236" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E236">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F236" s="2">
-        <v>45811.50931712963</v>
+        <v>45813.5819212963</v>
       </c>
       <c r="G236">
         <v>0</v>
@@ -6437,16 +6437,16 @@
         <v>1</v>
       </c>
       <c r="C247">
-        <v>1269</v>
+        <v>1261</v>
       </c>
       <c r="D247" s="2">
-        <v>45812.78299904546</v>
+        <v>45813.95795447831</v>
       </c>
       <c r="E247">
-        <v>1269</v>
+        <v>1261</v>
       </c>
       <c r="F247" s="2">
-        <v>45812.31732638889</v>
+        <v>45813.58277777778</v>
       </c>
       <c r="G247">
         <v>0</v>
@@ -6627,16 +6627,16 @@
         <v>1</v>
       </c>
       <c r="C255">
-        <v>-33</v>
+        <v>4</v>
       </c>
       <c r="D255" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E255">
-        <v>-33</v>
+        <v>4</v>
       </c>
       <c r="F255" s="2">
-        <v>45812.63135416667</v>
+        <v>45813.63554398148</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -6996,16 +6996,16 @@
         <v>1</v>
       </c>
       <c r="C270">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D270" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95782007044</v>
       </c>
       <c r="E270">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F270" s="2">
-        <v>45812.47226851852</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G270">
         <v>0</v>
@@ -7045,16 +7045,16 @@
         <v>1</v>
       </c>
       <c r="C272">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="D272" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E272">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="F272" s="2">
-        <v>45811.50931712963</v>
+        <v>45813.5819212963</v>
       </c>
       <c r="G272">
         <v>0</v>
@@ -7071,16 +7071,16 @@
         <v>1</v>
       </c>
       <c r="C273">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D273" s="2">
-        <v>45805.918751534</v>
+        <v>45813.95788194679</v>
       </c>
       <c r="E273">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F273" s="2">
-        <v>45805.70140046296</v>
+        <v>45813.67818287037</v>
       </c>
       <c r="G273">
         <v>0</v>
@@ -7097,16 +7097,16 @@
         <v>1</v>
       </c>
       <c r="C274">
-        <v>215</v>
+        <v>464</v>
       </c>
       <c r="D274" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95788197009</v>
       </c>
       <c r="E274">
-        <v>215</v>
+        <v>464</v>
       </c>
       <c r="F274" s="2">
-        <v>45811.72704861111</v>
+        <v>45813.68067129629</v>
       </c>
       <c r="G274">
         <v>0</v>
@@ -7310,16 +7310,16 @@
         <v>1</v>
       </c>
       <c r="C283">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D283" s="2">
-        <v>45811.92544186871</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E283">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F283" s="2">
-        <v>45811.42122685185</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G283">
         <v>0</v>
@@ -7408,16 +7408,16 @@
         <v>1</v>
       </c>
       <c r="C287">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="D287" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95782005877</v>
       </c>
       <c r="E287">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="F287" s="2">
-        <v>45812.48946759259</v>
+        <v>45813.42155092592</v>
       </c>
       <c r="G287">
         <v>0</v>
@@ -7509,16 +7509,16 @@
         <v>1</v>
       </c>
       <c r="C291">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="D291" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E291">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="F291" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.58258101852</v>
       </c>
       <c r="G291">
         <v>0</v>
@@ -7610,16 +7610,16 @@
         <v>1</v>
       </c>
       <c r="C295">
-        <v>415</v>
+        <v>373</v>
       </c>
       <c r="D295" s="2">
-        <v>45812.78303939045</v>
+        <v>45813.95793319555</v>
       </c>
       <c r="E295">
-        <v>415</v>
+        <v>373</v>
       </c>
       <c r="F295" s="2">
-        <v>45812.69229166667</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G295">
         <v>0</v>
@@ -7962,7 +7962,7 @@
         <v>1126</v>
       </c>
       <c r="F309" s="2">
-        <v>45811.76255787037</v>
+        <v>45813.51170138889</v>
       </c>
       <c r="G309">
         <v>0</v>
@@ -8071,16 +8071,16 @@
         <v>1</v>
       </c>
       <c r="C314">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D314" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E314">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="F314" s="2">
-        <v>45812.54806712963</v>
+        <v>45813.57359953703</v>
       </c>
       <c r="G314">
         <v>0</v>
@@ -8097,16 +8097,16 @@
         <v>1</v>
       </c>
       <c r="C315">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D315" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E315">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="F315" s="2">
-        <v>45811.49375</v>
+        <v>45813.57829861111</v>
       </c>
       <c r="G315">
         <v>0</v>
@@ -8169,16 +8169,16 @@
         <v>1</v>
       </c>
       <c r="C318">
-        <v>-28</v>
+        <v>30</v>
       </c>
       <c r="D318" s="2">
-        <v>45811.92552606984</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E318">
-        <v>-28</v>
+        <v>30</v>
       </c>
       <c r="F318" s="2">
-        <v>45811.75159722222</v>
+        <v>45813.63916666667</v>
       </c>
       <c r="G318">
         <v>0</v>
@@ -8374,16 +8374,16 @@
         <v>1</v>
       </c>
       <c r="C326">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D326" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E326">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F326" s="2">
-        <v>45812.65549768518</v>
+        <v>45813.57303240741</v>
       </c>
       <c r="G326">
         <v>0</v>
@@ -8772,16 +8772,16 @@
         <v>1</v>
       </c>
       <c r="C342">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D342" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E342">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F342" s="2">
-        <v>45811.47556712963</v>
+        <v>45813.57616898148</v>
       </c>
       <c r="G342">
         <v>0</v>
@@ -8870,16 +8870,16 @@
         <v>1</v>
       </c>
       <c r="C346">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D346" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E346">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F346" s="2">
-        <v>45811.68890046296</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G346">
         <v>0</v>
@@ -8965,16 +8965,16 @@
         <v>1</v>
       </c>
       <c r="C350">
-        <v>178</v>
+        <v>146</v>
       </c>
       <c r="D350" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95795449081</v>
       </c>
       <c r="E350">
-        <v>178</v>
+        <v>146</v>
       </c>
       <c r="F350" s="2">
-        <v>45811.50664351852</v>
+        <v>45813.58277777778</v>
       </c>
       <c r="G350">
         <v>0</v>
@@ -8991,16 +8991,16 @@
         <v>1</v>
       </c>
       <c r="C351">
-        <v>32</v>
+        <v>-112</v>
       </c>
       <c r="D351" s="2">
-        <v>45811.92544186871</v>
+        <v>45813.95795449081</v>
       </c>
       <c r="E351">
-        <v>32</v>
+        <v>-112</v>
       </c>
       <c r="F351" s="2">
-        <v>45811.41633101852</v>
+        <v>45813.63770833334</v>
       </c>
       <c r="G351">
         <v>0</v>
@@ -9115,16 +9115,16 @@
         <v>1</v>
       </c>
       <c r="C356">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D356" s="2">
-        <v>45810.72556744247</v>
+        <v>45813.95782007044</v>
       </c>
       <c r="E356">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F356" s="2">
-        <v>45810.44434027778</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G356">
         <v>0</v>
@@ -9164,16 +9164,16 @@
         <v>1</v>
       </c>
       <c r="C358">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D358" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95785145537</v>
       </c>
       <c r="E358">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F358" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.51621527778</v>
       </c>
       <c r="G358">
         <v>0</v>
@@ -9291,16 +9291,16 @@
         <v>1</v>
       </c>
       <c r="C363">
-        <v>730</v>
+        <v>692</v>
       </c>
       <c r="D363" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95788194679</v>
       </c>
       <c r="E363">
-        <v>730</v>
+        <v>692</v>
       </c>
       <c r="F363" s="2">
-        <v>45812.44633101852</v>
+        <v>45813.67818287037</v>
       </c>
       <c r="G363">
         <v>0</v>
@@ -9438,16 +9438,16 @@
         <v>1</v>
       </c>
       <c r="C369">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D369" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95785145537</v>
       </c>
       <c r="E369">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F369" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.51170138889</v>
       </c>
       <c r="G369">
         <v>0</v>
@@ -9487,16 +9487,16 @@
         <v>1</v>
       </c>
       <c r="C371">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D371" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95782005877</v>
       </c>
       <c r="E371">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F371" s="2">
-        <v>45811.50125</v>
+        <v>45813.42155092592</v>
       </c>
       <c r="G371">
         <v>0</v>
@@ -9764,16 +9764,16 @@
         <v>1</v>
       </c>
       <c r="C382">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D382" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95782005877</v>
       </c>
       <c r="E382">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="F382" s="2">
-        <v>45812.43199074074</v>
+        <v>45813.42155092592</v>
       </c>
       <c r="G382">
         <v>0</v>
@@ -9839,16 +9839,16 @@
         <v>1</v>
       </c>
       <c r="C385">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D385" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E385">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F385" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.58085648148</v>
       </c>
       <c r="G385">
         <v>0</v>
@@ -9865,16 +9865,16 @@
         <v>1</v>
       </c>
       <c r="C386">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="D386" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E386">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="F386" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.63309027778</v>
       </c>
       <c r="G386">
         <v>0</v>
@@ -9969,16 +9969,16 @@
         <v>1</v>
       </c>
       <c r="C390">
-        <v>-44</v>
+        <v>32</v>
       </c>
       <c r="D390" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95788193521</v>
       </c>
       <c r="E390">
-        <v>-44</v>
+        <v>32</v>
       </c>
       <c r="F390" s="2">
-        <v>45812.4777662037</v>
+        <v>45813.67373842592</v>
       </c>
       <c r="G390">
         <v>0</v>
@@ -10070,16 +10070,16 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D394" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95790534767</v>
       </c>
       <c r="E394">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F394" s="2">
-        <v>45812.65041666666</v>
+        <v>45813.57359953703</v>
       </c>
       <c r="G394">
         <v>0</v>
@@ -10278,7 +10278,7 @@
         <v>112</v>
       </c>
       <c r="F402" s="2">
-        <v>45811.72704861111</v>
+        <v>45813.51170138889</v>
       </c>
       <c r="G402">
         <v>0</v>
@@ -10321,16 +10321,16 @@
         <v>1</v>
       </c>
       <c r="C404">
-        <v>229</v>
+        <v>114</v>
       </c>
       <c r="D404" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E404">
-        <v>229</v>
+        <v>114</v>
       </c>
       <c r="F404" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.54864583333</v>
       </c>
       <c r="G404">
         <v>0</v>
@@ -10445,16 +10445,16 @@
         <v>1</v>
       </c>
       <c r="C409">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D409" s="2">
-        <v>45799.89532165734</v>
+        <v>45813.95782007044</v>
       </c>
       <c r="E409">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F409" s="2">
-        <v>45789.75767361111</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G409">
         <v>0</v>
@@ -10471,16 +10471,16 @@
         <v>1</v>
       </c>
       <c r="C410">
-        <v>-216</v>
+        <v>2236</v>
       </c>
       <c r="D410" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95788197009</v>
       </c>
       <c r="E410">
-        <v>-216</v>
+        <v>2236</v>
       </c>
       <c r="F410" s="2">
-        <v>45811.49375</v>
+        <v>45813.67957175926</v>
       </c>
       <c r="G410">
         <v>0</v>
@@ -10549,16 +10549,16 @@
         <v>1</v>
       </c>
       <c r="C413">
-        <v>258</v>
+        <v>198</v>
       </c>
       <c r="D413" s="2">
-        <v>45805.918751534</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E413">
-        <v>258</v>
+        <v>198</v>
       </c>
       <c r="F413" s="2">
-        <v>45805.70869212963</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G413">
         <v>0</v>
@@ -10624,16 +10624,16 @@
         <v>1</v>
       </c>
       <c r="C416">
-        <v>-24</v>
+        <v>71</v>
       </c>
       <c r="D416" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95788197009</v>
       </c>
       <c r="E416">
-        <v>-24</v>
+        <v>71</v>
       </c>
       <c r="F416" s="2">
-        <v>45811.47861111111</v>
+        <v>45813.67928240741</v>
       </c>
       <c r="G416">
         <v>0</v>
@@ -10673,16 +10673,16 @@
         <v>1</v>
       </c>
       <c r="C418">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="D418" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E418">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="F418" s="2">
-        <v>45811.72704861111</v>
+        <v>45813.58277777778</v>
       </c>
       <c r="G418">
         <v>0</v>
@@ -10771,16 +10771,16 @@
         <v>1</v>
       </c>
       <c r="C422">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D422" s="2">
-        <v>45810.72563721648</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E422">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F422" s="2">
-        <v>45810.75585648148</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G422">
         <v>0</v>
@@ -11088,16 +11088,16 @@
         <v>1</v>
       </c>
       <c r="C435">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D435" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E435">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F435" s="2">
-        <v>45811.68634259259</v>
+        <v>45813.58258101852</v>
       </c>
       <c r="G435">
         <v>0</v>
@@ -11140,16 +11140,16 @@
         <v>1</v>
       </c>
       <c r="C437">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D437" s="2">
-        <v>45795.04210567895</v>
+        <v>45813.95785145537</v>
       </c>
       <c r="E437">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F437" s="2">
-        <v>45776.72944444444</v>
+        <v>45813.51621527778</v>
       </c>
       <c r="G437">
         <v>0</v>
@@ -11192,16 +11192,16 @@
         <v>1</v>
       </c>
       <c r="C439">
-        <v>7</v>
+        <v>-3</v>
       </c>
       <c r="D439" s="2">
-        <v>45810.72556744247</v>
+        <v>45813.95793319555</v>
       </c>
       <c r="E439">
-        <v>7</v>
+        <v>-3</v>
       </c>
       <c r="F439" s="2">
-        <v>45810.44434027778</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G439">
         <v>0</v>
@@ -11296,16 +11296,16 @@
         <v>1</v>
       </c>
       <c r="C443">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D443" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E443">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F443" s="2">
-        <v>45812.48946759259</v>
+        <v>45813.57359953703</v>
       </c>
       <c r="G443">
         <v>0</v>
@@ -11728,16 +11728,16 @@
         <v>1</v>
       </c>
       <c r="C461">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D461" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E461">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F461" s="2">
-        <v>45811.42236111111</v>
+        <v>45813.58277777778</v>
       </c>
       <c r="G461">
         <v>0</v>
@@ -11832,16 +11832,16 @@
         <v>1</v>
       </c>
       <c r="C465">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D465" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95795447831</v>
       </c>
       <c r="E465">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="F465" s="2">
-        <v>45811.49467592593</v>
+        <v>45813.67818287037</v>
       </c>
       <c r="G465">
         <v>0</v>
@@ -11930,16 +11930,16 @@
         <v>1</v>
       </c>
       <c r="C469">
-        <v>-87</v>
+        <v>-104</v>
       </c>
       <c r="D469" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E469">
-        <v>-87</v>
+        <v>-104</v>
       </c>
       <c r="F469" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.58277777778</v>
       </c>
       <c r="G469">
         <v>0</v>
@@ -12005,16 +12005,16 @@
         <v>1</v>
       </c>
       <c r="C472">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D472" s="2">
-        <v>45810.72556744247</v>
+        <v>45813.95795447831</v>
       </c>
       <c r="E472">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F472" s="2">
-        <v>45810.44699074074</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G472">
         <v>0</v>
@@ -12207,16 +12207,16 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D480" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E480">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F480" s="2">
-        <v>45812.53040509259</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G480">
         <v>0</v>
@@ -13314,16 +13314,16 @@
         <v>1</v>
       </c>
       <c r="C525">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D525" s="2">
-        <v>45799.89534672352</v>
+        <v>45813.95782007044</v>
       </c>
       <c r="E525">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F525" s="2">
-        <v>45793.53142361111</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G525">
         <v>0</v>
@@ -13467,16 +13467,16 @@
         <v>1</v>
       </c>
       <c r="C531">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D531" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95782007044</v>
       </c>
       <c r="E531">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F531" s="2">
-        <v>45811.73097222222</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G531">
         <v>0</v>
@@ -14415,16 +14415,16 @@
         <v>1</v>
       </c>
       <c r="C570">
-        <v>2645</v>
+        <v>2644</v>
       </c>
       <c r="D570" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E570">
-        <v>2645</v>
+        <v>2644</v>
       </c>
       <c r="F570" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.58085648148</v>
       </c>
       <c r="G570">
         <v>0</v>
@@ -15207,16 +15207,16 @@
         <v>1</v>
       </c>
       <c r="C603">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D603" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95790539397</v>
       </c>
       <c r="E603">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F603" s="2">
-        <v>45811.47861111111</v>
+        <v>45813.57704861111</v>
       </c>
       <c r="G603">
         <v>0</v>
@@ -15956,16 +15956,16 @@
         <v>1</v>
       </c>
       <c r="C634">
-        <v>-12</v>
+        <v>26</v>
       </c>
       <c r="D634" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95788193521</v>
       </c>
       <c r="E634">
-        <v>-12</v>
+        <v>26</v>
       </c>
       <c r="F634" s="2">
-        <v>45811.50664351852</v>
+        <v>45813.66930555556</v>
       </c>
       <c r="G634">
         <v>0</v>
@@ -16385,16 +16385,16 @@
         <v>1</v>
       </c>
       <c r="C652">
-        <v>7</v>
+        <v>-5</v>
       </c>
       <c r="D652" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95793319555</v>
       </c>
       <c r="E652">
-        <v>7</v>
+        <v>-5</v>
       </c>
       <c r="F652" s="2">
-        <v>45811.50931712963</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G652">
         <v>0</v>
@@ -16509,16 +16509,16 @@
         <v>1</v>
       </c>
       <c r="C657">
-        <v>2160</v>
+        <v>2146</v>
       </c>
       <c r="D657" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E657">
-        <v>2160</v>
+        <v>2146</v>
       </c>
       <c r="F657" s="2">
-        <v>45812.63135416667</v>
+        <v>45813.60496527778</v>
       </c>
       <c r="G657">
         <v>0</v>
@@ -16584,16 +16584,16 @@
         <v>1</v>
       </c>
       <c r="C660">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D660" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E660">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F660" s="2">
-        <v>45812.53040509259</v>
+        <v>45813.5819212963</v>
       </c>
       <c r="G660">
         <v>0</v>
@@ -17094,16 +17094,16 @@
         <v>1</v>
       </c>
       <c r="C681">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D681" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95795449081</v>
       </c>
       <c r="E681">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F681" s="2">
-        <v>45812.53040509259</v>
+        <v>45813.78240740741</v>
       </c>
       <c r="G681">
         <v>0</v>
@@ -17342,16 +17342,16 @@
         <v>1</v>
       </c>
       <c r="C691">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D691" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95795449081</v>
       </c>
       <c r="E691">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F691" s="2">
-        <v>45812.44633101852</v>
+        <v>45813.82861111111</v>
       </c>
       <c r="G691">
         <v>0</v>
@@ -17573,16 +17573,16 @@
         <v>1</v>
       </c>
       <c r="C700">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="D700" s="2">
-        <v>45795.04208095842</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E700">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="F700" s="2">
-        <v>45758.39363425926</v>
+        <v>45813.54864583333</v>
       </c>
       <c r="G700">
         <v>0</v>
@@ -17599,16 +17599,16 @@
         <v>1</v>
       </c>
       <c r="C701">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D701" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E701">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F701" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.57766203704</v>
       </c>
       <c r="G701">
         <v>0</v>
@@ -17830,7 +17830,7 @@
         <v>165</v>
       </c>
       <c r="F710" s="2">
-        <v>45811.72704861111</v>
+        <v>45813.51170138889</v>
       </c>
       <c r="G710">
         <v>0</v>
@@ -18072,16 +18072,16 @@
         <v>1</v>
       </c>
       <c r="C720">
-        <v>586</v>
+        <v>571</v>
       </c>
       <c r="D720" s="2">
-        <v>45812.78306321269</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E720">
-        <v>586</v>
+        <v>571</v>
       </c>
       <c r="F720" s="2">
-        <v>45812.44633101852</v>
+        <v>45813.58108796296</v>
       </c>
       <c r="G720">
         <v>0</v>
@@ -18098,16 +18098,16 @@
         <v>1</v>
       </c>
       <c r="C721">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="D721" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E721">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="F721" s="2">
-        <v>45812.44633101852</v>
+        <v>45813.63019675926</v>
       </c>
       <c r="G721">
         <v>0</v>
@@ -18150,16 +18150,16 @@
         <v>1</v>
       </c>
       <c r="C723">
-        <v>14</v>
+        <v>-16</v>
       </c>
       <c r="D723" s="2">
-        <v>45811.92552607598</v>
+        <v>45813.95790535926</v>
       </c>
       <c r="E723">
-        <v>14</v>
+        <v>-16</v>
       </c>
       <c r="F723" s="2">
-        <v>45811.76435185185</v>
+        <v>45813.68569444444</v>
       </c>
       <c r="G723">
         <v>0</v>
@@ -18237,7 +18237,7 @@
         <v>93</v>
       </c>
       <c r="F726" s="2">
-        <v>45812.47731481482</v>
+        <v>45813.51170138889</v>
       </c>
       <c r="G726">
         <v>0</v>
@@ -18303,16 +18303,16 @@
         <v>1</v>
       </c>
       <c r="C729">
-        <v>-20</v>
+        <v>35</v>
       </c>
       <c r="D729" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95788193521</v>
       </c>
       <c r="E729">
-        <v>-20</v>
+        <v>35</v>
       </c>
       <c r="F729" s="2">
-        <v>45811.50931712963</v>
+        <v>45813.67116898148</v>
       </c>
       <c r="G729">
         <v>0</v>
@@ -18329,16 +18329,16 @@
         <v>1</v>
       </c>
       <c r="C730">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="D730" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95788197009</v>
       </c>
       <c r="E730">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="F730" s="2">
-        <v>45811.50931712963</v>
+        <v>45813.68012731482</v>
       </c>
       <c r="G730">
         <v>0</v>
@@ -18355,16 +18355,16 @@
         <v>1</v>
       </c>
       <c r="C731">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="D731" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95788193521</v>
       </c>
       <c r="E731">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="F731" s="2">
-        <v>45811.50664351852</v>
+        <v>45813.66902777777</v>
       </c>
       <c r="G731">
         <v>0</v>
@@ -18381,16 +18381,16 @@
         <v>1</v>
       </c>
       <c r="C732">
-        <v>349</v>
+        <v>321</v>
       </c>
       <c r="D732" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E732">
-        <v>349</v>
+        <v>321</v>
       </c>
       <c r="F732" s="2">
-        <v>45811.64200231482</v>
+        <v>45813.58277777778</v>
       </c>
       <c r="G732">
         <v>0</v>
@@ -18508,16 +18508,16 @@
         <v>1</v>
       </c>
       <c r="C737">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D737" s="2">
-        <v>45800.93204011993</v>
+        <v>45813.95793319555</v>
       </c>
       <c r="E737">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F737" s="2">
-        <v>45800.77331018518</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G737">
         <v>0</v>
@@ -18612,16 +18612,16 @@
         <v>1</v>
       </c>
       <c r="C741">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D741" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E741">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F741" s="2">
-        <v>45811.49467592593</v>
+        <v>45813.57855324074</v>
       </c>
       <c r="G741">
         <v>0</v>
@@ -19379,16 +19379,16 @@
         <v>1</v>
       </c>
       <c r="C772">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="D772" s="2">
-        <v>45812.78303939045</v>
+        <v>45813.95785145537</v>
       </c>
       <c r="E772">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="F772" s="2">
-        <v>45812.6909837963</v>
+        <v>45813.46407407407</v>
       </c>
       <c r="G772">
         <v>0</v>
@@ -19535,16 +19535,16 @@
         <v>1</v>
       </c>
       <c r="C778">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D778" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E778">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F778" s="2">
-        <v>45812.53040509259</v>
+        <v>45813.60496527778</v>
       </c>
       <c r="G778">
         <v>0</v>
@@ -20383,16 +20383,16 @@
         <v>1</v>
       </c>
       <c r="C812">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D812" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E812">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F812" s="2">
-        <v>45811.49375</v>
+        <v>45813.57680555555</v>
       </c>
       <c r="G812">
         <v>0</v>
@@ -20458,16 +20458,16 @@
         <v>1</v>
       </c>
       <c r="C815">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D815" s="2">
-        <v>45800.93188815672</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E815">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F815" s="2">
-        <v>45811.67939814815</v>
+        <v>45813.57766203704</v>
       </c>
       <c r="G815">
         <v>0</v>
@@ -20484,16 +20484,16 @@
         <v>1</v>
       </c>
       <c r="C816">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D816" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E816">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F816" s="2">
-        <v>45811.68032407408</v>
+        <v>45813.57766203704</v>
       </c>
       <c r="G816">
         <v>0</v>
@@ -20556,16 +20556,16 @@
         <v>1</v>
       </c>
       <c r="C819">
-        <v>-1</v>
+        <v>98</v>
       </c>
       <c r="D819" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E819">
-        <v>-1</v>
+        <v>98</v>
       </c>
       <c r="F819" s="2">
-        <v>45812.63878472222</v>
+        <v>45813.64146990741</v>
       </c>
       <c r="G819">
         <v>0</v>
@@ -20732,16 +20732,16 @@
         <v>1</v>
       </c>
       <c r="C826">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D826" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E826">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F826" s="2">
-        <v>45812.47731481482</v>
+        <v>45813.60496527778</v>
       </c>
       <c r="G826">
         <v>0</v>
@@ -21164,16 +21164,16 @@
         <v>1</v>
       </c>
       <c r="C844">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D844" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E844">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F844" s="2">
-        <v>45811.72704861111</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G844">
         <v>0</v>
@@ -21389,16 +21389,16 @@
         <v>1</v>
       </c>
       <c r="C853">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D853" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95782007044</v>
       </c>
       <c r="E853">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F853" s="2">
-        <v>45811.69520833333</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G853">
         <v>0</v>
@@ -21724,7 +21724,7 @@
         <v>0</v>
       </c>
       <c r="F866" s="2">
-        <v>45790.42966435185</v>
+        <v>45813.65351851852</v>
       </c>
       <c r="G866">
         <v>0</v>
@@ -21868,16 +21868,16 @@
         <v>1</v>
       </c>
       <c r="C872">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D872" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E872">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="F872" s="2">
-        <v>45812.43199074074</v>
+        <v>45813.58108796296</v>
       </c>
       <c r="G872">
         <v>0</v>
@@ -21972,16 +21972,16 @@
         <v>1</v>
       </c>
       <c r="C876">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D876" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E876">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="F876" s="2">
-        <v>45812.43199074074</v>
+        <v>45813.58258101852</v>
       </c>
       <c r="G876">
         <v>0</v>
@@ -22145,16 +22145,16 @@
         <v>1</v>
       </c>
       <c r="C883">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D883" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95795446759</v>
       </c>
       <c r="E883">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F883" s="2">
-        <v>45811.69520833333</v>
+        <v>45813.58277777778</v>
       </c>
       <c r="G883">
         <v>0</v>
@@ -22272,16 +22272,16 @@
         <v>1</v>
       </c>
       <c r="C888">
-        <v>195</v>
+        <v>-5</v>
       </c>
       <c r="D888" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785145537</v>
       </c>
       <c r="E888">
-        <v>195</v>
+        <v>-5</v>
       </c>
       <c r="F888" s="2">
-        <v>45811.50252314815</v>
+        <v>45813.46407407407</v>
       </c>
       <c r="G888">
         <v>0</v>
@@ -22627,16 +22627,16 @@
         <v>1</v>
       </c>
       <c r="C902">
-        <v>-43</v>
+        <v>57</v>
       </c>
       <c r="D902" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95790539397</v>
       </c>
       <c r="E902">
-        <v>-43</v>
+        <v>57</v>
       </c>
       <c r="F902" s="2">
-        <v>45812.44633101852</v>
+        <v>45813.62805555556</v>
       </c>
       <c r="G902">
         <v>0</v>
@@ -22806,16 +22806,16 @@
         <v>1</v>
       </c>
       <c r="C909">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D909" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E909">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="F909" s="2">
-        <v>45811.49467592593</v>
+        <v>45813.58085648148</v>
       </c>
       <c r="G909">
         <v>0</v>
@@ -24110,16 +24110,16 @@
         <v>1</v>
       </c>
       <c r="C961">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D961" s="2">
-        <v>45810.72559944464</v>
+        <v>45813.95785151322</v>
       </c>
       <c r="E961">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F961" s="2">
-        <v>45810.52887731481</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G961">
         <v>0</v>
@@ -24162,16 +24162,16 @@
         <v>1</v>
       </c>
       <c r="C963">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D963" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E963">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="F963" s="2">
-        <v>45811.69520833333</v>
+        <v>45813.58258101852</v>
       </c>
       <c r="G963">
         <v>0</v>
@@ -25738,16 +25738,16 @@
         <v>1</v>
       </c>
       <c r="C1025">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="D1025" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95793319555</v>
       </c>
       <c r="E1025">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="F1025" s="2">
-        <v>45812.44633101852</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G1025">
         <v>0</v>
@@ -25764,16 +25764,16 @@
         <v>1</v>
       </c>
       <c r="C1026">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="D1026" s="2">
-        <v>45806.77605776805</v>
+        <v>45813.95793319555</v>
       </c>
       <c r="E1026">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="F1026" s="2">
-        <v>45806.74983796296</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G1026">
         <v>0</v>
@@ -26099,7 +26099,7 @@
         <v>137</v>
       </c>
       <c r="F1039" s="2">
-        <v>45811.72704861111</v>
+        <v>45813.51170138889</v>
       </c>
       <c r="G1039">
         <v>0</v>
@@ -26676,16 +26676,16 @@
         <v>1</v>
       </c>
       <c r="C1062">
-        <v>681</v>
+        <v>661</v>
       </c>
       <c r="D1062" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E1062">
-        <v>681</v>
+        <v>661</v>
       </c>
       <c r="F1062" s="2">
-        <v>45812.53040509259</v>
+        <v>45813.58277777778</v>
       </c>
       <c r="G1062">
         <v>0</v>
@@ -27867,16 +27867,16 @@
         <v>1</v>
       </c>
       <c r="C1110">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D1110" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785151322</v>
       </c>
       <c r="E1110">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F1110" s="2">
-        <v>45811.66579861111</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G1110">
         <v>0</v>
@@ -28017,16 +28017,16 @@
         <v>1</v>
       </c>
       <c r="C1116">
-        <v>-87</v>
+        <v>5</v>
       </c>
       <c r="D1116" s="2">
-        <v>45812.78303939045</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E1116">
-        <v>-87</v>
+        <v>5</v>
       </c>
       <c r="F1116" s="2">
-        <v>45812.69229166667</v>
+        <v>45813.63752314815</v>
       </c>
       <c r="G1116">
         <v>0</v>
@@ -28173,16 +28173,16 @@
         <v>1</v>
       </c>
       <c r="C1122">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D1122" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E1122">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F1122" s="2">
-        <v>45812.53040509259</v>
+        <v>45813.60496527778</v>
       </c>
       <c r="G1122">
         <v>0</v>
@@ -28805,16 +28805,16 @@
         <v>1</v>
       </c>
       <c r="C1147">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="D1147" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95785151322</v>
       </c>
       <c r="E1147">
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="F1147" s="2">
-        <v>45812.43199074074</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G1147">
         <v>0</v>
@@ -28857,16 +28857,16 @@
         <v>1</v>
       </c>
       <c r="C1149">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D1149" s="2">
-        <v>45804.91952554927</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E1149">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F1149" s="2">
-        <v>45804.71377314815</v>
+        <v>45813.54864583333</v>
       </c>
       <c r="G1149">
         <v>0</v>
@@ -29752,16 +29752,16 @@
         <v>1</v>
       </c>
       <c r="C1184">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1184" s="2">
-        <v>45799.89532164588</v>
+        <v>45813.9578514438</v>
       </c>
       <c r="E1184">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1184" s="2">
-        <v>45786.47115740741</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G1184">
         <v>0</v>
@@ -29830,16 +29830,16 @@
         <v>1</v>
       </c>
       <c r="C1187">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D1187" s="2">
-        <v>45811.92544186871</v>
+        <v>45813.9578819583</v>
       </c>
       <c r="E1187">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F1187" s="2">
-        <v>45810.78246527778</v>
+        <v>45813.67818287037</v>
       </c>
       <c r="G1187">
         <v>0</v>
@@ -29986,16 +29986,16 @@
         <v>1</v>
       </c>
       <c r="C1193">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1193" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.9578819583</v>
       </c>
       <c r="E1193">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F1193" s="2">
-        <v>45811.67758101852</v>
+        <v>45813.67818287037</v>
       </c>
       <c r="G1193">
         <v>0</v>
@@ -30142,16 +30142,16 @@
         <v>1</v>
       </c>
       <c r="C1199">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D1199" s="2">
-        <v>45811.92544186871</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E1199">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F1199" s="2">
-        <v>45810.76871527778</v>
+        <v>45813.57788194445</v>
       </c>
       <c r="G1199">
         <v>0</v>
@@ -30760,16 +30760,16 @@
         <v>1</v>
       </c>
       <c r="C1223">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1223" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E1223">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1223" s="2">
-        <v>45812.5547337963</v>
+        <v>45813.60496527778</v>
       </c>
       <c r="G1223">
         <v>0</v>
@@ -31528,16 +31528,16 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>235</v>
+        <v>40</v>
       </c>
       <c r="D1253" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95788197009</v>
       </c>
       <c r="E1253">
-        <v>235</v>
+        <v>40</v>
       </c>
       <c r="F1253" s="2">
-        <v>45812.65041666666</v>
+        <v>45813.67865740741</v>
       </c>
       <c r="G1253">
         <v>0</v>
@@ -31733,16 +31733,16 @@
         <v>1</v>
       </c>
       <c r="C1261">
-        <v>199</v>
+        <v>-121</v>
       </c>
       <c r="D1261" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95795447831</v>
       </c>
       <c r="E1261">
-        <v>199</v>
+        <v>-121</v>
       </c>
       <c r="F1261" s="2">
-        <v>45812.47731481482</v>
+        <v>45813.54864583333</v>
       </c>
       <c r="G1261">
         <v>0</v>
@@ -32299,16 +32299,16 @@
         <v>1</v>
       </c>
       <c r="C1283">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1283" s="2">
-        <v>45795.04193352044</v>
+        <v>45813.95793319555</v>
       </c>
       <c r="E1283">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F1283" s="2">
-        <v>45674.62599537037</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G1283">
         <v>0</v>
@@ -32492,16 +32492,16 @@
         <v>1</v>
       </c>
       <c r="C1291">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1291" s="2">
-        <v>45806.77603756409</v>
+        <v>45813.95785145537</v>
       </c>
       <c r="E1291">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F1291" s="2">
-        <v>45806.67306712963</v>
+        <v>45813.51621527778</v>
       </c>
       <c r="G1291">
         <v>0</v>
@@ -33540,16 +33540,16 @@
         <v>1</v>
       </c>
       <c r="C1332">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1332" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95795447831</v>
       </c>
       <c r="E1332">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1332" s="2">
-        <v>45811.73181712963</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G1332">
         <v>0</v>
@@ -35067,16 +35067,16 @@
         <v>1</v>
       </c>
       <c r="C1392">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="D1392" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95790540554</v>
       </c>
       <c r="E1392">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="F1392" s="2">
-        <v>45812.44633101852</v>
+        <v>45813.63127314814</v>
       </c>
       <c r="G1392">
         <v>0</v>
@@ -35552,16 +35552,16 @@
         <v>1</v>
       </c>
       <c r="C1411">
-        <v>-20</v>
+        <v>95</v>
       </c>
       <c r="D1411" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95795446759</v>
       </c>
       <c r="E1411">
-        <v>-20</v>
+        <v>95</v>
       </c>
       <c r="F1411" s="2">
-        <v>45811.50125</v>
+        <v>45813.68358796297</v>
       </c>
       <c r="G1411">
         <v>0</v>
@@ -35630,16 +35630,16 @@
         <v>1</v>
       </c>
       <c r="C1414">
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="D1414" s="2">
-        <v>45799.89528859723</v>
+        <v>45813.95795449081</v>
       </c>
       <c r="E1414">
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="F1414" s="2">
-        <v>45784.64305555556</v>
+        <v>45813.7544212963</v>
       </c>
       <c r="G1414">
         <v>0</v>
@@ -36450,16 +36450,16 @@
         <v>1</v>
       </c>
       <c r="C1446">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D1446" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E1446">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="F1446" s="2">
-        <v>45812.65041666666</v>
+        <v>45813.54864583333</v>
       </c>
       <c r="G1446">
         <v>0</v>
@@ -36502,16 +36502,16 @@
         <v>1</v>
       </c>
       <c r="C1448">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D1448" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E1448">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F1448" s="2">
-        <v>45811.49467592593</v>
+        <v>45813.58085648148</v>
       </c>
       <c r="G1448">
         <v>0</v>
@@ -37988,16 +37988,16 @@
         <v>1</v>
       </c>
       <c r="C1507">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D1507" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E1507">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F1507" s="2">
-        <v>45812.53040509259</v>
+        <v>45813.57829861111</v>
       </c>
       <c r="G1507">
         <v>0</v>
@@ -39242,16 +39242,16 @@
         <v>1</v>
       </c>
       <c r="C1558">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D1558" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E1558">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F1558" s="2">
-        <v>45811.70625</v>
+        <v>45813.60496527778</v>
       </c>
       <c r="G1558">
         <v>0</v>
@@ -40223,16 +40223,16 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>6092</v>
+        <v>5951</v>
       </c>
       <c r="D1597" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95793319555</v>
       </c>
       <c r="E1597">
-        <v>6092</v>
+        <v>5951</v>
       </c>
       <c r="F1597" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G1597">
         <v>0</v>
@@ -41190,16 +41190,16 @@
         <v>1</v>
       </c>
       <c r="C1635">
-        <v>2773</v>
+        <v>2760</v>
       </c>
       <c r="D1635" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E1635">
-        <v>2773</v>
+        <v>2760</v>
       </c>
       <c r="F1635" s="2">
-        <v>45812.53040509259</v>
+        <v>45813.58108796296</v>
       </c>
       <c r="G1635">
         <v>0</v>
@@ -43727,16 +43727,16 @@
         <v>1</v>
       </c>
       <c r="C1738">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D1738" s="2">
-        <v>45806.77605776805</v>
+        <v>45813.95790535926</v>
       </c>
       <c r="E1738">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F1738" s="2">
-        <v>45806.74983796296</v>
+        <v>45813.68512731481</v>
       </c>
       <c r="G1738">
         <v>0</v>
@@ -45865,16 +45865,16 @@
         <v>1</v>
       </c>
       <c r="C1823">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D1823" s="2">
-        <v>45807.78640665444</v>
+        <v>45813.95782005877</v>
       </c>
       <c r="E1823">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F1823" s="2">
-        <v>45807.43805555555</v>
+        <v>45813.42155092592</v>
       </c>
       <c r="G1823">
         <v>0</v>
@@ -46399,16 +46399,16 @@
         <v>1</v>
       </c>
       <c r="C1844">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="D1844" s="2">
-        <v>45811.92544186871</v>
+        <v>45813.95785151322</v>
       </c>
       <c r="E1844">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="F1844" s="2">
-        <v>45810.76806712963</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G1844">
         <v>0</v>
@@ -47444,16 +47444,16 @@
         <v>1</v>
       </c>
       <c r="C1885">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D1885" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95788193521</v>
       </c>
       <c r="E1885">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F1885" s="2">
-        <v>45812.43199074074</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G1885">
         <v>0</v>
@@ -47888,16 +47888,16 @@
         <v>1</v>
       </c>
       <c r="C1903">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="D1903" s="2">
-        <v>45812.78303939045</v>
+        <v>45813.95785149008</v>
       </c>
       <c r="E1903">
-        <v>-2</v>
+        <v>10</v>
       </c>
       <c r="F1903" s="2">
-        <v>45812.44633101852</v>
+        <v>45813.63085648148</v>
       </c>
       <c r="G1903">
         <v>0</v>
@@ -50032,16 +50032,16 @@
         <v>1</v>
       </c>
       <c r="C1988">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="D1988" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95782005877</v>
       </c>
       <c r="E1988">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="F1988" s="2">
-        <v>45812.44633101852</v>
+        <v>45813.42049768518</v>
       </c>
       <c r="G1988">
         <v>0</v>
@@ -51059,16 +51059,16 @@
         <v>1</v>
       </c>
       <c r="C2029">
-        <v>-9</v>
+        <v>2</v>
       </c>
       <c r="D2029" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E2029">
-        <v>-9</v>
+        <v>2</v>
       </c>
       <c r="F2029" s="2">
-        <v>45812.54806712963</v>
+        <v>45813.58085648148</v>
       </c>
       <c r="G2029">
         <v>0</v>
@@ -51746,16 +51746,16 @@
         <v>1</v>
       </c>
       <c r="C2056">
-        <v>7</v>
+        <v>-5</v>
       </c>
       <c r="D2056" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95788197009</v>
       </c>
       <c r="E2056">
-        <v>7</v>
+        <v>-5</v>
       </c>
       <c r="F2056" s="2">
-        <v>45812.53496527778</v>
+        <v>45813.68033564815</v>
       </c>
       <c r="G2056">
         <v>0</v>
@@ -52026,16 +52026,16 @@
         <v>1</v>
       </c>
       <c r="C2067">
-        <v>47</v>
+        <v>-53</v>
       </c>
       <c r="D2067" s="2">
-        <v>45807.78640665444</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E2067">
-        <v>47</v>
+        <v>-53</v>
       </c>
       <c r="F2067" s="2">
-        <v>45807.44157407407</v>
+        <v>45813.54864583333</v>
       </c>
       <c r="G2067">
         <v>0</v>
@@ -54795,16 +54795,16 @@
         <v>1</v>
       </c>
       <c r="C2178">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="D2178" s="2">
-        <v>45811.92549991595</v>
+        <v>45813.95785150164</v>
       </c>
       <c r="E2178">
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="F2178" s="2">
-        <v>45811.67811342593</v>
+        <v>45813.64386574074</v>
       </c>
       <c r="G2178">
         <v>0</v>
@@ -54847,16 +54847,16 @@
         <v>1</v>
       </c>
       <c r="C2180">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D2180" s="2">
-        <v>45803.90694022291</v>
+        <v>45813.95793319555</v>
       </c>
       <c r="E2180">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F2180" s="2">
-        <v>45803.7415625</v>
+        <v>45813.71038194445</v>
       </c>
       <c r="G2180">
         <v>0</v>
@@ -56244,16 +56244,16 @@
         <v>1</v>
       </c>
       <c r="C2235">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2235" s="2">
-        <v>45804.91952554927</v>
+        <v>45813.95795447831</v>
       </c>
       <c r="E2235">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F2235" s="2">
-        <v>45804.59697916666</v>
+        <v>45813.65701388889</v>
       </c>
       <c r="G2235">
         <v>0</v>
@@ -56400,16 +56400,16 @@
         <v>1</v>
       </c>
       <c r="C2241">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="D2241" s="2">
-        <v>45810.72559945051</v>
+        <v>45813.95782005877</v>
       </c>
       <c r="E2241">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="F2241" s="2">
-        <v>45810.61395833334</v>
+        <v>45813.42155092592</v>
       </c>
       <c r="G2241">
         <v>0</v>
@@ -60020,7 +60020,7 @@
         <v>0</v>
       </c>
       <c r="F2386" s="2">
-        <v>45758.39503472222</v>
+        <v>45813.64251157407</v>
       </c>
       <c r="G2386">
         <v>0</v>
@@ -60340,16 +60340,16 @@
         <v>1</v>
       </c>
       <c r="C2399">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2399" s="2">
-        <v>45795.04199224871</v>
+        <v>45813.95795449081</v>
       </c>
       <c r="E2399">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2399" s="2">
-        <v>45686.76962962963</v>
+        <v>45813.82819444445</v>
       </c>
       <c r="G2399">
         <v>0</v>
@@ -60510,16 +60510,16 @@
         <v>1</v>
       </c>
       <c r="C2406">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D2406" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E2406">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F2406" s="2">
-        <v>45811.47164351852</v>
+        <v>45813.57788194445</v>
       </c>
       <c r="G2406">
         <v>0</v>
@@ -60767,16 +60767,16 @@
         <v>1</v>
       </c>
       <c r="C2416">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="D2416" s="2">
-        <v>45812.78306322403</v>
+        <v>45813.95785147848</v>
       </c>
       <c r="E2416">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="F2416" s="2">
-        <v>45812.70449074074</v>
+        <v>45813.5819212963</v>
       </c>
       <c r="G2416">
         <v>0</v>
@@ -61188,16 +61188,16 @@
         <v>1</v>
       </c>
       <c r="C2433">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D2433" s="2">
-        <v>45799.89545110933</v>
+        <v>45813.95782005877</v>
       </c>
       <c r="E2433">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="F2433" s="2">
-        <v>45783.46972222222</v>
+        <v>45813.42155092592</v>
       </c>
       <c r="G2433">
         <v>0</v>
@@ -61828,16 +61828,16 @@
         <v>1</v>
       </c>
       <c r="C2459">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2459" s="2">
-        <v>45811.92546678011</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E2459">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2459" s="2">
-        <v>45811.54368055556</v>
+        <v>45813.57788194445</v>
       </c>
       <c r="G2459">
         <v>0</v>
@@ -62361,16 +62361,16 @@
         <v>1</v>
       </c>
       <c r="C2481">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="D2481" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785145537</v>
       </c>
       <c r="E2481">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="F2481" s="2">
-        <v>45812.53040509259</v>
+        <v>45813.46293981482</v>
       </c>
       <c r="G2481">
         <v>0</v>
@@ -62387,16 +62387,16 @@
         <v>1</v>
       </c>
       <c r="C2482">
-        <v>398</v>
+        <v>198</v>
       </c>
       <c r="D2482" s="2">
-        <v>45812.78301989438</v>
+        <v>45813.95785146693</v>
       </c>
       <c r="E2482">
-        <v>398</v>
+        <v>198</v>
       </c>
       <c r="F2482" s="2">
-        <v>45812.53040509259</v>
+        <v>45813.54864583333</v>
       </c>
       <c r="G2482">
         <v>0</v>
@@ -62422,7 +62422,7 @@
         <v>821</v>
       </c>
       <c r="F2483" s="2">
-        <v>45812.70203703704</v>
+        <v>45813.51170138889</v>
       </c>
       <c r="G2483">
         <v>0</v>
@@ -62439,16 +62439,16 @@
         <v>1</v>
       </c>
       <c r="C2484">
-        <v>841</v>
+        <v>811</v>
       </c>
       <c r="D2484" s="2">
-        <v>45812.78306321269</v>
+        <v>45813.95785145537</v>
       </c>
       <c r="E2484">
-        <v>841</v>
+        <v>811</v>
       </c>
       <c r="F2484" s="2">
-        <v>45812.70203703704</v>
+        <v>45813.51170138889</v>
       </c>
       <c r="G2484">
         <v>0</v>
@@ -64159,13 +64159,16 @@
         <v>1</v>
       </c>
       <c r="C2555">
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="D2555" s="2">
-        <v>45811.92552608132</v>
+        <v>45813.95788197009</v>
       </c>
       <c r="E2555">
-        <v>0</v>
+        <v>-50</v>
+      </c>
+      <c r="F2555" s="2">
+        <v>45813.67865740741</v>
       </c>
       <c r="G2555">
         <v>0</v>
@@ -64182,13 +64185,16 @@
         <v>1</v>
       </c>
       <c r="C2556">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="D2556" s="2">
-        <v>45812.78301983239</v>
+        <v>45813.95785145537</v>
       </c>
       <c r="E2556">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F2556" s="2">
+        <v>45813.46293981482</v>
       </c>
       <c r="G2556">
         <v>0</v>
@@ -64217,6 +64223,29 @@
         <v>0</v>
       </c>
       <c r="H2557" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2558" spans="1:8">
+      <c r="A2558">
+        <v>43452065</v>
+      </c>
+      <c r="B2558">
+        <v>1</v>
+      </c>
+      <c r="C2558">
+        <v>0</v>
+      </c>
+      <c r="D2558" s="2">
+        <v>45813.95782005877</v>
+      </c>
+      <c r="E2558">
+        <v>0</v>
+      </c>
+      <c r="G2558">
+        <v>0</v>
+      </c>
+      <c r="H2558" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizei dados da bibi e da add
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -494,16 +494,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>45813.95782005877</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2">
-        <v>45813.426875</v>
+        <v>45814.64774305555</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -690,16 +690,16 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2">
-        <v>45813.95785145537</v>
+        <v>45814.82970463676</v>
       </c>
       <c r="E12">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F12" s="2">
-        <v>45813.46407407407</v>
+        <v>45814.61284722222</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -926,16 +926,16 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D22" s="2">
-        <v>45795.04210567895</v>
+        <v>45814.82966409007</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F22" s="2">
-        <v>45775.71903935185</v>
+        <v>45814.39601851852</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -952,16 +952,16 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2">
-        <v>45811.92546678011</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E23">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" s="2">
-        <v>45811.49901620371</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1194,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>3172</v>
+        <v>3161</v>
       </c>
       <c r="D33" s="2">
-        <v>45813.95788194679</v>
+        <v>45814.82970462521</v>
       </c>
       <c r="E33">
-        <v>3172</v>
+        <v>3161</v>
       </c>
       <c r="F33" s="2">
-        <v>45813.67818287037</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1589,16 +1589,16 @@
         <v>1</v>
       </c>
       <c r="C49">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D49" s="2">
-        <v>45813.95785149008</v>
+        <v>45814.82976436854</v>
       </c>
       <c r="E49">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F49" s="2">
-        <v>45813.60496527778</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -1765,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D56" s="2">
-        <v>45813.95795447831</v>
+        <v>45814.82966409007</v>
       </c>
       <c r="E56">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F56" s="2">
-        <v>45813.60496527778</v>
+        <v>45814.39652777778</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -1817,16 +1817,16 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D58" s="2">
-        <v>45813.95795446759</v>
+        <v>45814.82966409007</v>
       </c>
       <c r="E58">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F58" s="2">
-        <v>45813.57855324074</v>
+        <v>45814.39652777778</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -1941,16 +1941,16 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D63" s="2">
-        <v>45813.95795446759</v>
+        <v>45814.82976436854</v>
       </c>
       <c r="E63">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F63" s="2">
-        <v>45813.46293981482</v>
+        <v>45814.70711805556</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2088,16 +2088,16 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D69" s="2">
-        <v>45812.78306322403</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E69">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F69" s="2">
-        <v>45812.70449074074</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -2114,16 +2114,16 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D70" s="2">
-        <v>45813.95785150164</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E70">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F70" s="2">
-        <v>45813.65289351852</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2402,16 +2402,16 @@
         <v>1</v>
       </c>
       <c r="C82">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D82" s="2">
-        <v>45812.78301983239</v>
+        <v>45814.82966409007</v>
       </c>
       <c r="E82">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F82" s="2">
-        <v>45812.48946759259</v>
+        <v>45814.38376157408</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -2428,16 +2428,16 @@
         <v>1</v>
       </c>
       <c r="C83">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D83" s="2">
-        <v>45812.78301989438</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E83">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="F83" s="2">
-        <v>45812.53496527778</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -2477,16 +2477,16 @@
         <v>1</v>
       </c>
       <c r="C85">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D85" s="2">
-        <v>45812.78301983239</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E85">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85" s="2">
-        <v>45812.44633101852</v>
+        <v>45814.65319444444</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -2503,22 +2503,22 @@
         <v>1</v>
       </c>
       <c r="C86">
-        <v>-8</v>
+        <v>162</v>
       </c>
       <c r="D86" s="2">
-        <v>45813.95788194679</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E86">
-        <v>-8</v>
+        <v>-38</v>
       </c>
       <c r="F86" s="2">
-        <v>45813.67818287037</v>
+        <v>45814.38376157408</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="H86" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2529,16 +2529,16 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D87" s="2">
-        <v>45813.95785147848</v>
+        <v>45814.82966409007</v>
       </c>
       <c r="E87">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="F87" s="2">
-        <v>45813.58277777778</v>
+        <v>45814.38376157408</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -2702,16 +2702,16 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D94" s="2">
-        <v>45813.95785150164</v>
+        <v>45814.82980241515</v>
       </c>
       <c r="E94">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F94" s="2">
-        <v>45813.65432870371</v>
+        <v>45814.4477662037</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -2872,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>875</v>
+        <v>821</v>
       </c>
       <c r="D101" s="2">
-        <v>45813.95793318399</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E101">
-        <v>875</v>
+        <v>821</v>
       </c>
       <c r="F101" s="2">
-        <v>45813.71038194445</v>
+        <v>45814.70711805556</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -2921,10 +2921,10 @@
         <v>1</v>
       </c>
       <c r="C103">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="D103" s="2">
-        <v>45810.72563720519</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E103">
         <v>31</v>
@@ -2933,10 +2933,10 @@
         <v>45810.68862268519</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H103" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -3258,16 +3258,16 @@
         <v>1</v>
       </c>
       <c r="C117">
-        <v>1131</v>
+        <v>1125</v>
       </c>
       <c r="D117" s="2">
-        <v>45811.92552605522</v>
+        <v>45814.82970462521</v>
       </c>
       <c r="E117">
-        <v>1131</v>
+        <v>1125</v>
       </c>
       <c r="F117" s="2">
-        <v>45813.51170138889</v>
+        <v>45814.46266203704</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -3359,10 +3359,10 @@
         <v>1</v>
       </c>
       <c r="C121">
-        <v>22</v>
+        <v>682</v>
       </c>
       <c r="D121" s="2">
-        <v>45810.72559945051</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E121">
         <v>22</v>
@@ -3371,10 +3371,10 @@
         <v>45810.64912037037</v>
       </c>
       <c r="G121">
-        <v>0</v>
+        <v>660</v>
       </c>
       <c r="H121" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -3408,22 +3408,22 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>-13</v>
+        <v>483</v>
       </c>
       <c r="D123" s="2">
-        <v>45813.95785150164</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E123">
-        <v>-13</v>
+        <v>-17</v>
       </c>
       <c r="F123" s="2">
-        <v>45813.65701388889</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G123">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H123" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -3460,10 +3460,10 @@
         <v>1</v>
       </c>
       <c r="C125">
-        <v>202</v>
+        <v>607</v>
       </c>
       <c r="D125" s="2">
-        <v>45813.95788194679</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E125">
         <v>202</v>
@@ -3472,10 +3472,10 @@
         <v>45813.67818287037</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>405</v>
       </c>
       <c r="H125" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -3846,16 +3846,16 @@
         <v>1</v>
       </c>
       <c r="C141">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D141" s="2">
-        <v>45813.95785145537</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E141">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F141" s="2">
-        <v>45813.51621527778</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G141">
         <v>0</v>
@@ -3950,16 +3950,16 @@
         <v>1</v>
       </c>
       <c r="C145">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D145" s="2">
-        <v>45811.92544186871</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E145">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F145" s="2">
-        <v>45811.42236111111</v>
+        <v>45814.64479166667</v>
       </c>
       <c r="G145">
         <v>0</v>
@@ -4100,16 +4100,16 @@
         <v>1</v>
       </c>
       <c r="C151">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D151" s="2">
-        <v>45807.78640665444</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E151">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="F151" s="2">
-        <v>45813.63825231481</v>
+        <v>45814.64774305555</v>
       </c>
       <c r="G151">
         <v>0</v>
@@ -6149,16 +6149,16 @@
         <v>1</v>
       </c>
       <c r="C235">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D235" s="2">
-        <v>45810.72556745499</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E235">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F235" s="2">
-        <v>45810.51450231481</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G235">
         <v>0</v>
@@ -6437,16 +6437,16 @@
         <v>1</v>
       </c>
       <c r="C247">
-        <v>1261</v>
+        <v>1245</v>
       </c>
       <c r="D247" s="2">
-        <v>45813.95795447831</v>
+        <v>45814.82976436854</v>
       </c>
       <c r="E247">
-        <v>1261</v>
+        <v>1245</v>
       </c>
       <c r="F247" s="2">
-        <v>45813.58277777778</v>
+        <v>45814.70711805556</v>
       </c>
       <c r="G247">
         <v>0</v>
@@ -6996,16 +6996,16 @@
         <v>1</v>
       </c>
       <c r="C270">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D270" s="2">
-        <v>45813.95782007044</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E270">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="F270" s="2">
-        <v>45813.46293981482</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G270">
         <v>0</v>
@@ -7045,16 +7045,16 @@
         <v>1</v>
       </c>
       <c r="C272">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D272" s="2">
-        <v>45813.95785147848</v>
+        <v>45814.82966409007</v>
       </c>
       <c r="E272">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F272" s="2">
-        <v>45813.5819212963</v>
+        <v>45814.39601851852</v>
       </c>
       <c r="G272">
         <v>0</v>
@@ -7408,16 +7408,16 @@
         <v>1</v>
       </c>
       <c r="C287">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="D287" s="2">
-        <v>45813.95782005877</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E287">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="F287" s="2">
-        <v>45813.42155092592</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G287">
         <v>0</v>
@@ -7509,22 +7509,22 @@
         <v>1</v>
       </c>
       <c r="C291">
-        <v>61</v>
+        <v>659</v>
       </c>
       <c r="D291" s="2">
-        <v>45813.95785147848</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E291">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F291" s="2">
-        <v>45813.58258101852</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G291">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="H291" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="292" spans="1:8">
@@ -8169,16 +8169,16 @@
         <v>1</v>
       </c>
       <c r="C318">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D318" s="2">
-        <v>45813.95785150164</v>
+        <v>45814.82976436854</v>
       </c>
       <c r="E318">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F318" s="2">
-        <v>45813.63916666667</v>
+        <v>45814.70711805556</v>
       </c>
       <c r="G318">
         <v>0</v>
@@ -8247,16 +8247,16 @@
         <v>1</v>
       </c>
       <c r="C321">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D321" s="2">
-        <v>45812.78301989438</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E321">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F321" s="2">
-        <v>45812.5547337963</v>
+        <v>45814.52313657408</v>
       </c>
       <c r="G321">
         <v>0</v>
@@ -8374,16 +8374,16 @@
         <v>1</v>
       </c>
       <c r="C326">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D326" s="2">
-        <v>45813.95785146693</v>
+        <v>45814.82980241515</v>
       </c>
       <c r="E326">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="F326" s="2">
-        <v>45813.57303240741</v>
+        <v>45814.75739583333</v>
       </c>
       <c r="G326">
         <v>0</v>
@@ -8991,16 +8991,16 @@
         <v>1</v>
       </c>
       <c r="C351">
-        <v>-112</v>
+        <v>-152</v>
       </c>
       <c r="D351" s="2">
-        <v>45813.95795449081</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E351">
-        <v>-112</v>
+        <v>-152</v>
       </c>
       <c r="F351" s="2">
-        <v>45813.63770833334</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G351">
         <v>0</v>
@@ -9066,16 +9066,16 @@
         <v>1</v>
       </c>
       <c r="C354">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D354" s="2">
-        <v>45811.92544186871</v>
+        <v>45814.82980222279</v>
       </c>
       <c r="E354">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F354" s="2">
-        <v>45811.40138888889</v>
+        <v>45814.70711805556</v>
       </c>
       <c r="G354">
         <v>0</v>
@@ -9115,16 +9115,16 @@
         <v>1</v>
       </c>
       <c r="C356">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D356" s="2">
-        <v>45813.95782007044</v>
+        <v>45814.82976436854</v>
       </c>
       <c r="E356">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F356" s="2">
-        <v>45813.46293981482</v>
+        <v>45814.70711805556</v>
       </c>
       <c r="G356">
         <v>0</v>
@@ -9291,16 +9291,16 @@
         <v>1</v>
       </c>
       <c r="C363">
-        <v>692</v>
+        <v>682</v>
       </c>
       <c r="D363" s="2">
-        <v>45813.95788194679</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E363">
-        <v>692</v>
+        <v>682</v>
       </c>
       <c r="F363" s="2">
-        <v>45813.67818287037</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G363">
         <v>0</v>
@@ -9839,16 +9839,16 @@
         <v>1</v>
       </c>
       <c r="C385">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D385" s="2">
-        <v>45813.95785147848</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E385">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F385" s="2">
-        <v>45813.58085648148</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G385">
         <v>0</v>
@@ -9969,16 +9969,16 @@
         <v>1</v>
       </c>
       <c r="C390">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D390" s="2">
-        <v>45813.95788193521</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E390">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F390" s="2">
-        <v>45813.67373842592</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G390">
         <v>0</v>
@@ -10070,22 +10070,22 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>47</v>
+        <v>236</v>
       </c>
       <c r="D394" s="2">
-        <v>45813.95790534767</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E394">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F394" s="2">
-        <v>45813.57359953703</v>
+        <v>45814.65862268519</v>
       </c>
       <c r="G394">
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="H394" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="395" spans="1:8">
@@ -10122,10 +10122,10 @@
         <v>1</v>
       </c>
       <c r="C396">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D396" s="2">
-        <v>45812.78301983239</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E396">
         <v>3</v>
@@ -10134,10 +10134,10 @@
         <v>45812.32835648148</v>
       </c>
       <c r="G396">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H396" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="397" spans="1:8">
@@ -10269,16 +10269,16 @@
         <v>1</v>
       </c>
       <c r="C402">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="D402" s="2">
-        <v>45811.92549991595</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E402">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="F402" s="2">
-        <v>45813.51170138889</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G402">
         <v>0</v>
@@ -10321,16 +10321,16 @@
         <v>1</v>
       </c>
       <c r="C404">
-        <v>114</v>
+        <v>58</v>
       </c>
       <c r="D404" s="2">
-        <v>45813.95785146693</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E404">
-        <v>114</v>
+        <v>58</v>
       </c>
       <c r="F404" s="2">
-        <v>45813.54864583333</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G404">
         <v>0</v>
@@ -10445,16 +10445,16 @@
         <v>1</v>
       </c>
       <c r="C409">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D409" s="2">
-        <v>45813.95782007044</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E409">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F409" s="2">
-        <v>45813.46293981482</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G409">
         <v>0</v>
@@ -10471,16 +10471,16 @@
         <v>1</v>
       </c>
       <c r="C410">
-        <v>2236</v>
+        <v>1936</v>
       </c>
       <c r="D410" s="2">
-        <v>45813.95788197009</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E410">
-        <v>2236</v>
+        <v>1936</v>
       </c>
       <c r="F410" s="2">
-        <v>45813.67957175926</v>
+        <v>45814.46266203704</v>
       </c>
       <c r="G410">
         <v>0</v>
@@ -10575,16 +10575,16 @@
         <v>1</v>
       </c>
       <c r="C414">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D414" s="2">
-        <v>45812.78301989438</v>
+        <v>45814.8297848079</v>
       </c>
       <c r="E414">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F414" s="2">
-        <v>45812.66328703704</v>
+        <v>45814.39652777778</v>
       </c>
       <c r="G414">
         <v>0</v>
@@ -11088,16 +11088,16 @@
         <v>1</v>
       </c>
       <c r="C435">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D435" s="2">
-        <v>45813.95785147848</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E435">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F435" s="2">
-        <v>45813.58258101852</v>
+        <v>45814.53738425926</v>
       </c>
       <c r="G435">
         <v>0</v>
@@ -11114,16 +11114,16 @@
         <v>1</v>
       </c>
       <c r="C436">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D436" s="2">
-        <v>45811.92549991595</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E436">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="F436" s="2">
-        <v>45811.73181712963</v>
+        <v>45814.38376157408</v>
       </c>
       <c r="G436">
         <v>0</v>
@@ -12155,16 +12155,16 @@
         <v>1</v>
       </c>
       <c r="C478">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D478" s="2">
-        <v>45811.92549991595</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E478">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="F478" s="2">
-        <v>45811.70625</v>
+        <v>45814.464375</v>
       </c>
       <c r="G478">
         <v>0</v>
@@ -12207,16 +12207,16 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D480" s="2">
-        <v>45813.95785150164</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E480">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F480" s="2">
-        <v>45813.65701388889</v>
+        <v>45814.46266203704</v>
       </c>
       <c r="G480">
         <v>0</v>
@@ -12536,16 +12536,16 @@
         <v>1</v>
       </c>
       <c r="C493">
-        <v>47</v>
+        <v>547</v>
       </c>
       <c r="D493" s="2">
-        <v>45811.92549991595</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E493">
-        <v>47</v>
+        <v>547</v>
       </c>
       <c r="F493" s="2">
-        <v>45811.72346064815</v>
+        <v>45814.68706018518</v>
       </c>
       <c r="G493">
         <v>0</v>
@@ -12951,16 +12951,16 @@
         <v>1</v>
       </c>
       <c r="C510">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="D510" s="2">
-        <v>45812.78301983239</v>
+        <v>45814.82976436854</v>
       </c>
       <c r="E510">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="F510" s="2">
-        <v>45812.43105324074</v>
+        <v>45814.70711805556</v>
       </c>
       <c r="G510">
         <v>0</v>
@@ -13851,7 +13851,7 @@
         <v>24</v>
       </c>
       <c r="F546" s="2">
-        <v>45811.6834837963</v>
+        <v>45814.68097222222</v>
       </c>
       <c r="G546">
         <v>0</v>
@@ -14389,16 +14389,16 @@
         <v>1</v>
       </c>
       <c r="C569">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D569" s="2">
-        <v>45812.78301989438</v>
+        <v>45814.82972452114</v>
       </c>
       <c r="E569">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F569" s="2">
-        <v>45812.53040509259</v>
+        <v>45814.61704861111</v>
       </c>
       <c r="G569">
         <v>0</v>
@@ -14415,16 +14415,16 @@
         <v>1</v>
       </c>
       <c r="C570">
-        <v>2644</v>
+        <v>2624</v>
       </c>
       <c r="D570" s="2">
-        <v>45813.95785147848</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E570">
-        <v>2644</v>
+        <v>2624</v>
       </c>
       <c r="F570" s="2">
-        <v>45813.58085648148</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G570">
         <v>0</v>
@@ -15207,16 +15207,16 @@
         <v>1</v>
       </c>
       <c r="C603">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="D603" s="2">
-        <v>45813.95790539397</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E603">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="F603" s="2">
-        <v>45813.57704861111</v>
+        <v>45814.73384259259</v>
       </c>
       <c r="G603">
         <v>0</v>
@@ -15878,16 +15878,16 @@
         <v>1</v>
       </c>
       <c r="C631">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D631" s="2">
-        <v>45812.78301983239</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E631">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="F631" s="2">
-        <v>45812.44633101852</v>
+        <v>45814.6853587963</v>
       </c>
       <c r="G631">
         <v>0</v>
@@ -16509,16 +16509,16 @@
         <v>1</v>
       </c>
       <c r="C657">
-        <v>2146</v>
+        <v>2140</v>
       </c>
       <c r="D657" s="2">
-        <v>45813.95785149008</v>
+        <v>45814.82966410174</v>
       </c>
       <c r="E657">
-        <v>2146</v>
+        <v>2140</v>
       </c>
       <c r="F657" s="2">
-        <v>45813.60496527778</v>
+        <v>45814.39652777778</v>
       </c>
       <c r="G657">
         <v>0</v>
@@ -16535,16 +16535,16 @@
         <v>1</v>
       </c>
       <c r="C658">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D658" s="2">
-        <v>45812.78301989438</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E658">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F658" s="2">
-        <v>45812.53040509259</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G658">
         <v>0</v>
@@ -16584,16 +16584,16 @@
         <v>1</v>
       </c>
       <c r="C660">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="D660" s="2">
-        <v>45813.95785147848</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E660">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="F660" s="2">
-        <v>45813.5819212963</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G660">
         <v>0</v>
@@ -17342,16 +17342,16 @@
         <v>1</v>
       </c>
       <c r="C691">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D691" s="2">
-        <v>45813.95795449081</v>
+        <v>45814.82972452114</v>
       </c>
       <c r="E691">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="F691" s="2">
-        <v>45813.82861111111</v>
+        <v>45814.61704861111</v>
       </c>
       <c r="G691">
         <v>0</v>
@@ -17968,16 +17968,16 @@
         <v>1</v>
       </c>
       <c r="C716">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D716" s="2">
-        <v>45811.92549991595</v>
+        <v>45814.82972453323</v>
       </c>
       <c r="E716">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F716" s="2">
-        <v>45811.73097222222</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G716">
         <v>0</v>
@@ -18150,16 +18150,16 @@
         <v>1</v>
       </c>
       <c r="C723">
-        <v>-16</v>
+        <v>5</v>
       </c>
       <c r="D723" s="2">
-        <v>45813.95790535926</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E723">
-        <v>-16</v>
+        <v>5</v>
       </c>
       <c r="F723" s="2">
-        <v>45813.68569444444</v>
+        <v>45814.67725694444</v>
       </c>
       <c r="G723">
         <v>0</v>
@@ -18202,16 +18202,16 @@
         <v>1</v>
       </c>
       <c r="C725">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D725" s="2">
-        <v>45811.92544186871</v>
+        <v>45814.82972452114</v>
       </c>
       <c r="E725">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F725" s="2">
-        <v>45811.42122685185</v>
+        <v>45814.61704861111</v>
       </c>
       <c r="G725">
         <v>0</v>
@@ -18228,16 +18228,16 @@
         <v>1</v>
       </c>
       <c r="C726">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="D726" s="2">
-        <v>45812.78301983239</v>
+        <v>45814.82970462521</v>
       </c>
       <c r="E726">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="F726" s="2">
-        <v>45813.51170138889</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G726">
         <v>0</v>
@@ -18381,16 +18381,16 @@
         <v>1</v>
       </c>
       <c r="C732">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D732" s="2">
-        <v>45813.95785149008</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E732">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F732" s="2">
-        <v>45813.58277777778</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G732">
         <v>0</v>
@@ -18482,16 +18482,16 @@
         <v>1</v>
       </c>
       <c r="C736">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D736" s="2">
-        <v>45795.04190003897</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E736">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F736" s="2">
-        <v>45624.48908564815</v>
+        <v>45814.39601851852</v>
       </c>
       <c r="G736">
         <v>0</v>
@@ -20383,16 +20383,16 @@
         <v>1</v>
       </c>
       <c r="C812">
-        <v>-2</v>
+        <v>22</v>
       </c>
       <c r="D812" s="2">
-        <v>45813.95785146693</v>
+        <v>45814.82980241515</v>
       </c>
       <c r="E812">
-        <v>-2</v>
+        <v>22</v>
       </c>
       <c r="F812" s="2">
-        <v>45813.57680555555</v>
+        <v>45814.75879629629</v>
       </c>
       <c r="G812">
         <v>0</v>
@@ -20556,16 +20556,16 @@
         <v>1</v>
       </c>
       <c r="C819">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D819" s="2">
-        <v>45813.95785150164</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E819">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F819" s="2">
-        <v>45813.64146990741</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G819">
         <v>0</v>
@@ -20683,10 +20683,10 @@
         <v>1</v>
       </c>
       <c r="C824">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="D824" s="2">
-        <v>45799.89542739857</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E824">
         <v>35</v>
@@ -20695,10 +20695,10 @@
         <v>45793.38046296296</v>
       </c>
       <c r="G824">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H824" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="825" spans="1:8">
@@ -20781,16 +20781,16 @@
         <v>1</v>
       </c>
       <c r="C828">
-        <v>244</v>
+        <v>194</v>
       </c>
       <c r="D828" s="2">
-        <v>45799.89534672352</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E828">
-        <v>244</v>
+        <v>194</v>
       </c>
       <c r="F828" s="2">
-        <v>45793.37662037037</v>
+        <v>45814.53738425926</v>
       </c>
       <c r="G828">
         <v>0</v>
@@ -21415,16 +21415,16 @@
         <v>1</v>
       </c>
       <c r="C854">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D854" s="2">
-        <v>45811.92549991595</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E854">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F854" s="2">
-        <v>45811.69520833333</v>
+        <v>45814.64774305555</v>
       </c>
       <c r="G854">
         <v>0</v>
@@ -21868,16 +21868,16 @@
         <v>1</v>
       </c>
       <c r="C872">
-        <v>583</v>
+        <v>558</v>
       </c>
       <c r="D872" s="2">
-        <v>45813.95785147848</v>
+        <v>45814.82972452114</v>
       </c>
       <c r="E872">
-        <v>583</v>
+        <v>558</v>
       </c>
       <c r="F872" s="2">
-        <v>45813.58108796296</v>
+        <v>45814.61704861111</v>
       </c>
       <c r="G872">
         <v>0</v>
@@ -22145,16 +22145,16 @@
         <v>1</v>
       </c>
       <c r="C883">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D883" s="2">
-        <v>45813.95795446759</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E883">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F883" s="2">
-        <v>45813.58277777778</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G883">
         <v>0</v>
@@ -22806,16 +22806,16 @@
         <v>1</v>
       </c>
       <c r="C909">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="D909" s="2">
-        <v>45813.95785147848</v>
+        <v>45814.82980240628</v>
       </c>
       <c r="E909">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="F909" s="2">
-        <v>45813.58085648148</v>
+        <v>45814.75269675926</v>
       </c>
       <c r="G909">
         <v>0</v>
@@ -23161,16 +23161,16 @@
         <v>1</v>
       </c>
       <c r="C923">
-        <v>428</v>
+        <v>378</v>
       </c>
       <c r="D923" s="2">
-        <v>45810.72559946219</v>
+        <v>45814.82970463676</v>
       </c>
       <c r="E923">
-        <v>428</v>
+        <v>378</v>
       </c>
       <c r="F923" s="2">
-        <v>45810.6524074074</v>
+        <v>45814.38376157408</v>
       </c>
       <c r="G923">
         <v>0</v>
@@ -23187,16 +23187,16 @@
         <v>1</v>
       </c>
       <c r="C924">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D924" s="2">
-        <v>45812.78301989438</v>
+        <v>45814.82972452114</v>
       </c>
       <c r="E924">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F924" s="2">
-        <v>45812.63878472222</v>
+        <v>45814.61704861111</v>
       </c>
       <c r="G924">
         <v>0</v>
@@ -24110,16 +24110,16 @@
         <v>1</v>
       </c>
       <c r="C961">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D961" s="2">
-        <v>45813.95785151322</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E961">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F961" s="2">
-        <v>45813.65701388889</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G961">
         <v>0</v>
@@ -24999,16 +24999,16 @@
         <v>1</v>
       </c>
       <c r="C996">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="D996" s="2">
-        <v>45805.91875152234</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E996">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="F996" s="2">
-        <v>45805.65278935185</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G996">
         <v>0</v>
@@ -25155,16 +25155,16 @@
         <v>1</v>
       </c>
       <c r="C1002">
-        <v>105</v>
+        <v>20</v>
       </c>
       <c r="D1002" s="2">
-        <v>45807.78640657826</v>
+        <v>45814.82980241515</v>
       </c>
       <c r="E1002">
-        <v>105</v>
+        <v>20</v>
       </c>
       <c r="F1002" s="2">
-        <v>45807.43640046296</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G1002">
         <v>0</v>
@@ -25181,16 +25181,16 @@
         <v>1</v>
       </c>
       <c r="C1003">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D1003" s="2">
-        <v>45811.92544186871</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E1003">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="F1003" s="2">
-        <v>45811.40424768518</v>
+        <v>45814.39601851852</v>
       </c>
       <c r="G1003">
         <v>0</v>
@@ -25839,16 +25839,16 @@
         <v>1</v>
       </c>
       <c r="C1029">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1029" s="2">
-        <v>45795.04208095842</v>
+        <v>45814.82976436854</v>
       </c>
       <c r="E1029">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1029" s="2">
-        <v>45770.49887731481</v>
+        <v>45814.70711805556</v>
       </c>
       <c r="G1029">
         <v>0</v>
@@ -26676,16 +26676,16 @@
         <v>1</v>
       </c>
       <c r="C1062">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D1062" s="2">
-        <v>45813.95785149008</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E1062">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F1062" s="2">
-        <v>45813.58277777778</v>
+        <v>45814.65319444444</v>
       </c>
       <c r="G1062">
         <v>0</v>
@@ -27028,16 +27028,16 @@
         <v>1</v>
       </c>
       <c r="C1076">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="D1076" s="2">
-        <v>45795.04208095842</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E1076">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="F1076" s="2">
-        <v>45769.46112268518</v>
+        <v>45814.39601851852</v>
       </c>
       <c r="G1076">
         <v>0</v>
@@ -27867,16 +27867,16 @@
         <v>1</v>
       </c>
       <c r="C1110">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D1110" s="2">
-        <v>45813.95785151322</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E1110">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F1110" s="2">
-        <v>45813.65701388889</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G1110">
         <v>0</v>
@@ -28017,10 +28017,10 @@
         <v>1</v>
       </c>
       <c r="C1116">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="D1116" s="2">
-        <v>45813.95785149008</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E1116">
         <v>5</v>
@@ -28029,10 +28029,10 @@
         <v>45813.63752314815</v>
       </c>
       <c r="G1116">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="H1116" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1117" spans="1:8">
@@ -28173,16 +28173,16 @@
         <v>1</v>
       </c>
       <c r="C1122">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1122" s="2">
-        <v>45813.95785149008</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E1122">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1122" s="2">
-        <v>45813.60496527778</v>
+        <v>45814.64774305555</v>
       </c>
       <c r="G1122">
         <v>0</v>
@@ -28378,16 +28378,16 @@
         <v>1</v>
       </c>
       <c r="C1130">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1130" s="2">
-        <v>45799.89532166889</v>
+        <v>45814.82972452114</v>
       </c>
       <c r="E1130">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F1130" s="2">
-        <v>45791.69849537037</v>
+        <v>45814.61704861111</v>
       </c>
       <c r="G1130">
         <v>0</v>
@@ -28805,22 +28805,22 @@
         <v>1</v>
       </c>
       <c r="C1147">
-        <v>-5</v>
+        <v>56</v>
       </c>
       <c r="D1147" s="2">
-        <v>45813.95785151322</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E1147">
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="F1147" s="2">
-        <v>45813.65701388889</v>
+        <v>45814.74931712963</v>
       </c>
       <c r="G1147">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H1147" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1148" spans="1:8">
@@ -29039,16 +29039,16 @@
         <v>1</v>
       </c>
       <c r="C1156">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D1156" s="2">
-        <v>45799.89528857399</v>
+        <v>45814.82966409007</v>
       </c>
       <c r="E1156">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F1156" s="2">
-        <v>45779.53798611111</v>
+        <v>45814.39601851852</v>
       </c>
       <c r="G1156">
         <v>0</v>
@@ -29495,16 +29495,16 @@
         <v>1</v>
       </c>
       <c r="C1174">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D1174" s="2">
-        <v>45810.72563721648</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E1174">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F1174" s="2">
-        <v>45810.75585648148</v>
+        <v>45814.65319444444</v>
       </c>
       <c r="G1174">
         <v>0</v>
@@ -30760,16 +30760,16 @@
         <v>1</v>
       </c>
       <c r="C1223">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1223" s="2">
-        <v>45813.95785149008</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E1223">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1223" s="2">
-        <v>45813.60496527778</v>
+        <v>45814.52313657408</v>
       </c>
       <c r="G1223">
         <v>0</v>
@@ -31528,16 +31528,16 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1253" s="2">
-        <v>45813.95788197009</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E1253">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F1253" s="2">
-        <v>45813.67865740741</v>
+        <v>45814.65319444444</v>
       </c>
       <c r="G1253">
         <v>0</v>
@@ -31733,16 +31733,16 @@
         <v>1</v>
       </c>
       <c r="C1261">
-        <v>-121</v>
+        <v>23</v>
       </c>
       <c r="D1261" s="2">
-        <v>45813.95795447831</v>
+        <v>45814.82980240628</v>
       </c>
       <c r="E1261">
-        <v>-121</v>
+        <v>23</v>
       </c>
       <c r="F1261" s="2">
-        <v>45813.54864583333</v>
+        <v>45814.75055555555</v>
       </c>
       <c r="G1261">
         <v>0</v>
@@ -35015,16 +35015,16 @@
         <v>1</v>
       </c>
       <c r="C1390">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1390" s="2">
-        <v>45804.91954472794</v>
+        <v>45814.82976436854</v>
       </c>
       <c r="E1390">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F1390" s="2">
-        <v>45804.76886574074</v>
+        <v>45814.70711805556</v>
       </c>
       <c r="G1390">
         <v>0</v>
@@ -35041,16 +35041,16 @@
         <v>1</v>
       </c>
       <c r="C1391">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="D1391" s="2">
-        <v>45810.72559946219</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E1391">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="F1391" s="2">
-        <v>45810.6524074074</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G1391">
         <v>0</v>
@@ -35578,16 +35578,16 @@
         <v>1</v>
       </c>
       <c r="C1412">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D1412" s="2">
-        <v>45811.92549991595</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E1412">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="F1412" s="2">
-        <v>45811.71334490741</v>
+        <v>45814.74193287037</v>
       </c>
       <c r="G1412">
         <v>0</v>
@@ -36502,10 +36502,10 @@
         <v>1</v>
       </c>
       <c r="C1448">
-        <v>10</v>
+        <v>334</v>
       </c>
       <c r="D1448" s="2">
-        <v>45813.95785147848</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E1448">
         <v>10</v>
@@ -36514,10 +36514,10 @@
         <v>45813.58085648148</v>
       </c>
       <c r="G1448">
-        <v>0</v>
+        <v>324</v>
       </c>
       <c r="H1448" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="1449" spans="1:8">
@@ -37379,16 +37379,16 @@
         <v>1</v>
       </c>
       <c r="C1483">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="D1483" s="2">
-        <v>45811.92546678011</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E1483">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="F1483" s="2">
-        <v>45811.50252314815</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G1483">
         <v>0</v>
@@ -37988,16 +37988,16 @@
         <v>1</v>
       </c>
       <c r="C1507">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="D1507" s="2">
-        <v>45813.95785147848</v>
+        <v>45814.82976436854</v>
       </c>
       <c r="E1507">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="F1507" s="2">
-        <v>45813.57829861111</v>
+        <v>45814.46266203704</v>
       </c>
       <c r="G1507">
         <v>0</v>
@@ -38040,16 +38040,16 @@
         <v>1</v>
       </c>
       <c r="C1509">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1509" s="2">
-        <v>45811.92552606984</v>
+        <v>45814.82980241515</v>
       </c>
       <c r="E1509">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1509" s="2">
-        <v>45811.75563657407</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G1509">
         <v>0</v>
@@ -39242,16 +39242,16 @@
         <v>1</v>
       </c>
       <c r="C1558">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D1558" s="2">
-        <v>45813.95785149008</v>
+        <v>45814.82966410174</v>
       </c>
       <c r="E1558">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F1558" s="2">
-        <v>45813.60496527778</v>
+        <v>45814.39652777778</v>
       </c>
       <c r="G1558">
         <v>0</v>
@@ -39470,16 +39470,16 @@
         <v>1</v>
       </c>
       <c r="C1567">
-        <v>0</v>
+        <v>-64</v>
       </c>
       <c r="D1567" s="2">
-        <v>45806.77603763194</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E1567">
-        <v>0</v>
+        <v>-64</v>
       </c>
       <c r="F1567" s="2">
-        <v>45811.49850694444</v>
+        <v>45814.5771875</v>
       </c>
       <c r="G1567">
         <v>0</v>
@@ -40223,16 +40223,16 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>5951</v>
+        <v>5726</v>
       </c>
       <c r="D1597" s="2">
-        <v>45813.95793319555</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E1597">
-        <v>5951</v>
+        <v>5726</v>
       </c>
       <c r="F1597" s="2">
-        <v>45813.71038194445</v>
+        <v>45814.65319444444</v>
       </c>
       <c r="G1597">
         <v>0</v>
@@ -41703,16 +41703,16 @@
         <v>1</v>
       </c>
       <c r="C1656">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1656" s="2">
-        <v>45812.78301983239</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E1656">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F1656" s="2">
-        <v>45812.44633101852</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G1656">
         <v>0</v>
@@ -41729,16 +41729,16 @@
         <v>1</v>
       </c>
       <c r="C1657">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1657" s="2">
-        <v>45799.89542739857</v>
+        <v>45814.82976436854</v>
       </c>
       <c r="E1657">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F1657" s="2">
-        <v>45783.42384259259</v>
+        <v>45814.70711805556</v>
       </c>
       <c r="G1657">
         <v>0</v>
@@ -46171,16 +46171,16 @@
         <v>1</v>
       </c>
       <c r="C1835">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1835" s="2">
-        <v>45811.92546678011</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E1835">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1835" s="2">
-        <v>45811.50125</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G1835">
         <v>0</v>
@@ -46399,16 +46399,16 @@
         <v>1</v>
       </c>
       <c r="C1844">
-        <v>388</v>
+        <v>268</v>
       </c>
       <c r="D1844" s="2">
-        <v>45813.95785151322</v>
+        <v>45814.82970463676</v>
       </c>
       <c r="E1844">
-        <v>388</v>
+        <v>268</v>
       </c>
       <c r="F1844" s="2">
-        <v>45813.65701388889</v>
+        <v>45814.38376157408</v>
       </c>
       <c r="G1844">
         <v>0</v>
@@ -46699,16 +46699,16 @@
         <v>1</v>
       </c>
       <c r="C1856">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D1856" s="2">
-        <v>45804.91952554927</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E1856">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F1856" s="2">
-        <v>45804.42633101852</v>
+        <v>45814.67278935185</v>
       </c>
       <c r="G1856">
         <v>0</v>
@@ -46959,16 +46959,16 @@
         <v>1</v>
       </c>
       <c r="C1866">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D1866" s="2">
-        <v>45795.04169367771</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E1866">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F1866" s="2">
-        <v>45427.65541666667</v>
+        <v>45814.45145833334</v>
       </c>
       <c r="G1866">
         <v>0</v>
@@ -51746,16 +51746,16 @@
         <v>1</v>
       </c>
       <c r="C2056">
-        <v>-5</v>
+        <v>-21</v>
       </c>
       <c r="D2056" s="2">
-        <v>45813.95788197009</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E2056">
-        <v>-5</v>
+        <v>-21</v>
       </c>
       <c r="F2056" s="2">
-        <v>45813.68033564815</v>
+        <v>45814.64774305555</v>
       </c>
       <c r="G2056">
         <v>0</v>
@@ -52026,16 +52026,16 @@
         <v>1</v>
       </c>
       <c r="C2067">
-        <v>-53</v>
+        <v>271</v>
       </c>
       <c r="D2067" s="2">
-        <v>45813.95785146693</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E2067">
-        <v>-53</v>
+        <v>271</v>
       </c>
       <c r="F2067" s="2">
-        <v>45813.54864583333</v>
+        <v>45814.67518518519</v>
       </c>
       <c r="G2067">
         <v>0</v>
@@ -53007,10 +53007,10 @@
         <v>1</v>
       </c>
       <c r="C2106">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="D2106" s="2">
-        <v>45807.78640657826</v>
+        <v>45816.01481442774</v>
       </c>
       <c r="E2106">
         <v>-1</v>
@@ -53019,10 +53019,10 @@
         <v>45807.43640046296</v>
       </c>
       <c r="G2106">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H2106" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2107" spans="1:8">
@@ -55101,16 +55101,16 @@
         <v>1</v>
       </c>
       <c r="C2190">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2190" s="2">
-        <v>45811.92552606984</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E2190">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2190" s="2">
-        <v>45811.75335648148</v>
+        <v>45814.53738425926</v>
       </c>
       <c r="G2190">
         <v>0</v>
@@ -55615,16 +55615,16 @@
         <v>1</v>
       </c>
       <c r="C2210">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2210" s="2">
-        <v>45811.92544186871</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E2210">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2210" s="2">
-        <v>45810.78280092592</v>
+        <v>45814.53738425926</v>
       </c>
       <c r="G2210">
         <v>0</v>
@@ -58581,22 +58581,22 @@
         <v>1</v>
       </c>
       <c r="C2328">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="D2328" s="2">
-        <v>45810.72556745499</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E2328">
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="F2328" s="2">
-        <v>45784.75885416667</v>
+        <v>45814.64774305555</v>
       </c>
       <c r="G2328">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2328" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2329" spans="1:8">
@@ -61162,16 +61162,16 @@
         <v>1</v>
       </c>
       <c r="C2432">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D2432" s="2">
-        <v>45812.78301989438</v>
+        <v>45814.82978481724</v>
       </c>
       <c r="E2432">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F2432" s="2">
-        <v>45812.65634259259</v>
+        <v>45814.64774305555</v>
       </c>
       <c r="G2432">
         <v>0</v>
@@ -61188,16 +61188,16 @@
         <v>1</v>
       </c>
       <c r="C2433">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D2433" s="2">
-        <v>45813.95782005877</v>
+        <v>45814.82980241515</v>
       </c>
       <c r="E2433">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F2433" s="2">
-        <v>45813.42155092592</v>
+        <v>45814.75646990741</v>
       </c>
       <c r="G2433">
         <v>0</v>
@@ -62517,16 +62517,16 @@
         <v>1</v>
       </c>
       <c r="C2487">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D2487" s="2">
-        <v>45812.78301989438</v>
+        <v>45814.82968397064</v>
       </c>
       <c r="E2487">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F2487" s="2">
-        <v>45812.65958333333</v>
+        <v>45814.49446759259</v>
       </c>
       <c r="G2487">
         <v>0</v>
@@ -64159,16 +64159,16 @@
         <v>1</v>
       </c>
       <c r="C2555">
-        <v>-50</v>
+        <v>0</v>
       </c>
       <c r="D2555" s="2">
-        <v>45813.95788197009</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E2555">
-        <v>-50</v>
+        <v>0</v>
       </c>
       <c r="F2555" s="2">
-        <v>45813.67865740741</v>
+        <v>45814.67984953704</v>
       </c>
       <c r="G2555">
         <v>0</v>
@@ -64185,16 +64185,16 @@
         <v>1</v>
       </c>
       <c r="C2556">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="D2556" s="2">
-        <v>45813.95785145537</v>
+        <v>45814.82974449309</v>
       </c>
       <c r="E2556">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="F2556" s="2">
-        <v>45813.46293981482</v>
+        <v>45814.67895833333</v>
       </c>
       <c r="G2556">
         <v>0</v>

</xml_diff>

<commit_message>
atualizei dados da add
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2574" uniqueCount="10">
   <si>
     <t>id_produto</t>
   </si>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2558"/>
+  <dimension ref="A1:H2567"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -952,16 +952,16 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="D23" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.30486084756</v>
       </c>
       <c r="E23">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="F23" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.66995370371</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1194,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>3161</v>
+        <v>3155</v>
       </c>
       <c r="D33" s="2">
-        <v>45814.82970462521</v>
+        <v>45818.30489302581</v>
       </c>
       <c r="E33">
-        <v>3161</v>
+        <v>3155</v>
       </c>
       <c r="F33" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1739,16 +1739,16 @@
         <v>1</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D55" s="2">
-        <v>45795.04208095842</v>
+        <v>45818.30489301677</v>
       </c>
       <c r="E55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" s="2">
-        <v>45763.60134259259</v>
+        <v>45817.75368055556</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -1765,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D56" s="2">
-        <v>45814.82966409007</v>
+        <v>45818.30489301893</v>
       </c>
       <c r="E56">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F56" s="2">
-        <v>45814.39652777778</v>
+        <v>45817.75439814815</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -1817,16 +1817,16 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D58" s="2">
-        <v>45814.82966409007</v>
+        <v>45818.30489300755</v>
       </c>
       <c r="E58">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F58" s="2">
-        <v>45814.39652777778</v>
+        <v>45817.73993055556</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -1843,16 +1843,16 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D59" s="2">
-        <v>45813.95795446759</v>
+        <v>45818.30489300116</v>
       </c>
       <c r="E59">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F59" s="2">
-        <v>45813.57359953703</v>
+        <v>45817.71056712963</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -1941,16 +1941,16 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D63" s="2">
-        <v>45814.82976436854</v>
+        <v>45818.30486083002</v>
       </c>
       <c r="E63">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F63" s="2">
-        <v>45814.70711805556</v>
+        <v>45817.5053587963</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2114,16 +2114,16 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="D70" s="2">
-        <v>45814.82978481724</v>
+        <v>45818.30486085102</v>
       </c>
       <c r="E70">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="F70" s="2">
-        <v>45814.74193287037</v>
+        <v>45817.68067129629</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2437,7 +2437,7 @@
         <v>32</v>
       </c>
       <c r="F83" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.66995370371</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -2529,16 +2529,16 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D87" s="2">
-        <v>45814.82966409007</v>
+        <v>45818.30486081236</v>
       </c>
       <c r="E87">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F87" s="2">
-        <v>45814.38376157408</v>
+        <v>45817.39020833333</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -2702,16 +2702,16 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="D94" s="2">
-        <v>45814.82980241515</v>
+        <v>45818.30489301284</v>
       </c>
       <c r="E94">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="F94" s="2">
-        <v>45814.4477662037</v>
+        <v>45817.75225694444</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -2872,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>821</v>
+        <v>723</v>
       </c>
       <c r="D101" s="2">
-        <v>45814.82978481724</v>
+        <v>45818.30489302641</v>
       </c>
       <c r="E101">
-        <v>821</v>
+        <v>723</v>
       </c>
       <c r="F101" s="2">
-        <v>45814.70711805556</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -3209,16 +3209,16 @@
         <v>1</v>
       </c>
       <c r="C115">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D115" s="2">
-        <v>45813.95785150164</v>
+        <v>45818.30489302706</v>
       </c>
       <c r="E115">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F115" s="2">
-        <v>45813.65701388889</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -3258,16 +3258,16 @@
         <v>1</v>
       </c>
       <c r="C117">
-        <v>1125</v>
+        <v>1110</v>
       </c>
       <c r="D117" s="2">
-        <v>45814.82970462521</v>
+        <v>45818.30489301346</v>
       </c>
       <c r="E117">
-        <v>1125</v>
+        <v>1110</v>
       </c>
       <c r="F117" s="2">
-        <v>45814.46266203704</v>
+        <v>45817.75225694444</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -3333,16 +3333,16 @@
         <v>1</v>
       </c>
       <c r="C120">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D120" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.30486081295</v>
       </c>
       <c r="E120">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F120" s="2">
-        <v>45811.50252314815</v>
+        <v>45817.39020833333</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -3408,16 +3408,16 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>483</v>
+        <v>440</v>
       </c>
       <c r="D123" s="2">
-        <v>45816.01481442774</v>
+        <v>45818.30489301414</v>
       </c>
       <c r="E123">
-        <v>483</v>
+        <v>440</v>
       </c>
       <c r="F123" s="2">
-        <v>45815.96212962963</v>
+        <v>45817.75225694444</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -3846,16 +3846,16 @@
         <v>1</v>
       </c>
       <c r="C141">
-        <v>554</v>
+        <v>542</v>
       </c>
       <c r="D141" s="2">
-        <v>45814.82978481724</v>
+        <v>45818.30489301466</v>
       </c>
       <c r="E141">
-        <v>554</v>
+        <v>542</v>
       </c>
       <c r="F141" s="2">
-        <v>45814.74193287037</v>
+        <v>45817.75225694444</v>
       </c>
       <c r="G141">
         <v>0</v>
@@ -4100,16 +4100,16 @@
         <v>1</v>
       </c>
       <c r="C151">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D151" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.30486085203</v>
       </c>
       <c r="E151">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F151" s="2">
-        <v>45814.64774305555</v>
+        <v>45817.68385416667</v>
       </c>
       <c r="G151">
         <v>0</v>
@@ -4936,16 +4936,16 @@
         <v>1</v>
       </c>
       <c r="C185">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D185" s="2">
-        <v>45813.95788193521</v>
+        <v>45818.30486081362</v>
       </c>
       <c r="E185">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F185" s="2">
-        <v>45813.66761574074</v>
+        <v>45817.39020833333</v>
       </c>
       <c r="G185">
         <v>0</v>
@@ -5103,16 +5103,16 @@
         <v>1</v>
       </c>
       <c r="C192">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="D192" s="2">
-        <v>45812.78301989438</v>
+        <v>45818.3048608515</v>
       </c>
       <c r="E192">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="F192" s="2">
-        <v>45812.53496527778</v>
+        <v>45817.68160879629</v>
       </c>
       <c r="G192">
         <v>0</v>
@@ -5181,16 +5181,16 @@
         <v>1</v>
       </c>
       <c r="C195">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="D195" s="2">
-        <v>45813.95785150164</v>
+        <v>45818.30486082699</v>
       </c>
       <c r="E195">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="F195" s="2">
-        <v>45813.65701388889</v>
+        <v>45817.49925925926</v>
       </c>
       <c r="G195">
         <v>0</v>
@@ -5711,16 +5711,16 @@
         <v>1</v>
       </c>
       <c r="C217">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D217" s="2">
-        <v>45811.92549991595</v>
+        <v>45818.30486083706</v>
       </c>
       <c r="E217">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F217" s="2">
-        <v>45811.70625</v>
+        <v>45817.555</v>
       </c>
       <c r="G217">
         <v>0</v>
@@ -5933,16 +5933,16 @@
         <v>1</v>
       </c>
       <c r="C226">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D226" s="2">
-        <v>45810.72559946219</v>
+        <v>45818.30486083779</v>
       </c>
       <c r="E226">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F226" s="2">
-        <v>45810.64998842592</v>
+        <v>45817.555</v>
       </c>
       <c r="G226">
         <v>0</v>
@@ -6437,16 +6437,16 @@
         <v>1</v>
       </c>
       <c r="C247">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="D247" s="2">
-        <v>45814.82976436854</v>
+        <v>45818.30486082299</v>
       </c>
       <c r="E247">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="F247" s="2">
-        <v>45814.70711805556</v>
+        <v>45817.49490740741</v>
       </c>
       <c r="G247">
         <v>0</v>
@@ -6702,16 +6702,16 @@
         <v>1</v>
       </c>
       <c r="C258">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D258" s="2">
-        <v>45804.91952554927</v>
+        <v>45818.30486083855</v>
       </c>
       <c r="E258">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F258" s="2">
-        <v>45804.67836805555</v>
+        <v>45817.555</v>
       </c>
       <c r="G258">
         <v>0</v>
@@ -6823,16 +6823,16 @@
         <v>1</v>
       </c>
       <c r="C263">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D263" s="2">
-        <v>45811.92552606984</v>
+        <v>45818.30489300823</v>
       </c>
       <c r="E263">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F263" s="2">
-        <v>45811.75563657407</v>
+        <v>45817.73993055556</v>
       </c>
       <c r="G263">
         <v>0</v>
@@ -6898,16 +6898,16 @@
         <v>1</v>
       </c>
       <c r="C266">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="D266" s="2">
-        <v>45812.78301983239</v>
+        <v>45818.30489299829</v>
       </c>
       <c r="E266">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="F266" s="2">
-        <v>45812.47731481482</v>
+        <v>45817.69295138889</v>
       </c>
       <c r="G266">
         <v>0</v>
@@ -6996,16 +6996,16 @@
         <v>1</v>
       </c>
       <c r="C270">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="D270" s="2">
-        <v>45814.82968397064</v>
+        <v>45818.30486084807</v>
       </c>
       <c r="E270">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="F270" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.66995370371</v>
       </c>
       <c r="G270">
         <v>0</v>
@@ -7045,16 +7045,16 @@
         <v>1</v>
       </c>
       <c r="C272">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="D272" s="2">
-        <v>45814.82966409007</v>
+        <v>45818.30486083927</v>
       </c>
       <c r="E272">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="F272" s="2">
-        <v>45814.39601851852</v>
+        <v>45817.555</v>
       </c>
       <c r="G272">
         <v>0</v>
@@ -7071,16 +7071,16 @@
         <v>1</v>
       </c>
       <c r="C273">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D273" s="2">
-        <v>45813.95788194679</v>
+        <v>45818.30489301942</v>
       </c>
       <c r="E273">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F273" s="2">
-        <v>45813.67818287037</v>
+        <v>45817.7553587963</v>
       </c>
       <c r="G273">
         <v>0</v>
@@ -7097,16 +7097,16 @@
         <v>1</v>
       </c>
       <c r="C274">
-        <v>464</v>
+        <v>444</v>
       </c>
       <c r="D274" s="2">
-        <v>45813.95788197009</v>
+        <v>45818.30489300891</v>
       </c>
       <c r="E274">
-        <v>464</v>
+        <v>444</v>
       </c>
       <c r="F274" s="2">
-        <v>45813.68067129629</v>
+        <v>45817.73993055556</v>
       </c>
       <c r="G274">
         <v>0</v>
@@ -7417,7 +7417,7 @@
         <v>540</v>
       </c>
       <c r="F287" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.66995370371</v>
       </c>
       <c r="G287">
         <v>0</v>
@@ -7610,16 +7610,16 @@
         <v>1</v>
       </c>
       <c r="C295">
-        <v>373</v>
+        <v>354</v>
       </c>
       <c r="D295" s="2">
-        <v>45813.95793319555</v>
+        <v>45818.30489302766</v>
       </c>
       <c r="E295">
-        <v>373</v>
+        <v>354</v>
       </c>
       <c r="F295" s="2">
-        <v>45813.71038194445</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G295">
         <v>0</v>
@@ -7953,16 +7953,16 @@
         <v>1</v>
       </c>
       <c r="C309">
-        <v>1126</v>
+        <v>1118</v>
       </c>
       <c r="D309" s="2">
-        <v>45811.92552607598</v>
+        <v>45818.30486081876</v>
       </c>
       <c r="E309">
-        <v>1126</v>
+        <v>1118</v>
       </c>
       <c r="F309" s="2">
-        <v>45813.51170138889</v>
+        <v>45817.43152777778</v>
       </c>
       <c r="G309">
         <v>0</v>
@@ -8374,16 +8374,16 @@
         <v>1</v>
       </c>
       <c r="C326">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D326" s="2">
-        <v>45814.82980241515</v>
+        <v>45818.30486081776</v>
       </c>
       <c r="E326">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F326" s="2">
-        <v>45814.75739583333</v>
+        <v>45817.42730324074</v>
       </c>
       <c r="G326">
         <v>0</v>
@@ -8674,16 +8674,16 @@
         <v>1</v>
       </c>
       <c r="C338">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D338" s="2">
-        <v>45800.93175380815</v>
+        <v>45818.30489301519</v>
       </c>
       <c r="E338">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F338" s="2">
-        <v>45800.46056712963</v>
+        <v>45817.75225694444</v>
       </c>
       <c r="G338">
         <v>0</v>
@@ -8991,16 +8991,16 @@
         <v>1</v>
       </c>
       <c r="C351">
-        <v>-152</v>
+        <v>32</v>
       </c>
       <c r="D351" s="2">
-        <v>45814.82978481724</v>
+        <v>45818.30489300047</v>
       </c>
       <c r="E351">
-        <v>-152</v>
+        <v>32</v>
       </c>
       <c r="F351" s="2">
-        <v>45814.74193287037</v>
+        <v>45817.69565972222</v>
       </c>
       <c r="G351">
         <v>0</v>
@@ -9066,16 +9066,16 @@
         <v>1</v>
       </c>
       <c r="C354">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D354" s="2">
-        <v>45814.82980222279</v>
+        <v>45818.30486082787</v>
       </c>
       <c r="E354">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F354" s="2">
-        <v>45814.70711805556</v>
+        <v>45817.49925925926</v>
       </c>
       <c r="G354">
         <v>0</v>
@@ -9190,16 +9190,16 @@
         <v>1</v>
       </c>
       <c r="C359">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D359" s="2">
-        <v>45812.78306322403</v>
+        <v>45818.30486081928</v>
       </c>
       <c r="E359">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F359" s="2">
-        <v>45812.70449074074</v>
+        <v>45817.43152777778</v>
       </c>
       <c r="G359">
         <v>0</v>
@@ -9242,16 +9242,16 @@
         <v>1</v>
       </c>
       <c r="C361">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="D361" s="2">
-        <v>45807.78643077149</v>
+        <v>45818.30489301989</v>
       </c>
       <c r="E361">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="F361" s="2">
-        <v>45807.78542824074</v>
+        <v>45817.7553587963</v>
       </c>
       <c r="G361">
         <v>0</v>
@@ -9291,16 +9291,16 @@
         <v>1</v>
       </c>
       <c r="C363">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="D363" s="2">
-        <v>45814.82978481724</v>
+        <v>45818.30489302042</v>
       </c>
       <c r="E363">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="F363" s="2">
-        <v>45814.74193287037</v>
+        <v>45817.7553587963</v>
       </c>
       <c r="G363">
         <v>0</v>
@@ -9487,16 +9487,16 @@
         <v>1</v>
       </c>
       <c r="C371">
-        <v>179</v>
+        <v>107</v>
       </c>
       <c r="D371" s="2">
-        <v>45813.95782005877</v>
+        <v>45818.30486084376</v>
       </c>
       <c r="E371">
-        <v>179</v>
+        <v>107</v>
       </c>
       <c r="F371" s="2">
-        <v>45813.42155092592</v>
+        <v>45817.63928240741</v>
       </c>
       <c r="G371">
         <v>0</v>
@@ -9692,16 +9692,16 @@
         <v>1</v>
       </c>
       <c r="C379">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D379" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.30486082043</v>
       </c>
       <c r="E379">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F379" s="2">
-        <v>45811.52653935185</v>
+        <v>45817.43934027778</v>
       </c>
       <c r="G379">
         <v>0</v>
@@ -9891,16 +9891,16 @@
         <v>1</v>
       </c>
       <c r="C387">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D387" s="2">
-        <v>45812.78301989438</v>
+        <v>45818.30486084699</v>
       </c>
       <c r="E387">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F387" s="2">
-        <v>45812.63135416667</v>
+        <v>45817.664375</v>
       </c>
       <c r="G387">
         <v>0</v>
@@ -9969,16 +9969,16 @@
         <v>1</v>
       </c>
       <c r="C390">
-        <v>31</v>
+        <v>-1</v>
       </c>
       <c r="D390" s="2">
-        <v>45814.82968397064</v>
+        <v>45818.30489302825</v>
       </c>
       <c r="E390">
-        <v>31</v>
+        <v>-1</v>
       </c>
       <c r="F390" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G390">
         <v>0</v>
@@ -10070,16 +10070,16 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="D394" s="2">
-        <v>45816.01481442774</v>
+        <v>45818.30489299895</v>
       </c>
       <c r="E394">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="F394" s="2">
-        <v>45815.95642361111</v>
+        <v>45817.69565972222</v>
       </c>
       <c r="G394">
         <v>0</v>
@@ -10269,16 +10269,16 @@
         <v>1</v>
       </c>
       <c r="C402">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="D402" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.30489301573</v>
       </c>
       <c r="E402">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="F402" s="2">
-        <v>45814.49446759259</v>
+        <v>45817.75225694444</v>
       </c>
       <c r="G402">
         <v>0</v>
@@ -10419,16 +10419,16 @@
         <v>1</v>
       </c>
       <c r="C408">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D408" s="2">
-        <v>45811.92552606984</v>
+        <v>45818.30486081827</v>
       </c>
       <c r="E408">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F408" s="2">
-        <v>45811.75159722222</v>
+        <v>45817.42730324074</v>
       </c>
       <c r="G408">
         <v>0</v>
@@ -10673,16 +10673,16 @@
         <v>1</v>
       </c>
       <c r="C418">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="D418" s="2">
-        <v>45813.95785149008</v>
+        <v>45818.30489300957</v>
       </c>
       <c r="E418">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="F418" s="2">
-        <v>45813.58277777778</v>
+        <v>45817.73993055556</v>
       </c>
       <c r="G418">
         <v>0</v>
@@ -10843,16 +10843,16 @@
         <v>1</v>
       </c>
       <c r="C425">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D425" s="2">
-        <v>45812.78301989438</v>
+        <v>45818.3048608235</v>
       </c>
       <c r="E425">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F425" s="2">
-        <v>45812.63878472222</v>
+        <v>45817.49490740741</v>
       </c>
       <c r="G425">
         <v>0</v>
@@ -11140,16 +11140,16 @@
         <v>1</v>
       </c>
       <c r="C437">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D437" s="2">
-        <v>45813.95785145537</v>
+        <v>45818.30486083998</v>
       </c>
       <c r="E437">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F437" s="2">
-        <v>45813.51621527778</v>
+        <v>45817.555</v>
       </c>
       <c r="G437">
         <v>0</v>
@@ -11192,16 +11192,16 @@
         <v>1</v>
       </c>
       <c r="C439">
-        <v>-3</v>
+        <v>7</v>
       </c>
       <c r="D439" s="2">
-        <v>45813.95793319555</v>
+        <v>45818.30486082193</v>
       </c>
       <c r="E439">
-        <v>-3</v>
+        <v>7</v>
       </c>
       <c r="F439" s="2">
-        <v>45813.71038194445</v>
+        <v>45817.46255787037</v>
       </c>
       <c r="G439">
         <v>0</v>
@@ -11728,16 +11728,16 @@
         <v>1</v>
       </c>
       <c r="C461">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D461" s="2">
-        <v>45813.95785149008</v>
+        <v>45818.30489302886</v>
       </c>
       <c r="E461">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F461" s="2">
-        <v>45813.58277777778</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G461">
         <v>0</v>
@@ -12207,16 +12207,16 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D480" s="2">
-        <v>45814.82968397064</v>
+        <v>45818.30489300188</v>
       </c>
       <c r="E480">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F480" s="2">
-        <v>45814.46266203704</v>
+        <v>45817.71056712963</v>
       </c>
       <c r="G480">
         <v>0</v>
@@ -12951,16 +12951,16 @@
         <v>1</v>
       </c>
       <c r="C510">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="D510" s="2">
-        <v>45814.82976436854</v>
+        <v>45818.30489302096</v>
       </c>
       <c r="E510">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="F510" s="2">
-        <v>45814.70711805556</v>
+        <v>45817.7553587963</v>
       </c>
       <c r="G510">
         <v>0</v>
@@ -13467,16 +13467,16 @@
         <v>1</v>
       </c>
       <c r="C531">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D531" s="2">
-        <v>45813.95782007044</v>
+        <v>45818.30486082874</v>
       </c>
       <c r="E531">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F531" s="2">
-        <v>45813.46293981482</v>
+        <v>45817.49925925926</v>
       </c>
       <c r="G531">
         <v>0</v>
@@ -13816,16 +13816,16 @@
         <v>1</v>
       </c>
       <c r="C545">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D545" s="2">
-        <v>45799.895427387</v>
+        <v>45818.30489300693</v>
       </c>
       <c r="E545">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F545" s="2">
-        <v>45799.64056712963</v>
+        <v>45817.73076388889</v>
       </c>
       <c r="G545">
         <v>0</v>
@@ -14389,16 +14389,16 @@
         <v>1</v>
       </c>
       <c r="C569">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D569" s="2">
-        <v>45814.82972452114</v>
+        <v>45818.30489301023</v>
       </c>
       <c r="E569">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F569" s="2">
-        <v>45814.61704861111</v>
+        <v>45817.73993055556</v>
       </c>
       <c r="G569">
         <v>0</v>
@@ -14424,7 +14424,7 @@
         <v>2624</v>
       </c>
       <c r="F570" s="2">
-        <v>45814.49446759259</v>
+        <v>45817.66995370371</v>
       </c>
       <c r="G570">
         <v>0</v>
@@ -15939,7 +15939,7 @@
         <v>0</v>
       </c>
       <c r="F633" s="2">
-        <v>45812.47270833333</v>
+        <v>45817.54049768519</v>
       </c>
       <c r="G633">
         <v>0</v>
@@ -16509,16 +16509,16 @@
         <v>1</v>
       </c>
       <c r="C657">
-        <v>2140</v>
+        <v>2132</v>
       </c>
       <c r="D657" s="2">
-        <v>45814.82966410174</v>
+        <v>45818.30489302156</v>
       </c>
       <c r="E657">
-        <v>2140</v>
+        <v>2132</v>
       </c>
       <c r="F657" s="2">
-        <v>45814.39652777778</v>
+        <v>45817.7553587963</v>
       </c>
       <c r="G657">
         <v>0</v>
@@ -16535,16 +16535,16 @@
         <v>1</v>
       </c>
       <c r="C658">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D658" s="2">
-        <v>45814.82978481724</v>
+        <v>45818.30486082475</v>
       </c>
       <c r="E658">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F658" s="2">
-        <v>45814.74193287037</v>
+        <v>45817.49490740741</v>
       </c>
       <c r="G658">
         <v>0</v>
@@ -17290,16 +17290,16 @@
         <v>1</v>
       </c>
       <c r="C689">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="D689" s="2">
-        <v>45806.77600903736</v>
+        <v>45818.30486084076</v>
       </c>
       <c r="E689">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="F689" s="2">
-        <v>45806.61890046296</v>
+        <v>45817.555</v>
       </c>
       <c r="G689">
         <v>0</v>
@@ -17599,16 +17599,16 @@
         <v>1</v>
       </c>
       <c r="C701">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D701" s="2">
-        <v>45813.95785146693</v>
+        <v>45818.30489300293</v>
       </c>
       <c r="E701">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F701" s="2">
-        <v>45813.57766203704</v>
+        <v>45817.71056712963</v>
       </c>
       <c r="G701">
         <v>0</v>
@@ -18381,16 +18381,16 @@
         <v>1</v>
       </c>
       <c r="C732">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D732" s="2">
-        <v>45814.82968397064</v>
+        <v>45818.30486083475</v>
       </c>
       <c r="E732">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F732" s="2">
-        <v>45814.49446759259</v>
+        <v>45817.51208333333</v>
       </c>
       <c r="G732">
         <v>0</v>
@@ -18560,16 +18560,16 @@
         <v>1</v>
       </c>
       <c r="C739">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D739" s="2">
-        <v>45805.9187731686</v>
+        <v>45818.30486084728</v>
       </c>
       <c r="E739">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F739" s="2">
-        <v>45805.76938657407</v>
+        <v>45817.664375</v>
       </c>
       <c r="G739">
         <v>0</v>
@@ -19154,16 +19154,16 @@
         <v>1</v>
       </c>
       <c r="C763">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D763" s="2">
-        <v>45811.92549991595</v>
+        <v>45818.30486082933</v>
       </c>
       <c r="E763">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F763" s="2">
-        <v>45811.69520833333</v>
+        <v>45817.49925925926</v>
       </c>
       <c r="G763">
         <v>0</v>
@@ -19232,16 +19232,16 @@
         <v>1</v>
       </c>
       <c r="C766">
-        <v>-30</v>
+        <v>10</v>
       </c>
       <c r="D766" s="2">
-        <v>45811.92552607598</v>
+        <v>45818.30489301217</v>
       </c>
       <c r="E766">
-        <v>-30</v>
+        <v>10</v>
       </c>
       <c r="F766" s="2">
-        <v>45811.76255787037</v>
+        <v>45817.74609953703</v>
       </c>
       <c r="G766">
         <v>0</v>
@@ -19327,16 +19327,16 @@
         <v>1</v>
       </c>
       <c r="C770">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D770" s="2">
-        <v>45810.72559944464</v>
+        <v>45818.30489302945</v>
       </c>
       <c r="E770">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F770" s="2">
-        <v>45810.52887731481</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G770">
         <v>0</v>
@@ -19379,16 +19379,16 @@
         <v>1</v>
       </c>
       <c r="C772">
-        <v>233</v>
+        <v>158</v>
       </c>
       <c r="D772" s="2">
-        <v>45813.95785145537</v>
+        <v>45818.30489302205</v>
       </c>
       <c r="E772">
-        <v>233</v>
+        <v>158</v>
       </c>
       <c r="F772" s="2">
-        <v>45813.46407407407</v>
+        <v>45817.7553587963</v>
       </c>
       <c r="G772">
         <v>0</v>
@@ -20683,16 +20683,16 @@
         <v>1</v>
       </c>
       <c r="C824">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D824" s="2">
-        <v>45816.01481442774</v>
+        <v>45818.30486081409</v>
       </c>
       <c r="E824">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F824" s="2">
-        <v>45815.95763888889</v>
+        <v>45817.39020833333</v>
       </c>
       <c r="G824">
         <v>0</v>
@@ -20732,16 +20732,16 @@
         <v>1</v>
       </c>
       <c r="C826">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D826" s="2">
-        <v>45813.95785149008</v>
+        <v>45818.30489303007</v>
       </c>
       <c r="E826">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F826" s="2">
-        <v>45813.60496527778</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G826">
         <v>0</v>
@@ -20853,16 +20853,16 @@
         <v>1</v>
       </c>
       <c r="C831">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="D831" s="2">
-        <v>45811.92552605522</v>
+        <v>45818.30486083288</v>
       </c>
       <c r="E831">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="F831" s="2">
-        <v>45811.75072916667</v>
+        <v>45817.51131944444</v>
       </c>
       <c r="G831">
         <v>0</v>
@@ -21389,16 +21389,16 @@
         <v>1</v>
       </c>
       <c r="C853">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D853" s="2">
-        <v>45813.95782007044</v>
+        <v>45818.30489301757</v>
       </c>
       <c r="E853">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F853" s="2">
-        <v>45813.46293981482</v>
+        <v>45817.75368055556</v>
       </c>
       <c r="G853">
         <v>0</v>
@@ -21415,16 +21415,16 @@
         <v>1</v>
       </c>
       <c r="C854">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D854" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.3048608254</v>
       </c>
       <c r="E854">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F854" s="2">
-        <v>45814.64774305555</v>
+        <v>45817.49490740741</v>
       </c>
       <c r="G854">
         <v>0</v>
@@ -21868,16 +21868,16 @@
         <v>1</v>
       </c>
       <c r="C872">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D872" s="2">
-        <v>45814.82972452114</v>
+        <v>45818.30489302258</v>
       </c>
       <c r="E872">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="F872" s="2">
-        <v>45814.61704861111</v>
+        <v>45817.7553587963</v>
       </c>
       <c r="G872">
         <v>0</v>
@@ -22154,7 +22154,7 @@
         <v>76</v>
       </c>
       <c r="F883" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.66995370371</v>
       </c>
       <c r="G883">
         <v>0</v>
@@ -23196,7 +23196,7 @@
         <v>26</v>
       </c>
       <c r="F924" s="2">
-        <v>45814.61704861111</v>
+        <v>45817.66995370371</v>
       </c>
       <c r="G924">
         <v>0</v>
@@ -24119,7 +24119,7 @@
         <v>40</v>
       </c>
       <c r="F961" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.66995370371</v>
       </c>
       <c r="G961">
         <v>0</v>
@@ -24390,16 +24390,16 @@
         <v>1</v>
       </c>
       <c r="C972">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D972" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.30486082585</v>
       </c>
       <c r="E972">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F972" s="2">
-        <v>45811.4736574074</v>
+        <v>45817.49490740741</v>
       </c>
       <c r="G972">
         <v>0</v>
@@ -25533,16 +25533,16 @@
         <v>1</v>
       </c>
       <c r="C1017">
-        <v>445</v>
+        <v>424</v>
       </c>
       <c r="D1017" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.30489300357</v>
       </c>
       <c r="E1017">
-        <v>445</v>
+        <v>424</v>
       </c>
       <c r="F1017" s="2">
-        <v>45811.66579861111</v>
+        <v>45817.71056712963</v>
       </c>
       <c r="G1017">
         <v>0</v>
@@ -26676,16 +26676,16 @@
         <v>1</v>
       </c>
       <c r="C1062">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D1062" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.30489302317</v>
       </c>
       <c r="E1062">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="F1062" s="2">
-        <v>45814.65319444444</v>
+        <v>45817.7553587963</v>
       </c>
       <c r="G1062">
         <v>0</v>
@@ -27423,7 +27423,7 @@
         <v>4</v>
       </c>
       <c r="F1092" s="2">
-        <v>45811.50076388889</v>
+        <v>45817.77144675926</v>
       </c>
       <c r="G1092">
         <v>0</v>
@@ -27867,16 +27867,16 @@
         <v>1</v>
       </c>
       <c r="C1110">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D1110" s="2">
-        <v>45814.82968397064</v>
+        <v>45818.30489303031</v>
       </c>
       <c r="E1110">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F1110" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G1110">
         <v>0</v>
@@ -28173,16 +28173,16 @@
         <v>1</v>
       </c>
       <c r="C1122">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1122" s="2">
-        <v>45814.82978481724</v>
+        <v>45818.30489300424</v>
       </c>
       <c r="E1122">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F1122" s="2">
-        <v>45814.64774305555</v>
+        <v>45817.71056712963</v>
       </c>
       <c r="G1122">
         <v>0</v>
@@ -28309,7 +28309,7 @@
         <v>27</v>
       </c>
       <c r="F1127" s="2">
-        <v>45786.60893518518</v>
+        <v>45817.54049768519</v>
       </c>
       <c r="G1127">
         <v>0</v>
@@ -28805,16 +28805,16 @@
         <v>1</v>
       </c>
       <c r="C1147">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1147" s="2">
-        <v>45816.01481442774</v>
+        <v>45818.30486084976</v>
       </c>
       <c r="E1147">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1147" s="2">
-        <v>45815.95717592593</v>
+        <v>45817.66995370371</v>
       </c>
       <c r="G1147">
         <v>0</v>
@@ -29013,16 +29013,16 @@
         <v>1</v>
       </c>
       <c r="C1155">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1155" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.30489300488</v>
       </c>
       <c r="E1155">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1155" s="2">
-        <v>45811.45587962963</v>
+        <v>45817.71056712963</v>
       </c>
       <c r="G1155">
         <v>0</v>
@@ -31372,16 +31372,16 @@
         <v>1</v>
       </c>
       <c r="C1247">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D1247" s="2">
-        <v>45810.72563720519</v>
+        <v>45818.30486081455</v>
       </c>
       <c r="E1247">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F1247" s="2">
-        <v>45810.68862268519</v>
+        <v>45817.39020833333</v>
       </c>
       <c r="G1247">
         <v>0</v>
@@ -31528,16 +31528,16 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D1253" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.30489301086</v>
       </c>
       <c r="E1253">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F1253" s="2">
-        <v>45814.65319444444</v>
+        <v>45817.73993055556</v>
       </c>
       <c r="G1253">
         <v>0</v>
@@ -33384,16 +33384,16 @@
         <v>1</v>
       </c>
       <c r="C1326">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1326" s="2">
-        <v>45795.04171905605</v>
+        <v>45818.30486082246</v>
       </c>
       <c r="E1326">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1326" s="2">
-        <v>45469.53236111111</v>
+        <v>45817.46609953704</v>
       </c>
       <c r="G1326">
         <v>0</v>
@@ -33462,16 +33462,16 @@
         <v>1</v>
       </c>
       <c r="C1329">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D1329" s="2">
-        <v>45804.91954472794</v>
+        <v>45818.30489301625</v>
       </c>
       <c r="E1329">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F1329" s="2">
-        <v>45804.72743055555</v>
+        <v>45817.75225694444</v>
       </c>
       <c r="G1329">
         <v>0</v>
@@ -33540,16 +33540,16 @@
         <v>1</v>
       </c>
       <c r="C1332">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1332" s="2">
-        <v>45813.95795447831</v>
+        <v>45818.30489302384</v>
       </c>
       <c r="E1332">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1332" s="2">
-        <v>45813.46293981482</v>
+        <v>45817.7553587963</v>
       </c>
       <c r="G1332">
         <v>0</v>
@@ -33791,16 +33791,16 @@
         <v>1</v>
       </c>
       <c r="C1342">
-        <v>1244</v>
+        <v>1184</v>
       </c>
       <c r="D1342" s="2">
-        <v>45812.78306321269</v>
+        <v>45818.30486081507</v>
       </c>
       <c r="E1342">
-        <v>1244</v>
+        <v>1184</v>
       </c>
       <c r="F1342" s="2">
-        <v>45812.70203703704</v>
+        <v>45817.39020833333</v>
       </c>
       <c r="G1342">
         <v>0</v>
@@ -35630,16 +35630,16 @@
         <v>1</v>
       </c>
       <c r="C1414">
-        <v>-3</v>
+        <v>7</v>
       </c>
       <c r="D1414" s="2">
-        <v>45813.95795449081</v>
+        <v>45818.30486082094</v>
       </c>
       <c r="E1414">
-        <v>-3</v>
+        <v>7</v>
       </c>
       <c r="F1414" s="2">
-        <v>45813.7544212963</v>
+        <v>45817.45899305555</v>
       </c>
       <c r="G1414">
         <v>0</v>
@@ -36996,7 +36996,7 @@
         <v>0</v>
       </c>
       <c r="F1467" s="2">
-        <v>45705.77503472222</v>
+        <v>45817.77212962963</v>
       </c>
       <c r="G1467">
         <v>0</v>
@@ -37379,16 +37379,16 @@
         <v>1</v>
       </c>
       <c r="C1483">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D1483" s="2">
-        <v>45814.82968397064</v>
+        <v>45818.30486081611</v>
       </c>
       <c r="E1483">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F1483" s="2">
-        <v>45814.49446759259</v>
+        <v>45817.41581018519</v>
       </c>
       <c r="G1483">
         <v>0</v>
@@ -39470,16 +39470,16 @@
         <v>1</v>
       </c>
       <c r="C1567">
-        <v>-64</v>
+        <v>0</v>
       </c>
       <c r="D1567" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.30486084452</v>
       </c>
       <c r="E1567">
-        <v>-64</v>
+        <v>0</v>
       </c>
       <c r="F1567" s="2">
-        <v>45814.5771875</v>
+        <v>45817.64519675926</v>
       </c>
       <c r="G1567">
         <v>0</v>
@@ -40145,16 +40145,16 @@
         <v>1</v>
       </c>
       <c r="C1594">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1594" s="2">
-        <v>45812.78301989438</v>
+        <v>45818.30489302451</v>
       </c>
       <c r="E1594">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F1594" s="2">
-        <v>45812.65041666666</v>
+        <v>45817.7553587963</v>
       </c>
       <c r="G1594">
         <v>0</v>
@@ -40223,16 +40223,16 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>5726</v>
+        <v>5675</v>
       </c>
       <c r="D1597" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.30489303058</v>
       </c>
       <c r="E1597">
-        <v>5726</v>
+        <v>5675</v>
       </c>
       <c r="F1597" s="2">
-        <v>45814.65319444444</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G1597">
         <v>0</v>
@@ -41086,16 +41086,16 @@
         <v>1</v>
       </c>
       <c r="C1631">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D1631" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.30486084249</v>
       </c>
       <c r="E1631">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F1631" s="2">
-        <v>45811.49467592593</v>
+        <v>45817.6315625</v>
       </c>
       <c r="G1631">
         <v>0</v>
@@ -41190,16 +41190,16 @@
         <v>1</v>
       </c>
       <c r="C1635">
-        <v>2760</v>
+        <v>2679</v>
       </c>
       <c r="D1635" s="2">
-        <v>45813.95785147848</v>
+        <v>45818.30489301831</v>
       </c>
       <c r="E1635">
-        <v>2760</v>
+        <v>2679</v>
       </c>
       <c r="F1635" s="2">
-        <v>45813.58108796296</v>
+        <v>45817.75368055556</v>
       </c>
       <c r="G1635">
         <v>0</v>
@@ -41712,7 +41712,7 @@
         <v>0</v>
       </c>
       <c r="F1656" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.66995370371</v>
       </c>
       <c r="G1656">
         <v>0</v>
@@ -43762,7 +43762,7 @@
         <v>44</v>
       </c>
       <c r="F1739" s="2">
-        <v>45811.64603009259</v>
+        <v>45817.424375</v>
       </c>
       <c r="G1739">
         <v>0</v>
@@ -46180,7 +46180,7 @@
         <v>4</v>
       </c>
       <c r="F1835" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.66995370371</v>
       </c>
       <c r="G1835">
         <v>0</v>
@@ -46699,16 +46699,16 @@
         <v>1</v>
       </c>
       <c r="C1856">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D1856" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.30489300554</v>
       </c>
       <c r="E1856">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1856" s="2">
-        <v>45814.67278935185</v>
+        <v>45817.71056712963</v>
       </c>
       <c r="G1856">
         <v>0</v>
@@ -46959,16 +46959,16 @@
         <v>1</v>
       </c>
       <c r="C1866">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D1866" s="2">
-        <v>45814.82968397064</v>
+        <v>45818.30489299761</v>
       </c>
       <c r="E1866">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F1866" s="2">
-        <v>45814.45145833334</v>
+        <v>45817.68912037037</v>
       </c>
       <c r="G1866">
         <v>0</v>
@@ -48691,16 +48691,16 @@
         <v>1</v>
       </c>
       <c r="C1934">
-        <v>1</v>
+        <v>-9</v>
       </c>
       <c r="D1934" s="2">
-        <v>45804.91952554927</v>
+        <v>45818.30489299967</v>
       </c>
       <c r="E1934">
-        <v>1</v>
+        <v>-9</v>
       </c>
       <c r="F1934" s="2">
-        <v>45804.42633101852</v>
+        <v>45817.69565972222</v>
       </c>
       <c r="G1934">
         <v>0</v>
@@ -49937,7 +49937,7 @@
         <v>0</v>
       </c>
       <c r="D1984" s="2">
-        <v>45795.04169367771</v>
+        <v>45818.30489300624</v>
       </c>
       <c r="E1984">
         <v>0</v>
@@ -51472,16 +51472,16 @@
         <v>1</v>
       </c>
       <c r="C2045">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="D2045" s="2">
-        <v>45799.89542737551</v>
+        <v>45818.30486084311</v>
       </c>
       <c r="E2045">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="F2045" s="2">
-        <v>45799.6352662037</v>
+        <v>45817.6315625</v>
       </c>
       <c r="G2045">
         <v>0</v>
@@ -51746,16 +51746,16 @@
         <v>1</v>
       </c>
       <c r="C2056">
-        <v>-21</v>
+        <v>20</v>
       </c>
       <c r="D2056" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.30489302518</v>
       </c>
       <c r="E2056">
-        <v>-21</v>
+        <v>20</v>
       </c>
       <c r="F2056" s="2">
-        <v>45814.64774305555</v>
+        <v>45817.7553587963</v>
       </c>
       <c r="G2056">
         <v>0</v>
@@ -52580,7 +52580,7 @@
         <v>0</v>
       </c>
       <c r="F2089" s="2">
-        <v>45631.66751157407</v>
+        <v>45817.68456018518</v>
       </c>
       <c r="G2089">
         <v>0</v>
@@ -53454,16 +53454,16 @@
         <v>1</v>
       </c>
       <c r="C2124">
-        <v>291</v>
+        <v>211</v>
       </c>
       <c r="D2124" s="2">
-        <v>45810.72559945051</v>
+        <v>45818.30486081979</v>
       </c>
       <c r="E2124">
-        <v>291</v>
+        <v>211</v>
       </c>
       <c r="F2124" s="2">
-        <v>45810.63849537037</v>
+        <v>45817.43152777778</v>
       </c>
       <c r="G2124">
         <v>0</v>
@@ -56244,16 +56244,16 @@
         <v>1</v>
       </c>
       <c r="C2235">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2235" s="2">
-        <v>45813.95795447831</v>
+        <v>45818.30486081664</v>
       </c>
       <c r="E2235">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F2235" s="2">
-        <v>45813.65701388889</v>
+        <v>45817.41581018519</v>
       </c>
       <c r="G2235">
         <v>0</v>
@@ -58581,16 +58581,16 @@
         <v>1</v>
       </c>
       <c r="C2328">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D2328" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.30489299681</v>
       </c>
       <c r="E2328">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="F2328" s="2">
-        <v>45814.64774305555</v>
+        <v>45817.68517361111</v>
       </c>
       <c r="G2328">
         <v>0</v>
@@ -60767,16 +60767,16 @@
         <v>1</v>
       </c>
       <c r="C2416">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D2416" s="2">
-        <v>45813.95785147848</v>
+        <v>45818.30486081559</v>
       </c>
       <c r="E2416">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F2416" s="2">
-        <v>45813.5819212963</v>
+        <v>45817.39020833333</v>
       </c>
       <c r="G2416">
         <v>0</v>
@@ -61972,16 +61972,16 @@
         <v>1</v>
       </c>
       <c r="C2465">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D2465" s="2">
-        <v>45810.72563720519</v>
+        <v>45818.30489303097</v>
       </c>
       <c r="E2465">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="F2465" s="2">
-        <v>45810.66278935185</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G2465">
         <v>0</v>
@@ -62387,16 +62387,16 @@
         <v>1</v>
       </c>
       <c r="C2482">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="D2482" s="2">
-        <v>45813.95785146693</v>
+        <v>45818.30486084184</v>
       </c>
       <c r="E2482">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="F2482" s="2">
-        <v>45813.54864583333</v>
+        <v>45817.555</v>
       </c>
       <c r="G2482">
         <v>0</v>
@@ -62413,16 +62413,16 @@
         <v>1</v>
       </c>
       <c r="C2483">
-        <v>821</v>
+        <v>793</v>
       </c>
       <c r="D2483" s="2">
-        <v>45812.78306321269</v>
+        <v>45818.30489303119</v>
       </c>
       <c r="E2483">
-        <v>821</v>
+        <v>793</v>
       </c>
       <c r="F2483" s="2">
-        <v>45813.51170138889</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G2483">
         <v>0</v>
@@ -62439,16 +62439,16 @@
         <v>1</v>
       </c>
       <c r="C2484">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="D2484" s="2">
-        <v>45813.95785145537</v>
+        <v>45818.30489303141</v>
       </c>
       <c r="E2484">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="F2484" s="2">
-        <v>45813.51170138889</v>
+        <v>45817.7559837963</v>
       </c>
       <c r="G2484">
         <v>0</v>
@@ -64246,6 +64246,216 @@
         <v>0</v>
       </c>
       <c r="H2558" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:8">
+      <c r="A2559">
+        <v>43514052</v>
+      </c>
+      <c r="B2559">
+        <v>1</v>
+      </c>
+      <c r="C2559">
+        <v>0</v>
+      </c>
+      <c r="D2559" s="2">
+        <v>45818.30489303147</v>
+      </c>
+      <c r="E2559">
+        <v>0</v>
+      </c>
+      <c r="F2559" s="2">
+        <v>45817.76997685185</v>
+      </c>
+      <c r="G2559">
+        <v>0</v>
+      </c>
+      <c r="H2559" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2560" spans="1:8">
+      <c r="A2560">
+        <v>43514806</v>
+      </c>
+      <c r="B2560">
+        <v>1</v>
+      </c>
+      <c r="C2560">
+        <v>0</v>
+      </c>
+      <c r="D2560" s="2">
+        <v>45818.3048608199</v>
+      </c>
+      <c r="E2560">
+        <v>0</v>
+      </c>
+      <c r="G2560">
+        <v>0</v>
+      </c>
+      <c r="H2560" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:8">
+      <c r="A2561">
+        <v>43520877</v>
+      </c>
+      <c r="B2561">
+        <v>1</v>
+      </c>
+      <c r="C2561">
+        <v>0</v>
+      </c>
+      <c r="D2561" s="2">
+        <v>45818.30486084626</v>
+      </c>
+      <c r="E2561">
+        <v>0</v>
+      </c>
+      <c r="G2561">
+        <v>0</v>
+      </c>
+      <c r="H2561" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:8">
+      <c r="A2562">
+        <v>43521261</v>
+      </c>
+      <c r="B2562">
+        <v>1</v>
+      </c>
+      <c r="C2562">
+        <v>0</v>
+      </c>
+      <c r="D2562" s="2">
+        <v>45818.3048608464</v>
+      </c>
+      <c r="E2562">
+        <v>0</v>
+      </c>
+      <c r="G2562">
+        <v>0</v>
+      </c>
+      <c r="H2562" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2563" spans="1:8">
+      <c r="A2563">
+        <v>43537158</v>
+      </c>
+      <c r="B2563">
+        <v>1</v>
+      </c>
+      <c r="C2563">
+        <v>0</v>
+      </c>
+      <c r="D2563" s="2">
+        <v>45818.30489301126</v>
+      </c>
+      <c r="E2563">
+        <v>0</v>
+      </c>
+      <c r="G2563">
+        <v>0</v>
+      </c>
+      <c r="H2563" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2564" spans="1:8">
+      <c r="A2564">
+        <v>43537163</v>
+      </c>
+      <c r="B2564">
+        <v>1</v>
+      </c>
+      <c r="C2564">
+        <v>0</v>
+      </c>
+      <c r="D2564" s="2">
+        <v>45818.30489301113</v>
+      </c>
+      <c r="E2564">
+        <v>0</v>
+      </c>
+      <c r="G2564">
+        <v>0</v>
+      </c>
+      <c r="H2564" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2565" spans="1:8">
+      <c r="A2565">
+        <v>43537165</v>
+      </c>
+      <c r="B2565">
+        <v>1</v>
+      </c>
+      <c r="C2565">
+        <v>0</v>
+      </c>
+      <c r="D2565" s="2">
+        <v>45818.30489301101</v>
+      </c>
+      <c r="E2565">
+        <v>0</v>
+      </c>
+      <c r="G2565">
+        <v>0</v>
+      </c>
+      <c r="H2565" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2566" spans="1:8">
+      <c r="A2566">
+        <v>43537169</v>
+      </c>
+      <c r="B2566">
+        <v>1</v>
+      </c>
+      <c r="C2566">
+        <v>0</v>
+      </c>
+      <c r="D2566" s="2">
+        <v>45818.30489301139</v>
+      </c>
+      <c r="E2566">
+        <v>0</v>
+      </c>
+      <c r="G2566">
+        <v>0</v>
+      </c>
+      <c r="H2566" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:8">
+      <c r="A2567">
+        <v>43537173</v>
+      </c>
+      <c r="B2567">
+        <v>1</v>
+      </c>
+      <c r="C2567">
+        <v>0</v>
+      </c>
+      <c r="D2567" s="2">
+        <v>45818.30489301152</v>
+      </c>
+      <c r="E2567">
+        <v>0</v>
+      </c>
+      <c r="G2567">
+        <v>0</v>
+      </c>
+      <c r="H2567" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finalizando inatividade de produtos
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -1194,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>3155</v>
+        <v>3153</v>
       </c>
       <c r="D33" s="2">
-        <v>45818.30489302581</v>
+        <v>45818.80148693069</v>
       </c>
       <c r="E33">
-        <v>3155</v>
+        <v>3153</v>
       </c>
       <c r="F33" s="2">
-        <v>45817.7559837963</v>
+        <v>45818.40175925926</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1312,16 +1312,16 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D38" s="2">
-        <v>45810.72556745499</v>
+        <v>45818.80148693405</v>
       </c>
       <c r="E38">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F38" s="2">
-        <v>45810.51450231481</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -1765,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D56" s="2">
-        <v>45818.30489301893</v>
+        <v>45818.8014869416</v>
       </c>
       <c r="E56">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F56" s="2">
-        <v>45817.75439814815</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2402,16 +2402,16 @@
         <v>1</v>
       </c>
       <c r="C82">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D82" s="2">
-        <v>45814.82966409007</v>
+        <v>45818.80148693439</v>
       </c>
       <c r="E82">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F82" s="2">
-        <v>45814.38376157408</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -2477,16 +2477,16 @@
         <v>1</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D85" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.80148693339</v>
       </c>
       <c r="E85">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F85" s="2">
-        <v>45814.65319444444</v>
+        <v>45818.42027777778</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -2529,16 +2529,16 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D87" s="2">
-        <v>45818.30486081236</v>
+        <v>45818.80148695138</v>
       </c>
       <c r="E87">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F87" s="2">
-        <v>45817.39020833333</v>
+        <v>45818.7134375</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -2630,16 +2630,16 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="D91" s="2">
-        <v>45813.95782007044</v>
+        <v>45818.80148695299</v>
       </c>
       <c r="E91">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="F91" s="2">
-        <v>45813.46293981482</v>
+        <v>45818.71952546296</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -2872,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>723</v>
+        <v>580</v>
       </c>
       <c r="D101" s="2">
-        <v>45818.30489302641</v>
+        <v>45818.80148694194</v>
       </c>
       <c r="E101">
-        <v>723</v>
+        <v>580</v>
       </c>
       <c r="F101" s="2">
-        <v>45817.7559837963</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -2993,16 +2993,16 @@
         <v>1</v>
       </c>
       <c r="C106">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="D106" s="2">
-        <v>45813.95793319555</v>
+        <v>45818.80148695203</v>
       </c>
       <c r="E106">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="F106" s="2">
-        <v>45813.71038194445</v>
+        <v>45818.71346064815</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -3333,16 +3333,16 @@
         <v>1</v>
       </c>
       <c r="C120">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D120" s="2">
-        <v>45818.30486081295</v>
+        <v>45818.80148693471</v>
       </c>
       <c r="E120">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="F120" s="2">
-        <v>45817.39020833333</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -3434,16 +3434,16 @@
         <v>1</v>
       </c>
       <c r="C124">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D124" s="2">
-        <v>45811.92544186871</v>
+        <v>45818.80148694228</v>
       </c>
       <c r="E124">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F124" s="2">
-        <v>45810.78246527778</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -4936,16 +4936,16 @@
         <v>1</v>
       </c>
       <c r="C185">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D185" s="2">
-        <v>45818.30486081362</v>
+        <v>45818.80148693504</v>
       </c>
       <c r="E185">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F185" s="2">
-        <v>45817.39020833333</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G185">
         <v>0</v>
@@ -5181,16 +5181,16 @@
         <v>1</v>
       </c>
       <c r="C195">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="D195" s="2">
-        <v>45818.30486082699</v>
+        <v>45818.80148694695</v>
       </c>
       <c r="E195">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="F195" s="2">
-        <v>45817.49925925926</v>
+        <v>45818.66138888889</v>
       </c>
       <c r="G195">
         <v>0</v>
@@ -6627,16 +6627,16 @@
         <v>1</v>
       </c>
       <c r="C255">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D255" s="2">
-        <v>45813.95785149008</v>
+        <v>45818.8014869426</v>
       </c>
       <c r="E255">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="F255" s="2">
-        <v>45813.63554398148</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -7097,16 +7097,16 @@
         <v>1</v>
       </c>
       <c r="C274">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D274" s="2">
-        <v>45818.30489300891</v>
+        <v>45818.80148694293</v>
       </c>
       <c r="E274">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F274" s="2">
-        <v>45817.73993055556</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G274">
         <v>0</v>
@@ -7310,16 +7310,16 @@
         <v>1</v>
       </c>
       <c r="C283">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D283" s="2">
-        <v>45813.95785150164</v>
+        <v>45818.80148693536</v>
       </c>
       <c r="E283">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F283" s="2">
-        <v>45813.65701388889</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G283">
         <v>0</v>
@@ -7509,16 +7509,16 @@
         <v>1</v>
       </c>
       <c r="C291">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D291" s="2">
-        <v>45816.01481442774</v>
+        <v>45818.80148694325</v>
       </c>
       <c r="E291">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="F291" s="2">
-        <v>45815.96244212963</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G291">
         <v>0</v>
@@ -7610,16 +7610,16 @@
         <v>1</v>
       </c>
       <c r="C295">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="D295" s="2">
-        <v>45818.30489302766</v>
+        <v>45818.80148693572</v>
       </c>
       <c r="E295">
-        <v>354</v>
+        <v>288</v>
       </c>
       <c r="F295" s="2">
-        <v>45817.7559837963</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G295">
         <v>0</v>
@@ -7953,16 +7953,16 @@
         <v>1</v>
       </c>
       <c r="C309">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="D309" s="2">
-        <v>45818.30486081876</v>
+        <v>45818.80148693619</v>
       </c>
       <c r="E309">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="F309" s="2">
-        <v>45817.43152777778</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G309">
         <v>0</v>
@@ -8374,16 +8374,16 @@
         <v>1</v>
       </c>
       <c r="C326">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D326" s="2">
-        <v>45818.30486081776</v>
+        <v>45818.80148693661</v>
       </c>
       <c r="E326">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F326" s="2">
-        <v>45817.42730324074</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G326">
         <v>0</v>
@@ -8772,16 +8772,16 @@
         <v>1</v>
       </c>
       <c r="C342">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="D342" s="2">
-        <v>45813.95785146693</v>
+        <v>45818.80148694019</v>
       </c>
       <c r="E342">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="F342" s="2">
-        <v>45813.57616898148</v>
+        <v>45818.53353009259</v>
       </c>
       <c r="G342">
         <v>0</v>
@@ -9839,16 +9839,16 @@
         <v>1</v>
       </c>
       <c r="C385">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D385" s="2">
-        <v>45814.82978481724</v>
+        <v>45818.80148694391</v>
       </c>
       <c r="E385">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F385" s="2">
-        <v>45814.74193287037</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G385">
         <v>0</v>
@@ -10673,16 +10673,16 @@
         <v>1</v>
       </c>
       <c r="C418">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D418" s="2">
-        <v>45818.30489300957</v>
+        <v>45818.80148693696</v>
       </c>
       <c r="E418">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F418" s="2">
-        <v>45817.73993055556</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G418">
         <v>0</v>
@@ -12951,16 +12951,16 @@
         <v>1</v>
       </c>
       <c r="C510">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D510" s="2">
-        <v>45818.30489302096</v>
+        <v>45818.80148693114</v>
       </c>
       <c r="E510">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F510" s="2">
-        <v>45817.7553587963</v>
+        <v>45818.40175925926</v>
       </c>
       <c r="G510">
         <v>0</v>
@@ -13643,16 +13643,16 @@
         <v>1</v>
       </c>
       <c r="C538">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="D538" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.8014869473</v>
       </c>
       <c r="E538">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="F538" s="2">
-        <v>45811.45587962963</v>
+        <v>45818.704375</v>
       </c>
       <c r="G538">
         <v>0</v>
@@ -13744,16 +13744,16 @@
         <v>1</v>
       </c>
       <c r="C542">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D542" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.80148694778</v>
       </c>
       <c r="E542">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F542" s="2">
-        <v>45811.50252314815</v>
+        <v>45818.704375</v>
       </c>
       <c r="G542">
         <v>0</v>
@@ -14389,16 +14389,16 @@
         <v>1</v>
       </c>
       <c r="C569">
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="D569" s="2">
-        <v>45818.30489301023</v>
+        <v>45818.80148694661</v>
       </c>
       <c r="E569">
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="F569" s="2">
-        <v>45817.73993055556</v>
+        <v>45818.66094907407</v>
       </c>
       <c r="G569">
         <v>0</v>
@@ -14415,16 +14415,16 @@
         <v>1</v>
       </c>
       <c r="C570">
-        <v>2624</v>
+        <v>2622</v>
       </c>
       <c r="D570" s="2">
-        <v>45814.82968397064</v>
+        <v>45818.80148693728</v>
       </c>
       <c r="E570">
-        <v>2624</v>
+        <v>2622</v>
       </c>
       <c r="F570" s="2">
-        <v>45817.66995370371</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G570">
         <v>0</v>
@@ -15878,16 +15878,16 @@
         <v>1</v>
       </c>
       <c r="C631">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D631" s="2">
-        <v>45814.82974449309</v>
+        <v>45818.80148694831</v>
       </c>
       <c r="E631">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F631" s="2">
-        <v>45814.6853587963</v>
+        <v>45818.704375</v>
       </c>
       <c r="G631">
         <v>0</v>
@@ -17143,16 +17143,16 @@
         <v>1</v>
       </c>
       <c r="C683">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D683" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.80148694866</v>
       </c>
       <c r="E683">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F683" s="2">
-        <v>45811.45587962963</v>
+        <v>45818.704375</v>
       </c>
       <c r="G683">
         <v>0</v>
@@ -17342,16 +17342,16 @@
         <v>1</v>
       </c>
       <c r="C691">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D691" s="2">
-        <v>45814.82972452114</v>
+        <v>45818.80148693761</v>
       </c>
       <c r="E691">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F691" s="2">
-        <v>45814.61704861111</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G691">
         <v>0</v>
@@ -19154,16 +19154,16 @@
         <v>1</v>
       </c>
       <c r="C763">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D763" s="2">
-        <v>45818.30486082933</v>
+        <v>45818.80148694425</v>
       </c>
       <c r="E763">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F763" s="2">
-        <v>45817.49925925926</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G763">
         <v>0</v>
@@ -21363,16 +21363,16 @@
         <v>1</v>
       </c>
       <c r="C852">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="D852" s="2">
-        <v>45812.78301983239</v>
+        <v>45818.80148693794</v>
       </c>
       <c r="E852">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="F852" s="2">
-        <v>45812.471875</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G852">
         <v>0</v>
@@ -22145,16 +22145,16 @@
         <v>1</v>
       </c>
       <c r="C883">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D883" s="2">
-        <v>45814.82968397064</v>
+        <v>45818.80148694458</v>
       </c>
       <c r="E883">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F883" s="2">
-        <v>45817.66995370371</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G883">
         <v>0</v>
@@ -22350,16 +22350,16 @@
         <v>1</v>
       </c>
       <c r="C891">
-        <v>0</v>
+        <v>-80</v>
       </c>
       <c r="D891" s="2">
-        <v>45799.895451121</v>
+        <v>45818.80148694057</v>
       </c>
       <c r="E891">
-        <v>0</v>
+        <v>-80</v>
       </c>
       <c r="F891" s="2">
-        <v>45799.4196875</v>
+        <v>45818.53353009259</v>
       </c>
       <c r="G891">
         <v>0</v>
@@ -22552,16 +22552,16 @@
         <v>1</v>
       </c>
       <c r="C899">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D899" s="2">
-        <v>45795.04208095842</v>
+        <v>45818.80148694901</v>
       </c>
       <c r="E899">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F899" s="2">
-        <v>45763.62788194444</v>
+        <v>45818.704375</v>
       </c>
       <c r="G899">
         <v>0</v>
@@ -23161,16 +23161,16 @@
         <v>1</v>
       </c>
       <c r="C923">
-        <v>378</v>
+        <v>328</v>
       </c>
       <c r="D923" s="2">
-        <v>45814.82970463676</v>
+        <v>45818.80148693373</v>
       </c>
       <c r="E923">
-        <v>378</v>
+        <v>328</v>
       </c>
       <c r="F923" s="2">
-        <v>45814.38376157408</v>
+        <v>45818.42027777778</v>
       </c>
       <c r="G923">
         <v>0</v>
@@ -24263,16 +24263,16 @@
         <v>1</v>
       </c>
       <c r="C967">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D967" s="2">
-        <v>45795.04199234088</v>
+        <v>45818.80148695403</v>
       </c>
       <c r="E967">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F967" s="2">
-        <v>45708.74841435185</v>
+        <v>45818.704375</v>
       </c>
       <c r="G967">
         <v>0</v>
@@ -24390,16 +24390,16 @@
         <v>1</v>
       </c>
       <c r="C972">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D972" s="2">
-        <v>45818.30486082585</v>
+        <v>45818.80148694938</v>
       </c>
       <c r="E972">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F972" s="2">
-        <v>45817.49490740741</v>
+        <v>45818.704375</v>
       </c>
       <c r="G972">
         <v>0</v>
@@ -25155,16 +25155,16 @@
         <v>1</v>
       </c>
       <c r="C1002">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="D1002" s="2">
-        <v>45814.82980241515</v>
+        <v>45818.80148695243</v>
       </c>
       <c r="E1002">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="F1002" s="2">
-        <v>45814.49446759259</v>
+        <v>45818.71809027778</v>
       </c>
       <c r="G1002">
         <v>0</v>
@@ -26676,16 +26676,16 @@
         <v>1</v>
       </c>
       <c r="C1062">
-        <v>656</v>
+        <v>617</v>
       </c>
       <c r="D1062" s="2">
-        <v>45818.30489302317</v>
+        <v>45818.80148693828</v>
       </c>
       <c r="E1062">
-        <v>656</v>
+        <v>617</v>
       </c>
       <c r="F1062" s="2">
-        <v>45817.7553587963</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G1062">
         <v>0</v>
@@ -28173,16 +28173,16 @@
         <v>1</v>
       </c>
       <c r="C1122">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1122" s="2">
-        <v>45818.30489300424</v>
+        <v>45818.80148695171</v>
       </c>
       <c r="E1122">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1122" s="2">
-        <v>45817.71056712963</v>
+        <v>45818.7134375</v>
       </c>
       <c r="G1122">
         <v>0</v>
@@ -28453,16 +28453,16 @@
         <v>1</v>
       </c>
       <c r="C1133">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D1133" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.80148694971</v>
       </c>
       <c r="E1133">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F1133" s="2">
-        <v>45811.50125</v>
+        <v>45818.704375</v>
       </c>
       <c r="G1133">
         <v>0</v>
@@ -29013,16 +29013,16 @@
         <v>1</v>
       </c>
       <c r="C1155">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1155" s="2">
-        <v>45818.30489300488</v>
+        <v>45818.80148695005</v>
       </c>
       <c r="E1155">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1155" s="2">
-        <v>45817.71056712963</v>
+        <v>45818.704375</v>
       </c>
       <c r="G1155">
         <v>0</v>
@@ -29521,16 +29521,16 @@
         <v>1</v>
       </c>
       <c r="C1175">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="D1175" s="2">
-        <v>45812.78301983239</v>
+        <v>45818.80148695334</v>
       </c>
       <c r="E1175">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="F1175" s="2">
-        <v>45812.43199074074</v>
+        <v>45818.7203125</v>
       </c>
       <c r="G1175">
         <v>0</v>
@@ -29830,16 +29830,16 @@
         <v>1</v>
       </c>
       <c r="C1187">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D1187" s="2">
-        <v>45813.9578819583</v>
+        <v>45818.80148694491</v>
       </c>
       <c r="E1187">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F1187" s="2">
-        <v>45813.67818287037</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G1187">
         <v>0</v>
@@ -30734,16 +30734,16 @@
         <v>1</v>
       </c>
       <c r="C1222">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D1222" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.8014869315</v>
       </c>
       <c r="E1222">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F1222" s="2">
-        <v>45811.66614583333</v>
+        <v>45818.40175925926</v>
       </c>
       <c r="G1222">
         <v>0</v>
@@ -30887,16 +30887,16 @@
         <v>1</v>
       </c>
       <c r="C1228">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1228" s="2">
-        <v>45799.8954032937</v>
+        <v>45818.80148693191</v>
       </c>
       <c r="E1228">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1228" s="2">
-        <v>45799.43015046296</v>
+        <v>45818.40175925926</v>
       </c>
       <c r="G1228">
         <v>0</v>
@@ -31372,16 +31372,16 @@
         <v>1</v>
       </c>
       <c r="C1247">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D1247" s="2">
-        <v>45818.30486081455</v>
+        <v>45818.80148693859</v>
       </c>
       <c r="E1247">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F1247" s="2">
-        <v>45817.39020833333</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G1247">
         <v>0</v>
@@ -31528,16 +31528,16 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>22</v>
+        <v>-28</v>
       </c>
       <c r="D1253" s="2">
-        <v>45818.30489301086</v>
+        <v>45818.80148693892</v>
       </c>
       <c r="E1253">
-        <v>22</v>
+        <v>-28</v>
       </c>
       <c r="F1253" s="2">
-        <v>45817.73993055556</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G1253">
         <v>0</v>
@@ -32299,16 +32299,16 @@
         <v>1</v>
       </c>
       <c r="C1283">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="D1283" s="2">
-        <v>45813.95793319555</v>
+        <v>45818.8014869504</v>
       </c>
       <c r="E1283">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="F1283" s="2">
-        <v>45813.71038194445</v>
+        <v>45818.704375</v>
       </c>
       <c r="G1283">
         <v>0</v>
@@ -33358,16 +33358,16 @@
         <v>1</v>
       </c>
       <c r="C1325">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D1325" s="2">
-        <v>45799.8954032937</v>
+        <v>45818.80148695073</v>
       </c>
       <c r="E1325">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F1325" s="2">
-        <v>45106.65594907408</v>
+        <v>45818.704375</v>
       </c>
       <c r="G1325">
         <v>0</v>
@@ -33791,16 +33791,16 @@
         <v>1</v>
       </c>
       <c r="C1342">
-        <v>1184</v>
+        <v>1040</v>
       </c>
       <c r="D1342" s="2">
-        <v>45818.30486081507</v>
+        <v>45818.80148693925</v>
       </c>
       <c r="E1342">
-        <v>1184</v>
+        <v>1040</v>
       </c>
       <c r="F1342" s="2">
-        <v>45817.39020833333</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G1342">
         <v>0</v>
@@ -38040,16 +38040,16 @@
         <v>1</v>
       </c>
       <c r="C1509">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="D1509" s="2">
-        <v>45814.82980241515</v>
+        <v>45818.80148695368</v>
       </c>
       <c r="E1509">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="F1509" s="2">
-        <v>45814.49446759259</v>
+        <v>45818.72087962963</v>
       </c>
       <c r="G1509">
         <v>0</v>
@@ -39701,16 +39701,16 @@
         <v>1</v>
       </c>
       <c r="C1576">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1576" s="2">
-        <v>45811.92549991595</v>
+        <v>45818.80148693236</v>
       </c>
       <c r="E1576">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F1576" s="2">
-        <v>45811.72346064815</v>
+        <v>45818.40175925926</v>
       </c>
       <c r="G1576">
         <v>0</v>
@@ -40223,16 +40223,16 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>5675</v>
+        <v>5653</v>
       </c>
       <c r="D1597" s="2">
-        <v>45818.30489303058</v>
+        <v>45818.80148694525</v>
       </c>
       <c r="E1597">
-        <v>5675</v>
+        <v>5653</v>
       </c>
       <c r="F1597" s="2">
-        <v>45817.7559837963</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G1597">
         <v>0</v>
@@ -40298,16 +40298,16 @@
         <v>1</v>
       </c>
       <c r="C1600">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1600" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.80148693273</v>
       </c>
       <c r="E1600">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1600" s="2">
-        <v>45811.44629629629</v>
+        <v>45818.40175925926</v>
       </c>
       <c r="G1600">
         <v>0</v>
@@ -48639,16 +48639,16 @@
         <v>1</v>
       </c>
       <c r="C1932">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D1932" s="2">
-        <v>45795.04210567895</v>
+        <v>45818.80148694559</v>
       </c>
       <c r="E1932">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F1932" s="2">
-        <v>45776.66952546296</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G1932">
         <v>0</v>
@@ -48691,16 +48691,16 @@
         <v>1</v>
       </c>
       <c r="C1934">
-        <v>-9</v>
+        <v>21</v>
       </c>
       <c r="D1934" s="2">
-        <v>45818.30489299967</v>
+        <v>45818.80148694627</v>
       </c>
       <c r="E1934">
-        <v>-9</v>
+        <v>21</v>
       </c>
       <c r="F1934" s="2">
-        <v>45817.69565972222</v>
+        <v>45818.65571759259</v>
       </c>
       <c r="G1934">
         <v>0</v>
@@ -50883,16 +50883,16 @@
         <v>1</v>
       </c>
       <c r="C2022">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2022" s="2">
-        <v>45799.89545110933</v>
+        <v>45818.80148693304</v>
       </c>
       <c r="E2022">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2022" s="2">
-        <v>45785.70503472222</v>
+        <v>45818.40175925926</v>
       </c>
       <c r="G2022">
         <v>0</v>
@@ -50909,16 +50909,16 @@
         <v>1</v>
       </c>
       <c r="C2023">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D2023" s="2">
-        <v>45811.92546678011</v>
+        <v>45818.80148694593</v>
       </c>
       <c r="E2023">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F2023" s="2">
-        <v>45812.67899305555</v>
+        <v>45818.65388888889</v>
       </c>
       <c r="G2023">
         <v>0</v>
@@ -52372,16 +52372,16 @@
         <v>1</v>
       </c>
       <c r="C2081">
-        <v>0</v>
+        <v>-12</v>
       </c>
       <c r="D2081" s="2">
-        <v>45795.04177855738</v>
+        <v>45818.80148695105</v>
       </c>
       <c r="E2081">
-        <v>0</v>
+        <v>-12</v>
       </c>
       <c r="F2081" s="2">
-        <v>45518.74190972222</v>
+        <v>45818.704375</v>
       </c>
       <c r="G2081">
         <v>0</v>
@@ -60767,16 +60767,16 @@
         <v>1</v>
       </c>
       <c r="C2416">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D2416" s="2">
-        <v>45818.30486081559</v>
+        <v>45818.80148693962</v>
       </c>
       <c r="E2416">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F2416" s="2">
-        <v>45817.39020833333</v>
+        <v>45818.46909722222</v>
       </c>
       <c r="G2416">
         <v>0</v>
@@ -64314,6 +64314,9 @@
       <c r="E2561">
         <v>0</v>
       </c>
+      <c r="F2561" s="2">
+        <v>45818.63560185185</v>
+      </c>
       <c r="G2561">
         <v>0</v>
       </c>
@@ -64336,6 +64339,9 @@
       </c>
       <c r="E2562">
         <v>0</v>
+      </c>
+      <c r="F2562" s="2">
+        <v>45818.63516203704</v>
       </c>
       <c r="G2562">
         <v>0</v>

</xml_diff>

<commit_message>
atualizei dados bibi e add
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2596" uniqueCount="10">
   <si>
     <t>id_produto</t>
   </si>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2586"/>
+  <dimension ref="A1:H2589"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,16 +494,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="D4" s="2">
-        <v>45832.99937861314</v>
+        <v>45833.77620284099</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="F4" s="2">
-        <v>45832.4265162037</v>
+        <v>45833.69550925926</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -520,16 +520,16 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2">
-        <v>45831.83463792984</v>
+        <v>45833.77620283774</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F5" s="2">
-        <v>45831.81263888889</v>
+        <v>45833.59693287037</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -690,16 +690,16 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2">
-        <v>45832.99937863887</v>
+        <v>45833.77620284134</v>
       </c>
       <c r="E12">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="2">
-        <v>45832.75739583333</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -978,16 +978,16 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D24" s="2">
-        <v>45829.29943059705</v>
+        <v>45833.77618177847</v>
       </c>
       <c r="E24">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F24" s="2">
-        <v>45828.52178240741</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1194,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>2851</v>
+        <v>2831</v>
       </c>
       <c r="D33" s="2">
-        <v>45832.99937862625</v>
+        <v>45833.77620283895</v>
       </c>
       <c r="E33">
-        <v>2851</v>
+        <v>2831</v>
       </c>
       <c r="F33" s="2">
-        <v>45832.55858796297</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1765,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>339</v>
+        <v>297</v>
       </c>
       <c r="D56" s="2">
-        <v>45832.99937862444</v>
+        <v>45833.77620284142</v>
       </c>
       <c r="E56">
-        <v>339</v>
+        <v>297</v>
       </c>
       <c r="F56" s="2">
-        <v>45832.50936342592</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -1817,16 +1817,16 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D58" s="2">
-        <v>45832.99935919302</v>
+        <v>45833.77620284149</v>
       </c>
       <c r="E58">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F58" s="2">
-        <v>45832.40921296296</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -1843,16 +1843,16 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="D59" s="2">
-        <v>45825.8270770669</v>
+        <v>45833.77618177872</v>
       </c>
       <c r="E59">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="F59" s="2">
-        <v>45825.61604166667</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -1892,16 +1892,16 @@
         <v>1</v>
       </c>
       <c r="C61">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D61" s="2">
-        <v>45831.31672868288</v>
+        <v>45834.28681886554</v>
       </c>
       <c r="E61">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F61" s="2">
-        <v>45829.58444444444</v>
+        <v>45833.87444444445</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -1941,16 +1941,16 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D63" s="2">
-        <v>45831.83461824944</v>
+        <v>45833.77620283903</v>
       </c>
       <c r="E63">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F63" s="2">
-        <v>45831.63957175926</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2088,16 +2088,16 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>-3</v>
+        <v>33</v>
       </c>
       <c r="D69" s="2">
-        <v>45832.99937862792</v>
+        <v>45833.77618177396</v>
       </c>
       <c r="E69">
-        <v>-3</v>
+        <v>33</v>
       </c>
       <c r="F69" s="2">
-        <v>45832.61931712963</v>
+        <v>45833.47572916667</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -2114,16 +2114,16 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D70" s="2">
-        <v>45831.83463792157</v>
+        <v>45833.77618177376</v>
       </c>
       <c r="E70">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="F70" s="2">
-        <v>45831.81081018518</v>
+        <v>45833.47356481481</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2376,16 +2376,16 @@
         <v>1</v>
       </c>
       <c r="C81">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D81" s="2">
-        <v>45831.83463791914</v>
+        <v>45833.77620283993</v>
       </c>
       <c r="E81">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F81" s="2">
-        <v>45831.73116898148</v>
+        <v>45833.68471064815</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -2428,16 +2428,16 @@
         <v>1</v>
       </c>
       <c r="C83">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D83" s="2">
-        <v>45832.99935919479</v>
+        <v>45833.77618176836</v>
       </c>
       <c r="E83">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F83" s="2">
-        <v>45832.42351851852</v>
+        <v>45833.39194444445</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -2529,16 +2529,16 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D87" s="2">
-        <v>45832.99937862293</v>
+        <v>45833.77618176855</v>
       </c>
       <c r="E87">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F87" s="2">
-        <v>45832.44876157407</v>
+        <v>45833.39194444445</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -2630,16 +2630,16 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D91" s="2">
-        <v>45825.82710087817</v>
+        <v>45833.77618176876</v>
       </c>
       <c r="E91">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F91" s="2">
-        <v>45825.6681712963</v>
+        <v>45833.39194444445</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -2702,16 +2702,16 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="D94" s="2">
-        <v>45832.99937862756</v>
+        <v>45833.77620284</v>
       </c>
       <c r="E94">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="F94" s="2">
-        <v>45832.60596064815</v>
+        <v>45833.68471064815</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -2872,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>2850</v>
+        <v>2796</v>
       </c>
       <c r="D101" s="2">
-        <v>45832.99937863777</v>
+        <v>45833.77620284156</v>
       </c>
       <c r="E101">
-        <v>2850</v>
+        <v>2796</v>
       </c>
       <c r="F101" s="2">
-        <v>45832.73863425926</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -3258,16 +3258,16 @@
         <v>1</v>
       </c>
       <c r="C117">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="D117" s="2">
-        <v>45831.83461824039</v>
+        <v>45833.7761817699</v>
       </c>
       <c r="E117">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="F117" s="2">
-        <v>45831.47940972223</v>
+        <v>45833.42523148148</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -3359,16 +3359,16 @@
         <v>1</v>
       </c>
       <c r="C121">
-        <v>649</v>
+        <v>638</v>
       </c>
       <c r="D121" s="2">
-        <v>45832.99935919538</v>
+        <v>45833.7761817701</v>
       </c>
       <c r="E121">
-        <v>649</v>
+        <v>638</v>
       </c>
       <c r="F121" s="2">
-        <v>45832.42351851852</v>
+        <v>45833.42523148148</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -3408,16 +3408,16 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>437</v>
+        <v>416</v>
       </c>
       <c r="D123" s="2">
-        <v>45832.99935918899</v>
+        <v>45833.77618177892</v>
       </c>
       <c r="E123">
-        <v>437</v>
+        <v>416</v>
       </c>
       <c r="F123" s="2">
-        <v>45832.385</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -3434,16 +3434,16 @@
         <v>1</v>
       </c>
       <c r="C124">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D124" s="2">
-        <v>45831.83461825257</v>
+        <v>45833.77618177133</v>
       </c>
       <c r="E124">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F124" s="2">
-        <v>45831.67700231481</v>
+        <v>45833.42833333334</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -3460,16 +3460,16 @@
         <v>1</v>
       </c>
       <c r="C125">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D125" s="2">
-        <v>45832.99935919566</v>
+        <v>45833.77620283911</v>
       </c>
       <c r="E125">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F125" s="2">
-        <v>45832.42351851852</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -3486,16 +3486,16 @@
         <v>1</v>
       </c>
       <c r="C126">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D126" s="2">
-        <v>45831.83461825048</v>
+        <v>45834.28681886589</v>
       </c>
       <c r="E126">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="F126" s="2">
-        <v>45831.67092592592</v>
+        <v>45833.8759375</v>
       </c>
       <c r="G126">
         <v>0</v>
@@ -3846,16 +3846,16 @@
         <v>1</v>
       </c>
       <c r="C141">
-        <v>376</v>
+        <v>357</v>
       </c>
       <c r="D141" s="2">
-        <v>45831.83463791714</v>
+        <v>45833.77620284037</v>
       </c>
       <c r="E141">
-        <v>376</v>
+        <v>357</v>
       </c>
       <c r="F141" s="2">
-        <v>45831.69412037037</v>
+        <v>45833.68996527778</v>
       </c>
       <c r="G141">
         <v>0</v>
@@ -3950,16 +3950,16 @@
         <v>1</v>
       </c>
       <c r="C145">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D145" s="2">
-        <v>45827.49773230286</v>
+        <v>45833.77620284045</v>
       </c>
       <c r="E145">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F145" s="2">
-        <v>45827.44425925926</v>
+        <v>45833.68996527778</v>
       </c>
       <c r="G145">
         <v>0</v>
@@ -4345,16 +4345,16 @@
         <v>1</v>
       </c>
       <c r="C161">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D161" s="2">
-        <v>45829.29943060024</v>
+        <v>45833.77620284128</v>
       </c>
       <c r="E161">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F161" s="2">
-        <v>45828.62064814815</v>
+        <v>45833.73408564815</v>
       </c>
       <c r="G161">
         <v>0</v>
@@ -4397,16 +4397,16 @@
         <v>1</v>
       </c>
       <c r="C163">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D163" s="2">
-        <v>45831.8346182506</v>
+        <v>45833.77618177913</v>
       </c>
       <c r="E163">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F163" s="2">
-        <v>45831.67092592592</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G163">
         <v>0</v>
@@ -5449,16 +5449,16 @@
         <v>1</v>
       </c>
       <c r="C206">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D206" s="2">
-        <v>45831.83463792224</v>
+        <v>45833.77620284163</v>
       </c>
       <c r="E206">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F206" s="2">
-        <v>45831.81081018518</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G206">
         <v>0</v>
@@ -5521,16 +5521,16 @@
         <v>1</v>
       </c>
       <c r="C209">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D209" s="2">
-        <v>45832.99937862316</v>
+        <v>45833.77618177226</v>
       </c>
       <c r="E209">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F209" s="2">
-        <v>45832.44876157407</v>
+        <v>45833.44604166667</v>
       </c>
       <c r="G209">
         <v>0</v>
@@ -5711,16 +5711,16 @@
         <v>1</v>
       </c>
       <c r="C217">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="D217" s="2">
-        <v>45832.99937863368</v>
+        <v>45833.77620283873</v>
       </c>
       <c r="E217">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="F217" s="2">
-        <v>45832.66791666667</v>
+        <v>45833.66048611111</v>
       </c>
       <c r="G217">
         <v>0</v>
@@ -7045,16 +7045,16 @@
         <v>1</v>
       </c>
       <c r="C272">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="D272" s="2">
-        <v>45827.49771214504</v>
+        <v>45833.77618177247</v>
       </c>
       <c r="E272">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="F272" s="2">
-        <v>45826.54380787037</v>
+        <v>45833.44604166667</v>
       </c>
       <c r="G272">
         <v>0</v>
@@ -7071,16 +7071,16 @@
         <v>1</v>
       </c>
       <c r="C273">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D273" s="2">
-        <v>45831.83463792867</v>
+        <v>45833.77620283919</v>
       </c>
       <c r="E273">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F273" s="2">
-        <v>45831.81233796296</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G273">
         <v>0</v>
@@ -7097,16 +7097,16 @@
         <v>1</v>
       </c>
       <c r="C274">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D274" s="2">
-        <v>45832.99937863346</v>
+        <v>45833.77618177416</v>
       </c>
       <c r="E274">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F274" s="2">
-        <v>45832.66299768518</v>
+        <v>45833.48585648148</v>
       </c>
       <c r="G274">
         <v>0</v>
@@ -7261,16 +7261,16 @@
         <v>1</v>
       </c>
       <c r="C281">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D281" s="2">
-        <v>45832.99937861747</v>
+        <v>45833.77618177698</v>
       </c>
       <c r="E281">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="F281" s="2">
-        <v>45832.435625</v>
+        <v>45833.52773148148</v>
       </c>
       <c r="G281">
         <v>0</v>
@@ -7310,16 +7310,16 @@
         <v>1</v>
       </c>
       <c r="C283">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D283" s="2">
-        <v>45832.99935918979</v>
+        <v>45833.77618177031</v>
       </c>
       <c r="E283">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F283" s="2">
-        <v>45832.385</v>
+        <v>45833.42523148148</v>
       </c>
       <c r="G283">
         <v>0</v>
@@ -7509,16 +7509,16 @@
         <v>1</v>
       </c>
       <c r="C291">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="D291" s="2">
-        <v>45831.83461825269</v>
+        <v>45833.77620284171</v>
       </c>
       <c r="E291">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="F291" s="2">
-        <v>45831.67700231481</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G291">
         <v>0</v>
@@ -7535,16 +7535,16 @@
         <v>1</v>
       </c>
       <c r="C292">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D292" s="2">
-        <v>45831.83461825179</v>
+        <v>45833.77620284052</v>
       </c>
       <c r="E292">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F292" s="2">
-        <v>45831.67487268519</v>
+        <v>45833.68996527778</v>
       </c>
       <c r="G292">
         <v>0</v>
@@ -7610,16 +7610,16 @@
         <v>1</v>
       </c>
       <c r="C295">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D295" s="2">
-        <v>45832.99935919787</v>
+        <v>45833.77618177933</v>
       </c>
       <c r="E295">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F295" s="2">
-        <v>45832.42388888889</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G295">
         <v>0</v>
@@ -7904,16 +7904,16 @@
         <v>1</v>
       </c>
       <c r="C307">
-        <v>-5</v>
+        <v>15</v>
       </c>
       <c r="D307" s="2">
-        <v>45832.99937863387</v>
+        <v>45833.77618177206</v>
       </c>
       <c r="E307">
-        <v>-5</v>
+        <v>15</v>
       </c>
       <c r="F307" s="2">
-        <v>45832.66791666667</v>
+        <v>45833.44583333333</v>
       </c>
       <c r="G307">
         <v>0</v>
@@ -7953,16 +7953,16 @@
         <v>1</v>
       </c>
       <c r="C309">
-        <v>987</v>
+        <v>981</v>
       </c>
       <c r="D309" s="2">
-        <v>45825.82710088014</v>
+        <v>45833.77618177718</v>
       </c>
       <c r="E309">
-        <v>987</v>
+        <v>981</v>
       </c>
       <c r="F309" s="2">
-        <v>45825.69407407408</v>
+        <v>45833.53011574074</v>
       </c>
       <c r="G309">
         <v>0</v>
@@ -8426,16 +8426,16 @@
         <v>1</v>
       </c>
       <c r="C328">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="D328" s="2">
-        <v>45828.40527173349</v>
+        <v>45833.77620283881</v>
       </c>
       <c r="E328">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F328" s="2">
-        <v>45827.86532407408</v>
+        <v>45833.66048611111</v>
       </c>
       <c r="G328">
         <v>0</v>
@@ -8570,16 +8570,16 @@
         <v>1</v>
       </c>
       <c r="C334">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D334" s="2">
-        <v>45811.92544186871</v>
+        <v>45833.77618177437</v>
       </c>
       <c r="E334">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F334" s="2">
-        <v>45811.42236111111</v>
+        <v>45833.48585648148</v>
       </c>
       <c r="G334">
         <v>0</v>
@@ -8870,16 +8870,16 @@
         <v>1</v>
       </c>
       <c r="C346">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D346" s="2">
-        <v>45832.99937862861</v>
+        <v>45833.77618177954</v>
       </c>
       <c r="E346">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F346" s="2">
-        <v>45832.61931712963</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G346">
         <v>0</v>
@@ -8991,16 +8991,16 @@
         <v>1</v>
       </c>
       <c r="C351">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="D351" s="2">
-        <v>45831.83461825296</v>
+        <v>45833.77618177974</v>
       </c>
       <c r="E351">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="F351" s="2">
-        <v>45831.67700231481</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G351">
         <v>0</v>
@@ -9164,16 +9164,16 @@
         <v>1</v>
       </c>
       <c r="C358">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D358" s="2">
-        <v>45832.9993786354</v>
+        <v>45833.77618177677</v>
       </c>
       <c r="E358">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="F358" s="2">
-        <v>45832.71763888889</v>
+        <v>45833.52721064815</v>
       </c>
       <c r="G358">
         <v>0</v>
@@ -9242,16 +9242,16 @@
         <v>1</v>
       </c>
       <c r="C361">
-        <v>499</v>
+        <v>449</v>
       </c>
       <c r="D361" s="2">
-        <v>45832.99935918798</v>
+        <v>45833.77620284179</v>
       </c>
       <c r="E361">
-        <v>499</v>
+        <v>449</v>
       </c>
       <c r="F361" s="2">
-        <v>45831.91774305556</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G361">
         <v>0</v>
@@ -9291,16 +9291,16 @@
         <v>1</v>
       </c>
       <c r="C363">
-        <v>538</v>
+        <v>518</v>
       </c>
       <c r="D363" s="2">
-        <v>45831.83463792886</v>
+        <v>45833.77618177994</v>
       </c>
       <c r="E363">
-        <v>538</v>
+        <v>518</v>
       </c>
       <c r="F363" s="2">
-        <v>45831.81233796296</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G363">
         <v>0</v>
@@ -9487,16 +9487,16 @@
         <v>1</v>
       </c>
       <c r="C371">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D371" s="2">
-        <v>45832.9993591962</v>
+        <v>45833.77618177456</v>
       </c>
       <c r="E371">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F371" s="2">
-        <v>45832.42351851852</v>
+        <v>45833.48585648148</v>
       </c>
       <c r="G371">
         <v>0</v>
@@ -9692,16 +9692,16 @@
         <v>1</v>
       </c>
       <c r="C379">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D379" s="2">
-        <v>45831.83459785258</v>
+        <v>45833.77620283888</v>
       </c>
       <c r="E379">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F379" s="2">
-        <v>45831.4337962963</v>
+        <v>45833.66048611111</v>
       </c>
       <c r="G379">
         <v>0</v>
@@ -9865,16 +9865,16 @@
         <v>1</v>
       </c>
       <c r="C386">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D386" s="2">
-        <v>45828.40527173226</v>
+        <v>45833.77618178015</v>
       </c>
       <c r="E386">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F386" s="2">
-        <v>45827.60001157408</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G386">
         <v>0</v>
@@ -9969,16 +9969,16 @@
         <v>1</v>
       </c>
       <c r="C390">
-        <v>-4</v>
+        <v>7</v>
       </c>
       <c r="D390" s="2">
-        <v>45831.83463793078</v>
+        <v>45833.77618177357</v>
       </c>
       <c r="E390">
-        <v>-4</v>
+        <v>7</v>
       </c>
       <c r="F390" s="2">
-        <v>45831.81263888889</v>
+        <v>45833.45938657408</v>
       </c>
       <c r="G390">
         <v>0</v>
@@ -10070,16 +10070,16 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D394" s="2">
-        <v>45832.99937863841</v>
+        <v>45833.77620284007</v>
       </c>
       <c r="E394">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="F394" s="2">
-        <v>45832.75680555555</v>
+        <v>45833.68471064815</v>
       </c>
       <c r="G394">
         <v>0</v>
@@ -10295,16 +10295,16 @@
         <v>1</v>
       </c>
       <c r="C403">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D403" s="2">
-        <v>45812.78301983239</v>
+        <v>45833.77620284185</v>
       </c>
       <c r="E403">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F403" s="2">
-        <v>45812.32231481482</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G403">
         <v>0</v>
@@ -10321,16 +10321,16 @@
         <v>1</v>
       </c>
       <c r="C404">
-        <v>15</v>
+        <v>-2</v>
       </c>
       <c r="D404" s="2">
-        <v>45831.83461824765</v>
+        <v>45833.77620283926</v>
       </c>
       <c r="E404">
-        <v>15</v>
+        <v>-2</v>
       </c>
       <c r="F404" s="2">
-        <v>45831.53259259259</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G404">
         <v>0</v>
@@ -10771,16 +10771,16 @@
         <v>1</v>
       </c>
       <c r="C422">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="D422" s="2">
-        <v>45825.82707706292</v>
+        <v>45833.77618177052</v>
       </c>
       <c r="E422">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="F422" s="2">
-        <v>45825.49319444445</v>
+        <v>45833.42523148148</v>
       </c>
       <c r="G422">
         <v>0</v>
@@ -11930,16 +11930,16 @@
         <v>1</v>
       </c>
       <c r="C469">
-        <v>3056</v>
+        <v>3046</v>
       </c>
       <c r="D469" s="2">
-        <v>45831.83463792255</v>
+        <v>45833.7762028406</v>
       </c>
       <c r="E469">
-        <v>3056</v>
+        <v>3046</v>
       </c>
       <c r="F469" s="2">
-        <v>45831.81081018518</v>
+        <v>45833.68996527778</v>
       </c>
       <c r="G469">
         <v>0</v>
@@ -12207,16 +12207,16 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D480" s="2">
-        <v>45832.99937863564</v>
+        <v>45833.77618177747</v>
       </c>
       <c r="E480">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F480" s="2">
-        <v>45832.71763888889</v>
+        <v>45833.53011574074</v>
       </c>
       <c r="G480">
         <v>0</v>
@@ -12562,16 +12562,16 @@
         <v>1</v>
       </c>
       <c r="C494">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D494" s="2">
-        <v>45811.92546678011</v>
+        <v>45833.77620284332</v>
       </c>
       <c r="E494">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F494" s="2">
-        <v>45811.50252314815</v>
+        <v>45833.769375</v>
       </c>
       <c r="G494">
         <v>0</v>
@@ -12951,16 +12951,16 @@
         <v>1</v>
       </c>
       <c r="C510">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="D510" s="2">
-        <v>45832.99937862482</v>
+        <v>45833.77620283933</v>
       </c>
       <c r="E510">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="F510" s="2">
-        <v>45832.54928240741</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G510">
         <v>0</v>
@@ -13545,16 +13545,16 @@
         <v>1</v>
       </c>
       <c r="C534">
-        <v>1233</v>
+        <v>1228</v>
       </c>
       <c r="D534" s="2">
-        <v>45831.31672868149</v>
+        <v>45833.77620283941</v>
       </c>
       <c r="E534">
-        <v>1233</v>
+        <v>1228</v>
       </c>
       <c r="F534" s="2">
-        <v>45829.56215277778</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G534">
         <v>0</v>
@@ -13571,16 +13571,16 @@
         <v>1</v>
       </c>
       <c r="C535">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D535" s="2">
-        <v>45831.31672868136</v>
+        <v>45833.77620283949</v>
       </c>
       <c r="E535">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F535" s="2">
-        <v>45824.45626157407</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G535">
         <v>0</v>
@@ -13816,16 +13816,16 @@
         <v>1</v>
       </c>
       <c r="C545">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="D545" s="2">
-        <v>45831.83461825219</v>
+        <v>45833.77618177326</v>
       </c>
       <c r="E545">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="F545" s="2">
-        <v>45831.6752662037</v>
+        <v>45833.45819444444</v>
       </c>
       <c r="G545">
         <v>0</v>
@@ -14389,16 +14389,16 @@
         <v>1</v>
       </c>
       <c r="C569">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D569" s="2">
-        <v>45831.8346379229</v>
+        <v>45833.77620283781</v>
       </c>
       <c r="E569">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F569" s="2">
-        <v>45831.81081018518</v>
+        <v>45833.63289351852</v>
       </c>
       <c r="G569">
         <v>0</v>
@@ -14677,16 +14677,16 @@
         <v>1</v>
       </c>
       <c r="C581">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D581" s="2">
-        <v>45828.40527173851</v>
+        <v>45833.7762028408</v>
       </c>
       <c r="E581">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F581" s="2">
-        <v>45828.41831018519</v>
+        <v>45833.68996527778</v>
       </c>
       <c r="G581">
         <v>0</v>
@@ -15207,16 +15207,16 @@
         <v>1</v>
       </c>
       <c r="C603">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D603" s="2">
-        <v>45829.29943060602</v>
+        <v>45833.77618177637</v>
       </c>
       <c r="E603">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F603" s="2">
-        <v>45828.71103009259</v>
+        <v>45833.515625</v>
       </c>
       <c r="G603">
         <v>0</v>
@@ -15878,16 +15878,16 @@
         <v>1</v>
       </c>
       <c r="C631">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D631" s="2">
-        <v>45827.49773229961</v>
+        <v>45833.77618177476</v>
       </c>
       <c r="E631">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F631" s="2">
-        <v>45826.68226851852</v>
+        <v>45833.48585648148</v>
       </c>
       <c r="G631">
         <v>0</v>
@@ -16509,16 +16509,16 @@
         <v>1</v>
       </c>
       <c r="C657">
-        <v>1887</v>
+        <v>1870</v>
       </c>
       <c r="D657" s="2">
-        <v>45831.83461824778</v>
+        <v>45833.77620284192</v>
       </c>
       <c r="E657">
-        <v>1887</v>
+        <v>1870</v>
       </c>
       <c r="F657" s="2">
-        <v>45831.53259259259</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G657">
         <v>0</v>
@@ -16584,16 +16584,16 @@
         <v>1</v>
       </c>
       <c r="C660">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D660" s="2">
-        <v>45832.99937862932</v>
+        <v>45833.77620284199</v>
       </c>
       <c r="E660">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F660" s="2">
-        <v>45832.61931712963</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G660">
         <v>0</v>
@@ -17143,16 +17143,16 @@
         <v>1</v>
       </c>
       <c r="C683">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D683" s="2">
-        <v>45818.80148694866</v>
+        <v>45833.77618177496</v>
       </c>
       <c r="E683">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F683" s="2">
-        <v>45818.704375</v>
+        <v>45833.48585648148</v>
       </c>
       <c r="G683">
         <v>0</v>
@@ -17342,16 +17342,16 @@
         <v>1</v>
       </c>
       <c r="C691">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D691" s="2">
-        <v>45831.83463791593</v>
+        <v>45833.77618177767</v>
       </c>
       <c r="E691">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F691" s="2">
-        <v>45831.68162037037</v>
+        <v>45833.53011574074</v>
       </c>
       <c r="G691">
         <v>0</v>
@@ -18072,16 +18072,16 @@
         <v>1</v>
       </c>
       <c r="C720">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="D720" s="2">
-        <v>45832.99937863649</v>
+        <v>45833.77618177788</v>
       </c>
       <c r="E720">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="F720" s="2">
-        <v>45832.71763888889</v>
+        <v>45833.53011574074</v>
       </c>
       <c r="G720">
         <v>0</v>
@@ -18228,16 +18228,16 @@
         <v>1</v>
       </c>
       <c r="C726">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D726" s="2">
-        <v>45832.99935919039</v>
+        <v>45833.77618178036</v>
       </c>
       <c r="E726">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F726" s="2">
-        <v>45832.385</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G726">
         <v>0</v>
@@ -18381,16 +18381,16 @@
         <v>1</v>
       </c>
       <c r="C732">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D732" s="2">
-        <v>45831.83463791787</v>
+        <v>45833.77618177808</v>
       </c>
       <c r="E732">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F732" s="2">
-        <v>45831.69412037037</v>
+        <v>45833.53011574074</v>
       </c>
       <c r="G732">
         <v>0</v>
@@ -18560,16 +18560,16 @@
         <v>1</v>
       </c>
       <c r="C739">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D739" s="2">
-        <v>45818.30486084728</v>
+        <v>45833.77618178056</v>
       </c>
       <c r="E739">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F739" s="2">
-        <v>45817.664375</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G739">
         <v>0</v>
@@ -18739,16 +18739,16 @@
         <v>1</v>
       </c>
       <c r="C746">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D746" s="2">
-        <v>45820.9169528116</v>
+        <v>45833.77618177153</v>
       </c>
       <c r="E746">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F746" s="2">
-        <v>45820.4658449074</v>
+        <v>45833.42833333334</v>
       </c>
       <c r="G746">
         <v>0</v>
@@ -19154,16 +19154,16 @@
         <v>1</v>
       </c>
       <c r="C763">
-        <v>-19</v>
+        <v>-29</v>
       </c>
       <c r="D763" s="2">
-        <v>45831.8346182511</v>
+        <v>45833.77618176786</v>
       </c>
       <c r="E763">
-        <v>-19</v>
+        <v>-29</v>
       </c>
       <c r="F763" s="2">
-        <v>45831.67092592592</v>
+        <v>45833.38887731481</v>
       </c>
       <c r="G763">
         <v>0</v>
@@ -19379,16 +19379,16 @@
         <v>1</v>
       </c>
       <c r="C772">
-        <v>362</v>
+        <v>276</v>
       </c>
       <c r="D772" s="2">
-        <v>45831.83463792903</v>
+        <v>45833.77620284207</v>
       </c>
       <c r="E772">
-        <v>362</v>
+        <v>276</v>
       </c>
       <c r="F772" s="2">
-        <v>45831.81233796296</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G772">
         <v>0</v>
@@ -20005,16 +20005,16 @@
         <v>1</v>
       </c>
       <c r="C797">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D797" s="2">
-        <v>45811.92544186871</v>
+        <v>45833.77620284354</v>
       </c>
       <c r="E797">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F797" s="2">
-        <v>45810.78280092592</v>
+        <v>45833.79240740741</v>
       </c>
       <c r="G797">
         <v>0</v>
@@ -20031,16 +20031,16 @@
         <v>1</v>
       </c>
       <c r="C798">
-        <v>-148</v>
+        <v>52</v>
       </c>
       <c r="D798" s="2">
-        <v>45832.99937862425</v>
+        <v>45833.77620284362</v>
       </c>
       <c r="E798">
-        <v>-148</v>
+        <v>52</v>
       </c>
       <c r="F798" s="2">
-        <v>45832.46924768519</v>
+        <v>45833.79266203703</v>
       </c>
       <c r="G798">
         <v>0</v>
@@ -20331,16 +20331,16 @@
         <v>1</v>
       </c>
       <c r="C810">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D810" s="2">
-        <v>45832.99937862956</v>
+        <v>45833.77620283803</v>
       </c>
       <c r="E810">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F810" s="2">
-        <v>45832.61931712963</v>
+        <v>45833.65263888889</v>
       </c>
       <c r="G810">
         <v>0</v>
@@ -20732,16 +20732,16 @@
         <v>1</v>
       </c>
       <c r="C826">
-        <v>-13</v>
+        <v>1</v>
       </c>
       <c r="D826" s="2">
-        <v>45832.99937863479</v>
+        <v>45833.77620284015</v>
       </c>
       <c r="E826">
-        <v>-13</v>
+        <v>1</v>
       </c>
       <c r="F826" s="2">
-        <v>45832.69049768519</v>
+        <v>45833.68471064815</v>
       </c>
       <c r="G826">
         <v>0</v>
@@ -21164,16 +21164,16 @@
         <v>1</v>
       </c>
       <c r="C844">
-        <v>1</v>
+        <v>-11</v>
       </c>
       <c r="D844" s="2">
-        <v>45832.99935918635</v>
+        <v>45833.77620283956</v>
       </c>
       <c r="E844">
-        <v>1</v>
+        <v>-11</v>
       </c>
       <c r="F844" s="2">
-        <v>45831.91517361111</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G844">
         <v>0</v>
@@ -21389,16 +21389,16 @@
         <v>1</v>
       </c>
       <c r="C853">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D853" s="2">
-        <v>45832.99937863926</v>
+        <v>45833.77620284214</v>
       </c>
       <c r="E853">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F853" s="2">
-        <v>45832.7659375</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G853">
         <v>0</v>
@@ -21415,16 +21415,16 @@
         <v>1</v>
       </c>
       <c r="C854">
-        <v>6</v>
+        <v>241</v>
       </c>
       <c r="D854" s="2">
-        <v>45831.83463791619</v>
+        <v>45834.28681886503</v>
       </c>
       <c r="E854">
-        <v>6</v>
+        <v>241</v>
       </c>
       <c r="F854" s="2">
-        <v>45831.68162037037</v>
+        <v>45833.87168981481</v>
       </c>
       <c r="G854">
         <v>0</v>
@@ -22145,16 +22145,16 @@
         <v>1</v>
       </c>
       <c r="C883">
-        <v>398</v>
+        <v>376</v>
       </c>
       <c r="D883" s="2">
-        <v>45831.83461825337</v>
+        <v>45833.77620284105</v>
       </c>
       <c r="E883">
-        <v>398</v>
+        <v>376</v>
       </c>
       <c r="F883" s="2">
-        <v>45831.67700231481</v>
+        <v>45833.69550925926</v>
       </c>
       <c r="G883">
         <v>0</v>
@@ -22226,13 +22226,13 @@
         <v>0</v>
       </c>
       <c r="D886" s="2">
-        <v>45795.04177855738</v>
+        <v>45833.7762028431</v>
       </c>
       <c r="E886">
         <v>0</v>
       </c>
       <c r="F886" s="2">
-        <v>45148.66943287037</v>
+        <v>45833.76693287037</v>
       </c>
       <c r="G886">
         <v>0</v>
@@ -22272,16 +22272,16 @@
         <v>1</v>
       </c>
       <c r="C888">
-        <v>502</v>
+        <v>452</v>
       </c>
       <c r="D888" s="2">
-        <v>45832.99937862339</v>
+        <v>45833.77620284224</v>
       </c>
       <c r="E888">
-        <v>502</v>
+        <v>452</v>
       </c>
       <c r="F888" s="2">
-        <v>45832.44876157407</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G888">
         <v>0</v>
@@ -22298,16 +22298,16 @@
         <v>1</v>
       </c>
       <c r="C889">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D889" s="2">
-        <v>45829.29943059556</v>
+        <v>45833.77618177516</v>
       </c>
       <c r="E889">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F889" s="2">
-        <v>45828.50344907407</v>
+        <v>45833.48585648148</v>
       </c>
       <c r="G889">
         <v>0</v>
@@ -24162,16 +24162,16 @@
         <v>1</v>
       </c>
       <c r="C963">
-        <v>1623</v>
+        <v>1618</v>
       </c>
       <c r="D963" s="2">
-        <v>45831.83463792426</v>
+        <v>45833.77618176898</v>
       </c>
       <c r="E963">
-        <v>1623</v>
+        <v>1618</v>
       </c>
       <c r="F963" s="2">
-        <v>45831.81081018518</v>
+        <v>45833.39194444445</v>
       </c>
       <c r="G963">
         <v>0</v>
@@ -24341,16 +24341,16 @@
         <v>1</v>
       </c>
       <c r="C970">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D970" s="2">
-        <v>45795.04204563411</v>
+        <v>45833.77620284022</v>
       </c>
       <c r="E970">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F970" s="2">
-        <v>45749.50945601852</v>
+        <v>45833.68471064815</v>
       </c>
       <c r="G970">
         <v>0</v>
@@ -25155,16 +25155,16 @@
         <v>1</v>
       </c>
       <c r="C1002">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D1002" s="2">
-        <v>45827.49773229451</v>
+        <v>45833.77618178075</v>
       </c>
       <c r="E1002">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F1002" s="2">
-        <v>45826.55956018518</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G1002">
         <v>0</v>
@@ -25559,16 +25559,16 @@
         <v>1</v>
       </c>
       <c r="C1018">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D1018" s="2">
-        <v>45821.87952450374</v>
+        <v>45834.28681886329</v>
       </c>
       <c r="E1018">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F1018" s="2">
-        <v>45831.52096064815</v>
+        <v>45833.85578703704</v>
       </c>
       <c r="G1018">
         <v>0</v>
@@ -25712,16 +25712,16 @@
         <v>1</v>
       </c>
       <c r="C1024">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D1024" s="2">
-        <v>45828.40527173024</v>
+        <v>45833.77620284279</v>
       </c>
       <c r="E1024">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F1024" s="2">
-        <v>45827.55313657408</v>
+        <v>45833.73675925926</v>
       </c>
       <c r="G1024">
         <v>0</v>
@@ -25738,16 +25738,16 @@
         <v>1</v>
       </c>
       <c r="C1025">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="D1025" s="2">
-        <v>45831.83463792459</v>
+        <v>45833.77620283711</v>
       </c>
       <c r="E1025">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="F1025" s="2">
-        <v>45831.81081018518</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G1025">
         <v>0</v>
@@ -26471,16 +26471,16 @@
         <v>1</v>
       </c>
       <c r="C1054">
-        <v>-8</v>
+        <v>8</v>
       </c>
       <c r="D1054" s="2">
-        <v>45832.99937863693</v>
+        <v>45833.77620283797</v>
       </c>
       <c r="E1054">
-        <v>-8</v>
+        <v>8</v>
       </c>
       <c r="F1054" s="2">
-        <v>45832.71763888889</v>
+        <v>45833.65202546296</v>
       </c>
       <c r="G1054">
         <v>0</v>
@@ -26676,16 +26676,16 @@
         <v>1</v>
       </c>
       <c r="C1062">
-        <v>283</v>
+        <v>258</v>
       </c>
       <c r="D1062" s="2">
-        <v>45832.99937862973</v>
+        <v>45833.77620284113</v>
       </c>
       <c r="E1062">
-        <v>283</v>
+        <v>258</v>
       </c>
       <c r="F1062" s="2">
-        <v>45832.61931712963</v>
+        <v>45833.69792824074</v>
       </c>
       <c r="G1062">
         <v>0</v>
@@ -27466,16 +27466,16 @@
         <v>1</v>
       </c>
       <c r="C1094">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D1094" s="2">
-        <v>45821.87952450383</v>
+        <v>45833.77618177071</v>
       </c>
       <c r="E1094">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="F1094" s="2">
-        <v>45821.73368055555</v>
+        <v>45833.42523148148</v>
       </c>
       <c r="G1094">
         <v>0</v>
@@ -27564,16 +27564,16 @@
         <v>1</v>
       </c>
       <c r="C1098">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1098" s="2">
-        <v>45807.78640665444</v>
+        <v>45833.7762028403</v>
       </c>
       <c r="E1098">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1098" s="2">
-        <v>45831.52096064815</v>
+        <v>45833.68471064815</v>
       </c>
       <c r="G1098">
         <v>0</v>
@@ -27867,16 +27867,16 @@
         <v>1</v>
       </c>
       <c r="C1110">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D1110" s="2">
-        <v>45832.999359191</v>
+        <v>45833.77618177092</v>
       </c>
       <c r="E1110">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F1110" s="2">
-        <v>45832.385</v>
+        <v>45833.42523148148</v>
       </c>
       <c r="G1110">
         <v>0</v>
@@ -28173,16 +28173,16 @@
         <v>1</v>
       </c>
       <c r="C1122">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1122" s="2">
-        <v>45821.87952449879</v>
+        <v>45833.77618176814</v>
       </c>
       <c r="E1122">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1122" s="2">
-        <v>45821.60837962963</v>
+        <v>45833.38887731481</v>
       </c>
       <c r="G1122">
         <v>0</v>
@@ -28274,16 +28274,16 @@
         <v>1</v>
       </c>
       <c r="C1126">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="D1126" s="2">
-        <v>45832.99937861889</v>
+        <v>45833.77620284229</v>
       </c>
       <c r="E1126">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="F1126" s="2">
-        <v>45832.44447916667</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G1126">
         <v>0</v>
@@ -28453,16 +28453,16 @@
         <v>1</v>
       </c>
       <c r="C1133">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D1133" s="2">
-        <v>45825.82707705498</v>
+        <v>45833.77618177536</v>
       </c>
       <c r="E1133">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F1133" s="2">
-        <v>45825.41831018519</v>
+        <v>45833.48585648148</v>
       </c>
       <c r="G1133">
         <v>0</v>
@@ -28805,16 +28805,16 @@
         <v>1</v>
       </c>
       <c r="C1147">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D1147" s="2">
-        <v>45831.83463792493</v>
+        <v>45833.77620284236</v>
       </c>
       <c r="E1147">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F1147" s="2">
-        <v>45831.81081018518</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G1147">
         <v>0</v>
@@ -28857,16 +28857,16 @@
         <v>1</v>
       </c>
       <c r="C1149">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D1149" s="2">
-        <v>45831.83463791953</v>
+        <v>45833.77618177555</v>
       </c>
       <c r="E1149">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F1149" s="2">
-        <v>45831.73116898148</v>
+        <v>45833.48585648148</v>
       </c>
       <c r="G1149">
         <v>0</v>
@@ -28883,16 +28883,16 @@
         <v>1</v>
       </c>
       <c r="C1150">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D1150" s="2">
-        <v>45829.29943060463</v>
+        <v>45834.28681886363</v>
       </c>
       <c r="E1150">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F1150" s="2">
-        <v>45828.66594907407</v>
+        <v>45833.85730324074</v>
       </c>
       <c r="G1150">
         <v>0</v>
@@ -29039,16 +29039,16 @@
         <v>1</v>
       </c>
       <c r="C1156">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1156" s="2">
-        <v>45832.999378625</v>
+        <v>45833.77618177657</v>
       </c>
       <c r="E1156">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1156" s="2">
-        <v>45832.54928240741</v>
+        <v>45833.515625</v>
       </c>
       <c r="G1156">
         <v>0</v>
@@ -29495,16 +29495,16 @@
         <v>1</v>
       </c>
       <c r="C1174">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D1174" s="2">
-        <v>45832.99935919896</v>
+        <v>45833.77618177576</v>
       </c>
       <c r="E1174">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F1174" s="2">
-        <v>45832.4250925926</v>
+        <v>45833.48585648148</v>
       </c>
       <c r="G1174">
         <v>0</v>
@@ -29804,16 +29804,16 @@
         <v>1</v>
       </c>
       <c r="C1186">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D1186" s="2">
-        <v>45811.92552606984</v>
+        <v>45833.77620284091</v>
       </c>
       <c r="E1186">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F1186" s="2">
-        <v>45811.75252314815</v>
+        <v>45833.68996527778</v>
       </c>
       <c r="G1186">
         <v>0</v>
@@ -30896,7 +30896,7 @@
         <v>0</v>
       </c>
       <c r="F1228" s="2">
-        <v>45818.40175925926</v>
+        <v>45833.77162037037</v>
       </c>
       <c r="G1228">
         <v>0</v>
@@ -31450,16 +31450,16 @@
         <v>1</v>
       </c>
       <c r="C1250">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="D1250" s="2">
-        <v>45828.40527173905</v>
+        <v>45834.28681886417</v>
       </c>
       <c r="E1250">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="F1250" s="2">
-        <v>45828.41831018519</v>
+        <v>45833.86076388889</v>
       </c>
       <c r="G1250">
         <v>0</v>
@@ -31528,16 +31528,16 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>324</v>
+        <v>279</v>
       </c>
       <c r="D1253" s="2">
-        <v>45832.99937862989</v>
+        <v>45833.77620284244</v>
       </c>
       <c r="E1253">
-        <v>324</v>
+        <v>279</v>
       </c>
       <c r="F1253" s="2">
-        <v>45832.61931712963</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G1253">
         <v>0</v>
@@ -31577,16 +31577,16 @@
         <v>1</v>
       </c>
       <c r="C1255">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1255" s="2">
-        <v>45807.78640665444</v>
+        <v>45833.77618176919</v>
       </c>
       <c r="E1255">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F1255" s="2">
-        <v>45807.69802083333</v>
+        <v>45833.40459490741</v>
       </c>
       <c r="G1255">
         <v>0</v>
@@ -31733,16 +31733,16 @@
         <v>1</v>
       </c>
       <c r="C1261">
-        <v>-3</v>
+        <v>253</v>
       </c>
       <c r="D1261" s="2">
-        <v>45832.99937862519</v>
+        <v>45834.28681886605</v>
       </c>
       <c r="E1261">
-        <v>-3</v>
+        <v>253</v>
       </c>
       <c r="F1261" s="2">
-        <v>45832.54928240741</v>
+        <v>45833.91274305555</v>
       </c>
       <c r="G1261">
         <v>0</v>
@@ -33332,16 +33332,16 @@
         <v>1</v>
       </c>
       <c r="C1324">
-        <v>-3</v>
+        <v>7</v>
       </c>
       <c r="D1324" s="2">
-        <v>45832.99937863865</v>
+        <v>45833.77620283811</v>
       </c>
       <c r="E1324">
-        <v>-3</v>
+        <v>7</v>
       </c>
       <c r="F1324" s="2">
-        <v>45832.75680555555</v>
+        <v>45833.65372685185</v>
       </c>
       <c r="G1324">
         <v>0</v>
@@ -33791,16 +33791,16 @@
         <v>1</v>
       </c>
       <c r="C1342">
-        <v>562</v>
+        <v>542</v>
       </c>
       <c r="D1342" s="2">
-        <v>45832.99937862538</v>
+        <v>45833.77620283842</v>
       </c>
       <c r="E1342">
-        <v>562</v>
+        <v>542</v>
       </c>
       <c r="F1342" s="2">
-        <v>45832.54928240741</v>
+        <v>45833.66032407407</v>
       </c>
       <c r="G1342">
         <v>0</v>
@@ -34885,16 +34885,16 @@
         <v>1</v>
       </c>
       <c r="C1385">
-        <v>36</v>
+        <v>326</v>
       </c>
       <c r="D1385" s="2">
-        <v>45811.92549991595</v>
+        <v>45834.28681886399</v>
       </c>
       <c r="E1385">
-        <v>36</v>
+        <v>326</v>
       </c>
       <c r="F1385" s="2">
-        <v>45811.72346064815</v>
+        <v>45833.85784722222</v>
       </c>
       <c r="G1385">
         <v>0</v>
@@ -35604,16 +35604,16 @@
         <v>1</v>
       </c>
       <c r="C1413">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D1413" s="2">
-        <v>45811.92544186871</v>
+        <v>45833.7762028385</v>
       </c>
       <c r="E1413">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="F1413" s="2">
-        <v>45811.41633101852</v>
+        <v>45833.66032407407</v>
       </c>
       <c r="G1413">
         <v>0</v>
@@ -35841,7 +35841,7 @@
         <v>13</v>
       </c>
       <c r="F1422" s="2">
-        <v>45811.50125</v>
+        <v>45833.76759259259</v>
       </c>
       <c r="G1422">
         <v>0</v>
@@ -36271,16 +36271,16 @@
         <v>1</v>
       </c>
       <c r="C1439">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1439" s="2">
-        <v>45800.9319772456</v>
+        <v>45833.77618177827</v>
       </c>
       <c r="E1439">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F1439" s="2">
-        <v>45800.46056712963</v>
+        <v>45833.53011574074</v>
       </c>
       <c r="G1439">
         <v>0</v>
@@ -36450,16 +36450,16 @@
         <v>1</v>
       </c>
       <c r="C1446">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D1446" s="2">
-        <v>45825.28849841491</v>
+        <v>45833.77618177596</v>
       </c>
       <c r="E1446">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F1446" s="2">
-        <v>45824.45626157407</v>
+        <v>45833.48585648148</v>
       </c>
       <c r="G1446">
         <v>0</v>
@@ -36502,16 +36502,16 @@
         <v>1</v>
       </c>
       <c r="C1448">
-        <v>188</v>
+        <v>118</v>
       </c>
       <c r="D1448" s="2">
-        <v>45832.99937863062</v>
+        <v>45833.77620284251</v>
       </c>
       <c r="E1448">
-        <v>188</v>
+        <v>118</v>
       </c>
       <c r="F1448" s="2">
-        <v>45832.62121527778</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G1448">
         <v>0</v>
@@ -37962,16 +37962,16 @@
         <v>1</v>
       </c>
       <c r="C1506">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D1506" s="2">
-        <v>45812.78301983239</v>
+        <v>45833.77620284294</v>
       </c>
       <c r="E1506">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F1506" s="2">
-        <v>45812.32796296296</v>
+        <v>45833.76515046296</v>
       </c>
       <c r="G1506">
         <v>0</v>
@@ -37988,16 +37988,16 @@
         <v>1</v>
       </c>
       <c r="C1507">
-        <v>-51</v>
+        <v>242</v>
       </c>
       <c r="D1507" s="2">
-        <v>45832.99937863008</v>
+        <v>45834.28681886305</v>
       </c>
       <c r="E1507">
-        <v>-51</v>
+        <v>242</v>
       </c>
       <c r="F1507" s="2">
-        <v>45832.61931712963</v>
+        <v>45833.85539351852</v>
       </c>
       <c r="G1507">
         <v>0</v>
@@ -39701,16 +39701,16 @@
         <v>1</v>
       </c>
       <c r="C1576">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D1576" s="2">
-        <v>45832.99937861426</v>
+        <v>45833.77620283971</v>
       </c>
       <c r="E1576">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F1576" s="2">
-        <v>45832.43322916667</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G1576">
         <v>0</v>
@@ -40145,16 +40145,16 @@
         <v>1</v>
       </c>
       <c r="C1594">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="D1594" s="2">
-        <v>45831.83463793174</v>
+        <v>45833.77620283723</v>
       </c>
       <c r="E1594">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="F1594" s="2">
-        <v>45831.81263888889</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G1594">
         <v>0</v>
@@ -40223,16 +40223,16 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>4845</v>
+        <v>4785</v>
       </c>
       <c r="D1597" s="2">
-        <v>45832.99937863797</v>
+        <v>45833.77620284258</v>
       </c>
       <c r="E1597">
-        <v>4845</v>
+        <v>4785</v>
       </c>
       <c r="F1597" s="2">
-        <v>45832.73863425926</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G1597">
         <v>0</v>
@@ -40298,16 +40298,16 @@
         <v>1</v>
       </c>
       <c r="C1600">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1600" s="2">
-        <v>45832.99937863024</v>
+        <v>45833.77620283866</v>
       </c>
       <c r="E1600">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1600" s="2">
-        <v>45832.61931712963</v>
+        <v>45833.66032407407</v>
       </c>
       <c r="G1600">
         <v>0</v>
@@ -41190,16 +41190,16 @@
         <v>1</v>
       </c>
       <c r="C1635">
-        <v>2657</v>
+        <v>2588</v>
       </c>
       <c r="D1635" s="2">
-        <v>45832.9993786256</v>
+        <v>45833.77620284265</v>
       </c>
       <c r="E1635">
-        <v>2657</v>
+        <v>2588</v>
       </c>
       <c r="F1635" s="2">
-        <v>45832.54928240741</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G1635">
         <v>0</v>
@@ -41576,16 +41576,16 @@
         <v>1</v>
       </c>
       <c r="C1651">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D1651" s="2">
-        <v>45831.83463791655</v>
+        <v>45833.77620284302</v>
       </c>
       <c r="E1651">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F1651" s="2">
-        <v>45831.68162037037</v>
+        <v>45833.76623842592</v>
       </c>
       <c r="G1651">
         <v>0</v>
@@ -41703,16 +41703,16 @@
         <v>1</v>
       </c>
       <c r="C1656">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D1656" s="2">
-        <v>45825.82707706397</v>
+        <v>45834.28681886452</v>
       </c>
       <c r="E1656">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F1656" s="2">
-        <v>45825.49319444445</v>
+        <v>45833.87039351852</v>
       </c>
       <c r="G1656">
         <v>0</v>
@@ -41729,16 +41729,16 @@
         <v>1</v>
       </c>
       <c r="C1657">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="D1657" s="2">
-        <v>45814.82976436854</v>
+        <v>45834.28681886521</v>
       </c>
       <c r="E1657">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="F1657" s="2">
-        <v>45814.70711805556</v>
+        <v>45833.87199074074</v>
       </c>
       <c r="G1657">
         <v>0</v>
@@ -42439,7 +42439,7 @@
         <v>0</v>
       </c>
       <c r="F1685" s="2">
-        <v>45708.39260416666</v>
+        <v>45833.76810185185</v>
       </c>
       <c r="G1685">
         <v>0</v>
@@ -42721,16 +42721,16 @@
         <v>1</v>
       </c>
       <c r="C1697">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1697" s="2">
-        <v>45820.91697502176</v>
+        <v>45833.77618177616</v>
       </c>
       <c r="E1697">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F1697" s="2">
-        <v>45820.7009375</v>
+        <v>45833.48585648148</v>
       </c>
       <c r="G1697">
         <v>0</v>
@@ -44220,16 +44220,16 @@
         <v>1</v>
       </c>
       <c r="C1758">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D1758" s="2">
-        <v>45799.89545110933</v>
+        <v>45834.28681886347</v>
       </c>
       <c r="E1758">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="F1758" s="2">
-        <v>45782.65509259259</v>
+        <v>45833.85653935185</v>
       </c>
       <c r="G1758">
         <v>0</v>
@@ -45533,16 +45533,16 @@
         <v>1</v>
       </c>
       <c r="C1810">
-        <v>-5</v>
+        <v>15</v>
       </c>
       <c r="D1810" s="2">
-        <v>45832.99937863459</v>
+        <v>45833.77618177173</v>
       </c>
       <c r="E1810">
-        <v>-5</v>
+        <v>15</v>
       </c>
       <c r="F1810" s="2">
-        <v>45832.66791666667</v>
+        <v>45833.43788194445</v>
       </c>
       <c r="G1810">
         <v>0</v>
@@ -45891,16 +45891,16 @@
         <v>1</v>
       </c>
       <c r="C1824">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1824" s="2">
-        <v>45831.83463791691</v>
+        <v>45833.77618176959</v>
       </c>
       <c r="E1824">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1824" s="2">
-        <v>45831.69243055556</v>
+        <v>45833.42410879629</v>
       </c>
       <c r="G1824">
         <v>0</v>
@@ -46699,16 +46699,16 @@
         <v>1</v>
       </c>
       <c r="C1856">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1856" s="2">
-        <v>45832.99937863735</v>
+        <v>45833.77620283733</v>
       </c>
       <c r="E1856">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F1856" s="2">
-        <v>45832.71763888889</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G1856">
         <v>0</v>
@@ -46829,16 +46829,16 @@
         <v>1</v>
       </c>
       <c r="C1861">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1861" s="2">
-        <v>45795.04190003897</v>
+        <v>45833.77620283978</v>
       </c>
       <c r="E1861">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1861" s="2">
-        <v>45659.72599537037</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G1861">
         <v>0</v>
@@ -46864,7 +46864,7 @@
         <v>0</v>
       </c>
       <c r="F1862" s="2">
-        <v>45812.32642361111</v>
+        <v>45833.77251157408</v>
       </c>
       <c r="G1862">
         <v>0</v>
@@ -47268,16 +47268,16 @@
         <v>1</v>
       </c>
       <c r="C1878">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D1878" s="2">
-        <v>45806.77603763194</v>
+        <v>45833.77618177266</v>
       </c>
       <c r="E1878">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F1878" s="2">
-        <v>45806.74783564815</v>
+        <v>45833.44604166667</v>
       </c>
       <c r="G1878">
         <v>0</v>
@@ -48122,16 +48122,16 @@
         <v>1</v>
       </c>
       <c r="C1912">
-        <v>71</v>
+        <v>239</v>
       </c>
       <c r="D1912" s="2">
-        <v>45828.4052717394</v>
+        <v>45834.28681886538</v>
       </c>
       <c r="E1912">
-        <v>71</v>
+        <v>239</v>
       </c>
       <c r="F1912" s="2">
-        <v>45828.41831018519</v>
+        <v>45833.87310185185</v>
       </c>
       <c r="G1912">
         <v>0</v>
@@ -50909,16 +50909,16 @@
         <v>1</v>
       </c>
       <c r="C2023">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="D2023" s="2">
-        <v>45831.83461825165</v>
+        <v>45834.2868188647</v>
       </c>
       <c r="E2023">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="F2023" s="2">
-        <v>45831.67092592592</v>
+        <v>45833.87069444444</v>
       </c>
       <c r="G2023">
         <v>0</v>
@@ -50935,16 +50935,16 @@
         <v>1</v>
       </c>
       <c r="C2024">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="D2024" s="2">
-        <v>45812.78303939045</v>
+        <v>45834.28681886487</v>
       </c>
       <c r="E2024">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="F2024" s="2">
-        <v>45812.67899305555</v>
+        <v>45833.8713425926</v>
       </c>
       <c r="G2024">
         <v>0</v>
@@ -51160,16 +51160,16 @@
         <v>1</v>
       </c>
       <c r="C2033">
-        <v>-5</v>
+        <v>65</v>
       </c>
       <c r="D2033" s="2">
-        <v>45827.49773229471</v>
+        <v>45834.28681886572</v>
       </c>
       <c r="E2033">
-        <v>-5</v>
+        <v>65</v>
       </c>
       <c r="F2033" s="2">
-        <v>45826.55956018518</v>
+        <v>45833.87530092592</v>
       </c>
       <c r="G2033">
         <v>0</v>
@@ -51899,16 +51899,16 @@
         <v>1</v>
       </c>
       <c r="C2062">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="D2062" s="2">
-        <v>45795.0420164208</v>
+        <v>45833.77620283788</v>
       </c>
       <c r="E2062">
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="F2062" s="2">
-        <v>45730.70069444444</v>
+        <v>45833.63289351852</v>
       </c>
       <c r="G2062">
         <v>0</v>
@@ -52958,16 +52958,16 @@
         <v>1</v>
       </c>
       <c r="C2104">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2104" s="2">
-        <v>45811.92546678011</v>
+        <v>45833.77618176939</v>
       </c>
       <c r="E2104">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2104" s="2">
-        <v>45811.50252314815</v>
+        <v>45833.40459490741</v>
       </c>
       <c r="G2104">
         <v>0</v>
@@ -53959,16 +53959,16 @@
         <v>1</v>
       </c>
       <c r="C2144">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D2144" s="2">
-        <v>45799.89545110933</v>
+        <v>45833.77618177286</v>
       </c>
       <c r="E2144">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F2144" s="2">
-        <v>45792.48434027778</v>
+        <v>45833.44604166667</v>
       </c>
       <c r="G2144">
         <v>0</v>
@@ -55883,16 +55883,16 @@
         <v>1</v>
       </c>
       <c r="C2221">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2221" s="2">
-        <v>45795.04190003897</v>
+        <v>45833.77620283985</v>
       </c>
       <c r="E2221">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2221" s="2">
-        <v>45656.66517361111</v>
+        <v>45833.68387731481</v>
       </c>
       <c r="G2221">
         <v>0</v>
@@ -56400,16 +56400,16 @@
         <v>1</v>
       </c>
       <c r="C2241">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D2241" s="2">
-        <v>45832.9993786382</v>
+        <v>45833.77620284271</v>
       </c>
       <c r="E2241">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F2241" s="2">
-        <v>45832.73863425926</v>
+        <v>45833.73585648148</v>
       </c>
       <c r="G2241">
         <v>0</v>
@@ -58555,16 +58555,16 @@
         <v>1</v>
       </c>
       <c r="C2327">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D2327" s="2">
-        <v>45831.83461825205</v>
+        <v>45833.7762028412</v>
       </c>
       <c r="E2327">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F2327" s="2">
-        <v>45831.67487268519</v>
+        <v>45833.69792824074</v>
       </c>
       <c r="G2327">
         <v>0</v>
@@ -59853,10 +59853,13 @@
         <v>0</v>
       </c>
       <c r="D2379" s="2">
-        <v>45795.04193352044</v>
+        <v>45833.77620283819</v>
       </c>
       <c r="E2379">
         <v>0</v>
+      </c>
+      <c r="F2379" s="2">
+        <v>45833.6553587963</v>
       </c>
       <c r="G2379">
         <v>0</v>
@@ -60767,16 +60770,16 @@
         <v>1</v>
       </c>
       <c r="C2416">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="D2416" s="2">
-        <v>45831.83463791669</v>
+        <v>45833.77618177112</v>
       </c>
       <c r="E2416">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F2416" s="2">
-        <v>45831.68162037037</v>
+        <v>45833.42523148148</v>
       </c>
       <c r="G2416">
         <v>0</v>
@@ -61972,16 +61975,16 @@
         <v>1</v>
       </c>
       <c r="C2465">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D2465" s="2">
-        <v>45831.83463793192</v>
+        <v>45833.77618177306</v>
       </c>
       <c r="E2465">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F2465" s="2">
-        <v>45831.81263888889</v>
+        <v>45833.44604166667</v>
       </c>
       <c r="G2465">
         <v>0</v>
@@ -62361,16 +62364,16 @@
         <v>1</v>
       </c>
       <c r="C2481">
-        <v>288</v>
+        <v>203</v>
       </c>
       <c r="D2481" s="2">
-        <v>45832.99937862582</v>
+        <v>45833.77620283741</v>
       </c>
       <c r="E2481">
-        <v>288</v>
+        <v>203</v>
       </c>
       <c r="F2481" s="2">
-        <v>45832.54928240741</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G2481">
         <v>0</v>
@@ -62387,16 +62390,16 @@
         <v>1</v>
       </c>
       <c r="C2482">
-        <v>913</v>
+        <v>834</v>
       </c>
       <c r="D2482" s="2">
-        <v>45832.99937862607</v>
+        <v>45833.77620283749</v>
       </c>
       <c r="E2482">
-        <v>913</v>
+        <v>834</v>
       </c>
       <c r="F2482" s="2">
-        <v>45832.54928240741</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G2482">
         <v>0</v>
@@ -62413,16 +62416,16 @@
         <v>1</v>
       </c>
       <c r="C2483">
-        <v>1173</v>
+        <v>1137</v>
       </c>
       <c r="D2483" s="2">
-        <v>45832.99935918752</v>
+        <v>45833.77620283757</v>
       </c>
       <c r="E2483">
-        <v>1173</v>
+        <v>1137</v>
       </c>
       <c r="F2483" s="2">
-        <v>45831.91746527778</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G2483">
         <v>0</v>
@@ -62439,16 +62442,16 @@
         <v>1</v>
       </c>
       <c r="C2484">
-        <v>577</v>
+        <v>494</v>
       </c>
       <c r="D2484" s="2">
-        <v>45831.83461824854</v>
+        <v>45833.77620283764</v>
       </c>
       <c r="E2484">
-        <v>577</v>
+        <v>494</v>
       </c>
       <c r="F2484" s="2">
-        <v>45831.53259259259</v>
+        <v>45833.54157407407</v>
       </c>
       <c r="G2484">
         <v>0</v>
@@ -64830,6 +64833,9 @@
       <c r="E2582">
         <v>0</v>
       </c>
+      <c r="F2582" s="2">
+        <v>45833.65579861111</v>
+      </c>
       <c r="G2582">
         <v>0</v>
       </c>
@@ -64929,6 +64935,81 @@
         <v>0</v>
       </c>
       <c r="H2586" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2587" spans="1:8">
+      <c r="A2587">
+        <v>43873951</v>
+      </c>
+      <c r="B2587">
+        <v>1</v>
+      </c>
+      <c r="C2587">
+        <v>-1</v>
+      </c>
+      <c r="D2587" s="2">
+        <v>45833.7762028428</v>
+      </c>
+      <c r="E2587">
+        <v>-1</v>
+      </c>
+      <c r="F2587" s="2">
+        <v>45833.68996527778</v>
+      </c>
+      <c r="G2587">
+        <v>0</v>
+      </c>
+      <c r="H2587" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2588" spans="1:8">
+      <c r="A2588">
+        <v>43874050</v>
+      </c>
+      <c r="B2588">
+        <v>1</v>
+      </c>
+      <c r="C2588">
+        <v>0</v>
+      </c>
+      <c r="D2588" s="2">
+        <v>45833.77620283766</v>
+      </c>
+      <c r="E2588">
+        <v>0</v>
+      </c>
+      <c r="G2588">
+        <v>0</v>
+      </c>
+      <c r="H2588" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2589" spans="1:8">
+      <c r="A2589">
+        <v>43883152</v>
+      </c>
+      <c r="B2589">
+        <v>1</v>
+      </c>
+      <c r="C2589">
+        <v>144</v>
+      </c>
+      <c r="D2589" s="2">
+        <v>45834.28681886436</v>
+      </c>
+      <c r="E2589">
+        <v>144</v>
+      </c>
+      <c r="F2589" s="2">
+        <v>45833.86863425926</v>
+      </c>
+      <c r="G2589">
+        <v>0</v>
+      </c>
+      <c r="H2589" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizei dados add e bibi
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2609" uniqueCount="10">
   <si>
     <t>id_produto</t>
   </si>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2599"/>
+  <dimension ref="A1:H2602"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,16 +494,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>-3</v>
       </c>
       <c r="D4" s="2">
-        <v>45839.88101717283</v>
+        <v>45840.80861854634</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>-3</v>
       </c>
       <c r="F4" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -520,16 +520,16 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2">
-        <v>45839.88099823055</v>
+        <v>45840.80861854191</v>
       </c>
       <c r="E5">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>45839.6671412037</v>
+        <v>45840.69604166667</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -952,16 +952,16 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="2">
-        <v>45839.88101716927</v>
+        <v>45840.80859799153</v>
       </c>
       <c r="E23">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F23" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.38353009259</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1194,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>2634</v>
+        <v>2601</v>
       </c>
       <c r="D33" s="2">
-        <v>45839.88099821127</v>
+        <v>45840.80859799837</v>
       </c>
       <c r="E33">
-        <v>2634</v>
+        <v>2601</v>
       </c>
       <c r="F33" s="2">
-        <v>45839.53225694445</v>
+        <v>45840.48958333334</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1765,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>243</v>
+        <v>193</v>
       </c>
       <c r="D56" s="2">
-        <v>45839.88101716644</v>
+        <v>45840.80861854657</v>
       </c>
       <c r="E56">
-        <v>243</v>
+        <v>193</v>
       </c>
       <c r="F56" s="2">
-        <v>45839.69537037037</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -1817,16 +1817,16 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="D58" s="2">
-        <v>45839.33732491444</v>
+        <v>45840.80861855218</v>
       </c>
       <c r="E58">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="F58" s="2">
-        <v>45838.7697337963</v>
+        <v>45840.70408564815</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -1843,16 +1843,16 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D59" s="2">
-        <v>45839.33732491323</v>
+        <v>45840.80859799736</v>
       </c>
       <c r="E59">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="F59" s="2">
-        <v>45838.76819444444</v>
+        <v>45840.48582175926</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -1941,16 +1941,16 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D63" s="2">
-        <v>45839.8810171666</v>
+        <v>45840.80859799984</v>
       </c>
       <c r="E63">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F63" s="2">
-        <v>45839.69537037037</v>
+        <v>45840.51295138889</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2088,16 +2088,16 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D69" s="2">
-        <v>45839.8810171694</v>
+        <v>45840.80861854216</v>
       </c>
       <c r="E69">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="F69" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -2114,16 +2114,16 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D70" s="2">
-        <v>45839.88101717587</v>
+        <v>45840.80861854237</v>
       </c>
       <c r="E70">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F70" s="2">
-        <v>45839.78440972222</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2376,16 +2376,16 @@
         <v>1</v>
       </c>
       <c r="C81">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D81" s="2">
-        <v>45839.88099822195</v>
+        <v>45840.80861854681</v>
       </c>
       <c r="E81">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F81" s="2">
-        <v>45839.63525462963</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -2402,16 +2402,16 @@
         <v>1</v>
       </c>
       <c r="C82">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D82" s="2">
-        <v>45839.88097972267</v>
+        <v>45840.8085980047</v>
       </c>
       <c r="E82">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F82" s="2">
-        <v>45839.42005787037</v>
+        <v>45840.65059027778</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -2428,16 +2428,16 @@
         <v>1</v>
       </c>
       <c r="C83">
-        <v>220</v>
+        <v>181</v>
       </c>
       <c r="D83" s="2">
-        <v>45839.88099823508</v>
+        <v>45840.80861854704</v>
       </c>
       <c r="E83">
-        <v>220</v>
+        <v>181</v>
       </c>
       <c r="F83" s="2">
-        <v>45839.68895833333</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -2477,16 +2477,16 @@
         <v>1</v>
       </c>
       <c r="C85">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D85" s="2">
-        <v>45839.88099823522</v>
+        <v>45840.80859800373</v>
       </c>
       <c r="E85">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F85" s="2">
-        <v>45839.68895833333</v>
+        <v>45840.62773148148</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -2503,16 +2503,16 @@
         <v>1</v>
       </c>
       <c r="C86">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="D86" s="2">
-        <v>45839.88099822219</v>
+        <v>45840.80861854728</v>
       </c>
       <c r="E86">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="F86" s="2">
-        <v>45839.63525462963</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -2529,16 +2529,16 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D87" s="2">
-        <v>45839.88101716954</v>
+        <v>45840.80861854751</v>
       </c>
       <c r="E87">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F87" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -2604,16 +2604,16 @@
         <v>1</v>
       </c>
       <c r="C90">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D90" s="2">
-        <v>45839.33732490868</v>
+        <v>45840.80859800224</v>
       </c>
       <c r="E90">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F90" s="2">
-        <v>45838.72313657407</v>
+        <v>45840.56913194444</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -2630,16 +2630,16 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D91" s="2">
-        <v>45839.88099821146</v>
+        <v>45840.80859799853</v>
       </c>
       <c r="E91">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F91" s="2">
-        <v>45839.53225694445</v>
+        <v>45840.48958333334</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -2702,16 +2702,16 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D94" s="2">
-        <v>45839.88101717598</v>
+        <v>45840.80861855553</v>
       </c>
       <c r="E94">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="F94" s="2">
-        <v>45839.78440972222</v>
+        <v>45840.73303240741</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -2751,16 +2751,16 @@
         <v>1</v>
       </c>
       <c r="C96">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D96" s="2">
-        <v>45839.88097972295</v>
+        <v>45840.80861855617</v>
       </c>
       <c r="E96">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F96" s="2">
-        <v>45839.42005787037</v>
+        <v>45840.75590277778</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -2800,16 +2800,16 @@
         <v>1</v>
       </c>
       <c r="C98">
-        <v>552</v>
+        <v>512</v>
       </c>
       <c r="D98" s="2">
-        <v>45839.33730491879</v>
+        <v>45840.80861854261</v>
       </c>
       <c r="E98">
-        <v>552</v>
+        <v>512</v>
       </c>
       <c r="F98" s="2">
-        <v>45838.51489583333</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -2872,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>1358</v>
+        <v>1043</v>
       </c>
       <c r="D101" s="2">
-        <v>45839.88101717301</v>
+        <v>45840.8086185526</v>
       </c>
       <c r="E101">
-        <v>1358</v>
+        <v>1043</v>
       </c>
       <c r="F101" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.70496527778</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -2921,16 +2921,16 @@
         <v>1</v>
       </c>
       <c r="C103">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D103" s="2">
-        <v>45839.33728134933</v>
+        <v>45840.80861855284</v>
       </c>
       <c r="E103">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F103" s="2">
-        <v>45838.49497685185</v>
+        <v>45840.70496527778</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -2993,16 +2993,16 @@
         <v>1</v>
       </c>
       <c r="C106">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D106" s="2">
-        <v>45839.88101717314</v>
+        <v>45840.80859800486</v>
       </c>
       <c r="E106">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F106" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.65059027778</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -3258,16 +3258,16 @@
         <v>1</v>
       </c>
       <c r="C117">
-        <v>983</v>
+        <v>973</v>
       </c>
       <c r="D117" s="2">
-        <v>45839.88099822243</v>
+        <v>45840.80859800338</v>
       </c>
       <c r="E117">
-        <v>983</v>
+        <v>973</v>
       </c>
       <c r="F117" s="2">
-        <v>45839.63525462963</v>
+        <v>45840.62440972222</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -3333,16 +3333,16 @@
         <v>1</v>
       </c>
       <c r="C120">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D120" s="2">
-        <v>45839.33730492832</v>
+        <v>45840.80859800502</v>
       </c>
       <c r="E120">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F120" s="2">
-        <v>45838.72134259259</v>
+        <v>45840.65059027778</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -3408,16 +3408,16 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D123" s="2">
-        <v>45839.88099822574</v>
+        <v>45840.80861854774</v>
       </c>
       <c r="E123">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="F123" s="2">
-        <v>45839.63565972223</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -3460,16 +3460,16 @@
         <v>1</v>
       </c>
       <c r="C125">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="D125" s="2">
-        <v>45839.88099821493</v>
+        <v>45840.80859800091</v>
       </c>
       <c r="E125">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="F125" s="2">
-        <v>45839.54896990741</v>
+        <v>45840.54755787037</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -3846,16 +3846,16 @@
         <v>1</v>
       </c>
       <c r="C141">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="D141" s="2">
-        <v>45839.88099822783</v>
+        <v>45840.80861854798</v>
       </c>
       <c r="E141">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="F141" s="2">
-        <v>45839.6484837963</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G141">
         <v>0</v>
@@ -3950,16 +3950,16 @@
         <v>1</v>
       </c>
       <c r="C145">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D145" s="2">
-        <v>45839.88099823544</v>
+        <v>45840.80859799486</v>
       </c>
       <c r="E145">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F145" s="2">
-        <v>45839.68895833333</v>
+        <v>45840.42106481481</v>
       </c>
       <c r="G145">
         <v>0</v>
@@ -4100,16 +4100,16 @@
         <v>1</v>
       </c>
       <c r="C151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D151" s="2">
-        <v>45839.88099821805</v>
+        <v>45840.80861855239</v>
       </c>
       <c r="E151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F151" s="2">
-        <v>45839.55863425926</v>
+        <v>45840.70408564815</v>
       </c>
       <c r="G151">
         <v>0</v>
@@ -4345,16 +4345,16 @@
         <v>1</v>
       </c>
       <c r="C161">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D161" s="2">
-        <v>45833.77620284128</v>
+        <v>45840.80859800107</v>
       </c>
       <c r="E161">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F161" s="2">
-        <v>45833.73408564815</v>
+        <v>45840.54755787037</v>
       </c>
       <c r="G161">
         <v>0</v>
@@ -4397,16 +4397,16 @@
         <v>1</v>
       </c>
       <c r="C163">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D163" s="2">
-        <v>45833.77618177913</v>
+        <v>45840.8086185346</v>
       </c>
       <c r="E163">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F163" s="2">
-        <v>45833.54157407407</v>
+        <v>45840.67962962963</v>
       </c>
       <c r="G163">
         <v>0</v>
@@ -4691,16 +4691,16 @@
         <v>1</v>
       </c>
       <c r="C175">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="D175" s="2">
-        <v>45839.88099823565</v>
+        <v>45840.80861855575</v>
       </c>
       <c r="E175">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="F175" s="2">
-        <v>45839.68895833333</v>
+        <v>45840.7536574074</v>
       </c>
       <c r="G175">
         <v>0</v>
@@ -4936,16 +4936,16 @@
         <v>1</v>
       </c>
       <c r="C185">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D185" s="2">
-        <v>45839.33732491286</v>
+        <v>45840.80859800518</v>
       </c>
       <c r="E185">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F185" s="2">
-        <v>45838.76719907407</v>
+        <v>45840.65059027778</v>
       </c>
       <c r="G185">
         <v>0</v>
@@ -5103,16 +5103,16 @@
         <v>1</v>
       </c>
       <c r="C192">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D192" s="2">
-        <v>45839.88099822274</v>
+        <v>45840.80859800665</v>
       </c>
       <c r="E192">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F192" s="2">
-        <v>45839.63525462963</v>
+        <v>45840.67293981482</v>
       </c>
       <c r="G192">
         <v>0</v>
@@ -5181,16 +5181,16 @@
         <v>1</v>
       </c>
       <c r="C195">
-        <v>10</v>
+        <v>-6</v>
       </c>
       <c r="D195" s="2">
-        <v>45839.88099823108</v>
+        <v>45840.8086185482</v>
       </c>
       <c r="E195">
-        <v>10</v>
+        <v>-6</v>
       </c>
       <c r="F195" s="2">
-        <v>45839.6756712963</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G195">
         <v>0</v>
@@ -5302,16 +5302,16 @@
         <v>1</v>
       </c>
       <c r="C200">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="D200" s="2">
-        <v>45839.88099821163</v>
+        <v>45840.80859799619</v>
       </c>
       <c r="E200">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="F200" s="2">
-        <v>45839.53225694445</v>
+        <v>45840.44622685185</v>
       </c>
       <c r="G200">
         <v>0</v>
@@ -5711,16 +5711,16 @@
         <v>1</v>
       </c>
       <c r="C217">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D217" s="2">
-        <v>45839.88101717353</v>
+        <v>45840.80859799434</v>
       </c>
       <c r="E217">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F217" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.41077546297</v>
       </c>
       <c r="G217">
         <v>0</v>
@@ -5737,16 +5737,16 @@
         <v>1</v>
       </c>
       <c r="C218">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D218" s="2">
-        <v>45839.88099822136</v>
+        <v>45840.80859800136</v>
       </c>
       <c r="E218">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F218" s="2">
-        <v>45839.63506944444</v>
+        <v>45840.54755787037</v>
       </c>
       <c r="G218">
         <v>0</v>
@@ -6149,16 +6149,16 @@
         <v>1</v>
       </c>
       <c r="C235">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="D235" s="2">
-        <v>45839.88101716808</v>
+        <v>45840.80861853628</v>
       </c>
       <c r="E235">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="F235" s="2">
-        <v>45839.74771990741</v>
+        <v>45840.68016203704</v>
       </c>
       <c r="G235">
         <v>0</v>
@@ -6437,16 +6437,16 @@
         <v>1</v>
       </c>
       <c r="C247">
-        <v>783</v>
+        <v>705</v>
       </c>
       <c r="D247" s="2">
-        <v>45839.88101716968</v>
+        <v>45840.80861853909</v>
       </c>
       <c r="E247">
-        <v>783</v>
+        <v>705</v>
       </c>
       <c r="F247" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.68561342593</v>
       </c>
       <c r="G247">
         <v>0</v>
@@ -6627,16 +6627,16 @@
         <v>1</v>
       </c>
       <c r="C255">
-        <v>1134</v>
+        <v>1088</v>
       </c>
       <c r="D255" s="2">
-        <v>45839.88099821231</v>
+        <v>45840.80861854846</v>
       </c>
       <c r="E255">
-        <v>1134</v>
+        <v>1088</v>
       </c>
       <c r="F255" s="2">
-        <v>45839.53225694445</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -6996,16 +6996,16 @@
         <v>1</v>
       </c>
       <c r="C270">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="D270" s="2">
-        <v>45839.88099823588</v>
+        <v>45840.80861854867</v>
       </c>
       <c r="E270">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="F270" s="2">
-        <v>45839.68895833333</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G270">
         <v>0</v>
@@ -7045,16 +7045,16 @@
         <v>1</v>
       </c>
       <c r="C272">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D272" s="2">
-        <v>45839.33734442695</v>
+        <v>45840.80861855704</v>
       </c>
       <c r="E272">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F272" s="2">
-        <v>45838.77438657408</v>
+        <v>45840.75967592592</v>
       </c>
       <c r="G272">
         <v>0</v>
@@ -7097,16 +7097,16 @@
         <v>1</v>
       </c>
       <c r="C274">
-        <v>91</v>
+        <v>201</v>
       </c>
       <c r="D274" s="2">
-        <v>45839.88101717365</v>
+        <v>45840.8086185412</v>
       </c>
       <c r="E274">
-        <v>91</v>
+        <v>201</v>
       </c>
       <c r="F274" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.69284722222</v>
       </c>
       <c r="G274">
         <v>0</v>
@@ -7310,16 +7310,16 @@
         <v>1</v>
       </c>
       <c r="C283">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D283" s="2">
-        <v>45839.88099821831</v>
+        <v>45840.80859800534</v>
       </c>
       <c r="E283">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="F283" s="2">
-        <v>45839.55863425926</v>
+        <v>45840.65059027778</v>
       </c>
       <c r="G283">
         <v>0</v>
@@ -7509,16 +7509,16 @@
         <v>1</v>
       </c>
       <c r="C291">
-        <v>460</v>
+        <v>442</v>
       </c>
       <c r="D291" s="2">
-        <v>45839.88101717612</v>
+        <v>45840.80861854285</v>
       </c>
       <c r="E291">
-        <v>460</v>
+        <v>442</v>
       </c>
       <c r="F291" s="2">
-        <v>45839.78440972222</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G291">
         <v>0</v>
@@ -7535,16 +7535,16 @@
         <v>1</v>
       </c>
       <c r="C292">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D292" s="2">
-        <v>45839.3373249169</v>
+        <v>45840.80859799637</v>
       </c>
       <c r="E292">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F292" s="2">
-        <v>45838.77349537037</v>
+        <v>45840.44622685185</v>
       </c>
       <c r="G292">
         <v>0</v>
@@ -7619,7 +7619,7 @@
         <v>-49</v>
       </c>
       <c r="F295" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G295">
         <v>0</v>
@@ -7953,16 +7953,16 @@
         <v>1</v>
       </c>
       <c r="C309">
-        <v>941</v>
+        <v>928</v>
       </c>
       <c r="D309" s="2">
-        <v>45839.88099822318</v>
+        <v>45840.80859799868</v>
       </c>
       <c r="E309">
-        <v>941</v>
+        <v>928</v>
       </c>
       <c r="F309" s="2">
-        <v>45839.63525462963</v>
+        <v>45840.48958333334</v>
       </c>
       <c r="G309">
         <v>0</v>
@@ -8071,16 +8071,16 @@
         <v>1</v>
       </c>
       <c r="C314">
-        <v>19</v>
+        <v>-9</v>
       </c>
       <c r="D314" s="2">
-        <v>45839.88101716712</v>
+        <v>45840.80861854419</v>
       </c>
       <c r="E314">
-        <v>19</v>
+        <v>-9</v>
       </c>
       <c r="F314" s="2">
-        <v>45839.71052083333</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G314">
         <v>0</v>
@@ -8097,16 +8097,16 @@
         <v>1</v>
       </c>
       <c r="C315">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D315" s="2">
-        <v>45839.33732491481</v>
+        <v>45840.80861853678</v>
       </c>
       <c r="E315">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F315" s="2">
-        <v>45838.76998842593</v>
+        <v>45840.68217592593</v>
       </c>
       <c r="G315">
         <v>0</v>
@@ -8169,16 +8169,16 @@
         <v>1</v>
       </c>
       <c r="C318">
-        <v>1021</v>
+        <v>991</v>
       </c>
       <c r="D318" s="2">
-        <v>45839.88099822066</v>
+        <v>45840.80859799519</v>
       </c>
       <c r="E318">
-        <v>1021</v>
+        <v>991</v>
       </c>
       <c r="F318" s="2">
-        <v>45839.63486111111</v>
+        <v>45840.42267361111</v>
       </c>
       <c r="G318">
         <v>0</v>
@@ -8221,16 +8221,16 @@
         <v>1</v>
       </c>
       <c r="C320">
-        <v>129</v>
+        <v>-1</v>
       </c>
       <c r="D320" s="2">
-        <v>45828.4052717326</v>
+        <v>45840.80859800679</v>
       </c>
       <c r="E320">
-        <v>129</v>
+        <v>-1</v>
       </c>
       <c r="F320" s="2">
-        <v>45827.85460648148</v>
+        <v>45840.67293981482</v>
       </c>
       <c r="G320">
         <v>0</v>
@@ -8247,16 +8247,16 @@
         <v>1</v>
       </c>
       <c r="C321">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D321" s="2">
-        <v>45839.33732490897</v>
+        <v>45840.80859800389</v>
       </c>
       <c r="E321">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F321" s="2">
-        <v>45838.72313657407</v>
+        <v>45840.62773148148</v>
       </c>
       <c r="G321">
         <v>0</v>
@@ -8374,16 +8374,16 @@
         <v>1</v>
       </c>
       <c r="C326">
-        <v>1068</v>
+        <v>1053</v>
       </c>
       <c r="D326" s="2">
-        <v>45839.88099823656</v>
+        <v>45840.80861854913</v>
       </c>
       <c r="E326">
-        <v>1068</v>
+        <v>1053</v>
       </c>
       <c r="F326" s="2">
-        <v>45839.68895833333</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G326">
         <v>0</v>
@@ -8870,16 +8870,16 @@
         <v>1</v>
       </c>
       <c r="C346">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D346" s="2">
-        <v>45839.88097972143</v>
+        <v>45840.80861854935</v>
       </c>
       <c r="E346">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F346" s="2">
-        <v>45839.41645833333</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G346">
         <v>0</v>
@@ -8991,16 +8991,16 @@
         <v>1</v>
       </c>
       <c r="C351">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="D351" s="2">
-        <v>45839.88101717404</v>
+        <v>45840.808618537</v>
       </c>
       <c r="E351">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="F351" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.68217592593</v>
       </c>
       <c r="G351">
         <v>0</v>
@@ -9066,16 +9066,16 @@
         <v>1</v>
       </c>
       <c r="C354">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D354" s="2">
-        <v>45839.33730493007</v>
+        <v>45840.8085979946</v>
       </c>
       <c r="E354">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="F354" s="2">
-        <v>45838.72134259259</v>
+        <v>45840.41077546297</v>
       </c>
       <c r="G354">
         <v>0</v>
@@ -9190,16 +9190,16 @@
         <v>1</v>
       </c>
       <c r="C359">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D359" s="2">
-        <v>45839.88099823437</v>
+        <v>45840.80859800289</v>
       </c>
       <c r="E359">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F359" s="2">
-        <v>45839.68684027778</v>
+        <v>45840.62070601852</v>
       </c>
       <c r="G359">
         <v>0</v>
@@ -9291,16 +9291,16 @@
         <v>1</v>
       </c>
       <c r="C363">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="D363" s="2">
-        <v>45839.33734443277</v>
+        <v>45840.80861855308</v>
       </c>
       <c r="E363">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="F363" s="2">
-        <v>45838.79094907407</v>
+        <v>45840.70496527778</v>
       </c>
       <c r="G363">
         <v>0</v>
@@ -9487,16 +9487,16 @@
         <v>1</v>
       </c>
       <c r="C371">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D371" s="2">
-        <v>45839.88099822834</v>
+        <v>45840.80859799654</v>
       </c>
       <c r="E371">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F371" s="2">
-        <v>45839.6484837963</v>
+        <v>45840.44622685185</v>
       </c>
       <c r="G371">
         <v>0</v>
@@ -9614,16 +9614,16 @@
         <v>1</v>
       </c>
       <c r="C376">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D376" s="2">
-        <v>45839.88099820774</v>
+        <v>45840.80861854956</v>
       </c>
       <c r="E376">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F376" s="2">
-        <v>45839.48964120371</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G376">
         <v>0</v>
@@ -9692,16 +9692,16 @@
         <v>1</v>
       </c>
       <c r="C379">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D379" s="2">
-        <v>45839.88099823161</v>
+        <v>45840.80861854977</v>
       </c>
       <c r="E379">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F379" s="2">
-        <v>45839.67738425926</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G379">
         <v>0</v>
@@ -9813,16 +9813,16 @@
         <v>1</v>
       </c>
       <c r="C384">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D384" s="2">
-        <v>45835.41886850383</v>
+        <v>45840.80861853438</v>
       </c>
       <c r="E384">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F384" s="2">
-        <v>45838.61395833334</v>
+        <v>45840.67901620371</v>
       </c>
       <c r="G384">
         <v>0</v>
@@ -9839,16 +9839,16 @@
         <v>1</v>
       </c>
       <c r="C385">
-        <v>109</v>
+        <v>209</v>
       </c>
       <c r="D385" s="2">
-        <v>45839.88101717416</v>
+        <v>45840.8086185365</v>
       </c>
       <c r="E385">
-        <v>109</v>
+        <v>209</v>
       </c>
       <c r="F385" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.68038194445</v>
       </c>
       <c r="G385">
         <v>0</v>
@@ -9969,16 +9969,16 @@
         <v>1</v>
       </c>
       <c r="C390">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="D390" s="2">
-        <v>45839.88099822598</v>
+        <v>45840.80859800404</v>
       </c>
       <c r="E390">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="F390" s="2">
-        <v>45839.63565972223</v>
+        <v>45840.62773148148</v>
       </c>
       <c r="G390">
         <v>0</v>
@@ -10070,16 +10070,16 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="D394" s="2">
-        <v>45839.8810171743</v>
+        <v>45840.80861854444</v>
       </c>
       <c r="E394">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="F394" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G394">
         <v>0</v>
@@ -10096,16 +10096,16 @@
         <v>1</v>
       </c>
       <c r="C395">
-        <v>-23</v>
+        <v>37</v>
       </c>
       <c r="D395" s="2">
-        <v>45839.88101717006</v>
+        <v>45840.80861855196</v>
       </c>
       <c r="E395">
-        <v>-23</v>
+        <v>37</v>
       </c>
       <c r="F395" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.70306712963</v>
       </c>
       <c r="G395">
         <v>0</v>
@@ -10269,16 +10269,16 @@
         <v>1</v>
       </c>
       <c r="C402">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="D402" s="2">
-        <v>45839.88099821527</v>
+        <v>45840.80859799884</v>
       </c>
       <c r="E402">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="F402" s="2">
-        <v>45839.54896990741</v>
+        <v>45840.48958333334</v>
       </c>
       <c r="G402">
         <v>0</v>
@@ -10321,16 +10321,16 @@
         <v>1</v>
       </c>
       <c r="C404">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="D404" s="2">
-        <v>45839.33728134477</v>
+        <v>45840.80861854469</v>
       </c>
       <c r="E404">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="F404" s="2">
-        <v>45838.38143518518</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G404">
         <v>0</v>
@@ -10445,16 +10445,16 @@
         <v>1</v>
       </c>
       <c r="C409">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D409" s="2">
-        <v>45814.82968397064</v>
+        <v>45840.80859800156</v>
       </c>
       <c r="E409">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F409" s="2">
-        <v>45814.49446759259</v>
+        <v>45840.54755787037</v>
       </c>
       <c r="G409">
         <v>0</v>
@@ -10471,16 +10471,16 @@
         <v>1</v>
       </c>
       <c r="C410">
-        <v>1657</v>
+        <v>1353</v>
       </c>
       <c r="D410" s="2">
-        <v>45839.88101717443</v>
+        <v>45840.80861854494</v>
       </c>
       <c r="E410">
-        <v>1657</v>
+        <v>1353</v>
       </c>
       <c r="F410" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G410">
         <v>0</v>
@@ -10673,16 +10673,16 @@
         <v>1</v>
       </c>
       <c r="C418">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D418" s="2">
-        <v>45839.88101717467</v>
+        <v>45840.80859800553</v>
       </c>
       <c r="E418">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F418" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.65059027778</v>
       </c>
       <c r="G418">
         <v>0</v>
@@ -11270,16 +11270,16 @@
         <v>1</v>
       </c>
       <c r="C442">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D442" s="2">
-        <v>45828.4052717349</v>
+        <v>45840.80861854996</v>
       </c>
       <c r="E442">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F442" s="2">
-        <v>45827.89302083333</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G442">
         <v>0</v>
@@ -11832,16 +11832,16 @@
         <v>1</v>
       </c>
       <c r="C465">
-        <v>-8</v>
+        <v>15</v>
       </c>
       <c r="D465" s="2">
-        <v>45839.88097972397</v>
+        <v>45840.80861855639</v>
       </c>
       <c r="E465">
-        <v>-8</v>
+        <v>15</v>
       </c>
       <c r="F465" s="2">
-        <v>45839.42005787037</v>
+        <v>45840.75590277778</v>
       </c>
       <c r="G465">
         <v>0</v>
@@ -11930,16 +11930,16 @@
         <v>1</v>
       </c>
       <c r="C469">
-        <v>2926</v>
+        <v>2906</v>
       </c>
       <c r="D469" s="2">
-        <v>45839.88101717018</v>
+        <v>45840.80861855018</v>
       </c>
       <c r="E469">
-        <v>2926</v>
+        <v>2906</v>
       </c>
       <c r="F469" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G469">
         <v>0</v>
@@ -12005,16 +12005,16 @@
         <v>1</v>
       </c>
       <c r="C472">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D472" s="2">
-        <v>45836.30888098924</v>
+        <v>45840.80861855447</v>
       </c>
       <c r="E472">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F472" s="2">
-        <v>45835.52792824074</v>
+        <v>45840.7230787037</v>
       </c>
       <c r="G472">
         <v>0</v>
@@ -12155,16 +12155,16 @@
         <v>1</v>
       </c>
       <c r="C478">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="D478" s="2">
-        <v>45814.82968397064</v>
+        <v>45840.80861853484</v>
       </c>
       <c r="E478">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="F478" s="2">
-        <v>45814.464375</v>
+        <v>45840.67962962963</v>
       </c>
       <c r="G478">
         <v>0</v>
@@ -12207,16 +12207,16 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="D480" s="2">
-        <v>45839.88099821862</v>
+        <v>45840.80861855725</v>
       </c>
       <c r="E480">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="F480" s="2">
-        <v>45839.55863425926</v>
+        <v>45840.75967592592</v>
       </c>
       <c r="G480">
         <v>0</v>
@@ -12334,16 +12334,16 @@
         <v>1</v>
       </c>
       <c r="C485">
-        <v>-4</v>
+        <v>8</v>
       </c>
       <c r="D485" s="2">
-        <v>45839.3373249156</v>
+        <v>45840.80859800074</v>
       </c>
       <c r="E485">
-        <v>-4</v>
+        <v>8</v>
       </c>
       <c r="F485" s="2">
-        <v>45838.77019675926</v>
+        <v>45840.53643518518</v>
       </c>
       <c r="G485">
         <v>0</v>
@@ -12637,16 +12637,16 @@
         <v>1</v>
       </c>
       <c r="C497">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D497" s="2">
-        <v>45799.89528859723</v>
+        <v>45840.80861853723</v>
       </c>
       <c r="E497">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F497" s="2">
-        <v>45784.64763888889</v>
+        <v>45840.68217592593</v>
       </c>
       <c r="G497">
         <v>0</v>
@@ -12951,16 +12951,16 @@
         <v>1</v>
       </c>
       <c r="C510">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="D510" s="2">
-        <v>45839.88101716859</v>
+        <v>45840.80861853746</v>
       </c>
       <c r="E510">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F510" s="2">
-        <v>45839.77019675926</v>
+        <v>45840.68217592593</v>
       </c>
       <c r="G510">
         <v>0</v>
@@ -13392,16 +13392,16 @@
         <v>1</v>
       </c>
       <c r="C528">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D528" s="2">
-        <v>45839.33730491703</v>
+        <v>45840.80859799535</v>
       </c>
       <c r="E528">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="F528" s="2">
-        <v>45838.49497685185</v>
+        <v>45840.42267361111</v>
       </c>
       <c r="G528">
         <v>0</v>
@@ -14389,16 +14389,16 @@
         <v>1</v>
       </c>
       <c r="C569">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="D569" s="2">
-        <v>45839.88099821052</v>
+        <v>45840.80861853981</v>
       </c>
       <c r="E569">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="F569" s="2">
-        <v>45839.49836805555</v>
+        <v>45840.68615740741</v>
       </c>
       <c r="G569">
         <v>0</v>
@@ -14415,16 +14415,16 @@
         <v>1</v>
       </c>
       <c r="C570">
-        <v>2501</v>
+        <v>2496</v>
       </c>
       <c r="D570" s="2">
-        <v>45839.8809982137</v>
+        <v>45840.80861853509</v>
       </c>
       <c r="E570">
-        <v>2501</v>
+        <v>2496</v>
       </c>
       <c r="F570" s="2">
-        <v>45839.54788194445</v>
+        <v>45840.67962962963</v>
       </c>
       <c r="G570">
         <v>0</v>
@@ -14510,16 +14510,16 @@
         <v>1</v>
       </c>
       <c r="C574">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D574" s="2">
-        <v>45839.88101717638</v>
+        <v>45840.80859800648</v>
       </c>
       <c r="E574">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F574" s="2">
-        <v>45839.78440972222</v>
+        <v>45840.67111111111</v>
       </c>
       <c r="G574">
         <v>0</v>
@@ -14677,16 +14677,16 @@
         <v>1</v>
       </c>
       <c r="C581">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="D581" s="2">
-        <v>45839.33730493072</v>
+        <v>45840.80859800016</v>
       </c>
       <c r="E581">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="F581" s="2">
-        <v>45838.72134259259</v>
+        <v>45840.51476851852</v>
       </c>
       <c r="G581">
         <v>0</v>
@@ -15158,16 +15158,16 @@
         <v>1</v>
       </c>
       <c r="C601">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="D601" s="2">
-        <v>45812.78303939045</v>
+        <v>45840.80861853769</v>
       </c>
       <c r="E601">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="F601" s="2">
-        <v>45812.43105324074</v>
+        <v>45840.68217592593</v>
       </c>
       <c r="G601">
         <v>0</v>
@@ -15878,16 +15878,16 @@
         <v>1</v>
       </c>
       <c r="C631">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D631" s="2">
-        <v>45839.88097971993</v>
+        <v>45840.80859799013</v>
       </c>
       <c r="E631">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F631" s="2">
-        <v>45839.39861111111</v>
+        <v>45840.37972222222</v>
       </c>
       <c r="G631">
         <v>0</v>
@@ -16509,16 +16509,16 @@
         <v>1</v>
       </c>
       <c r="C657">
-        <v>1824</v>
+        <v>1798</v>
       </c>
       <c r="D657" s="2">
-        <v>45839.88099821888</v>
+        <v>45840.80859800569</v>
       </c>
       <c r="E657">
-        <v>1824</v>
+        <v>1798</v>
       </c>
       <c r="F657" s="2">
-        <v>45839.55863425926</v>
+        <v>45840.65059027778</v>
       </c>
       <c r="G657">
         <v>0</v>
@@ -16535,16 +16535,16 @@
         <v>1</v>
       </c>
       <c r="C658">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D658" s="2">
-        <v>45839.88099822885</v>
+        <v>45840.80861854518</v>
       </c>
       <c r="E658">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F658" s="2">
-        <v>45839.6484837963</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G658">
         <v>0</v>
@@ -16584,16 +16584,16 @@
         <v>1</v>
       </c>
       <c r="C660">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="D660" s="2">
-        <v>45839.88101717649</v>
+        <v>45840.80861853534</v>
       </c>
       <c r="E660">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F660" s="2">
-        <v>45839.78440972222</v>
+        <v>45840.67962962963</v>
       </c>
       <c r="G660">
         <v>0</v>
@@ -17599,16 +17599,16 @@
         <v>1</v>
       </c>
       <c r="C701">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D701" s="2">
-        <v>45839.33734442785</v>
+        <v>45840.80859799901</v>
       </c>
       <c r="E701">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="F701" s="2">
-        <v>45838.77438657408</v>
+        <v>45840.48958333334</v>
       </c>
       <c r="G701">
         <v>0</v>
@@ -18072,16 +18072,16 @@
         <v>1</v>
       </c>
       <c r="C720">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D720" s="2">
-        <v>45839.88101717662</v>
+        <v>45840.80859799061</v>
       </c>
       <c r="E720">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F720" s="2">
-        <v>45839.78440972222</v>
+        <v>45840.37972222222</v>
       </c>
       <c r="G720">
         <v>0</v>
@@ -18098,16 +18098,16 @@
         <v>1</v>
       </c>
       <c r="C721">
-        <v>6</v>
+        <v>-9</v>
       </c>
       <c r="D721" s="2">
-        <v>45839.33734442807</v>
+        <v>45840.80859799754</v>
       </c>
       <c r="E721">
-        <v>6</v>
+        <v>-9</v>
       </c>
       <c r="F721" s="2">
-        <v>45838.77438657408</v>
+        <v>45840.48582175926</v>
       </c>
       <c r="G721">
         <v>0</v>
@@ -18228,16 +18228,16 @@
         <v>1</v>
       </c>
       <c r="C726">
-        <v>-20</v>
+        <v>-6</v>
       </c>
       <c r="D726" s="2">
-        <v>45839.88099823288</v>
+        <v>45840.80861855745</v>
       </c>
       <c r="E726">
-        <v>-20</v>
+        <v>-6</v>
       </c>
       <c r="F726" s="2">
-        <v>45839.68337962963</v>
+        <v>45840.75967592592</v>
       </c>
       <c r="G726">
         <v>0</v>
@@ -18381,16 +18381,16 @@
         <v>1</v>
       </c>
       <c r="C732">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D732" s="2">
-        <v>45839.88101717043</v>
+        <v>45840.8086185533</v>
       </c>
       <c r="E732">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F732" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.70496527778</v>
       </c>
       <c r="G732">
         <v>0</v>
@@ -19007,16 +19007,16 @@
         <v>1</v>
       </c>
       <c r="C757">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D757" s="2">
-        <v>45839.88099821913</v>
+        <v>45840.80861855041</v>
       </c>
       <c r="E757">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F757" s="2">
-        <v>45839.55863425926</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G757">
         <v>0</v>
@@ -19353,16 +19353,16 @@
         <v>1</v>
       </c>
       <c r="C771">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D771" s="2">
-        <v>45839.33730493113</v>
+        <v>45840.8085979918</v>
       </c>
       <c r="E771">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F771" s="2">
-        <v>45838.72134259259</v>
+        <v>45840.38353009259</v>
       </c>
       <c r="G771">
         <v>0</v>
@@ -19535,16 +19535,16 @@
         <v>1</v>
       </c>
       <c r="C778">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="D778" s="2">
-        <v>45839.33730492173</v>
+        <v>45840.80861853885</v>
       </c>
       <c r="E778">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="F778" s="2">
-        <v>45838.63927083334</v>
+        <v>45840.68482638889</v>
       </c>
       <c r="G778">
         <v>0</v>
@@ -20005,16 +20005,16 @@
         <v>1</v>
       </c>
       <c r="C797">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="D797" s="2">
-        <v>45839.88101717057</v>
+        <v>45840.80861855403</v>
       </c>
       <c r="E797">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="F797" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.7078587963</v>
       </c>
       <c r="G797">
         <v>0</v>
@@ -20331,16 +20331,16 @@
         <v>1</v>
       </c>
       <c r="C810">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="D810" s="2">
-        <v>45839.88101717079</v>
+        <v>45840.80861853389</v>
       </c>
       <c r="E810">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="F810" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.67560185185</v>
       </c>
       <c r="G810">
         <v>0</v>
@@ -20357,16 +20357,16 @@
         <v>1</v>
       </c>
       <c r="C811">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="D811" s="2">
-        <v>45839.88101717494</v>
+        <v>45840.80859800617</v>
       </c>
       <c r="E811">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F811" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.66892361111</v>
       </c>
       <c r="G811">
         <v>0</v>
@@ -20458,16 +20458,16 @@
         <v>1</v>
       </c>
       <c r="C815">
-        <v>-6</v>
+        <v>18</v>
       </c>
       <c r="D815" s="2">
-        <v>45839.88101717105</v>
+        <v>45840.80861853356</v>
       </c>
       <c r="E815">
-        <v>-6</v>
+        <v>18</v>
       </c>
       <c r="F815" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.67481481482</v>
       </c>
       <c r="G815">
         <v>0</v>
@@ -20732,16 +20732,16 @@
         <v>1</v>
       </c>
       <c r="C826">
-        <v>-23</v>
+        <v>-20</v>
       </c>
       <c r="D826" s="2">
-        <v>45839.88101716726</v>
+        <v>45840.80861855469</v>
       </c>
       <c r="E826">
-        <v>-23</v>
+        <v>-20</v>
       </c>
       <c r="F826" s="2">
-        <v>45839.73105324074</v>
+        <v>45840.7236574074</v>
       </c>
       <c r="G826">
         <v>0</v>
@@ -21724,7 +21724,7 @@
         <v>0</v>
       </c>
       <c r="F866" s="2">
-        <v>45832.60554398148</v>
+        <v>45840.7325462963</v>
       </c>
       <c r="G866">
         <v>0</v>
@@ -21868,16 +21868,16 @@
         <v>1</v>
       </c>
       <c r="C872">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="D872" s="2">
-        <v>45839.88099822698</v>
+        <v>45840.80859800176</v>
       </c>
       <c r="E872">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="F872" s="2">
-        <v>45839.63565972223</v>
+        <v>45840.54755787037</v>
       </c>
       <c r="G872">
         <v>0</v>
@@ -22145,16 +22145,16 @@
         <v>1</v>
       </c>
       <c r="C883">
-        <v>15</v>
+        <v>468</v>
       </c>
       <c r="D883" s="2">
-        <v>45839.88101717508</v>
+        <v>45840.80861855511</v>
       </c>
       <c r="E883">
-        <v>15</v>
+        <v>468</v>
       </c>
       <c r="F883" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.73126157407</v>
       </c>
       <c r="G883">
         <v>0</v>
@@ -22171,16 +22171,16 @@
         <v>1</v>
       </c>
       <c r="C884">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D884" s="2">
-        <v>45839.88099822911</v>
+        <v>45840.80859799209</v>
       </c>
       <c r="E884">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F884" s="2">
-        <v>45839.6484837963</v>
+        <v>45840.38353009259</v>
       </c>
       <c r="G884">
         <v>0</v>
@@ -22272,16 +22272,16 @@
         <v>1</v>
       </c>
       <c r="C888">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="D888" s="2">
-        <v>45839.88099821591</v>
+        <v>45840.80861855353</v>
       </c>
       <c r="E888">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="F888" s="2">
-        <v>45839.54896990741</v>
+        <v>45840.70496527778</v>
       </c>
       <c r="G888">
         <v>0</v>
@@ -22627,16 +22627,16 @@
         <v>1</v>
       </c>
       <c r="C902">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D902" s="2">
-        <v>45839.88099820951</v>
+        <v>45840.8085979967</v>
       </c>
       <c r="E902">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F902" s="2">
-        <v>45839.49008101852</v>
+        <v>45840.44622685185</v>
       </c>
       <c r="G902">
         <v>0</v>
@@ -22806,16 +22806,16 @@
         <v>1</v>
       </c>
       <c r="C909">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D909" s="2">
-        <v>45839.33732491606</v>
+        <v>45840.80859799602</v>
       </c>
       <c r="E909">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F909" s="2">
-        <v>45838.77019675926</v>
+        <v>45840.44586805555</v>
       </c>
       <c r="G909">
         <v>0</v>
@@ -23187,16 +23187,16 @@
         <v>1</v>
       </c>
       <c r="C924">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="D924" s="2">
-        <v>45839.88099821993</v>
+        <v>45840.80859799771</v>
       </c>
       <c r="E924">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="F924" s="2">
-        <v>45839.55863425926</v>
+        <v>45840.48582175926</v>
       </c>
       <c r="G924">
         <v>0</v>
@@ -23695,16 +23695,16 @@
         <v>1</v>
       </c>
       <c r="C944">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D944" s="2">
-        <v>45839.33732491089</v>
+        <v>45840.80859799346</v>
       </c>
       <c r="E944">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="F944" s="2">
-        <v>45838.73396990741</v>
+        <v>45840.39509259259</v>
       </c>
       <c r="G944">
         <v>0</v>
@@ -24136,16 +24136,16 @@
         <v>1</v>
       </c>
       <c r="C962">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="D962" s="2">
-        <v>45839.33730493139</v>
+        <v>45840.80861855061</v>
       </c>
       <c r="E962">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="F962" s="2">
-        <v>45838.72134259259</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G962">
         <v>0</v>
@@ -24162,16 +24162,16 @@
         <v>1</v>
       </c>
       <c r="C963">
-        <v>1455</v>
+        <v>1442</v>
       </c>
       <c r="D963" s="2">
-        <v>45839.88101716338</v>
+        <v>45840.80859799918</v>
       </c>
       <c r="E963">
-        <v>1455</v>
+        <v>1442</v>
       </c>
       <c r="F963" s="2">
-        <v>45839.68895833333</v>
+        <v>45840.48958333334</v>
       </c>
       <c r="G963">
         <v>0</v>
@@ -24999,16 +24999,16 @@
         <v>1</v>
       </c>
       <c r="C996">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D996" s="2">
-        <v>45839.33730492187</v>
+        <v>45840.80861854541</v>
       </c>
       <c r="E996">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="F996" s="2">
-        <v>45838.64166666667</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G996">
         <v>0</v>
@@ -25155,16 +25155,16 @@
         <v>1</v>
       </c>
       <c r="C1002">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D1002" s="2">
-        <v>45839.33732490925</v>
+        <v>45840.80861855081</v>
       </c>
       <c r="E1002">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F1002" s="2">
-        <v>45838.72313657407</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G1002">
         <v>0</v>
@@ -25533,16 +25533,16 @@
         <v>1</v>
       </c>
       <c r="C1017">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="D1017" s="2">
-        <v>45839.88099822935</v>
+        <v>45840.80859800454</v>
       </c>
       <c r="E1017">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="F1017" s="2">
-        <v>45839.6484837963</v>
+        <v>45840.6453587963</v>
       </c>
       <c r="G1017">
         <v>0</v>
@@ -25712,16 +25712,16 @@
         <v>1</v>
       </c>
       <c r="C1024">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D1024" s="2">
-        <v>45839.33730493154</v>
+        <v>45840.808618551</v>
       </c>
       <c r="E1024">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="F1024" s="2">
-        <v>45838.72134259259</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G1024">
         <v>0</v>
@@ -26676,16 +26676,16 @@
         <v>1</v>
       </c>
       <c r="C1062">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="D1062" s="2">
-        <v>45839.3373444333</v>
+        <v>45840.80859800585</v>
       </c>
       <c r="E1062">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="F1062" s="2">
-        <v>45838.79094907407</v>
+        <v>45840.65059027778</v>
       </c>
       <c r="G1062">
         <v>0</v>
@@ -27841,16 +27841,16 @@
         <v>1</v>
       </c>
       <c r="C1109">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1109" s="2">
-        <v>45795.04201639877</v>
+        <v>45840.80861855682</v>
       </c>
       <c r="E1109">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1109" s="2">
-        <v>45712.67925925926</v>
+        <v>45840.67798611111</v>
       </c>
       <c r="G1109">
         <v>0</v>
@@ -27867,16 +27867,16 @@
         <v>1</v>
       </c>
       <c r="C1110">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D1110" s="2">
-        <v>45836.30888099061</v>
+        <v>45840.80859800192</v>
       </c>
       <c r="E1110">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F1110" s="2">
-        <v>45835.52792824074</v>
+        <v>45840.54755787037</v>
       </c>
       <c r="G1110">
         <v>0</v>
@@ -28173,16 +28173,16 @@
         <v>1</v>
       </c>
       <c r="C1122">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D1122" s="2">
-        <v>45839.88097972424</v>
+        <v>45840.8085980042</v>
       </c>
       <c r="E1122">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F1122" s="2">
-        <v>45839.42005787037</v>
+        <v>45840.62773148148</v>
       </c>
       <c r="G1122">
         <v>0</v>
@@ -28274,16 +28274,16 @@
         <v>1</v>
       </c>
       <c r="C1126">
-        <v>648</v>
+        <v>612</v>
       </c>
       <c r="D1126" s="2">
-        <v>45839.33730493201</v>
+        <v>45840.80861854563</v>
       </c>
       <c r="E1126">
-        <v>648</v>
+        <v>612</v>
       </c>
       <c r="F1126" s="2">
-        <v>45838.72134259259</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G1126">
         <v>0</v>
@@ -28935,16 +28935,16 @@
         <v>1</v>
       </c>
       <c r="C1152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1152" s="2">
-        <v>45839.3373249113</v>
+        <v>45840.80859800323</v>
       </c>
       <c r="E1152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1152" s="2">
-        <v>45838.73396990741</v>
+        <v>45840.62177083334</v>
       </c>
       <c r="G1152">
         <v>0</v>
@@ -28987,16 +28987,16 @@
         <v>1</v>
       </c>
       <c r="C1154">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D1154" s="2">
-        <v>45835.41884528493</v>
+        <v>45840.80859799787</v>
       </c>
       <c r="E1154">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F1154" s="2">
-        <v>45834.66123842593</v>
+        <v>45840.48582175926</v>
       </c>
       <c r="G1154">
         <v>0</v>
@@ -29013,16 +29013,16 @@
         <v>1</v>
       </c>
       <c r="C1155">
-        <v>2</v>
+        <v>-13</v>
       </c>
       <c r="D1155" s="2">
-        <v>45839.88097972023</v>
+        <v>45840.80859799803</v>
       </c>
       <c r="E1155">
-        <v>2</v>
+        <v>-13</v>
       </c>
       <c r="F1155" s="2">
-        <v>45839.39861111111</v>
+        <v>45840.48582175926</v>
       </c>
       <c r="G1155">
         <v>0</v>
@@ -29986,16 +29986,16 @@
         <v>1</v>
       </c>
       <c r="C1193">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="D1193" s="2">
-        <v>45839.88099823135</v>
+        <v>45840.80861855121</v>
       </c>
       <c r="E1193">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="F1193" s="2">
-        <v>45839.6762037037</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G1193">
         <v>0</v>
@@ -30038,16 +30038,16 @@
         <v>1</v>
       </c>
       <c r="C1195">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1195" s="2">
-        <v>45839.33730491848</v>
+        <v>45840.80859799503</v>
       </c>
       <c r="E1195">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1195" s="2">
-        <v>45838.50037037037</v>
+        <v>45840.42232638889</v>
       </c>
       <c r="G1195">
         <v>0</v>
@@ -31528,16 +31528,16 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>1120</v>
+        <v>1095</v>
       </c>
       <c r="D1253" s="2">
-        <v>45839.88101717134</v>
+        <v>45840.80859799821</v>
       </c>
       <c r="E1253">
-        <v>1120</v>
+        <v>1095</v>
       </c>
       <c r="F1253" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.48582175926</v>
       </c>
       <c r="G1253">
         <v>0</v>
@@ -31577,16 +31577,16 @@
         <v>1</v>
       </c>
       <c r="C1255">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="D1255" s="2">
-        <v>45839.33732491167</v>
+        <v>45840.80859799999</v>
       </c>
       <c r="E1255">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="F1255" s="2">
-        <v>45838.73396990741</v>
+        <v>45840.51420138889</v>
       </c>
       <c r="G1255">
         <v>0</v>
@@ -32348,16 +32348,16 @@
         <v>1</v>
       </c>
       <c r="C1285">
-        <v>-5</v>
+        <v>245</v>
       </c>
       <c r="D1285" s="2">
-        <v>45839.33732491176</v>
+        <v>45840.80859799966</v>
       </c>
       <c r="E1285">
-        <v>-5</v>
+        <v>245</v>
       </c>
       <c r="F1285" s="2">
-        <v>45838.73396990741</v>
+        <v>45840.51243055556</v>
       </c>
       <c r="G1285">
         <v>0</v>
@@ -33540,16 +33540,16 @@
         <v>1</v>
       </c>
       <c r="C1332">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D1332" s="2">
-        <v>45839.88101716472</v>
+        <v>45840.80861853933</v>
       </c>
       <c r="E1332">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F1332" s="2">
-        <v>45839.68895833333</v>
+        <v>45840.68561342593</v>
       </c>
       <c r="G1332">
         <v>0</v>
@@ -33791,16 +33791,16 @@
         <v>1</v>
       </c>
       <c r="C1342">
-        <v>1201</v>
+        <v>1133</v>
       </c>
       <c r="D1342" s="2">
-        <v>45839.88099821626</v>
+        <v>45840.80859800601</v>
       </c>
       <c r="E1342">
-        <v>1201</v>
+        <v>1133</v>
       </c>
       <c r="F1342" s="2">
-        <v>45839.54896990741</v>
+        <v>45840.65059027778</v>
       </c>
       <c r="G1342">
         <v>0</v>
@@ -34481,16 +34481,16 @@
         <v>1</v>
       </c>
       <c r="C1369">
-        <v>-1</v>
+        <v>43</v>
       </c>
       <c r="D1369" s="2">
-        <v>45836.30888098675</v>
+        <v>45840.80861854611</v>
       </c>
       <c r="E1369">
-        <v>-1</v>
+        <v>43</v>
       </c>
       <c r="F1369" s="2">
-        <v>45835.41170138889</v>
+        <v>45840.69929398148</v>
       </c>
       <c r="G1369">
         <v>0</v>
@@ -34966,16 +34966,16 @@
         <v>1</v>
       </c>
       <c r="C1388">
-        <v>-29</v>
+        <v>221</v>
       </c>
       <c r="D1388" s="2">
-        <v>45839.33732491187</v>
+        <v>45840.80859799376</v>
       </c>
       <c r="E1388">
-        <v>-29</v>
+        <v>221</v>
       </c>
       <c r="F1388" s="2">
-        <v>45838.73396990741</v>
+        <v>45840.39947916667</v>
       </c>
       <c r="G1388">
         <v>0</v>
@@ -35298,16 +35298,16 @@
         <v>1</v>
       </c>
       <c r="C1401">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D1401" s="2">
-        <v>45839.3373049325</v>
+        <v>45840.80859800257</v>
       </c>
       <c r="E1401">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F1401" s="2">
-        <v>45838.72134259259</v>
+        <v>45840.39284722223</v>
       </c>
       <c r="G1401">
         <v>0</v>
@@ -35347,16 +35347,16 @@
         <v>1</v>
       </c>
       <c r="C1403">
-        <v>-45</v>
+        <v>-4</v>
       </c>
       <c r="D1403" s="2">
-        <v>45839.33730492424</v>
+        <v>45840.80861855425</v>
       </c>
       <c r="E1403">
-        <v>-45</v>
+        <v>-4</v>
       </c>
       <c r="F1403" s="2">
-        <v>45838.66369212963</v>
+        <v>45840.72278935185</v>
       </c>
       <c r="G1403">
         <v>0</v>
@@ -35555,16 +35555,16 @@
         <v>1</v>
       </c>
       <c r="C1411">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D1411" s="2">
-        <v>45839.33732491267</v>
+        <v>45840.80859800633</v>
       </c>
       <c r="E1411">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="F1411" s="2">
-        <v>45838.76650462963</v>
+        <v>45840.66932870371</v>
       </c>
       <c r="G1411">
         <v>0</v>
@@ -35581,16 +35581,16 @@
         <v>1</v>
       </c>
       <c r="C1412">
-        <v>37</v>
+        <v>-13</v>
       </c>
       <c r="D1412" s="2">
-        <v>45839.88101716487</v>
+        <v>45840.80861853957</v>
       </c>
       <c r="E1412">
-        <v>37</v>
+        <v>-13</v>
       </c>
       <c r="F1412" s="2">
-        <v>45839.68895833333</v>
+        <v>45840.68561342593</v>
       </c>
       <c r="G1412">
         <v>0</v>
@@ -35809,16 +35809,16 @@
         <v>1</v>
       </c>
       <c r="C1421">
-        <v>-1</v>
+        <v>49</v>
       </c>
       <c r="D1421" s="2">
-        <v>45839.33732491616</v>
+        <v>45840.808598007</v>
       </c>
       <c r="E1421">
-        <v>-1</v>
+        <v>49</v>
       </c>
       <c r="F1421" s="2">
-        <v>45838.77019675926</v>
+        <v>45840.67443287037</v>
       </c>
       <c r="G1421">
         <v>0</v>
@@ -36453,16 +36453,16 @@
         <v>1</v>
       </c>
       <c r="C1446">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D1446" s="2">
-        <v>45839.33728134513</v>
+        <v>45840.80859799092</v>
       </c>
       <c r="E1446">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F1446" s="2">
-        <v>45838.38143518518</v>
+        <v>45840.37972222222</v>
       </c>
       <c r="G1446">
         <v>0</v>
@@ -36505,16 +36505,16 @@
         <v>1</v>
       </c>
       <c r="C1448">
-        <v>93</v>
+        <v>-3</v>
       </c>
       <c r="D1448" s="2">
-        <v>45839.33732491624</v>
+        <v>45840.80859799934</v>
       </c>
       <c r="E1448">
-        <v>93</v>
+        <v>-3</v>
       </c>
       <c r="F1448" s="2">
-        <v>45838.77019675926</v>
+        <v>45840.48958333334</v>
       </c>
       <c r="G1448">
         <v>0</v>
@@ -36583,16 +36583,16 @@
         <v>1</v>
       </c>
       <c r="C1451">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D1451" s="2">
-        <v>45839.88099820743</v>
+        <v>45840.80861853413</v>
       </c>
       <c r="E1451">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F1451" s="2">
-        <v>45607.63697916667</v>
+        <v>45840.67635416667</v>
       </c>
       <c r="G1451">
         <v>0</v>
@@ -37382,16 +37382,16 @@
         <v>1</v>
       </c>
       <c r="C1483">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="D1483" s="2">
-        <v>45835.41886853277</v>
+        <v>45840.80859799687</v>
       </c>
       <c r="E1483">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="F1483" s="2">
-        <v>45835.41170138889</v>
+        <v>45840.44622685185</v>
       </c>
       <c r="G1483">
         <v>0</v>
@@ -37861,16 +37861,16 @@
         <v>1</v>
       </c>
       <c r="C1502">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1502" s="2">
-        <v>45795.04190003897</v>
+        <v>45840.80861855661</v>
       </c>
       <c r="E1502">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F1502" s="2">
-        <v>45660.45600694444</v>
+        <v>45840.37972222222</v>
       </c>
       <c r="G1502">
         <v>0</v>
@@ -37991,16 +37991,16 @@
         <v>1</v>
       </c>
       <c r="C1507">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="D1507" s="2">
-        <v>45839.33734442838</v>
+        <v>45840.80861855143</v>
       </c>
       <c r="E1507">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="F1507" s="2">
-        <v>45838.77438657408</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G1507">
         <v>0</v>
@@ -39245,16 +39245,16 @@
         <v>1</v>
       </c>
       <c r="C1558">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D1558" s="2">
-        <v>45839.33730493266</v>
+        <v>45840.80859800436</v>
       </c>
       <c r="E1558">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F1558" s="2">
-        <v>45838.72134259259</v>
+        <v>45840.62773148148</v>
       </c>
       <c r="G1558">
         <v>0</v>
@@ -39473,16 +39473,16 @@
         <v>1</v>
       </c>
       <c r="C1567">
-        <v>0</v>
+        <v>-140</v>
       </c>
       <c r="D1567" s="2">
-        <v>45818.30486084452</v>
+        <v>45840.80861853558</v>
       </c>
       <c r="E1567">
-        <v>0</v>
+        <v>-140</v>
       </c>
       <c r="F1567" s="2">
-        <v>45838.78050925926</v>
+        <v>45840.67962962963</v>
       </c>
       <c r="G1567">
         <v>0</v>
@@ -39704,16 +39704,16 @@
         <v>1</v>
       </c>
       <c r="C1576">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D1576" s="2">
-        <v>45835.41886853368</v>
+        <v>45840.80859799566</v>
       </c>
       <c r="E1576">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F1576" s="2">
-        <v>45835.41170138889</v>
+        <v>45840.42353009259</v>
       </c>
       <c r="G1576">
         <v>0</v>
@@ -40148,16 +40148,16 @@
         <v>1</v>
       </c>
       <c r="C1594">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D1594" s="2">
-        <v>45839.88099822721</v>
+        <v>45840.80861855175</v>
       </c>
       <c r="E1594">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F1594" s="2">
-        <v>45839.63565972223</v>
+        <v>45840.70297453704</v>
       </c>
       <c r="G1594">
         <v>0</v>
@@ -40226,16 +40226,16 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>4346</v>
+        <v>4190</v>
       </c>
       <c r="D1597" s="2">
-        <v>45839.88101717736</v>
+        <v>45840.80861855596</v>
       </c>
       <c r="E1597">
-        <v>4346</v>
+        <v>4190</v>
       </c>
       <c r="F1597" s="2">
-        <v>45839.78440972222</v>
+        <v>45840.7536574074</v>
       </c>
       <c r="G1597">
         <v>0</v>
@@ -41193,16 +41193,16 @@
         <v>1</v>
       </c>
       <c r="C1635">
-        <v>2358</v>
+        <v>1734</v>
       </c>
       <c r="D1635" s="2">
-        <v>45839.33732491652</v>
+        <v>45840.80861853581</v>
       </c>
       <c r="E1635">
-        <v>2358</v>
+        <v>1734</v>
       </c>
       <c r="F1635" s="2">
-        <v>45838.77019675926</v>
+        <v>45840.67962962963</v>
       </c>
       <c r="G1635">
         <v>0</v>
@@ -41680,16 +41680,16 @@
         <v>1</v>
       </c>
       <c r="C1655">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D1655" s="2">
-        <v>45806.77600903736</v>
+        <v>45840.80861853791</v>
       </c>
       <c r="E1655">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="F1655" s="2">
-        <v>45806.51422453704</v>
+        <v>45840.68217592593</v>
       </c>
       <c r="G1655">
         <v>0</v>
@@ -41706,16 +41706,16 @@
         <v>1</v>
       </c>
       <c r="C1656">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D1656" s="2">
-        <v>45839.33734443568</v>
+        <v>45840.80859800208</v>
       </c>
       <c r="E1656">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F1656" s="2">
-        <v>45838.8253125</v>
+        <v>45840.54755787037</v>
       </c>
       <c r="G1656">
         <v>0</v>
@@ -43707,16 +43707,16 @@
         <v>1</v>
       </c>
       <c r="C1737">
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="D1737" s="2">
-        <v>45839.88101717747</v>
+        <v>45840.80861854168</v>
       </c>
       <c r="E1737">
-        <v>-6</v>
+        <v>6</v>
       </c>
       <c r="F1737" s="2">
-        <v>45839.78440972222</v>
+        <v>45840.69471064815</v>
       </c>
       <c r="G1737">
         <v>0</v>
@@ -43759,16 +43759,16 @@
         <v>1</v>
       </c>
       <c r="C1739">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D1739" s="2">
-        <v>45839.33730491971</v>
+        <v>45840.80859800307</v>
       </c>
       <c r="E1739">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F1739" s="2">
-        <v>45838.53253472222</v>
+        <v>45840.62070601852</v>
       </c>
       <c r="G1739">
         <v>0</v>
@@ -44099,16 +44099,16 @@
         <v>1</v>
       </c>
       <c r="C1753">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D1753" s="2">
-        <v>45839.88101717535</v>
+        <v>45840.80861855491</v>
       </c>
       <c r="E1753">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F1753" s="2">
-        <v>45839.78400462963</v>
+        <v>45840.72748842592</v>
       </c>
       <c r="G1753">
         <v>0</v>
@@ -44930,16 +44930,16 @@
         <v>1</v>
       </c>
       <c r="C1786">
-        <v>-48</v>
+        <v>0</v>
       </c>
       <c r="D1786" s="2">
-        <v>45839.88099822984</v>
+        <v>45840.80861854142</v>
       </c>
       <c r="E1786">
-        <v>-48</v>
+        <v>0</v>
       </c>
       <c r="F1786" s="2">
-        <v>45839.6484837963</v>
+        <v>45840.69409722222</v>
       </c>
       <c r="G1786">
         <v>0</v>
@@ -45871,16 +45871,16 @@
         <v>1</v>
       </c>
       <c r="C1823">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D1823" s="2">
-        <v>45835.41884528953</v>
+        <v>45840.8085979955</v>
       </c>
       <c r="E1823">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F1823" s="2">
-        <v>45834.68826388889</v>
+        <v>45840.42267361111</v>
       </c>
       <c r="G1823">
         <v>0</v>
@@ -46405,16 +46405,16 @@
         <v>1</v>
       </c>
       <c r="C1844">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="D1844" s="2">
-        <v>45839.337344436</v>
+        <v>45840.8085979995</v>
       </c>
       <c r="E1844">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="F1844" s="2">
-        <v>45839.36480324074</v>
+        <v>45840.48958333334</v>
       </c>
       <c r="G1844">
         <v>0</v>
@@ -48463,16 +48463,16 @@
         <v>1</v>
       </c>
       <c r="C1925">
-        <v>-1</v>
+        <v>23</v>
       </c>
       <c r="D1925" s="2">
-        <v>45839.8809982101</v>
+        <v>45840.80859799319</v>
       </c>
       <c r="E1925">
-        <v>-1</v>
+        <v>23</v>
       </c>
       <c r="F1925" s="2">
-        <v>45839.49008101852</v>
+        <v>45840.39346064815</v>
       </c>
       <c r="G1925">
         <v>0</v>
@@ -49017,16 +49017,16 @@
         <v>1</v>
       </c>
       <c r="C1947">
-        <v>-8</v>
+        <v>2</v>
       </c>
       <c r="D1947" s="2">
-        <v>45839.8810171684</v>
+        <v>45840.80859799405</v>
       </c>
       <c r="E1947">
-        <v>-8</v>
+        <v>2</v>
       </c>
       <c r="F1947" s="2">
-        <v>45839.75399305556</v>
+        <v>45840.40810185186</v>
       </c>
       <c r="G1947">
         <v>0</v>
@@ -49043,16 +49043,16 @@
         <v>1</v>
       </c>
       <c r="C1948">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D1948" s="2">
-        <v>45839.88101716914</v>
+        <v>45840.80861853814</v>
       </c>
       <c r="E1948">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F1948" s="2">
-        <v>45839.77019675926</v>
+        <v>45840.68217592593</v>
       </c>
       <c r="G1948">
         <v>0</v>
@@ -51065,16 +51065,16 @@
         <v>1</v>
       </c>
       <c r="C2029">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="D2029" s="2">
-        <v>45839.33732491671</v>
+        <v>45840.80859800032</v>
       </c>
       <c r="E2029">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F2029" s="2">
-        <v>45838.77019675926</v>
+        <v>45840.51508101852</v>
       </c>
       <c r="G2029">
         <v>0</v>
@@ -52032,16 +52032,16 @@
         <v>1</v>
       </c>
       <c r="C2067">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D2067" s="2">
-        <v>45839.33730492453</v>
+        <v>45840.80861854587</v>
       </c>
       <c r="E2067">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F2067" s="2">
-        <v>45838.66369212963</v>
+        <v>45840.69724537037</v>
       </c>
       <c r="G2067">
         <v>0</v>
@@ -52912,16 +52912,16 @@
         <v>1</v>
       </c>
       <c r="C2102">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="D2102" s="2">
-        <v>45795.04177855738</v>
+        <v>45840.80861853837</v>
       </c>
       <c r="E2102">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="F2102" s="2">
-        <v>45505.47642361111</v>
+        <v>45840.68217592593</v>
       </c>
       <c r="G2102">
         <v>0</v>
@@ -53186,16 +53186,16 @@
         <v>1</v>
       </c>
       <c r="C2113">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D2113" s="2">
-        <v>45839.33732490797</v>
+        <v>45840.80861853859</v>
       </c>
       <c r="E2113">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F2113" s="2">
-        <v>45839.68895833333</v>
+        <v>45840.68248842593</v>
       </c>
       <c r="G2113">
         <v>0</v>
@@ -56354,16 +56354,16 @@
         <v>1</v>
       </c>
       <c r="C2239">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D2239" s="2">
-        <v>45795.04199234088</v>
+        <v>45840.8086358626</v>
       </c>
       <c r="E2239">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F2239" s="2">
-        <v>45700.79064814815</v>
+        <v>45840.75967592592</v>
       </c>
       <c r="G2239">
         <v>0</v>
@@ -58561,16 +58561,16 @@
         <v>1</v>
       </c>
       <c r="C2327">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2327" s="2">
-        <v>45839.3373444286</v>
+        <v>45840.80861854018</v>
       </c>
       <c r="E2327">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2327" s="2">
-        <v>45838.77438657408</v>
+        <v>45840.68648148148</v>
       </c>
       <c r="G2327">
         <v>0</v>
@@ -58587,16 +58587,16 @@
         <v>1</v>
       </c>
       <c r="C2328">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D2328" s="2">
-        <v>45831.83461824009</v>
+        <v>45840.80861854043</v>
       </c>
       <c r="E2328">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F2328" s="2">
-        <v>45831.46164351852</v>
+        <v>45840.68708333333</v>
       </c>
       <c r="G2328">
         <v>0</v>
@@ -60023,16 +60023,16 @@
         <v>1</v>
       </c>
       <c r="C2386">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D2386" s="2">
-        <v>45839.33732491416</v>
+        <v>45840.80859800058</v>
       </c>
       <c r="E2386">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F2386" s="2">
-        <v>45838.7684375</v>
+        <v>45840.53359953704</v>
       </c>
       <c r="G2386">
         <v>0</v>
@@ -60779,16 +60779,16 @@
         <v>1</v>
       </c>
       <c r="C2416">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D2416" s="2">
-        <v>45839.88101717259</v>
+        <v>45840.8085980024</v>
       </c>
       <c r="E2416">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="F2416" s="2">
-        <v>45839.78326388889</v>
+        <v>45840.57128472222</v>
       </c>
       <c r="G2416">
         <v>0</v>
@@ -60880,16 +60880,16 @@
         <v>1</v>
       </c>
       <c r="C2420">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D2420" s="2">
-        <v>45839.33730492745</v>
+        <v>45840.80859799237</v>
       </c>
       <c r="E2420">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F2420" s="2">
-        <v>45838.71241898148</v>
+        <v>45840.38622685185</v>
       </c>
       <c r="G2420">
         <v>0</v>
@@ -61987,16 +61987,16 @@
         <v>1</v>
       </c>
       <c r="C2465">
-        <v>11</v>
+        <v>-13</v>
       </c>
       <c r="D2465" s="2">
-        <v>45833.77618177306</v>
+        <v>45840.80859800356</v>
       </c>
       <c r="E2465">
-        <v>11</v>
+        <v>-13</v>
       </c>
       <c r="F2465" s="2">
-        <v>45833.44604166667</v>
+        <v>45840.62440972222</v>
       </c>
       <c r="G2465">
         <v>0</v>
@@ -62203,16 +62203,16 @@
         <v>1</v>
       </c>
       <c r="C2474">
-        <v>-15</v>
+        <v>12</v>
       </c>
       <c r="D2474" s="2">
-        <v>45835.41886850681</v>
+        <v>45840.80861854095</v>
       </c>
       <c r="E2474">
-        <v>-15</v>
+        <v>12</v>
       </c>
       <c r="F2474" s="2">
-        <v>45838.61395833334</v>
+        <v>45840.68773148148</v>
       </c>
       <c r="G2474">
         <v>0</v>
@@ -62428,16 +62428,16 @@
         <v>1</v>
       </c>
       <c r="C2483">
-        <v>851</v>
+        <v>841</v>
       </c>
       <c r="D2483" s="2">
-        <v>45839.88099821725</v>
+        <v>45840.80861855375</v>
       </c>
       <c r="E2483">
-        <v>851</v>
+        <v>841</v>
       </c>
       <c r="F2483" s="2">
-        <v>45839.54896990741</v>
+        <v>45840.70496527778</v>
       </c>
       <c r="G2483">
         <v>0</v>
@@ -62532,16 +62532,16 @@
         <v>1</v>
       </c>
       <c r="C2487">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="D2487" s="2">
-        <v>45839.88097972114</v>
+        <v>45840.80859799265</v>
       </c>
       <c r="E2487">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="F2487" s="2">
-        <v>45839.40539351852</v>
+        <v>45840.39229166666</v>
       </c>
       <c r="G2487">
         <v>0</v>
@@ -63736,16 +63736,16 @@
         <v>1</v>
       </c>
       <c r="C2537">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="D2537" s="2">
-        <v>45839.33732490848</v>
+        <v>45840.80859799123</v>
       </c>
       <c r="E2537">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F2537" s="2">
-        <v>45838.72134259259</v>
+        <v>45840.38086805555</v>
       </c>
       <c r="G2537">
         <v>0</v>
@@ -63834,16 +63834,16 @@
         <v>1</v>
       </c>
       <c r="C2541">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="D2541" s="2">
-        <v>45839.88097972471</v>
+        <v>45840.80861853605</v>
       </c>
       <c r="E2541">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="F2541" s="2">
-        <v>45839.42005787037</v>
+        <v>45840.68011574074</v>
       </c>
       <c r="G2541">
         <v>0</v>
@@ -65082,16 +65082,16 @@
         <v>1</v>
       </c>
       <c r="C2592">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="D2592" s="2">
-        <v>45839.88099821752</v>
+        <v>45840.80859799703</v>
       </c>
       <c r="E2592">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="F2592" s="2">
-        <v>45839.39861111111</v>
+        <v>45840.46775462963</v>
       </c>
       <c r="G2592">
         <v>0</v>
@@ -65108,16 +65108,16 @@
         <v>1</v>
       </c>
       <c r="C2593">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="D2593" s="2">
-        <v>45839.88099821776</v>
+        <v>45840.8085979972</v>
       </c>
       <c r="E2593">
-        <v>-25</v>
+        <v>0</v>
       </c>
       <c r="F2593" s="2">
-        <v>45839.39861111111</v>
+        <v>45840.46829861111</v>
       </c>
       <c r="G2593">
         <v>0</v>
@@ -65267,6 +65267,81 @@
         <v>0</v>
       </c>
       <c r="H2599" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:8">
+      <c r="A2600">
+        <v>43993277</v>
+      </c>
+      <c r="B2600">
+        <v>1</v>
+      </c>
+      <c r="C2600">
+        <v>0</v>
+      </c>
+      <c r="D2600" s="2">
+        <v>45840.8085979957</v>
+      </c>
+      <c r="E2600">
+        <v>0</v>
+      </c>
+      <c r="G2600">
+        <v>0</v>
+      </c>
+      <c r="H2600" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:8">
+      <c r="A2601">
+        <v>43996292</v>
+      </c>
+      <c r="B2601">
+        <v>1</v>
+      </c>
+      <c r="C2601">
+        <v>0</v>
+      </c>
+      <c r="D2601" s="2">
+        <v>45840.80861853656</v>
+      </c>
+      <c r="E2601">
+        <v>0</v>
+      </c>
+      <c r="F2601" s="2">
+        <v>45840.68118055556</v>
+      </c>
+      <c r="G2601">
+        <v>0</v>
+      </c>
+      <c r="H2601" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:8">
+      <c r="A2602">
+        <v>44002959</v>
+      </c>
+      <c r="B2602">
+        <v>1</v>
+      </c>
+      <c r="C2602">
+        <v>-3</v>
+      </c>
+      <c r="D2602" s="2">
+        <v>45840.8086185538</v>
+      </c>
+      <c r="E2602">
+        <v>-3</v>
+      </c>
+      <c r="F2602" s="2">
+        <v>45840.70496527778</v>
+      </c>
+      <c r="G2602">
+        <v>0</v>
+      </c>
+      <c r="H2602" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizei dados da add e bibi
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2674" uniqueCount="10">
   <si>
     <t>id_produto</t>
   </si>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2660"/>
+  <dimension ref="A1:H2667"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,16 +494,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D4" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E4">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F4" s="2">
-        <v>45865.99837962963</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1194,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>3364</v>
+        <v>3353</v>
       </c>
       <c r="D33" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E33">
-        <v>3364</v>
+        <v>3353</v>
       </c>
       <c r="F33" s="2">
-        <v>45863.44744212963</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1312,16 +1312,16 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D38" s="2">
-        <v>45860.36531218661</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E38">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F38" s="2">
-        <v>45859.57789351852</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -1765,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>410</v>
+        <v>384</v>
       </c>
       <c r="D56" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E56">
-        <v>410</v>
+        <v>384</v>
       </c>
       <c r="F56" s="2">
-        <v>45865.94875</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -1826,7 +1826,7 @@
         <v>252</v>
       </c>
       <c r="F58" s="2">
-        <v>45863.45354166667</v>
+        <v>45866.56369212963</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -2088,16 +2088,16 @@
         <v>1</v>
       </c>
       <c r="C69">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D69" s="2">
-        <v>45860.36531218661</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E69">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F69" s="2">
-        <v>45859.72820601852</v>
+        <v>45866.54819444445</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -2114,16 +2114,16 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>14890</v>
+        <v>14864</v>
       </c>
       <c r="D70" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E70">
-        <v>14890</v>
+        <v>14864</v>
       </c>
       <c r="F70" s="2">
-        <v>45865.96047453704</v>
+        <v>45866.67512731482</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2376,16 +2376,16 @@
         <v>1</v>
       </c>
       <c r="C81">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D81" s="2">
-        <v>45863.33292844877</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E81">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F81" s="2">
-        <v>45862.47730324074</v>
+        <v>45866.44237268518</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -2402,16 +2402,16 @@
         <v>1</v>
       </c>
       <c r="C82">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D82" s="2">
-        <v>45861.89452460439</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E82">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F82" s="2">
-        <v>45861.46820601852</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -2529,16 +2529,16 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D87" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E87">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F87" s="2">
-        <v>45863.68854166667</v>
+        <v>45866.66629629629</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -2630,16 +2630,16 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="D91" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E91">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="F91" s="2">
-        <v>45863.54273148148</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -2702,16 +2702,16 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D94" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E94">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F94" s="2">
-        <v>45863.654375</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -2872,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>5354</v>
+        <v>5302</v>
       </c>
       <c r="D101" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E101">
-        <v>5354</v>
+        <v>5302</v>
       </c>
       <c r="F101" s="2">
-        <v>45863.68796296296</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -2921,16 +2921,16 @@
         <v>1</v>
       </c>
       <c r="C103">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D103" s="2">
-        <v>45863.33292844877</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E103">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F103" s="2">
-        <v>45862.4884375</v>
+        <v>45866.3953125</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -2993,16 +2993,16 @@
         <v>1</v>
       </c>
       <c r="C106">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D106" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E106">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F106" s="2">
-        <v>45863.68796296296</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -3258,16 +3258,16 @@
         <v>1</v>
       </c>
       <c r="C117">
-        <v>902</v>
+        <v>895</v>
       </c>
       <c r="D117" s="2">
-        <v>45861.89452460439</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E117">
-        <v>902</v>
+        <v>895</v>
       </c>
       <c r="F117" s="2">
-        <v>45861.46744212963</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -3333,16 +3333,16 @@
         <v>1</v>
       </c>
       <c r="C120">
-        <v>9</v>
+        <v>-2</v>
       </c>
       <c r="D120" s="2">
-        <v>45863.33290171585</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E120">
-        <v>9</v>
+        <v>-2</v>
       </c>
       <c r="F120" s="2">
-        <v>45862.4025462963</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -3359,16 +3359,16 @@
         <v>1</v>
       </c>
       <c r="C121">
-        <v>592</v>
+        <v>581</v>
       </c>
       <c r="D121" s="2">
-        <v>45863.33292844877</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E121">
-        <v>592</v>
+        <v>581</v>
       </c>
       <c r="F121" s="2">
-        <v>45862.4884375</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -3408,16 +3408,16 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D123" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E123">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F123" s="2">
-        <v>45863.68854166667</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -3460,16 +3460,16 @@
         <v>1</v>
       </c>
       <c r="C125">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D125" s="2">
-        <v>45863.33292844877</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E125">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F125" s="2">
-        <v>45862.4884375</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -3846,16 +3846,16 @@
         <v>1</v>
       </c>
       <c r="C141">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="D141" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E141">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="F141" s="2">
-        <v>45866.02469907407</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G141">
         <v>0</v>
@@ -3950,16 +3950,16 @@
         <v>1</v>
       </c>
       <c r="C145">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D145" s="2">
-        <v>45860.36531218661</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E145">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F145" s="2">
-        <v>45859.72820601852</v>
+        <v>45866.44237268518</v>
       </c>
       <c r="G145">
         <v>0</v>
@@ -4936,16 +4936,16 @@
         <v>1</v>
       </c>
       <c r="C185">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D185" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E185">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F185" s="2">
-        <v>45865.95337962963</v>
+        <v>45866.39487268519</v>
       </c>
       <c r="G185">
         <v>0</v>
@@ -5181,16 +5181,16 @@
         <v>1</v>
       </c>
       <c r="C195">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D195" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E195">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F195" s="2">
-        <v>45865.99903935185</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G195">
         <v>0</v>
@@ -5521,16 +5521,16 @@
         <v>1</v>
       </c>
       <c r="C209">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D209" s="2">
-        <v>45856.2770322055</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E209">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F209" s="2">
-        <v>45855.62951388889</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G209">
         <v>0</v>
@@ -5711,16 +5711,16 @@
         <v>1</v>
       </c>
       <c r="C217">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D217" s="2">
-        <v>45860.91580999861</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E217">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F217" s="2">
-        <v>45860.71293981482</v>
+        <v>45866.67512731482</v>
       </c>
       <c r="G217">
         <v>0</v>
@@ -5737,16 +5737,16 @@
         <v>1</v>
       </c>
       <c r="C218">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D218" s="2">
-        <v>45863.33290171585</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E218">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F218" s="2">
-        <v>45862.4021875</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G218">
         <v>0</v>
@@ -6627,16 +6627,16 @@
         <v>1</v>
       </c>
       <c r="C255">
-        <v>965</v>
+        <v>935</v>
       </c>
       <c r="D255" s="2">
-        <v>45863.33290171585</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E255">
-        <v>965</v>
+        <v>935</v>
       </c>
       <c r="F255" s="2">
-        <v>45862.40175925926</v>
+        <v>45866.51460648148</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -7310,16 +7310,16 @@
         <v>1</v>
       </c>
       <c r="C283">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D283" s="2">
-        <v>45863.33292844877</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E283">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F283" s="2">
-        <v>45862.44537037037</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G283">
         <v>0</v>
@@ -7509,16 +7509,16 @@
         <v>1</v>
       </c>
       <c r="C291">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D291" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E291">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F291" s="2">
-        <v>45863.68767361111</v>
+        <v>45866.54819444445</v>
       </c>
       <c r="G291">
         <v>0</v>
@@ -8374,16 +8374,16 @@
         <v>1</v>
       </c>
       <c r="C326">
-        <v>978</v>
+        <v>933</v>
       </c>
       <c r="D326" s="2">
-        <v>45861.89452460439</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E326">
-        <v>978</v>
+        <v>933</v>
       </c>
       <c r="F326" s="2">
-        <v>45861.46744212963</v>
+        <v>45866.6896412037</v>
       </c>
       <c r="G326">
         <v>0</v>
@@ -8870,16 +8870,16 @@
         <v>1</v>
       </c>
       <c r="C346">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D346" s="2">
-        <v>45863.33292844877</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E346">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F346" s="2">
-        <v>45862.4884375</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G346">
         <v>0</v>
@@ -9164,16 +9164,16 @@
         <v>1</v>
       </c>
       <c r="C358">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D358" s="2">
-        <v>45863.33292844877</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E358">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F358" s="2">
-        <v>45862.44537037037</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G358">
         <v>0</v>
@@ -9291,16 +9291,16 @@
         <v>1</v>
       </c>
       <c r="C363">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D363" s="2">
-        <v>45861.89454635836</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E363">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F363" s="2">
-        <v>45861.68965277778</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G363">
         <v>0</v>
@@ -9865,16 +9865,16 @@
         <v>1</v>
       </c>
       <c r="C386">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D386" s="2">
-        <v>45855.27896249622</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E386">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F386" s="2">
-        <v>45854.49162037037</v>
+        <v>45866.40174768519</v>
       </c>
       <c r="G386">
         <v>0</v>
@@ -9969,16 +9969,16 @@
         <v>1</v>
       </c>
       <c r="C390">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="D390" s="2">
-        <v>45863.33292844877</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E390">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="F390" s="2">
-        <v>45862.47730324074</v>
+        <v>45866.51460648148</v>
       </c>
       <c r="G390">
         <v>0</v>
@@ -10070,16 +10070,16 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="D394" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E394">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="F394" s="2">
-        <v>45863.70143518518</v>
+        <v>45866.75055555555</v>
       </c>
       <c r="G394">
         <v>0</v>
@@ -10321,16 +10321,16 @@
         <v>1</v>
       </c>
       <c r="C404">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="D404" s="2">
-        <v>45859.36420046808</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E404">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="F404" s="2">
-        <v>45856.65395833334</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G404">
         <v>0</v>
@@ -10549,16 +10549,16 @@
         <v>1</v>
       </c>
       <c r="C413">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="D413" s="2">
-        <v>45856.27701193687</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E413">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="F413" s="2">
-        <v>45855.39675925926</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G413">
         <v>0</v>
@@ -10673,16 +10673,16 @@
         <v>1</v>
       </c>
       <c r="C418">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="D418" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E418">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="F418" s="2">
-        <v>45863.68854166667</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G418">
         <v>0</v>
@@ -10771,16 +10771,16 @@
         <v>1</v>
       </c>
       <c r="C422">
-        <v>969</v>
+        <v>938</v>
       </c>
       <c r="D422" s="2">
-        <v>45860.91580999861</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E422">
-        <v>969</v>
+        <v>938</v>
       </c>
       <c r="F422" s="2">
-        <v>45860.67273148148</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G422">
         <v>0</v>
@@ -12207,16 +12207,16 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D480" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E480">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F480" s="2">
-        <v>45863.71251157407</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G480">
         <v>0</v>
@@ -12951,16 +12951,16 @@
         <v>1</v>
       </c>
       <c r="C510">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D510" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E510">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F510" s="2">
-        <v>45863.45354166667</v>
+        <v>45866.634375</v>
       </c>
       <c r="G510">
         <v>0</v>
@@ -13643,16 +13643,16 @@
         <v>1</v>
       </c>
       <c r="C538">
-        <v>559</v>
+        <v>524</v>
       </c>
       <c r="D538" s="2">
-        <v>45852.8954981397</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E538">
-        <v>559</v>
+        <v>524</v>
       </c>
       <c r="F538" s="2">
-        <v>45852.68399305556</v>
+        <v>45866.75055555555</v>
       </c>
       <c r="G538">
         <v>0</v>
@@ -13842,16 +13842,16 @@
         <v>1</v>
       </c>
       <c r="C546">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D546" s="2">
-        <v>45854.2677277031</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E546">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F546" s="2">
-        <v>45853.4324537037</v>
+        <v>45866.634375</v>
       </c>
       <c r="G546">
         <v>0</v>
@@ -14703,16 +14703,16 @@
         <v>1</v>
       </c>
       <c r="C582">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D582" s="2">
-        <v>45849.2922031681</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E582">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F582" s="2">
-        <v>45848.7749537037</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G582">
         <v>0</v>
@@ -15158,16 +15158,16 @@
         <v>1</v>
       </c>
       <c r="C601">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D601" s="2">
-        <v>45860.91580999861</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E601">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F601" s="2">
-        <v>45860.44378472222</v>
+        <v>45866.75055555555</v>
       </c>
       <c r="G601">
         <v>0</v>
@@ -15207,16 +15207,16 @@
         <v>1</v>
       </c>
       <c r="C603">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D603" s="2">
-        <v>45847.81181622412</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E603">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F603" s="2">
-        <v>45839.49008101852</v>
+        <v>45866.634375</v>
       </c>
       <c r="G603">
         <v>0</v>
@@ -15642,16 +15642,16 @@
         <v>1</v>
       </c>
       <c r="C621">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D621" s="2">
-        <v>45863.33290171585</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E621">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F621" s="2">
-        <v>45862.4021875</v>
+        <v>45866.634375</v>
       </c>
       <c r="G621">
         <v>0</v>
@@ -15878,16 +15878,16 @@
         <v>1</v>
       </c>
       <c r="C631">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D631" s="2">
-        <v>45856.2770322055</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E631">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F631" s="2">
-        <v>45855.69512731482</v>
+        <v>45866.75055555555</v>
       </c>
       <c r="G631">
         <v>0</v>
@@ -16518,7 +16518,7 @@
         <v>1422</v>
       </c>
       <c r="F657" s="2">
-        <v>45863.66641203704</v>
+        <v>45866.50738425926</v>
       </c>
       <c r="G657">
         <v>0</v>
@@ -16544,7 +16544,7 @@
         <v>0</v>
       </c>
       <c r="F658" s="2">
-        <v>45855.44644675926</v>
+        <v>45866.3953125</v>
       </c>
       <c r="G658">
         <v>0</v>
@@ -16584,16 +16584,16 @@
         <v>1</v>
       </c>
       <c r="C660">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D660" s="2">
-        <v>45860.36531218661</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E660">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F660" s="2">
-        <v>45859.57789351852</v>
+        <v>45866.634375</v>
       </c>
       <c r="G660">
         <v>0</v>
@@ -17290,16 +17290,16 @@
         <v>1</v>
       </c>
       <c r="C689">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D689" s="2">
-        <v>45860.36531218661</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E689">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F689" s="2">
-        <v>45859.57789351852</v>
+        <v>45866.40746527778</v>
       </c>
       <c r="G689">
         <v>0</v>
@@ -18228,16 +18228,16 @@
         <v>1</v>
       </c>
       <c r="C726">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="D726" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E726">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="F726" s="2">
-        <v>45866.02767361111</v>
+        <v>45866.40174768519</v>
       </c>
       <c r="G726">
         <v>0</v>
@@ -19327,16 +19327,16 @@
         <v>1</v>
       </c>
       <c r="C770">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D770" s="2">
-        <v>45847.81183474588</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E770">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F770" s="2">
-        <v>45841.66082175926</v>
+        <v>45866.66208333334</v>
       </c>
       <c r="G770">
         <v>0</v>
@@ -19483,16 +19483,16 @@
         <v>1</v>
       </c>
       <c r="C776">
-        <v>2333</v>
+        <v>2285</v>
       </c>
       <c r="D776" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E776">
-        <v>2333</v>
+        <v>2285</v>
       </c>
       <c r="F776" s="2">
-        <v>45866.01584490741</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G776">
         <v>0</v>
@@ -19535,16 +19535,16 @@
         <v>1</v>
       </c>
       <c r="C778">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D778" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E778">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F778" s="2">
-        <v>45866.00836805555</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G778">
         <v>0</v>
@@ -20256,16 +20256,16 @@
         <v>1</v>
       </c>
       <c r="C807">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="D807" s="2">
-        <v>45847.81154045185</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E807">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="F807" s="2">
-        <v>45729.72135416666</v>
+        <v>45866.634375</v>
       </c>
       <c r="G807">
         <v>0</v>
@@ -20556,16 +20556,16 @@
         <v>1</v>
       </c>
       <c r="C819">
-        <v>39</v>
+        <v>-21</v>
       </c>
       <c r="D819" s="2">
-        <v>45859.36420046808</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E819">
-        <v>39</v>
+        <v>-21</v>
       </c>
       <c r="F819" s="2">
-        <v>45856.74554398148</v>
+        <v>45866.634375</v>
       </c>
       <c r="G819">
         <v>0</v>
@@ -20608,16 +20608,16 @@
         <v>1</v>
       </c>
       <c r="C821">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D821" s="2">
-        <v>45849.2922031681</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E821">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F821" s="2">
-        <v>45848.7749537037</v>
+        <v>45866.76775462963</v>
       </c>
       <c r="G821">
         <v>0</v>
@@ -20683,16 +20683,16 @@
         <v>1</v>
       </c>
       <c r="C824">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D824" s="2">
-        <v>45861.89452460439</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E824">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F824" s="2">
-        <v>45861.46744212963</v>
+        <v>45866.3953125</v>
       </c>
       <c r="G824">
         <v>0</v>
@@ -21164,16 +21164,16 @@
         <v>1</v>
       </c>
       <c r="C844">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D844" s="2">
-        <v>45863.33292844877</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E844">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F844" s="2">
-        <v>45862.47730324074</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G844">
         <v>0</v>
@@ -21363,16 +21363,16 @@
         <v>1</v>
       </c>
       <c r="C852">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D852" s="2">
-        <v>45852.8954981397</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E852">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F852" s="2">
-        <v>45852.66924768518</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G852">
         <v>0</v>
@@ -21389,16 +21389,16 @@
         <v>1</v>
       </c>
       <c r="C853">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D853" s="2">
-        <v>45860.91583892083</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E853">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F853" s="2">
-        <v>45860.76299768518</v>
+        <v>45866.40174768519</v>
       </c>
       <c r="G853">
         <v>0</v>
@@ -21415,16 +21415,16 @@
         <v>1</v>
       </c>
       <c r="C854">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D854" s="2">
-        <v>45860.91583892083</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E854">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="F854" s="2">
-        <v>45860.76325231481</v>
+        <v>45866.76775462963</v>
       </c>
       <c r="G854">
         <v>0</v>
@@ -23161,16 +23161,16 @@
         <v>1</v>
       </c>
       <c r="C923">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="D923" s="2">
-        <v>45861.89452460439</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E923">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="F923" s="2">
-        <v>45861.46744212963</v>
+        <v>45866.39487268519</v>
       </c>
       <c r="G923">
         <v>0</v>
@@ -23848,16 +23848,16 @@
         <v>1</v>
       </c>
       <c r="C950">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D950" s="2">
-        <v>45847.81161766584</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E950">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F950" s="2">
-        <v>45806.44422453704</v>
+        <v>45866.75055555555</v>
       </c>
       <c r="G950">
         <v>0</v>
@@ -26347,16 +26347,16 @@
         <v>1</v>
       </c>
       <c r="C1049">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D1049" s="2">
-        <v>45847.81181622412</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1049">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F1049" s="2">
-        <v>45838.72313657407</v>
+        <v>45866.67512731482</v>
       </c>
       <c r="G1049">
         <v>0</v>
@@ -26546,16 +26546,16 @@
         <v>1</v>
       </c>
       <c r="C1057">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1057" s="2">
-        <v>45849.29218469877</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1057">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F1057" s="2">
-        <v>45848.48304398148</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G1057">
         <v>0</v>
@@ -26659,7 +26659,7 @@
         <v>26</v>
       </c>
       <c r="F1061" s="2">
-        <v>45863.66641203704</v>
+        <v>45866.50738425926</v>
       </c>
       <c r="G1061">
         <v>0</v>
@@ -26676,16 +26676,16 @@
         <v>1</v>
       </c>
       <c r="C1062">
-        <v>528</v>
+        <v>475</v>
       </c>
       <c r="D1062" s="2">
-        <v>45861.89452460439</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1062">
-        <v>528</v>
+        <v>475</v>
       </c>
       <c r="F1062" s="2">
-        <v>45861.46744212963</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G1062">
         <v>0</v>
@@ -27466,16 +27466,16 @@
         <v>1</v>
       </c>
       <c r="C1094">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D1094" s="2">
-        <v>45847.81183474588</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1094">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F1094" s="2">
-        <v>45841.76172453703</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G1094">
         <v>0</v>
@@ -27867,16 +27867,16 @@
         <v>1</v>
       </c>
       <c r="C1110">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D1110" s="2">
-        <v>45863.33290171585</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1110">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="F1110" s="2">
-        <v>45862.40175925926</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G1110">
         <v>0</v>
@@ -28453,16 +28453,16 @@
         <v>1</v>
       </c>
       <c r="C1133">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D1133" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1133">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F1133" s="2">
-        <v>45863.66303240741</v>
+        <v>45866.634375</v>
       </c>
       <c r="G1133">
         <v>0</v>
@@ -28805,16 +28805,16 @@
         <v>1</v>
       </c>
       <c r="C1147">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1147" s="2">
-        <v>45860.91580999861</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1147">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1147" s="2">
-        <v>45860.51488425926</v>
+        <v>45866.54819444445</v>
       </c>
       <c r="G1147">
         <v>0</v>
@@ -29039,16 +29039,16 @@
         <v>1</v>
       </c>
       <c r="C1156">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1156" s="2">
-        <v>45847.81179644933</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1156">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1156" s="2">
-        <v>45833.515625</v>
+        <v>45866.634375</v>
       </c>
       <c r="G1156">
         <v>0</v>
@@ -29495,16 +29495,16 @@
         <v>1</v>
       </c>
       <c r="C1174">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D1174" s="2">
-        <v>45860.36531218661</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1174">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F1174" s="2">
-        <v>45859.57789351852</v>
+        <v>45866.634375</v>
       </c>
       <c r="G1174">
         <v>0</v>
@@ -29674,16 +29674,16 @@
         <v>1</v>
       </c>
       <c r="C1181">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D1181" s="2">
-        <v>45847.81185513067</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1181">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F1181" s="2">
-        <v>45845.52229166667</v>
+        <v>45866.76775462963</v>
       </c>
       <c r="G1181">
         <v>0</v>
@@ -29804,16 +29804,16 @@
         <v>1</v>
       </c>
       <c r="C1186">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1186" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1186">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1186" s="2">
-        <v>45866.02258101852</v>
+        <v>45866.6896412037</v>
       </c>
       <c r="G1186">
         <v>0</v>
@@ -30142,16 +30142,16 @@
         <v>1</v>
       </c>
       <c r="C1199">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1199" s="2">
-        <v>45850.2785639081</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1199">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F1199" s="2">
-        <v>45849.72677083333</v>
+        <v>45866.40174768519</v>
       </c>
       <c r="G1199">
         <v>0</v>
@@ -31372,16 +31372,16 @@
         <v>1</v>
       </c>
       <c r="C1247">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D1247" s="2">
-        <v>45861.89452460439</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1247">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F1247" s="2">
-        <v>45861.46744212963</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G1247">
         <v>0</v>
@@ -31528,16 +31528,16 @@
         <v>1</v>
       </c>
       <c r="C1253">
-        <v>1021</v>
+        <v>967</v>
       </c>
       <c r="D1253" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1253">
-        <v>1021</v>
+        <v>967</v>
       </c>
       <c r="F1253" s="2">
-        <v>45865.97634259259</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G1253">
         <v>0</v>
@@ -31733,16 +31733,16 @@
         <v>1</v>
       </c>
       <c r="C1261">
-        <v>188</v>
+        <v>146</v>
       </c>
       <c r="D1261" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1261">
-        <v>188</v>
+        <v>146</v>
       </c>
       <c r="F1261" s="2">
-        <v>45863.66641203704</v>
+        <v>45866.69045138889</v>
       </c>
       <c r="G1261">
         <v>0</v>
@@ -33341,7 +33341,7 @@
         <v>8</v>
       </c>
       <c r="F1324" s="2">
-        <v>45865.92921296296</v>
+        <v>45866.50738425926</v>
       </c>
       <c r="G1324">
         <v>0</v>
@@ -33791,16 +33791,16 @@
         <v>1</v>
       </c>
       <c r="C1342">
-        <v>1467</v>
+        <v>1277</v>
       </c>
       <c r="D1342" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1342">
-        <v>1467</v>
+        <v>1277</v>
       </c>
       <c r="F1342" s="2">
-        <v>45863.66303240741</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G1342">
         <v>0</v>
@@ -35018,16 +35018,16 @@
         <v>1</v>
       </c>
       <c r="C1390">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1390" s="2">
-        <v>45863.33290171585</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1390">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1390" s="2">
-        <v>45862.4025462963</v>
+        <v>45866.39070601852</v>
       </c>
       <c r="G1390">
         <v>0</v>
@@ -35607,16 +35607,16 @@
         <v>1</v>
       </c>
       <c r="C1413">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D1413" s="2">
-        <v>45847.81179644933</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1413">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F1413" s="2">
-        <v>45835.72380787037</v>
+        <v>45866.39070601852</v>
       </c>
       <c r="G1413">
         <v>0</v>
@@ -35809,16 +35809,16 @@
         <v>1</v>
       </c>
       <c r="C1421">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D1421" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1421">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F1421" s="2">
-        <v>45863.54273148148</v>
+        <v>45866.634375</v>
       </c>
       <c r="G1421">
         <v>0</v>
@@ -35835,16 +35835,16 @@
         <v>1</v>
       </c>
       <c r="C1422">
-        <v>6</v>
+        <v>-14</v>
       </c>
       <c r="D1422" s="2">
-        <v>45847.81181622412</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1422">
-        <v>6</v>
+        <v>-14</v>
       </c>
       <c r="F1422" s="2">
-        <v>45838.73396990741</v>
+        <v>45866.634375</v>
       </c>
       <c r="G1422">
         <v>0</v>
@@ -36505,16 +36505,16 @@
         <v>1</v>
       </c>
       <c r="C1448">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D1448" s="2">
-        <v>45856.27705170162</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1448">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F1448" s="2">
-        <v>45855.74673611111</v>
+        <v>45866.634375</v>
       </c>
       <c r="G1448">
         <v>0</v>
@@ -37965,16 +37965,16 @@
         <v>1</v>
       </c>
       <c r="C1506">
-        <v>6</v>
+        <v>-4</v>
       </c>
       <c r="D1506" s="2">
-        <v>45847.81179644933</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1506">
-        <v>6</v>
+        <v>-4</v>
       </c>
       <c r="F1506" s="2">
-        <v>45834.43447916667</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G1506">
         <v>0</v>
@@ -40151,16 +40151,16 @@
         <v>1</v>
       </c>
       <c r="C1594">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D1594" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1594">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F1594" s="2">
-        <v>45863.44744212963</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G1594">
         <v>0</v>
@@ -40229,16 +40229,16 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>11689</v>
+        <v>11669</v>
       </c>
       <c r="D1597" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1597">
-        <v>11689</v>
+        <v>11669</v>
       </c>
       <c r="F1597" s="2">
-        <v>45863.68796296296</v>
+        <v>45866.634375</v>
       </c>
       <c r="G1597">
         <v>0</v>
@@ -40936,16 +40936,16 @@
         <v>1</v>
       </c>
       <c r="C1625">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D1625" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1625">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="F1625" s="2">
-        <v>45863.43357638889</v>
+        <v>45866.76775462963</v>
       </c>
       <c r="G1625">
         <v>0</v>
@@ -41196,16 +41196,16 @@
         <v>1</v>
       </c>
       <c r="C1635">
-        <v>1559</v>
+        <v>1524</v>
       </c>
       <c r="D1635" s="2">
-        <v>45863.33292844877</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E1635">
-        <v>1559</v>
+        <v>1524</v>
       </c>
       <c r="F1635" s="2">
-        <v>45862.44537037037</v>
+        <v>45866.64810185185</v>
       </c>
       <c r="G1635">
         <v>0</v>
@@ -41582,16 +41582,16 @@
         <v>1</v>
       </c>
       <c r="C1651">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1651" s="2">
-        <v>45847.81181622412</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1651">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1651" s="2">
-        <v>45838.79201388889</v>
+        <v>45866.39070601852</v>
       </c>
       <c r="G1651">
         <v>0</v>
@@ -46414,16 +46414,16 @@
         <v>1</v>
       </c>
       <c r="C1844">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="D1844" s="2">
-        <v>45859.36421881544</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1844">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="F1844" s="2">
-        <v>45859.36511574074</v>
+        <v>45866.39487268519</v>
       </c>
       <c r="G1844">
         <v>0</v>
@@ -46714,16 +46714,16 @@
         <v>1</v>
       </c>
       <c r="C1856">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1856" s="2">
-        <v>45854.26776722976</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1856">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F1856" s="2">
-        <v>45853.75052083333</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G1856">
         <v>0</v>
@@ -48498,16 +48498,16 @@
         <v>1</v>
       </c>
       <c r="C1926">
-        <v>0</v>
+        <v>-22</v>
       </c>
       <c r="D1926" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E1926">
-        <v>0</v>
+        <v>-22</v>
       </c>
       <c r="F1926" s="2">
-        <v>45863.66641203704</v>
+        <v>45866.50738425926</v>
       </c>
       <c r="G1926">
         <v>0</v>
@@ -50460,16 +50460,16 @@
         <v>1</v>
       </c>
       <c r="C2004">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2004" s="2">
-        <v>45854.26776722976</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E2004">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2004" s="2">
-        <v>45853.76050925926</v>
+        <v>45866.54819444445</v>
       </c>
       <c r="G2004">
         <v>0</v>
@@ -50953,16 +50953,16 @@
         <v>1</v>
       </c>
       <c r="C2024">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D2024" s="2">
-        <v>45860.91583892083</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E2024">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F2024" s="2">
-        <v>45860.76325231481</v>
+        <v>45866.6896412037</v>
       </c>
       <c r="G2024">
         <v>0</v>
@@ -52852,16 +52852,16 @@
         <v>1</v>
       </c>
       <c r="C2099">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2099" s="2">
-        <v>45855.27896249622</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E2099">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2099" s="2">
-        <v>45854.69638888889</v>
+        <v>45866.54819444445</v>
       </c>
       <c r="G2099">
         <v>0</v>
@@ -58608,16 +58608,16 @@
         <v>1</v>
       </c>
       <c r="C2328">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2328" s="2">
-        <v>45852.89547361292</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E2328">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F2328" s="2">
-        <v>45852.39309027778</v>
+        <v>45866.39487268519</v>
       </c>
       <c r="G2328">
         <v>0</v>
@@ -58712,16 +58712,16 @@
         <v>1</v>
       </c>
       <c r="C2332">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2332" s="2">
-        <v>45847.81179644933</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E2332">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2332" s="2">
-        <v>45838.52734953703</v>
+        <v>45866.56876157408</v>
       </c>
       <c r="G2332">
         <v>0</v>
@@ -62400,16 +62400,16 @@
         <v>1</v>
       </c>
       <c r="C2481">
-        <v>837</v>
+        <v>817</v>
       </c>
       <c r="D2481" s="2">
-        <v>45861.89452460439</v>
+        <v>45867.31615610872</v>
       </c>
       <c r="E2481">
-        <v>837</v>
+        <v>817</v>
       </c>
       <c r="F2481" s="2">
-        <v>45861.47043981482</v>
+        <v>45866.634375</v>
       </c>
       <c r="G2481">
         <v>0</v>
@@ -62426,16 +62426,16 @@
         <v>1</v>
       </c>
       <c r="C2482">
-        <v>1329</v>
+        <v>1298</v>
       </c>
       <c r="D2482" s="2">
-        <v>45866.27545220916</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E2482">
-        <v>1329</v>
+        <v>1298</v>
       </c>
       <c r="F2482" s="2">
-        <v>45863.69969907407</v>
+        <v>45866.56369212963</v>
       </c>
       <c r="G2482">
         <v>0</v>
@@ -62478,16 +62478,16 @@
         <v>1</v>
       </c>
       <c r="C2484">
-        <v>2424</v>
+        <v>2393</v>
       </c>
       <c r="D2484" s="2">
-        <v>45866.27547163953</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E2484">
-        <v>2424</v>
+        <v>2393</v>
       </c>
       <c r="F2484" s="2">
-        <v>45865.95244212963</v>
+        <v>45866.56173611111</v>
       </c>
       <c r="G2484">
         <v>0</v>
@@ -65202,7 +65202,7 @@
         <v>0</v>
       </c>
       <c r="D2595" s="2">
-        <v>45847.81181622412</v>
+        <v>45867.31613801513</v>
       </c>
       <c r="E2595">
         <v>0</v>
@@ -66787,6 +66787,173 @@
         <v>0</v>
       </c>
       <c r="H2660" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:8">
+      <c r="A2661">
+        <v>44410833</v>
+      </c>
+      <c r="B2661">
+        <v>1</v>
+      </c>
+      <c r="C2661">
+        <v>-4</v>
+      </c>
+      <c r="D2661" s="2">
+        <v>45867.31613801513</v>
+      </c>
+      <c r="E2661">
+        <v>-4</v>
+      </c>
+      <c r="F2661" s="2">
+        <v>45866.40174768519</v>
+      </c>
+      <c r="G2661">
+        <v>0</v>
+      </c>
+      <c r="H2661" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:8">
+      <c r="A2662">
+        <v>44425887</v>
+      </c>
+      <c r="B2662">
+        <v>1</v>
+      </c>
+      <c r="C2662">
+        <v>0</v>
+      </c>
+      <c r="D2662" s="2">
+        <v>45867.31615610872</v>
+      </c>
+      <c r="E2662">
+        <v>0</v>
+      </c>
+      <c r="G2662">
+        <v>0</v>
+      </c>
+      <c r="H2662" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:8">
+      <c r="A2663">
+        <v>44425902</v>
+      </c>
+      <c r="B2663">
+        <v>1</v>
+      </c>
+      <c r="C2663">
+        <v>0</v>
+      </c>
+      <c r="D2663" s="2">
+        <v>45867.31615610872</v>
+      </c>
+      <c r="E2663">
+        <v>0</v>
+      </c>
+      <c r="G2663">
+        <v>0</v>
+      </c>
+      <c r="H2663" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:8">
+      <c r="A2664">
+        <v>44425916</v>
+      </c>
+      <c r="B2664">
+        <v>1</v>
+      </c>
+      <c r="C2664">
+        <v>0</v>
+      </c>
+      <c r="D2664" s="2">
+        <v>45867.31615610872</v>
+      </c>
+      <c r="E2664">
+        <v>0</v>
+      </c>
+      <c r="G2664">
+        <v>0</v>
+      </c>
+      <c r="H2664" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:8">
+      <c r="A2665">
+        <v>44425922</v>
+      </c>
+      <c r="B2665">
+        <v>1</v>
+      </c>
+      <c r="C2665">
+        <v>0</v>
+      </c>
+      <c r="D2665" s="2">
+        <v>45867.31615610872</v>
+      </c>
+      <c r="E2665">
+        <v>0</v>
+      </c>
+      <c r="G2665">
+        <v>0</v>
+      </c>
+      <c r="H2665" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:8">
+      <c r="A2666">
+        <v>44425932</v>
+      </c>
+      <c r="B2666">
+        <v>1</v>
+      </c>
+      <c r="C2666">
+        <v>0</v>
+      </c>
+      <c r="D2666" s="2">
+        <v>45867.31615610872</v>
+      </c>
+      <c r="E2666">
+        <v>0</v>
+      </c>
+      <c r="G2666">
+        <v>0</v>
+      </c>
+      <c r="H2666" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:8">
+      <c r="A2667">
+        <v>44426813</v>
+      </c>
+      <c r="B2667">
+        <v>1</v>
+      </c>
+      <c r="C2667">
+        <v>-2</v>
+      </c>
+      <c r="D2667" s="2">
+        <v>45867.31615610872</v>
+      </c>
+      <c r="E2667">
+        <v>-2</v>
+      </c>
+      <c r="F2667" s="2">
+        <v>45866.76090277778</v>
+      </c>
+      <c r="G2667">
+        <v>0</v>
+      </c>
+      <c r="H2667" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizei bases bibi e add
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
+++ b/dados/ADD/Dados_ADD_PF/analise_consistencia_estoque.xlsx
@@ -494,16 +494,16 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D4" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E4">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F4" s="2">
-        <v>45866.56173611111</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -520,16 +520,16 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D5" s="2">
-        <v>45861.89454635836</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E5">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F5" s="2">
-        <v>45861.78336805556</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1194,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <v>3353</v>
+        <v>3312</v>
       </c>
       <c r="D33" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E33">
-        <v>3353</v>
+        <v>3312</v>
       </c>
       <c r="F33" s="2">
-        <v>45866.69045138889</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1765,16 +1765,16 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>384</v>
+        <v>293</v>
       </c>
       <c r="D56" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E56">
-        <v>384</v>
+        <v>293</v>
       </c>
       <c r="F56" s="2">
-        <v>45866.69045138889</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -1817,16 +1817,16 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D58" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E58">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F58" s="2">
-        <v>45866.56369212963</v>
+        <v>45867.42962962963</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -1843,16 +1843,16 @@
         <v>1</v>
       </c>
       <c r="C59">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D59" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E59">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F59" s="2">
-        <v>45865.949375</v>
+        <v>45867.6208912037</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -1941,16 +1941,16 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D63" s="2">
-        <v>45863.33292844877</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E63">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F63" s="2">
-        <v>45862.4884375</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2114,16 +2114,16 @@
         <v>1</v>
       </c>
       <c r="C70">
-        <v>14864</v>
+        <v>7</v>
       </c>
       <c r="D70" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E70">
-        <v>14864</v>
+        <v>7</v>
       </c>
       <c r="F70" s="2">
-        <v>45866.67512731482</v>
+        <v>45867.7325</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2140,16 +2140,16 @@
         <v>1</v>
       </c>
       <c r="C71">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D71" s="2">
-        <v>45863.33290171585</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E71">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F71" s="2">
-        <v>45862.4025462963</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -2402,16 +2402,16 @@
         <v>1</v>
       </c>
       <c r="C82">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D82" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E82">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F82" s="2">
-        <v>45866.64810185185</v>
+        <v>45867.53143518518</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -2477,16 +2477,16 @@
         <v>1</v>
       </c>
       <c r="C85">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D85" s="2">
-        <v>45860.91580999861</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E85">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F85" s="2">
-        <v>45860.40890046296</v>
+        <v>45867.53143518518</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -2503,16 +2503,16 @@
         <v>1</v>
       </c>
       <c r="C86">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D86" s="2">
-        <v>45860.91580999861</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E86">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F86" s="2">
-        <v>45860.53869212963</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -2529,16 +2529,16 @@
         <v>1</v>
       </c>
       <c r="C87">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D87" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E87">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F87" s="2">
-        <v>45866.66629629629</v>
+        <v>45867.53143518518</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -2630,16 +2630,16 @@
         <v>1</v>
       </c>
       <c r="C91">
-        <v>280</v>
+        <v>-2131</v>
       </c>
       <c r="D91" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E91">
-        <v>280</v>
+        <v>-2131</v>
       </c>
       <c r="F91" s="2">
-        <v>45866.69045138889</v>
+        <v>45867.7325</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -2702,16 +2702,16 @@
         <v>1</v>
       </c>
       <c r="C94">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D94" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E94">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F94" s="2">
-        <v>45866.69045138889</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -2872,16 +2872,16 @@
         <v>1</v>
       </c>
       <c r="C101">
-        <v>5302</v>
+        <v>4835</v>
       </c>
       <c r="D101" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E101">
-        <v>5302</v>
+        <v>4835</v>
       </c>
       <c r="F101" s="2">
-        <v>45866.64810185185</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -2993,16 +2993,16 @@
         <v>1</v>
       </c>
       <c r="C106">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D106" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E106">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F106" s="2">
-        <v>45866.64810185185</v>
+        <v>45867.42921296296</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -3114,16 +3114,16 @@
         <v>1</v>
       </c>
       <c r="C111">
-        <v>36562</v>
+        <v>1462</v>
       </c>
       <c r="D111" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E111">
         <v>0</v>
       </c>
       <c r="G111">
-        <v>36562</v>
+        <v>1462</v>
       </c>
       <c r="H111" t="s">
         <v>9</v>
@@ -3160,16 +3160,16 @@
         <v>1</v>
       </c>
       <c r="C113">
-        <v>24</v>
+        <v>-11</v>
       </c>
       <c r="D113" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E113">
-        <v>24</v>
+        <v>-11</v>
       </c>
       <c r="F113" s="2">
-        <v>45863.66188657407</v>
+        <v>45867.53143518518</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -3209,16 +3209,16 @@
         <v>1</v>
       </c>
       <c r="C115">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D115" s="2">
-        <v>45863.33290171585</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E115">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="F115" s="2">
-        <v>45862.42978009259</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -3333,16 +3333,16 @@
         <v>1</v>
       </c>
       <c r="C120">
-        <v>-2</v>
+        <v>88</v>
       </c>
       <c r="D120" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E120">
-        <v>-2</v>
+        <v>88</v>
       </c>
       <c r="F120" s="2">
-        <v>45866.64810185185</v>
+        <v>45867.64997685186</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -3359,16 +3359,16 @@
         <v>1</v>
       </c>
       <c r="C121">
-        <v>581</v>
+        <v>571</v>
       </c>
       <c r="D121" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E121">
-        <v>581</v>
+        <v>571</v>
       </c>
       <c r="F121" s="2">
-        <v>45866.56173611111</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -3408,16 +3408,16 @@
         <v>1</v>
       </c>
       <c r="C123">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D123" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E123">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F123" s="2">
-        <v>45866.56173611111</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -3495,7 +3495,7 @@
         <v>4</v>
       </c>
       <c r="F126" s="2">
-        <v>45863.54273148148</v>
+        <v>45867.53375</v>
       </c>
       <c r="G126">
         <v>0</v>
@@ -3535,16 +3535,16 @@
         <v>1</v>
       </c>
       <c r="C128">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D128" s="2">
-        <v>45847.81181622412</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E128">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F128" s="2">
-        <v>45856.66791666667</v>
+        <v>45867.63021990741</v>
       </c>
       <c r="G128">
         <v>0</v>
@@ -4074,16 +4074,16 @@
         <v>1</v>
       </c>
       <c r="C150">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D150" s="2">
-        <v>45860.91580999861</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E150">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F150" s="2">
-        <v>45860.40890046296</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G150">
         <v>0</v>
@@ -5077,16 +5077,16 @@
         <v>1</v>
       </c>
       <c r="C191">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="D191" s="2">
-        <v>45847.81185513067</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E191">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="F191" s="2">
-        <v>45845.45762731481</v>
+        <v>45867.40572916667</v>
       </c>
       <c r="G191">
         <v>0</v>
@@ -5711,16 +5711,16 @@
         <v>1</v>
       </c>
       <c r="C217">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D217" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E217">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F217" s="2">
-        <v>45866.67512731482</v>
+        <v>45867.71851851852</v>
       </c>
       <c r="G217">
         <v>0</v>
@@ -5737,16 +5737,16 @@
         <v>1</v>
       </c>
       <c r="C218">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D218" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E218">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F218" s="2">
-        <v>45866.69045138889</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G218">
         <v>0</v>
@@ -6175,16 +6175,16 @@
         <v>1</v>
       </c>
       <c r="C236">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D236" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E236">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F236" s="2">
-        <v>45863.68796296296</v>
+        <v>45867.42962962963</v>
       </c>
       <c r="G236">
         <v>0</v>
@@ -6627,16 +6627,16 @@
         <v>1</v>
       </c>
       <c r="C255">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D255" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E255">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F255" s="2">
-        <v>45866.51460648148</v>
+        <v>45867.3937962963</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -6996,16 +6996,16 @@
         <v>1</v>
       </c>
       <c r="C270">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D270" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E270">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F270" s="2">
-        <v>45865.99730324074</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G270">
         <v>0</v>
@@ -7509,16 +7509,16 @@
         <v>1</v>
       </c>
       <c r="C291">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D291" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E291">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F291" s="2">
-        <v>45866.54819444445</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G291">
         <v>0</v>
@@ -7904,16 +7904,16 @@
         <v>1</v>
       </c>
       <c r="C307">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D307" s="2">
-        <v>45847.81177677388</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E307">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F307" s="2">
-        <v>45833.44583333333</v>
+        <v>45867.40884259259</v>
       </c>
       <c r="G307">
         <v>0</v>
@@ -7953,16 +7953,16 @@
         <v>1</v>
       </c>
       <c r="C309">
-        <v>1405</v>
+        <v>1392</v>
       </c>
       <c r="D309" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E309">
-        <v>1405</v>
+        <v>1392</v>
       </c>
       <c r="F309" s="2">
-        <v>45866.02601851852</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G309">
         <v>0</v>
@@ -8169,16 +8169,16 @@
         <v>1</v>
       </c>
       <c r="C318">
-        <v>513</v>
+        <v>493</v>
       </c>
       <c r="D318" s="2">
-        <v>45860.91580999861</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E318">
-        <v>513</v>
+        <v>493</v>
       </c>
       <c r="F318" s="2">
-        <v>45860.53869212963</v>
+        <v>45867.42962962963</v>
       </c>
       <c r="G318">
         <v>0</v>
@@ -8870,16 +8870,16 @@
         <v>1</v>
       </c>
       <c r="C346">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D346" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E346">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="F346" s="2">
-        <v>45866.56173611111</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G346">
         <v>0</v>
@@ -9066,16 +9066,16 @@
         <v>1</v>
       </c>
       <c r="C354">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D354" s="2">
-        <v>45847.8118756755</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E354">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F354" s="2">
-        <v>45846.50909722222</v>
+        <v>45867.71851851852</v>
       </c>
       <c r="G354">
         <v>0</v>
@@ -9190,16 +9190,16 @@
         <v>1</v>
       </c>
       <c r="C359">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D359" s="2">
-        <v>45852.89547361292</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E359">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F359" s="2">
-        <v>45852.65956018519</v>
+        <v>45867.40572916667</v>
       </c>
       <c r="G359">
         <v>0</v>
@@ -9291,16 +9291,16 @@
         <v>1</v>
       </c>
       <c r="C363">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="D363" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E363">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="F363" s="2">
-        <v>45866.69045138889</v>
+        <v>45867.44495370371</v>
       </c>
       <c r="G363">
         <v>0</v>
@@ -9487,16 +9487,16 @@
         <v>1</v>
       </c>
       <c r="C371">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D371" s="2">
-        <v>45859.36421881544</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E371">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F371" s="2">
-        <v>45856.76034722223</v>
+        <v>45867.54620370371</v>
       </c>
       <c r="G371">
         <v>0</v>
@@ -9969,16 +9969,16 @@
         <v>1</v>
       </c>
       <c r="C390">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D390" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E390">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="F390" s="2">
-        <v>45866.51460648148</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G390">
         <v>0</v>
@@ -10070,16 +10070,16 @@
         <v>1</v>
       </c>
       <c r="C394">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D394" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E394">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="F394" s="2">
-        <v>45866.75055555555</v>
+        <v>45867.53254629629</v>
       </c>
       <c r="G394">
         <v>0</v>
@@ -10122,22 +10122,22 @@
         <v>1</v>
       </c>
       <c r="C396">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D396" s="2">
-        <v>45847.81181622412</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E396">
-        <v>6</v>
+        <v>1462</v>
       </c>
       <c r="F396" s="2">
-        <v>45838.79269675926</v>
+        <v>45867.7325</v>
       </c>
       <c r="G396">
-        <v>0</v>
+        <v>1458</v>
       </c>
       <c r="H396" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="397" spans="1:8">
@@ -10269,16 +10269,16 @@
         <v>1</v>
       </c>
       <c r="C402">
-        <v>271</v>
+        <v>223</v>
       </c>
       <c r="D402" s="2">
-        <v>45863.33290171585</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E402">
-        <v>271</v>
+        <v>223</v>
       </c>
       <c r="F402" s="2">
-        <v>45862.4021875</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G402">
         <v>0</v>
@@ -10295,16 +10295,16 @@
         <v>1</v>
       </c>
       <c r="C403">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D403" s="2">
-        <v>45861.89452460439</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E403">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F403" s="2">
-        <v>45861.47043981482</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G403">
         <v>0</v>
@@ -10549,16 +10549,16 @@
         <v>1</v>
       </c>
       <c r="C413">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D413" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E413">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="F413" s="2">
-        <v>45866.56173611111</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G413">
         <v>0</v>
@@ -10852,7 +10852,7 @@
         <v>133</v>
       </c>
       <c r="F425" s="2">
-        <v>45863.54273148148</v>
+        <v>45867.53375</v>
       </c>
       <c r="G425">
         <v>0</v>
@@ -11244,16 +11244,16 @@
         <v>1</v>
       </c>
       <c r="C441">
-        <v>-72</v>
+        <v>-70</v>
       </c>
       <c r="D441" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E441">
-        <v>-72</v>
+        <v>-70</v>
       </c>
       <c r="F441" s="2">
-        <v>45863.74745370371</v>
+        <v>45867.64740740741</v>
       </c>
       <c r="G441">
         <v>0</v>
@@ -11296,16 +11296,16 @@
         <v>1</v>
       </c>
       <c r="C443">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D443" s="2">
-        <v>45863.33292844877</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E443">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F443" s="2">
-        <v>45862.62569444445</v>
+        <v>45867.53143518518</v>
       </c>
       <c r="G443">
         <v>0</v>
@@ -12005,16 +12005,16 @@
         <v>1</v>
       </c>
       <c r="C472">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D472" s="2">
-        <v>45861.89452460439</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E472">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F472" s="2">
-        <v>45861.47043981482</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G472">
         <v>0</v>
@@ -12207,16 +12207,16 @@
         <v>1</v>
       </c>
       <c r="C480">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D480" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E480">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F480" s="2">
-        <v>45866.69045138889</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G480">
         <v>0</v>
@@ -12951,16 +12951,16 @@
         <v>1</v>
       </c>
       <c r="C510">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D510" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E510">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F510" s="2">
-        <v>45866.634375</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G510">
         <v>0</v>
@@ -12977,16 +12977,16 @@
         <v>1</v>
       </c>
       <c r="C511">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D511" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E511">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="F511" s="2">
-        <v>45863.66163194444</v>
+        <v>45867.42693287037</v>
       </c>
       <c r="G511">
         <v>0</v>
@@ -13467,16 +13467,16 @@
         <v>1</v>
       </c>
       <c r="C531">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D531" s="2">
-        <v>45855.27896249622</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E531">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F531" s="2">
-        <v>45854.69638888889</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G531">
         <v>0</v>
@@ -13571,16 +13571,16 @@
         <v>1</v>
       </c>
       <c r="C535">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="D535" s="2">
-        <v>45856.2770322055</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E535">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="F535" s="2">
-        <v>45855.69512731482</v>
+        <v>45867.4334375</v>
       </c>
       <c r="G535">
         <v>0</v>
@@ -14389,16 +14389,16 @@
         <v>1</v>
       </c>
       <c r="C569">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D569" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E569">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F569" s="2">
-        <v>45863.68796296296</v>
+        <v>45867.70488425926</v>
       </c>
       <c r="G569">
         <v>0</v>
@@ -14415,16 +14415,16 @@
         <v>1</v>
       </c>
       <c r="C570">
-        <v>2268</v>
+        <v>2264</v>
       </c>
       <c r="D570" s="2">
-        <v>45863.33290171585</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E570">
-        <v>2268</v>
+        <v>2264</v>
       </c>
       <c r="F570" s="2">
-        <v>45862.4025462963</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G570">
         <v>0</v>
@@ -15446,13 +15446,16 @@
         <v>1</v>
       </c>
       <c r="C613">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="D613" s="2">
-        <v>45847.81159828727</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E613">
-        <v>0</v>
+        <v>-20</v>
+      </c>
+      <c r="F613" s="2">
+        <v>45867.74648148148</v>
       </c>
       <c r="G613">
         <v>0</v>
@@ -15956,16 +15959,16 @@
         <v>1</v>
       </c>
       <c r="C634">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D634" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E634">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F634" s="2">
-        <v>45865.95358796296</v>
+        <v>45867.40572916667</v>
       </c>
       <c r="G634">
         <v>0</v>
@@ -16385,16 +16388,16 @@
         <v>1</v>
       </c>
       <c r="C652">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D652" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E652">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F652" s="2">
-        <v>45865.95395833333</v>
+        <v>45867.40572916667</v>
       </c>
       <c r="G652">
         <v>0</v>
@@ -16509,16 +16512,16 @@
         <v>1</v>
       </c>
       <c r="C657">
-        <v>1422</v>
+        <v>1375</v>
       </c>
       <c r="D657" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E657">
-        <v>1422</v>
+        <v>1375</v>
       </c>
       <c r="F657" s="2">
-        <v>45866.50738425926</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G657">
         <v>0</v>
@@ -17290,16 +17293,16 @@
         <v>1</v>
       </c>
       <c r="C689">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="D689" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E689">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="F689" s="2">
-        <v>45866.40746527778</v>
+        <v>45867.53254629629</v>
       </c>
       <c r="G689">
         <v>0</v>
@@ -17417,16 +17420,16 @@
         <v>1</v>
       </c>
       <c r="C694">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D694" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E694">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F694" s="2">
-        <v>45865.98148148148</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G694">
         <v>0</v>
@@ -17599,16 +17602,16 @@
         <v>1</v>
       </c>
       <c r="C701">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D701" s="2">
-        <v>45863.33292844877</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E701">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="F701" s="2">
-        <v>45862.47730324074</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G701">
         <v>0</v>
@@ -17648,16 +17651,16 @@
         <v>1</v>
       </c>
       <c r="C703">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D703" s="2">
-        <v>45861.89454635836</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E703">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F703" s="2">
-        <v>45861.65526620371</v>
+        <v>45867.43670138889</v>
       </c>
       <c r="G703">
         <v>0</v>
@@ -18381,16 +18384,16 @@
         <v>1</v>
       </c>
       <c r="C732">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="D732" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E732">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="F732" s="2">
-        <v>45863.68854166667</v>
+        <v>45867.44495370371</v>
       </c>
       <c r="G732">
         <v>0</v>
@@ -19379,16 +19382,16 @@
         <v>1</v>
       </c>
       <c r="C772">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="D772" s="2">
-        <v>45861.89454635836</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E772">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="F772" s="2">
-        <v>45861.70517361111</v>
+        <v>45867.40884259259</v>
       </c>
       <c r="G772">
         <v>0</v>
@@ -19483,16 +19486,16 @@
         <v>1</v>
       </c>
       <c r="C776">
-        <v>2285</v>
+        <v>2223</v>
       </c>
       <c r="D776" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E776">
-        <v>2285</v>
+        <v>2223</v>
       </c>
       <c r="F776" s="2">
-        <v>45866.64810185185</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G776">
         <v>0</v>
@@ -19561,16 +19564,16 @@
         <v>1</v>
       </c>
       <c r="C779">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="D779" s="2">
-        <v>45860.91580999861</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E779">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="F779" s="2">
-        <v>45860.40890046296</v>
+        <v>45867.53143518518</v>
       </c>
       <c r="G779">
         <v>0</v>
@@ -20256,16 +20259,16 @@
         <v>1</v>
       </c>
       <c r="C807">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D807" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E807">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F807" s="2">
-        <v>45866.634375</v>
+        <v>45867.76055555556</v>
       </c>
       <c r="G807">
         <v>0</v>
@@ -20556,16 +20559,16 @@
         <v>1</v>
       </c>
       <c r="C819">
-        <v>-21</v>
+        <v>79</v>
       </c>
       <c r="D819" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E819">
-        <v>-21</v>
+        <v>79</v>
       </c>
       <c r="F819" s="2">
-        <v>45866.634375</v>
+        <v>45867.64820601852</v>
       </c>
       <c r="G819">
         <v>0</v>
@@ -20732,16 +20735,16 @@
         <v>1</v>
       </c>
       <c r="C826">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="D826" s="2">
-        <v>45863.33292844877</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E826">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="F826" s="2">
-        <v>45862.44537037037</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G826">
         <v>0</v>
@@ -21389,16 +21392,16 @@
         <v>1</v>
       </c>
       <c r="C853">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D853" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E853">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F853" s="2">
-        <v>45866.40174768519</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G853">
         <v>0</v>
@@ -21868,16 +21871,16 @@
         <v>1</v>
       </c>
       <c r="C872">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="D872" s="2">
-        <v>45856.2770322055</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E872">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="F872" s="2">
-        <v>45855.69381944444</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G872">
         <v>0</v>
@@ -22653,16 +22656,16 @@
         <v>1</v>
       </c>
       <c r="C903">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D903" s="2">
-        <v>45847.81154045185</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E903">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F903" s="2">
-        <v>45757.50258101852</v>
+        <v>45867.40572916667</v>
       </c>
       <c r="G903">
         <v>0</v>
@@ -23187,16 +23190,16 @@
         <v>1</v>
       </c>
       <c r="C924">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="D924" s="2">
-        <v>45863.33292844877</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E924">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="F924" s="2">
-        <v>45862.42978009259</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G924">
         <v>0</v>
@@ -23213,16 +23216,16 @@
         <v>1</v>
       </c>
       <c r="C925">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D925" s="2">
-        <v>45860.36531218661</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E925">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F925" s="2">
-        <v>45859.61006944445</v>
+        <v>45867.42921296296</v>
       </c>
       <c r="G925">
         <v>0</v>
@@ -23874,16 +23877,16 @@
         <v>1</v>
       </c>
       <c r="C951">
-        <v>13</v>
+        <v>-187</v>
       </c>
       <c r="D951" s="2">
-        <v>45847.81175720668</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E951">
-        <v>13</v>
+        <v>-187</v>
       </c>
       <c r="F951" s="2">
-        <v>45756.50815972222</v>
+        <v>45867.53143518518</v>
       </c>
       <c r="G951">
         <v>0</v>
@@ -24162,16 +24165,16 @@
         <v>1</v>
       </c>
       <c r="C963">
-        <v>1378</v>
+        <v>1368</v>
       </c>
       <c r="D963" s="2">
-        <v>45863.33292844877</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E963">
-        <v>1378</v>
+        <v>1368</v>
       </c>
       <c r="F963" s="2">
-        <v>45862.47730324074</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G963">
         <v>0</v>
@@ -24390,16 +24393,16 @@
         <v>1</v>
       </c>
       <c r="C972">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D972" s="2">
-        <v>45856.2770322055</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E972">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="F972" s="2">
-        <v>45855.69512731482</v>
+        <v>45867.44495370371</v>
       </c>
       <c r="G972">
         <v>0</v>
@@ -25533,16 +25536,16 @@
         <v>1</v>
       </c>
       <c r="C1017">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D1017" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1017">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F1017" s="2">
-        <v>45863.66303240741</v>
+        <v>45867.4334375</v>
       </c>
       <c r="G1017">
         <v>0</v>
@@ -26321,16 +26324,16 @@
         <v>1</v>
       </c>
       <c r="C1048">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1048" s="2">
-        <v>45847.81177677388</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1048">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1048" s="2">
-        <v>45829.55180555556</v>
+        <v>45867.4334375</v>
       </c>
       <c r="G1048">
         <v>0</v>
@@ -26347,16 +26350,16 @@
         <v>1</v>
       </c>
       <c r="C1049">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D1049" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1049">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F1049" s="2">
-        <v>45866.67512731482</v>
+        <v>45867.65412037037</v>
       </c>
       <c r="G1049">
         <v>0</v>
@@ -26676,16 +26679,16 @@
         <v>1</v>
       </c>
       <c r="C1062">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D1062" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1062">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="F1062" s="2">
-        <v>45866.64810185185</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G1062">
         <v>0</v>
@@ -27867,16 +27870,16 @@
         <v>1</v>
       </c>
       <c r="C1110">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D1110" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1110">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="F1110" s="2">
-        <v>45866.64810185185</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G1110">
         <v>0</v>
@@ -28274,16 +28277,16 @@
         <v>1</v>
       </c>
       <c r="C1126">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D1126" s="2">
-        <v>45852.89547361292</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1126">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="F1126" s="2">
-        <v>45852.39138888889</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G1126">
         <v>0</v>
@@ -28805,16 +28808,16 @@
         <v>1</v>
       </c>
       <c r="C1147">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1147" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1147">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F1147" s="2">
-        <v>45866.54819444445</v>
+        <v>45867.70488425926</v>
       </c>
       <c r="G1147">
         <v>0</v>
@@ -28857,16 +28860,16 @@
         <v>1</v>
       </c>
       <c r="C1149">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D1149" s="2">
-        <v>45860.91583892083</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1149">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F1149" s="2">
-        <v>45860.76299768518</v>
+        <v>45867.44495370371</v>
       </c>
       <c r="G1149">
         <v>0</v>
@@ -29143,16 +29146,16 @@
         <v>1</v>
       </c>
       <c r="C1160">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1160" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1160">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1160" s="2">
-        <v>45866.00791666667</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G1160">
         <v>0</v>
@@ -30038,16 +30041,16 @@
         <v>1</v>
       </c>
       <c r="C1195">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1195" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1195">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F1195" s="2">
-        <v>45865.99628472222</v>
+        <v>45867.42921296296</v>
       </c>
       <c r="G1195">
         <v>0</v>
@@ -30734,16 +30737,16 @@
         <v>1</v>
       </c>
       <c r="C1222">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1222" s="2">
-        <v>45847.81179644933</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1222">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F1222" s="2">
-        <v>45835.76293981481</v>
+        <v>45867.54620370371</v>
       </c>
       <c r="G1222">
         <v>0</v>
@@ -32492,16 +32495,16 @@
         <v>1</v>
       </c>
       <c r="C1291">
-        <v>502</v>
+        <v>2</v>
       </c>
       <c r="D1291" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1291">
-        <v>502</v>
+        <v>2</v>
       </c>
       <c r="F1291" s="2">
-        <v>45865.93864583333</v>
+        <v>45867.7325</v>
       </c>
       <c r="G1291">
         <v>0</v>
@@ -33462,16 +33465,16 @@
         <v>1</v>
       </c>
       <c r="C1329">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1329" s="2">
-        <v>45861.89454635836</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1329">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F1329" s="2">
-        <v>45861.67886574074</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G1329">
         <v>0</v>
@@ -33540,16 +33543,16 @@
         <v>1</v>
       </c>
       <c r="C1332">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D1332" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1332">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F1332" s="2">
-        <v>45863.71251157407</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G1332">
         <v>0</v>
@@ -33791,16 +33794,16 @@
         <v>1</v>
       </c>
       <c r="C1342">
-        <v>1277</v>
+        <v>1263</v>
       </c>
       <c r="D1342" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1342">
-        <v>1277</v>
+        <v>1263</v>
       </c>
       <c r="F1342" s="2">
-        <v>45866.64810185185</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G1342">
         <v>0</v>
@@ -34865,13 +34868,13 @@
         <v>0</v>
       </c>
       <c r="D1384" s="2">
-        <v>45847.81159828727</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1384">
         <v>0</v>
       </c>
       <c r="F1384" s="2">
-        <v>45530.4959837963</v>
+        <v>45867.76094907407</v>
       </c>
       <c r="G1384">
         <v>0</v>
@@ -35018,16 +35021,16 @@
         <v>1</v>
       </c>
       <c r="C1390">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1390" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1390">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1390" s="2">
-        <v>45866.39070601852</v>
+        <v>45867.43670138889</v>
       </c>
       <c r="G1390">
         <v>0</v>
@@ -35581,16 +35584,16 @@
         <v>1</v>
       </c>
       <c r="C1412">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="D1412" s="2">
-        <v>45860.91583892083</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1412">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="F1412" s="2">
-        <v>45860.76325231481</v>
+        <v>45867.78262731482</v>
       </c>
       <c r="G1412">
         <v>0</v>
@@ -35616,7 +35619,7 @@
         <v>51</v>
       </c>
       <c r="F1413" s="2">
-        <v>45866.39070601852</v>
+        <v>45867.47743055555</v>
       </c>
       <c r="G1413">
         <v>0</v>
@@ -35809,16 +35812,16 @@
         <v>1</v>
       </c>
       <c r="C1421">
-        <v>126</v>
+        <v>176</v>
       </c>
       <c r="D1421" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1421">
-        <v>126</v>
+        <v>176</v>
       </c>
       <c r="F1421" s="2">
-        <v>45866.634375</v>
+        <v>45867.53375</v>
       </c>
       <c r="G1421">
         <v>0</v>
@@ -35835,16 +35838,16 @@
         <v>1</v>
       </c>
       <c r="C1422">
-        <v>-14</v>
+        <v>22</v>
       </c>
       <c r="D1422" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1422">
-        <v>-14</v>
+        <v>22</v>
       </c>
       <c r="F1422" s="2">
-        <v>45866.634375</v>
+        <v>45867.64895833333</v>
       </c>
       <c r="G1422">
         <v>0</v>
@@ -35991,16 +35994,16 @@
         <v>1</v>
       </c>
       <c r="C1428">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D1428" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1428">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F1428" s="2">
-        <v>45863.68796296296</v>
+        <v>45867.42962962963</v>
       </c>
       <c r="G1428">
         <v>0</v>
@@ -36453,16 +36456,16 @@
         <v>1</v>
       </c>
       <c r="C1446">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D1446" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1446">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F1446" s="2">
-        <v>45863.66303240741</v>
+        <v>45867.44495370371</v>
       </c>
       <c r="G1446">
         <v>0</v>
@@ -36505,16 +36508,16 @@
         <v>1</v>
       </c>
       <c r="C1448">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="D1448" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1448">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="F1448" s="2">
-        <v>45866.634375</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G1448">
         <v>0</v>
@@ -37965,16 +37968,16 @@
         <v>1</v>
       </c>
       <c r="C1506">
-        <v>-4</v>
+        <v>14</v>
       </c>
       <c r="D1506" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1506">
-        <v>-4</v>
+        <v>14</v>
       </c>
       <c r="F1506" s="2">
-        <v>45866.56173611111</v>
+        <v>45867.64167824074</v>
       </c>
       <c r="G1506">
         <v>0</v>
@@ -37991,16 +37994,16 @@
         <v>1</v>
       </c>
       <c r="C1507">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D1507" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1507">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F1507" s="2">
-        <v>45863.68854166667</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G1507">
         <v>0</v>
@@ -38043,16 +38046,16 @@
         <v>1</v>
       </c>
       <c r="C1509">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D1509" s="2">
-        <v>45866.27545220916</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1509">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F1509" s="2">
-        <v>45863.6689699074</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G1509">
         <v>0</v>
@@ -40151,16 +40154,16 @@
         <v>1</v>
       </c>
       <c r="C1594">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D1594" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1594">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F1594" s="2">
-        <v>45866.56173611111</v>
+        <v>45867.4334375</v>
       </c>
       <c r="G1594">
         <v>0</v>
@@ -40229,16 +40232,16 @@
         <v>1</v>
       </c>
       <c r="C1597">
-        <v>11669</v>
+        <v>11606</v>
       </c>
       <c r="D1597" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1597">
-        <v>11669</v>
+        <v>11606</v>
       </c>
       <c r="F1597" s="2">
-        <v>45866.634375</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G1597">
         <v>0</v>
@@ -40304,16 +40307,16 @@
         <v>1</v>
       </c>
       <c r="C1600">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D1600" s="2">
-        <v>45847.81185513067</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1600">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F1600" s="2">
-        <v>45845.44905092593</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G1600">
         <v>0</v>
@@ -40936,16 +40939,16 @@
         <v>1</v>
       </c>
       <c r="C1625">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="D1625" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1625">
-        <v>-1</v>
+        <v>11</v>
       </c>
       <c r="F1625" s="2">
-        <v>45866.76775462963</v>
+        <v>45867.64342592593</v>
       </c>
       <c r="G1625">
         <v>0</v>
@@ -41709,16 +41712,16 @@
         <v>1</v>
       </c>
       <c r="C1656">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D1656" s="2">
-        <v>45861.89452460439</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1656">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F1656" s="2">
-        <v>45861.44936342593</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G1656">
         <v>0</v>
@@ -46414,16 +46417,16 @@
         <v>1</v>
       </c>
       <c r="C1844">
-        <v>708</v>
+        <v>688</v>
       </c>
       <c r="D1844" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1844">
-        <v>708</v>
+        <v>688</v>
       </c>
       <c r="F1844" s="2">
-        <v>45866.39487268519</v>
+        <v>45867.69244212963</v>
       </c>
       <c r="G1844">
         <v>0</v>
@@ -47052,16 +47055,16 @@
         <v>1</v>
       </c>
       <c r="C1869">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D1869" s="2">
-        <v>45854.26774868267</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E1869">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F1869" s="2">
-        <v>45853.60497685185</v>
+        <v>45867.75194444445</v>
       </c>
       <c r="G1869">
         <v>0</v>
@@ -48498,16 +48501,16 @@
         <v>1</v>
       </c>
       <c r="C1926">
-        <v>-22</v>
+        <v>2</v>
       </c>
       <c r="D1926" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1926">
-        <v>-22</v>
+        <v>2</v>
       </c>
       <c r="F1926" s="2">
-        <v>45866.50738425926</v>
+        <v>45867.65579861111</v>
       </c>
       <c r="G1926">
         <v>0</v>
@@ -49851,16 +49854,16 @@
         <v>1</v>
       </c>
       <c r="C1980">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="D1980" s="2">
-        <v>45847.81185513067</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E1980">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="F1980" s="2">
-        <v>45845.78077546296</v>
+        <v>45867.44495370371</v>
       </c>
       <c r="G1980">
         <v>0</v>
@@ -51178,16 +51181,16 @@
         <v>1</v>
       </c>
       <c r="C2033">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2033" s="2">
-        <v>45856.2770322055</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E2033">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2033" s="2">
-        <v>45855.68418981481</v>
+        <v>45867.65923611111</v>
       </c>
       <c r="G2033">
         <v>0</v>
@@ -54871,16 +54874,16 @@
         <v>1</v>
       </c>
       <c r="C2180">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D2180" s="2">
-        <v>45847.8118756755</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E2180">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F2180" s="2">
-        <v>45846.42060185185</v>
+        <v>45867.40572916667</v>
       </c>
       <c r="G2180">
         <v>0</v>
@@ -61115,7 +61118,7 @@
         <v>0</v>
       </c>
       <c r="F2428" s="2">
-        <v>45839.67329861111</v>
+        <v>45867.6462962963</v>
       </c>
       <c r="G2428">
         <v>0</v>
@@ -62400,16 +62403,16 @@
         <v>1</v>
       </c>
       <c r="C2481">
-        <v>817</v>
+        <v>797</v>
       </c>
       <c r="D2481" s="2">
-        <v>45867.31615610872</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E2481">
-        <v>817</v>
+        <v>797</v>
       </c>
       <c r="F2481" s="2">
-        <v>45866.634375</v>
+        <v>45867.44495370371</v>
       </c>
       <c r="G2481">
         <v>0</v>
@@ -62426,16 +62429,16 @@
         <v>1</v>
       </c>
       <c r="C2482">
-        <v>1298</v>
+        <v>1243</v>
       </c>
       <c r="D2482" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E2482">
-        <v>1298</v>
+        <v>1243</v>
       </c>
       <c r="F2482" s="2">
-        <v>45866.56369212963</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G2482">
         <v>0</v>
@@ -62452,16 +62455,16 @@
         <v>1</v>
       </c>
       <c r="C2483">
-        <v>1389</v>
+        <v>1364</v>
       </c>
       <c r="D2483" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E2483">
-        <v>1389</v>
+        <v>1364</v>
       </c>
       <c r="F2483" s="2">
-        <v>45865.95275462963</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G2483">
         <v>0</v>
@@ -62478,16 +62481,16 @@
         <v>1</v>
       </c>
       <c r="C2484">
-        <v>2393</v>
+        <v>2348</v>
       </c>
       <c r="D2484" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E2484">
-        <v>2393</v>
+        <v>2348</v>
       </c>
       <c r="F2484" s="2">
-        <v>45866.56173611111</v>
+        <v>45867.68675925926</v>
       </c>
       <c r="G2484">
         <v>0</v>
@@ -66285,16 +66288,16 @@
         <v>1</v>
       </c>
       <c r="C2640">
-        <v>18720</v>
+        <v>180</v>
       </c>
       <c r="D2640" s="2">
-        <v>45860.36533241235</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E2640">
-        <v>18720</v>
+        <v>180</v>
       </c>
       <c r="F2640" s="2">
-        <v>45859.75748842592</v>
+        <v>45867.7325</v>
       </c>
       <c r="G2640">
         <v>0</v>
@@ -66319,6 +66322,9 @@
       <c r="E2641">
         <v>0</v>
       </c>
+      <c r="F2641" s="2">
+        <v>45867.74561342593</v>
+      </c>
       <c r="G2641">
         <v>0</v>
       </c>
@@ -66334,16 +66340,16 @@
         <v>1</v>
       </c>
       <c r="C2642">
-        <v>7416</v>
+        <v>0</v>
       </c>
       <c r="D2642" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E2642">
-        <v>7416</v>
+        <v>0</v>
       </c>
       <c r="F2642" s="2">
-        <v>45865.9516087963</v>
+        <v>45867.7325</v>
       </c>
       <c r="G2642">
         <v>0</v>
@@ -66360,16 +66366,16 @@
         <v>1</v>
       </c>
       <c r="C2643">
-        <v>7416</v>
+        <v>0</v>
       </c>
       <c r="D2643" s="2">
-        <v>45866.27547163953</v>
+        <v>45868.26747174406</v>
       </c>
       <c r="E2643">
-        <v>7416</v>
+        <v>0</v>
       </c>
       <c r="F2643" s="2">
-        <v>45865.95298611111</v>
+        <v>45867.7325</v>
       </c>
       <c r="G2643">
         <v>0</v>
@@ -66798,16 +66804,16 @@
         <v>1</v>
       </c>
       <c r="C2661">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="D2661" s="2">
-        <v>45867.31613801513</v>
+        <v>45868.26744750624</v>
       </c>
       <c r="E2661">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="F2661" s="2">
-        <v>45866.40174768519</v>
+        <v>45867.63637731481</v>
       </c>
       <c r="G2661">
         <v>0</v>

</xml_diff>